<commit_message>
A bunch of new data and api changes.
</commit_message>
<xml_diff>
--- a/Data/Podaci.xlsx
+++ b/Data/Podaci.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/domagojrunjak/Documents/Zavrsni rad/zavrsni-rad/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D537FB7-6BD6-664A-9128-1173766D4175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E290B8D3-52F3-634D-99B1-47620705B65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3100" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-3100" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Županije" sheetId="1" r:id="rId1"/>
     <sheet name="Država" sheetId="2" r:id="rId2"/>
+    <sheet name="Hrvatska povijest" sheetId="3" r:id="rId3"/>
+    <sheet name="Gradovi" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="258">
   <si>
     <t>Naziv županije</t>
   </si>
@@ -336,18 +338,830 @@
     <t>Klima u unutrašnjosti Hrvatske je umjereno kontinentalna, u gorskoj Hrvatskoj pretplaninska i planinska, u primorskom dijelu mediteranska (sa suhim i toplim ljetima te vlažnim i blagim zimama), a u zaleđu submediteranska (s nešto hladnijim zimama i toplijim ljetima).
 S prosječno 2.600 sunčanih sati u godini jadranska je obala jedna od najsunčanijih u Sredozemlju, a prosječna temperatura mora ljeti je od 25 °C do 27 °C, što Hrvatsku čini turistički atraktivnom lokacijom.</t>
   </si>
+  <si>
+    <t>Kameno doba</t>
+  </si>
+  <si>
+    <t>Metalno doba</t>
+  </si>
+  <si>
+    <t>Doba Grka, Ilira i Rimljana</t>
+  </si>
+  <si>
+    <t>Dolazak Hrvata</t>
+  </si>
+  <si>
+    <t>Hrvatsko Kraljevstvo</t>
+  </si>
+  <si>
+    <t>Personalna unija s Ugarskom</t>
+  </si>
+  <si>
+    <t>Ratovi s Osmanlijama</t>
+  </si>
+  <si>
+    <t>Habsburška monarhija</t>
+  </si>
+  <si>
+    <t>Hrvatski narodni preporod</t>
+  </si>
+  <si>
+    <t>Prva Jugoslavija</t>
+  </si>
+  <si>
+    <t>Nezavisna država Hrvatska</t>
+  </si>
+  <si>
+    <t>SFR Jugoslavija</t>
+  </si>
+  <si>
+    <t>Neovisna Hrvatska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na prostoru Hrvatske je otkriveno pedesetak nalazišta čovjeka kamenog doba. U pećini Šandalja I u blizini Pule pronađeni su najstariji predmeti oblikovani rukom na tlu Hrvatske. Izrađeni su od kamena, a obrađeni okresivanjem. Najvažnije nalazište otkrio je Dragutin Gorjanović-Kramberger 1899. godine u spilji na Hušnjakovom brdu kraj Krapine gdje je našao ostatke neandertalskog čovjeka i njegova oruđa. Nalazišta krapinskog pračovjeka jedno je od najvažnijih u Europi. Živio je oko 130 tisuća godina prije Krista.
+Ljudi mlađeg kamenog doba na prostoru Hrvatske su živjeli u plodnim nizinama rijeka i uz Jadransko more. Prema prostoru najvažnijih nalazišta razlikujemo četiri kulture. Starčevačka kultura se prostirala dijelom sjeverne Hrvatske, a nositelji su ratari i stočari koji su živjeli u sojenicama i proizvodili keramiku koju su bojali crvenom bojom. Sopotska kultura prostirala se na prostoru Slavonije. Danilska kultura se prostirala uz obale Jadrana. Hvarska kultura se prostirala južnim dalmatinskim otocima. Danilska i Hvarska kultura pripadaju krugu impresso keramike koja se odlikuje posudama crveno smeđe boje ukrašenima otiscima školjaka, morskim puževa i zarezima učinjenim oštrim predmetima. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na prijelazu iz mlađeg kamenog u metalno doba na prostoru Srijema i Slavonije prostirala se Vučedolska kultura. Na prostoru kraj Dunava pronađena su kuće pravokutnog oblika, oružje od glačanog kamena te kalupi za lijevanje bakrenih sjekira. Glasovit je nalaz posude u obliku ptice poznat pod nazivom Vučedolska golubica. Najvažnija kultura ranog brončanog doba na tlu kontinentalne Hrvatske je vinkovačka kultura, a na tlu južne Hrvatske cetinska kultura. Obje od njih, na različit način i u različitom obimu nastavljaju tradiciju vučedolske kulture. Ostala važnija nalazišta su Nezakcij u Istri, Donja Dolina na Savi i Ripač na Uni. U kasnom brončanom dobu proširila se sjevernom Hrvatskom kultura polja sa žarama, nazvana prema glinenim posudama u koje se polagao pepeo pokojnika, s nalazištima kraj Virovitice, Zagreba i Velike Gorice.
+U željeznom dobu pojavili su se prvi poznati narodi na hrvatskom tlu. Keltski narodi pojavili su se u IV. stoljeću prije Krista, a živjeli su na području sjeverno od Save i Kupe. Sa sobom su donijeli lončarsko kolo i umijeće kovanja novca. Od keltskih plemena na panonskom tlu treba spomenuti Skordiske i Tauriske. Iliri su živjeli na prostoru južno od Save, a najvažniji narodi su Histri, Liburni, Japodi, Delmati i Ardijejci. Oni su gradili kamene utvrde koje se nazivaju gradine. Stanovnici priobalja su bili poznati po brodograditeljskom i pomorskom umijeću. Poznati po gradnji brodova i gusarenju bili su Liburni. Male i brze lađe kojima su plovili zvale su se lembi. Rimljani su po liburnskome uzoru izgrađivali vlastite ratne brodove koje su prozvali liburne. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grci svoje kolonije na istočnim jadranskim obalama osnivaju krajem VI. stoljeća prije Krista. Prva naseobina je bila Korkira Melajna na Korčuli koji su osnovali stanovnici otoka Krfa. Sirakuški tiranin Dionizije Stariji osnovao je koloniju Issu na otoku Visu. U blizini Lumbarde na Korčuli je osnovana kolonija o čijem osnivanju svjedoči zapis Lumbardska psefizma. Stanovnici otoka Para osnovali su Far u Starom Gradu na Hvaru, a važne kolonije su i Tragurij u Trogiru i Epetij u Stobreču. Između kolonija i matičnog polisa razvijale su se snažne kulturne i trgovačke veze.
+Gusarenje ilirskih naroda dovelo ih je u sukob s Rimljanima koji su od kraljice Teute tražili da svojim podanicima zabrani gusarenje, no ona je to odbila. Rimljani pokreću tri ilirska rata kojima uništavaju Ilirsko kraljevstvo koje je 167. godine prije Krista podijeljeno na tri oblasti pod vrhovnom rimskom vlašću. Konačno osvajanje završeno tek početkom prvog stoljeća.
+Tada je uspostavljena granica na Dunavu, a jedinstveni Ilirik je podijeljen na dvije rimske provincije Panoniju i Dalmaciju. Ilirske provincije zbog zemljopisnog položaja i prirodnih bogatstava ubrajale su se u važnije pokrajine Carstva. Najstarije kolonije u Dalmaciji bile su Salona, sjedište rimskog namjesnika i gospodarsko središte, Narona kao trgovačko i lučko središte te Jadera i Pola. U Panonija najvažnije su bile Siscija i Sirmij. Jedan od najvažnijih rimskih spomenika uopće je palača cara Dioklecijana podignuta nedaleko Salone. Pulski amfiteatar bio je jedan od najvećih u Carstvu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hrvati su narod koji je doselio u područje današnje Hrvatske tijekom sedmog stoljeća. Pitanje etnogeneze Hrvata je još otvoreno, a najpopularnije teorije o podrijetlu Hrvata su slavenska, iranska i gotska teorija. Tijekom seobe Hrvati su se dijelili na nekoliko plemena. Nakon dolaska i dugotrajnih borbi Hrvati su pobijedili Avare i zavladali njihovom zemljom. Prostor koji su naselili nalazio se između rijeke Drave i obala Jadranskog mora. Starosjedilačko romansko stanovništvo preseljava u priobalne utvrđene gradove pod bizantskom vlašću i u nepristupačne planinke krajeve Dinarida. To stanovništvo će se tijekom stoljeća pojaviti u nizinama pod imenom Vlasi. Kad su došli u novu domovinu Hrvati su bili mnogobošci. U dodiru s kršćanskim starosjediocima polako prihvaćaju kršćanstvo. Ulogu u pokrštavanju imali su Bizantski i franački misionari te benediktinci koji donose zapadne kulturne utjecaje.
+Na području Hrvatske Slaveni organiziraju nekoliko malih državnih zajednica – sklavinija, od kojih su najvažnije kneževina Hrvatska u priobalju i Donja Panonija. Prvi vladar koji je u svoj vladarski naslov stavio hrvatsko ime i koji sebe u darovnici iz 852. godine sebe naziva milošću Božjom knez Hrvata je Trpimir I., osnivač narodne dinastije Trpimirovića. Knez Branimir o svom dolasku na vlast u pismu obavještava papu Ivana VIII. U uzvratnom pismu od 21. svibnja 879. godine papa obavještava Branimira da je blagoslovio njega, njegov narod i državu, što je ustvari prvo međunarodno priznanje neovisnosti Hrvatske. Kameni ulomak iz šopota kraj Benkovca spominje Branimira kao kneza Hrvata, i to je najstariji kameni zapis hrvatskog imena. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nakon razdoblja vladanja hrvatskih knezova prvi kralj Hrvatske postaje Tomislav iz loze Trpimirovića oko 925. godine. Tomislav, koji je vojno porazio Mađare i kao bizantski saveznik potukao bugarsku vojsku, ujedinio je Posavsku i Primorsku Hrvatsku i stvorio državu znatne veličine. Na upravu je dobio i bizantsku Dalmaciju. Po podacima iz zapisa bizantskog cara Konstantina Porfirogeneta koji su očito pretjerani saznajemo da je hrvatska vojna moć u X. stoljeću zasigurno bila velika. Stjepan Držislav postaje prvi hrvatski okrunjeni kralj s titulom kralj Hrvatske i Dalmacije.
+Srednjovjekovno hrvatsko kraljevstvo doseglo je vrhunac pod kraljevima Petrom Krešimirom IV. (1058. – 1074.) i Dmitrom Zvonimirom (1075. – 1089.). Petar Krešimir pod svoju je upravu stavio dalmatinske gradove, Slavoniju te pripojio Neretvansku kneževinu i dijelove Bosne. Zvonimir je od legata tadašnjeg pape Grgura VII. Gebizona 1075. godine u crkvi u Solinu okrunjen za kralja Hrvatske i Dalmacije. Iz tog vremena potječe Bašćanska ploča prvi dokument zapisan na hrvatskom jeziku na glagoljici. </t>
+  </si>
+  <si>
+    <t>Hrvati su 1102. godine Pactom Conventom izabrali ugarskoga kralja Kolomana Arpadovića za kralja Hrvatske. Otada su Hrvatska i Ugarska bile povezane osobom vladara sve do 1918. godine. Takvu vrstu državne zajednice nazivamo personalna unija. Kralj Ladislav je 1094. godine osnovao biskupiju u Zagrebu, a prvi biskup je bio češki redovnik Duh. Tijekom stoljeća vode se obrambeni ratovi s Venecijom koja pokušava zavladati hrvatskom obalom Jadrana. Uz pomoć križarske vojske 1202. osvojen je Zadar. Slabljenjem središnje kraljeve vlasti, kralj Andrija II. prisiljen je 1222. godine sazvati državni sabor i donijeti Zlatnu bulu, dokument kojim ograničava svoju vlast u korist plemstva. Započinje uspon velikaških obitelji od kojih su najvažniji Frankapani i Šubići. Vrhunac moći Šubići doživljavaju oko 1300. godine kada Pavao I. nosi naslov ban Hrvata i gospodar Bosne.
+Vinodolski zakonik iz 1288. godine najstariji je sačuvani zakonik napisan na hrvatskom jeziku. Osnivaju se brojni slobodni kraljevski gradovi koji od kralja dobivaju samoupravu, najrazvijeniji je Gradec kraj biskupskog Zagreba. Krunidbom Karla Roberta na prijestolje stupa nova dinastija Anžuvinaca. Ludovik I. uspostavlja jaku kraljevsku vlast slamanjem moći velikaša i provođenjem brojnih gospodarskih, poreznih i vojnih reformi. U savezništvu s Genovom poražena je Mletačka Republika te se mirom u Zadru 1358. godine mletački dužd odriče svakog prava na Dalmaciju. Dubrovnik priznaje vlast hrvatsko-ugarskog kralja te se ubrzo počinje nazivati Republikom. U dinastičkim borbama na prijestolje dolazi Žigmund Luksemburški. Godine 1409. drugi pretendent na prijestolje Ladislav Napuljski prodaje mletačkom duždu za 100 000 dukata svoja kraljevska prava na Dalmaciju (tj. Zadar s utvrdom i zadarskim kotarom, otok Pag, dvije utvrde u hrvatskom zaleđu, Novigrad i Vranu, ali i sva prava na cijelu Dalmaciju, što znači i one njezine dijelove koji su u tom času priznavali Sigismundovu vlast.).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tijekom Žigmundove vladavine po prvi puta Hrvatskoj prijeti osmanska opasnost. Organizira se obrambeni sustav osnivanjem hrvatskog, slavonskog i usorskog tabora koji se nakon Žigmundove smrti pokazuje neuspješnim. Padom Bosne 1463. godine pod Osmansku vlast Matija Korvin osniva Srebreničku i Jajačku banovinu. Osmanlije su 1493. godine teško porazile hrvatsku plemićku vojsku na Krbavskom polju. Hrvatski ban i biskup Petar Berislavić uspješno brani Hrvatsku. Knez Bernardin Frankapan na njemačkom državnom saboru u Nürnbergu poziva na pomoć Hrvatskoj nazivajući je štitom kršćanstva. Bernardinov sin Krsto spada među najznačajnije hrvatske srednjovjekovne vojskovođe. Porazom na Mohačkom polju 1526. godine od osmanskog sultana Sulejmana I. ugasila se srednjovjekovna hrvatsko-ugarska država. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na saboru u Cetingradu 1527. godine hrvatsko je plemstvo izabralo Ferdinanda Habsburškog za hrvatskog kralja. Time je Hrvatska ušla u personalnu uniju sa zemljama Habsburške Monarhije. Time je čuvana svijest o zasebnosti Hrvatskog kraljevstva. Junaštvom se proslavio Nikola Jurišić koji je obranio Kiseg od premoćne osmanske vojske i tako obranio Beč od osvajanja. Osmanlije su krenule u novi pohod na Beč 1566. godine predvođeni Sulejmanom Veličanstvenim i velikim vezirom Mehmed-pašom Sokolovićem. U Opsadi Sigeta nakon junačkog otpora, braneći grad od 100.000 osmanskih vojnika, pogiba Nikola Šubić Zrinski jedan od najvećih velikana u hrvatskoj povijesti. Kardinal Richelieu bitku kod Sigeta je nazvao bitkom koja je spasila civilizaciju. Godine 1592. pada važna utvrda Bihać, a nekada slavno Hrvatsko Kraljevstvo je svedeno na ostatke ostataka, a hrvatske zemlje su pogođene snažnim iseljavanjem stanovništva. Godine 1558. Hrvatski i Slavonski sabor spojili su se u jedinstveni Hrvatski sabor.
+Osmanlije 1593. godine doživljavaju poraz u bitki kod Siska. Osniva se Vojna Krajina, sustav obrambenih utvrda pod zapovjedništvom Dvorskog ratnog vijeća. Najvažnija utvrda je Karlovac. Na opustošenu zemlju naseljava se vlaško stanovništvo. Zbog zasluga u obrani Hrvatske pripadnici starih hrvatskih obitelji Zrinski i Frankapani nazivaju se skrbnicima i zaštitnicima Hrvatske. Nikola Zrinski pali veliki most kod Osijeka kojim su Osmanlije prodirale u Europu. Zbog sjajnih pobjeda odlikovali su ga i nagradili španjolski kralj Filip IV. i francuski kralj Luj XIV. Nezadovoljni centralističkom politikom bečkog dvora hrvatski i ugarski plemići pružaju otpor želeći samo otjerati Osmanlije uz pomoć zapadnoeuropskih sila, ponajprije Francuske. Vođe pobune Petar Zrinski i Fran Krsto Frankapan pogubljeni su u Bečkom Novom Mjestu 30. travnja 1671. godine. Time je skršen otpor hrvatskog plemstva, a posjedi Zrinskih i Frankapana došli su pod vlast Dvorske komore.
+Na osvojenim područjima provodi se islamizacija iako Osmanlije prihvaćaju činjenicu da dio pokorenih naroda pripada kršćanskoj vjeri. Pri tome su tolerantniji bili prema pravoslavnim crkvama nego prema katolicima jer je Katolička crkva često poticala zapadne države protiv Osmanlija. Jedino su franjevci mogli slobodno djelovati na području Osmanskog Carstva. Kršćani su morali plaćati visoke poreze tako da mnogi iseljavaju. Organizira se otpor koji pružaju hajduci i uskoci. 
+Jedini dio hrvatskoga prostora koji se samostalno razvijao bila je Dubrovačka Republika koja je s 200 brodova imala jednu od najvećih trgovačkih mornarica u Europi. Isusovac Bartol Kašić piše 1604. godine prvu gramatiku hrvatskog jezika. Isusovci osnivaju 1607. godine gimnaziju u Zagrebu. Kralj Leopold I. dodijelio joj je naslov akademije čime je osnovano Sveučilište u Zagrebu, najstarije sveučilište s neprekinutim djelovanjem u Jugoistočnoj Europi. Najvažniji hrvatski barokni književnik Ivan Gundulić djeluje u Dubrovniku, a povjesničar Ivan Lučić spada u sam vrh europske povijesne znanosti sedamnaestog stoljeća. </t>
+  </si>
+  <si>
+    <t>Oslobađanje Hrvatske od Osmanlija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nakon pobjede nad Osmanlijama kod Beča 1683. godine organizira se Sveta liga, savez Habsburške Monarhije, Mletačke Republike i Poljske. Oslobađanje Slavonije organizira franjevac Luka Ibrišimović, a u Lici otpor organizira Marko Mesić. Mirom u Srijemskim Karlovcima 1699. godine velik dio hrvatskog prostora je oslobođen vlasti Osmanlija. Ipak oslobođeni prostor je postao dio Vojne Krajne. Mir u Požarevcu 1718. godine označio je kraj vojne opasnosti od Osmanskog Carstva. Hrvatski sabor 1712. godine prihvaća Pragmatičku sankciju. Provodi se plansko naseljavanje s kojim u Hrvatsku dolaze Nijemci, Česi, Slovaci i Srbi.
+Marija Terezija provodi brojne upravne, porezne i vojne reforme. Osniva se Hrvatsko kraljevsko vijeće 1767. godine, prva moderna vlada. Za vrijeme cara Josipa II. provodi se snažna germanizacija pa se hrvatsko plemstvo okreće suradnji s ugarskim. Na zajedničkom Ugarskom saboru 1790. godine od hrvatske je strane predložena veća financijska ovisnost te podvrgnost Ugarskom kraljevskom vijeću što su Mađari oduševljeno prihvatili. U to vrijeme nastaje ideja o jedinstvenoj mađarskoj nacionalnoj državi od Karpata do Jadrana kao odgovor na germanizaciju Beča u kojoj bi mađarski jezik postao službeni za sve. Hrvatski izaslanici na Saboru odlučno odbijaju uvođenje mađarskog jezika kao službenog. Po prvi puta izbio je spor oko jezika koji će se u sljedećem stoljeću smatrati glavnim obilježjem nacije. Požunskim mirom 1805. godine hrvatska obala dolazi pod francusku vlast te su organizirane Ilirske pokrajine. Na Bečkom kongresu 1815. godine Dalmacija i Istra dolaze pod austrijsku vlast ali nisu sjedinjene s ostatkom Hrvatske. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Razjedinjenost hrvatskih zemalja pokazao je osnovni cilj hrvatske politike u 19. stoljeću – ujedinjenje hrvatskih krajeva u jedinstvenu cjelinu. Zagrebački biskup Maksimilijan Vrhovac pomaže pretpreporodne napore. Ljudevit Gaj stvara krug građanskih intelektualaca koji postaje jezgra kulturnog i nacionalnog preporoda Hrvatske. Pripadnici tog pokreta nazivaju se ilircima, a pokret se naziva Ilirskim pokretom. Grof Janko Drašković piše Disertaciju, prvi hrvatski politički program. U Zagrebu 1835. godine počinju izlaziti Novine horvatske. Objavljena je pjesma Horvatska domovina Antuna Mihanovića koja će poslije postati hrvatska himna. Matica ilirska osnovana je 1842. godine. Ivan Kukuljević Sakcinski održava 1843. godine u Hrvatskom saboru prvi zastupnički govor na hrvatskom jeziku. Srpanjske žrtve svečano su pokopane 1845. godine. Hrvatski sabor jednoglasno je 1847. godine proglasio hrvatski jezik službenim.
+Revolucionarne 1848. godine formulirana su Zahtijevanja naroda. Hrvatskim banom postaje Josip Jelačić. U Hrvatskoj je 25. travnja 1848. godine ukinuto kmetstvo. Osnovano je Bansko vijeće te je sazvan prvi zastupnički Sabor u hrvatskoj povijesti. Jelačić je s hrvatskom vojskom prešao Dravu i zaratio s Mađarima. Nakon revolucije 1849. godine Franjo Josip proglašava oktroirani Ustav. Započeta je snažna germanizacija. Na Saboru 1861. godine grupiraju se političke stranke: Narodna stranka, Stranka prava i Unionistička stranka. </t>
+  </si>
+  <si>
+    <t>Hrvatsko-ugarska nagodba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hrvatsko-ugarska nagodba sklopljena je 1868. godine kojom su uređena zajednička pitanja, a prevagnuli su mađarski interesi. Ugarska je priznala Kraljevini Hrvatskoj položaj političkog naroda i teritorijalnu cjelokupnost. Hrvatska je slala zastupnike u Ugarski sabor te je bila financijski oštećena i podređena Ugarskoj. Riječkom krpicom Rijeka dolazi pod mađarsku vlast. Propala je Kvaternikova Rakovička buna. U ovom razdoblju djeluje Ante Starčević, otac domovine. U Dalmaciji se vodi politička borba narodnjaka i autonomaša. U Istri djeluje Juraj Dobrila. Banom postaje Ivan Mažuranić koji provodi modernizaciju zemlje. Godine 1874. godine utemeljeno je moderno Sveučilište u Zagrebu. Godine 1881. Vojna Krajina je sjedinjena s ostatkom Hrvatske. Dolaskom na vlast bana Khuen-Hédervárya 1883. godine sljedećih dvadeset godina provodi se jaka mađarizacija. Srpska manjina dobiva privilegirani položaj. Održani su veliki protumađarski prosvjedi 1903. godine. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nakon Prvog svjetskog rata i raspada Austro-Ugarske, Hrvatska je ušla u Kraljevinu Srba, Hrvata i Slovenaca. Istra, Rijeka i Zadar potpali su pod talijansku vlast. Kraljevina SHS je 1929. godine preimenovana u Kraljevinu Jugoslaviju. Godine 1939. osniva se samoupravna banovina Hrvatska. </t>
+  </si>
+  <si>
+    <t>Za vrijeme Drugoga svjetskog rata dio današnjega područja Republike Hrvatske bio je unutar granica Nezavisne Države Hrvatske (1941. – 1945.). Hrvatski narod isprva je podržavao ustašku vlast, no došlo je do progona Srba koje Hrvati kao katolici nisu mogli prihvatiti. Talijanski poglavar Mussolini želio se domoći jadranske obale, zbog čega je prisilio poglavnika Antu Pavelića da mu je preda. Stoga su 18. svibnja potpisani Rimski ugovori kojima je Italija prisvojila većinu Jadrana, no Pavelić je uspio ograničiti njezine zahtjeve i spasiti dio hrvatske obale.[7] U to su doba Istra, Zadar, Cres, Lošinj, Lastovo i Rijeka nastavili biti dio Kraljevine Italije kojoj su pripali Rapalskim ugovorom nakon I. svjetskog rata; a vlasti NDH – koja je nastala upravo zauzimanjem Italije nakon raspada Kraljevine Jugoslavije u travnju 1941. godine - morale su Italiji prepustiti skoro sve hrvatske otoke, Split, Šibenik, Trogir i dio dalmatinskog zaleđa (5380 km2 ozemlja s oko 380.000 stanovnika te pretežni dio hrvatskog teritorijalnog mora). Međimurje i Baranju je sebi pripojila Kraljevina Mađarska; NDH nije priznala pripojenje Međimurja, ali nije imala ni načina da Mađarskoj oduzme to područje. NDH je ubrzo došla u loše odnose s Italijom, koja je u pojasu od linije Karlovac – Mostar praktično suspendirala vlast NDH i zabranila lociranje njenih oružanih snaga (na početku teg skromnog broja i snage), nastojeći kontrolirati to područje u suradnji s četnicima.
+Nakon kapitulacije Italije u rujnu 1943. godine su vlasti NDH u tim krajevima imale veću ulogu, ali samo onoliko koliko je to odgovaralo Njemačkoj, koja je privolila vodstvo NDH da dopusti novačenje hrvatskih vojnih obveznika u Wehrmacht i SS (pri čemu se iz proračuna NDH plaćalo troškove njemačkih postrojbi) te čak uspostavu Njemačke policije u Hrvatskoj, izravno odgovorne vlastima u Berlinu. Povijesno pravo hrvatskoga naroda na punu državnu suverenost izraženo Ustavom Republike Hrvatske temelji se među ostalim i na odlukama ZAVNOH-a izraženim nasuprot proglašenju NDH.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snažan partizanski pokret i paralelna narodna vlast na oslobođenim područjima te oslobađanje vlastitim snagama dovode do toga da je nakon rata Hrvatska postala dio nove, socijalističke Jugoslavije.
+Krajem 1960-ih godina javljaju se zahtjevi za razvlaštenje federalne vlasti, jačanje tržišne privrede te se kritiziraju unitarističke i centralističke tendencije u Jugoslaviji. Višegodišnja kretanja prerastaju u pravi nacionalni pokret čija su središta Matica hrvatska, studenti te mlađi komunistički političari u Centralnom komitetu KPH od kojih su najpoznatiji Miko Tripalo i Savka Dabčević-Kučar. Pokret se posebno proširio do proljeća 1971. godine pa je i nazvan Hrvatsko proljeće. Širenje pokreta izaziva kritike u drugim jugoslavenskim republikama te Josip Broz Tito smjenjuje hrvatski politički vrh. Ipak ustavnim promjenama, a osobito donošenjem Ustava 1974. godine snažno je ojačan republički individualitet.
+Titovom smrću 1980. godine nestaje element koji je svojom karizmom i autoritetom osiguravao koheziju visoko složenog sustava prepunog različitosti unutar Jugoslavije. Početak teške političke kriza prati gospodarska kriza, nastala sudarom tržišnih elemenata i elemenata planske privrede te afirmacija nacionalnih interesa. Radikalizacija zahtjeva u Srbiji koja na političko vodstvo dovodi Slobodana Miloševića dovodi do raspada SKJ. Krajem osamdesetih godina počinju se osnivati političke stranke te se priznaje višestranački sustav. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na prvim cišestranačkim izborima 1990. premoćnu pobjedu ostvaruje HDZ predvođen Franjom Tuđmanom te se 30. svibnja konstituira višestranački Hrvatski sabor. Novi Ustav Republike Hrvatske od 22. prosinca 1990. (poznat i kao Božićni Ustav) više nije bio ustav jedne komunističke države, a iz naziva se izbacuje naznaka Socijalistička: od tada ime države glasi: Republika Hrvatska. Na Referendumu o hrvatskoj samostalnosti održanom 19. svibnja 1991. većina od 93,24 % birača opredjeljuje se za samostalnu i neovisnu državu. Slijedom te odluke Sabor je 25. lipnja 1991. donio Ustavnu odluku o suverenosti i samostalnosti Republike Hrvatske kojim se Hrvatska uspostavlja kao neovisna država. Neuspjehom u rješavanju jugoslavenske krize 8. listopada 1991. raskida sve državnopravne sveze s dosadašnjom SFRJ.
+Oružanom pobunom dijela srpskog stanovništva počinje Domovinski rat, koji je završio 1995. hrvatskom pobjedom u operaciji Oluja. Hrvatska je 22. svibnja 1992. primljena u Ujedinjene narode kao punopravni član. Drugu polovicu devedesetih karakterizira loša gospodarska situacija uzrokovana prelaskom na tržišno gospodarstvo, netransparentnom privatizacijom i posljedicama rata. Na parlamentarnim izborima 2000. pobjeđuje koalicija šest stranaka u koju su uključeni SDP, HSLS, HSS, HNS, LS i IDS. Premijer je Ivica Račan. Stjepan Mesić je izabran za predsjednika 2000., a reizabran 2005.. Na vlast 2003. dolazi reformirani HDZ predvođen Ivom Sanaderom koji osvaja drugi mandat kao premijer nakon pobjede na izborima 2007. Razdoblje nakon 2000. karakterizira razvoj i rast gospodarstva do svjetske recesije 2008. godine.
+Još od svog osamostaljenja glavni vanjskopolitički ciljevi Republike Hrvatske bili su ulazak u euroatlantske integracije, prije svega ulazak u Europsku uniju i NATO. Od 1. travnja 2009. članica je NATO-a, dok je 3. listopada 2005. Hrvatska započela pristupne pregovore za ulazak u Europsku uniju. Hrvatska je postala 28. članica Europske unije 1. srpnja 2013. 
+Od 1. siječnja 2023. službena valuta u Hrvatskoj postao je euro. Istoga dana Hrvatska je i službeno postala članica Schengenskoga prostora. </t>
+  </si>
+  <si>
+    <t>Naziv grada</t>
+  </si>
+  <si>
+    <t>Odredišna pošta</t>
+  </si>
+  <si>
+    <t>Pozivni broj</t>
+  </si>
+  <si>
+    <t>Županija</t>
+  </si>
+  <si>
+    <t>10000 Zagreb</t>
+  </si>
+  <si>
+    <t>Registracijska oznaka</t>
+  </si>
+  <si>
+    <t>Zemljopisna širina</t>
+  </si>
+  <si>
+    <t>Zemljopisna visina</t>
+  </si>
+  <si>
+    <t>45.8</t>
+  </si>
+  <si>
+    <t>15.97</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>46.16</t>
+  </si>
+  <si>
+    <t>15.87</t>
+  </si>
+  <si>
+    <t>44000 Sisak</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>Na području grada Siska pratimo kontinuitet urbanog življenja više od dvije tisuće godina tijekom kojih je grad proživljavao burne trenutke uspona i padova. Prostori današnjih sisačkih ulica mijenjali su svoj izgled prateći promjene kultura i civilizacija, stilova i načina života svojih stanovnika. Temelji planske koncepcije razvoja Siska, najuočljiviji u njegovoj najužoj povijesnoj jezgri, skriveni su u nestalom gradu ispod živog grada. Jedan je od rijetkih europskih gradova kod kojega uz kontinuitet trajanja naselja možemo pratiti i kontinuitet njegovog naziva: Segesta, Segestica, iz predrimskog razdoblja, Siscia u vrijeme Rimskog Carstva, Siscium u ranom srednjem vijeku, Sissek, Sziszek, Sciteck, Zysek, Sziscium, Scytzyc, Zitech, Scyteck, Sziszak, pa sve do hrvatskog naziva Sisak. Naseljen je od prapovijesnih vremena. Sojeničko naselje na desnoj obali Kupe poznato je od razdoblja starijeg željeznog doba. U razdoblju mlađeg željeznog doba poznat je i oppidum Segestica kojega 35. godine pr. Kr. osvaja budući rimski car Oktavijan. Novo naselje Siscia razvija se na lijevoj obali Kupe. Prvobitno postoji kao vojni logor koji se tijekom 1. st. razvija u civilno naselje koje je car Vespazijan 71. god. proglasio kolonijom. U Sisciji se tijekom 3. st. razvija ranokršćanska zajednica i biskupija. U posljednjim velikim progonima kršćana početkom 4. st. stradava siscijanski biskup Kvirin, danas štovan kao zaštitnik grada Siska. Tijekom 5. i 6. st. uslijed sve većeg priljeva barbara, nastavlja se propadanje Siscije, a kraj antičkog grada dogodio se oko 600. god. zauzimanjem Siscije od Avara i Slavena. Život se na ovim prostorima nastavlja, iako ne u dotadašnjem opsegu. Kneževina Ljudevita Posavskog, koja se prostirala u zapadnim dijelovima Panonske nizine, odigrala je bitnu ulogu u borbi protiv franačke vlasti na početku 9. st. Sisak je bio središte trogodišnjeg otpora Ljudevita Posavskog, a nakon iscrpljujućih borbi i njegovog povlačenja, grad potpada pod vlast Ludovika Njemačkog. O zbivanjima na ovim prostorima neko vrijeme nema pisanih podataka. Godine 928. spominjanjem na splitskom crkvenom saboru, potvrđuje se kako još uvijek postoji sisačka biskupija. Od godine 1215., zemaljski feudalni gospodar Siska i područja oko njega postaje Zagrebački kaptol i Sisak u njegovom vlasništvu ostaje do 19. stoljeća. Naselje egzistira kao mirno trgovačko i poljoprivredno središte sve do 16. st. i razdoblja bojeva s prodirućim osmanlijskim snagama. Sisak je postao najvažnija obrambena točka sjeverozapadnog dijela Hrvatske. Nakon brojnih pokušaja prodora, opsjeda i razaranja, godine 1593. godine, osmanlijske snage zaustavljene su u Sisku čime je onemogućen njihov prodor prema ostalim dijelovima Hrvatske, ali i srednje i zapadne Europe. Nakon iscrpljujućeg ratovanja slijede stoljeća oporavka a od 17. stoljeća započinje i ponovni nagli razvitak gradskog načina života. Oslobađanjem tradicionalnih trgovačkih putova, Sisak postaje značajna riječna luka, a vodeni transport pokretačka snaga razvoja grada.
+Grad se razvija uz obadvije obale rijeke Kupe: kao Vojni Sisak s desne i Civilni Sisak s lijeve obale. Oba naselja okrenuta su jedno prema drugom i istovremeno prema rijeci koja za njih znači život. Godine 1874., dva sisačka naselja ujedinjavaju se u jedinstveno gradsko središte koje dobiva status slobodnog kraljevskog grada. Započinje nagla urbanizacija; gradnja infrastrukture, uređenje ulica, trgova, gradnja brojnih objekata javne namjene. Razvojem trgovine, obrta i industrije, doseljavanjem sve većeg broja stanovništva, prometnom povezanošću, stvaraju se preduvjeti za uspon društvenog života grada. Na prijelazu 19. u 20. st. dolazi do stagnacije trgovine i obrta, a sve prisutnija mala industrijska postrojenja prerastaju u značajne industrijske pogone, uz koje se, van uže gradske jezgre, stvaraju industrijska predgrađa i nova stambena naselja, koja se svojim izgledom bitno razlikuju od stare gradske jezgre.
+Sisačka povijest promatrana kroz stoljeća, primjer je ponavljanja povijesnih iskustava. Dva su osnovna čimbenika diktirala razvoj Siska: vojni i gospodarstveni. Izmjenjujući se, oni su ga u pojedinim povijesnim razdobljima dovodili u središte pozornosti, da bi onda opet ostajao zaboravljen i prepušten sebi. Dokaz tomu su i događaji s kraja 20. stoljeća, kada se Sisak, po tko zna koji puta našao suočen s ratnim strahotama. Neizazvana agresija bez ikakvog moralnog opravdanja, obrušila se na grad i njegove stanovnike, ne vjerujući ono što je Sisak toliko puta u svojoj povijesti dokazao: on je ovdje, postoji i traje. Opstat će kao svjedok prošlosti i opstanka onih koji ovdje obitavaju stoljećima.</t>
+  </si>
+  <si>
+    <t>1869.</t>
+  </si>
+  <si>
+    <t>1880.</t>
+  </si>
+  <si>
+    <t>1890.</t>
+  </si>
+  <si>
+    <t>1910.</t>
+  </si>
+  <si>
+    <t>1921.</t>
+  </si>
+  <si>
+    <t>1948.</t>
+  </si>
+  <si>
+    <t>1953.</t>
+  </si>
+  <si>
+    <t>1971.</t>
+  </si>
+  <si>
+    <t>1981.</t>
+  </si>
+  <si>
+    <t>45.48</t>
+  </si>
+  <si>
+    <t>16.36</t>
+  </si>
+  <si>
+    <t>KA</t>
+  </si>
+  <si>
+    <t>45.5</t>
+  </si>
+  <si>
+    <t>15.54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karlovac je relativno mlado naselje kojem se zna točan datum nastanka - 13. srpnja 1579. godine. Po naredbi Karla II. Štajerskog, osnovan je kao tvrđava radi zaštite od turskih osvajanja, u ravnici na utoku Korane u Kupu, podno stare gradine Dubovac. Franz Vaniček navodi podatak da je tvrđava izgrađena na 900 turskih lubanja.[5] Ime je dobio po osnivaču, austrijskom nadvojvodi Karlu. Građen je po zamisli idealnog renesansnog grada u obliku šesterokrake zvijezde sa središnjim trgom i ulicama koje se sijeku pod pravim kutom.
+Od osnivanja do 1693. godine grad Karlovac bio je pod vojnom upravom, a tek tada dobiva ograničenu samoupravu. Slobodnim kraljevskim gradom postaje 1776. godine.
+Tijekom 18. i 19. stoljeća, ponajviše zahvaljujući procvatu trgovine i lađarstva Kupom, Karlovac je slovio za jedan od najbogatijih i najrazvijenijih hrvatskih gradova. O tome svjedoči i podatak kako su početkom 19. stoljeća upravo Karlovčani plaćali najveći porez od svih hrvatskih gradova. U Karlovcu je Stranka prava 13. travnja 1896. osnovala svoj ogranak.[6] Pokazala se uspješnom, jer od 1896. do 1920. godine, dala je Karlovcu četvoricu gradonačelnika (Josip Vrbanić, Ivan Banjavčić, Božidar Vinković i Gustav Modrušan).[6][7] U tom je razdoblju po industriji i izdavačkoj djelatnosti Karlovac bio među najznačajnijim gradovima u Hrvatskoj.[6]
+Grad Karlovac je u početku Domovinskog rata bio gotovo okupiran grad jer je u njemu i bližoj okolici tadašnja Jugoslavenska narodna armija (JNA) imala 19 vojnih objekata s raspoređenim vojnim snagama. Pravilnom i mudrom organizacijom otpora, sve vojarne u gradu i bližoj okolici su osvojene, a vojska iseljena iz grada, no taj proces nije prošao mirno. Najteže su trenutke grad i njegovi stanovnici proživljavali od sredine listopada 1991. do siječnja 1992. godine, kada su svakodnevno bili izloženi granatiranju. Osobito težak trodnevni napad s pokušajem osvajanja grada bio je 4. listopada, a grad je opet bio u velikoj neizvjesnosti kad je neprijateljska JNA uz pomoć pobunjenih Srba izvukla teško oružje i mehanizaciju iz vojarne u Logorištu. U razdoblju do siječnja 1992. poginulo je 255 ljudi, dok je više od tisuću ranjeno.
+Žestoki napadi uslijedili su i u svibnju 1992., u srpnju i rujnu 1993., te u svibnju i kolovozu 1995. godine. Grad i okolica definitivno su oslobođeni 7. kolovoza 1995. godine. </t>
+  </si>
+  <si>
+    <t>42000 Varaždin</t>
+  </si>
+  <si>
+    <t>VŽ</t>
+  </si>
+  <si>
+    <t>U špilji Vindija u Donjoj Voći kod Varaždina pronađeni su najbolje sačuvani ostaci neandertalaca na svijetu, stari oko 30 000 godina.
+Prema arheološkim nalazima, područje grada bilo je naseljeno još u rimsko doba, o čemu svjedoče i imena dviju danas postojećih ulica – Via Militum i Via Petovia (današnje ulice Braće Radić i Optujska).
+U sjeverozapadnoj Hrvatskoj, na desnoj obali rijeke Drave nalazi se grad Varaždin, danas sjedište Varaždinske županije, grad obrtnika i male industrije, ali i sačuvanog bogatog kulturnog i povijesnog naslijeđa.
+Prirodni uvjeti oduvijek su  ljudima bili privlačni i pogodni za život, o čemu nam govore mnogobrojni poznati arheološki lokaliteti kao što su špilja Vindija, Punikve kod Ivanca, špilja Vilenica kod Novog Marofa te pronađeni ostatci materijalne baštine.
+Vrijeme rimske dominacije u samom gradu ostavilo je malo tragova, ali je ovuda prolazila važna rimska cesta koja je povezivala Ptuj, Varaždinske Toplice i Sisak s Osijekom.
+U povijesnim izvorima najstarije podatke o Varaždinu, o imenu grada  koji se ovdje spominje pod nazivom  Guarestin, o njegovim stanovnicima i Guaresdienses, imenima varaždinskih župana Beleé i Motmira, nalazimo u ispravi kralja Bele III. izdanoj 1181. godine kojom presuđuje u sukobu oko posjeda Varaždinske Toplice između Zagrebačkog kaptola i varaždinskog župana Beleéa.
+Svoj najznačajniji politički razvoj Varaždin će doživjeti osnivanjem Kraljevskog namjesničkog vijeća čiji rad kraljica Marija Terezija stavlja u Varaždin te na taj način grad postaje glavno sjedište Banske Hrvatske. U to vrijeme hrvatski ban i kapetan Franjo Nadasdy živi u Varaždinu, u palači Drašković, gdje se u jednom krilu palače održavaju i sjednice Kraljevskog namjesničkog vijeća, u razdoblju od 1767. do 1776. g.
+Veliki požar 1776. godine (25. travnja) u kojem su izgorjele dvije trećine grada, predstavlja kraj političkog i upravnog razvoja grada kao banskog sjedišta. Iz dokumenata je vidljivo da postoji niz zanimanja obrtnika prisutnih u gradu dugi niz godina, ali se početkom 18. stoljeća javljaju i neka nova, otvorena je manufaktura čokolade DAGNESE, prisutno je pivarstvo i svilarstvo, zabilježen je pokušaj uzgajanja riže (od Ivana Saltnera), a grad posjeduje i ciglanu. Nova su pravila dobili cehovi mesara, čohaša i lončara. Dopunjena su pravila ceha stolara, bravara, puškara, tokara, staklara i gumbarskog ceha.
+Između trgovaca dolazi do čestih svađa. Ovdje se često radi o borbi unutar cehovske i slobodne trgovine pa je Hrvatski sabor odredio da će cijenu robe određivati podžupani. Carica Marija Terezija je, sagledavajući cjelokupni život stanovništva, nastojala  poboljšati i zdravstveno stanje stanovništva pa u grad  dovodi gradskog fizika i liječnika Ivana Baptista Lalangua. U grad je po njenom nalogu stigao i Adalbert Barić s ciljem da ovdje osnuje Kameralni studij.
+Početkom 18. stoljeća gradi se Kapucinska crkva i samostan. Novi duh varaždinskom osnovnom školstvu donose uršulinke koje 1703. dolaze u grad. One ovdje grade crkvu, samostan i školu. Ukinućem isusovačkog reda gimnazija prelazi u ruke pavlina. 
+Glazbeni život Varaždina obilježit će Ivan Werner, Leopold Ebner i Jan K. Wanhal. Crkve čuvaju slikarske radove Joakima Shidta, Blaža Grubera te Ivana Rangera. Društveni život „Malog Beča“ ogledat će se u organizaciji mnogobrojnih zabava i plesova građana i plemića prisutnih u gradu. U palačama i kurijama  vodi se raskošan život koji je opisao Adam Oršić. Prve su se kazališne predstave izvodile u Isusovačkoj gimnaziji, no 1773. pojavljuje se i kazališna družina.
+Grof Stjepan Niczky je u naše krajeve donio ideju o slobodnom zidarstvu koje je imalo odjeka među plemstvom ovog područja. U gradu nastaje građanska četa, a zbog čestih požara organiziraju se i vatrogasne družine.
+Kraj 18. stoljeća u našem kraju je obilježen strahom  pred napoleonskim četama. U gradu se smještaju ranjenici u privremene bolnice u Zakmardijevoj palači i Isusovačkoj gimnaziji.
+Društvene i političke promjene koje će do sredine 19. stoljeća rezultirati  novim idejama u razvijanju nacionalne svijesti, odrazit će se i na razvoj gradske uprave. Početkom stoljeća ruše se gradski bedemi i izgrađuje dio nekadašnjih grabišta.
+Ideje Hrvatskog narodnog preporoda u Varaždinu će naći široki odjek. Ljudevit Gaj, jedan od vodećih preporoditelja  bio je varaždinski gimnazijalac, a 1832. kao odvjetnički perovođa u Varaždinu, i ovdje je mnoge ljude oduševio za svoje ideje. Ovdje živi Metel Ožegović čijom je velikom zaslugom 1837. godine otvorena Narodna čitaonica. U blizini živi i grof Janko Drašković, u Varaždinu djeluju Ivan Kukuljević, Tomo Blažek te drugi ilirci.
+Događanja 1848. godine ostavit će trag i u zbivanjima u varaždinskoj okolici. Gradsko zastupstvo raspravljalo je o pozivu hrvatskim rodoljubima na veliku političku skupštinu u Zagrebu 25. ožujka. Te su se godine Varaždinci pobunili protiv Židova, a 30. svibnja sastala  se velika skupština Varaždinske županije koja je zaključila da više ne priznaje Erdödijevce za nasljedne župane. Donesen je i novi grb i županijska zastava. Od 7. rujna iste godine ban Josip Jelačić boravi u Varaždinu, a  11. rujna s hrvatskom vojskom prelazi Dravu i kreće u smirivanje Mađara.
+Secesija Varaždinu daje novi smjer u načinu gradnje pa je početkom 20. stoljeća sagrađena zgrada nove pošte. Tada u grad dolazi telefon, a grof Marko Bombelles doveo je u naš kraj prvi automobil i aktivno sudjelovao u akcijama automobilskog društva. 
+Prvi svjetski rat u Varaždin donosi mobilizaciju vojnih obveznika. Varaždinci odlaze na različita bojišta, a u gradu se organiziraju bolnice za prihvat ranjenika. Ulaskom u novu državu, Kraljevinu Jugoslaviju, već 1919. godine dolazi do oružane pobune koja je brzo ugušena, a sudionici poslani u zatvor u Niš.
+U vrijeme Drugog svjetskog rata na našem je području nastala Velika župa Zagorje kojoj je Varaždin bio središte. Formiranjem Nezavisne Države Hrvatske i u našem gradu jedni pristaju uz antifašizam, a drugi ostaju lojalni postojećem režimu.
+Nakon Drugog svjetskog rata stvara se novi poredak, socijalizam. U grad se doseljava mnogo novog stanovništva pa se na taj način mijenja društvena struktura ovog područja. Provodi se nacionalizacija i konfiskacija pa velik broj građana ostaje bez svojeg dotadašnjeg vlasništva. Gospodarstvo grada sve se više oslanja na novi oblik proizvodnje, na tvornice i poduzeća kao što su LTA, Koka, Kalnik i sl. uz već postojeći Varteks i Svilanu.
+Gradnjom novih zgrada nastaju nova naselja. Širenjem grada se urbana i komunalna infrastruktura razvija. U gradu se otvaraju nove osnovne i srednje škole i fakulteti. Povijesna se jezgra zaštićuje kao spomenik kulture, razvija se kulturni život, prosvjeta i socijale ustanove. Uvodi se samoupravljanje i društveno vlasništvo. Sedamdesete će i u naše krajeve donijeti buđenje nacionalne svijesti koje će biti nasilno prekinuto. 
+Nakon Titove smrti dolazi do raspada Jugoslavije. U tom procesu i u Domovinskom ratu od 1990. – 1995. godine, Varaždin ima važnu ulogu.  Osvajanjem vojarni i oslobađanjem grada od JNA, Varaždin će osvojenim naoružanjem pripomoći osamostaljenju Hrvatske. Stvaranjem hrvatske države Varaždin postaje sjedište novoustrojene županije.
+Razdoblje Bachova apsolutizma odrazit će se i u našim krajevima u sprovođenju germanizacije. Velikom pritisku mađarizacije grad je bio izložen nakon nastanka Austro-Ugarske Monarhije,  u vrijeme Radoslava Rubida Zichyja, varaždinskog župana od 1886.-1906. godine koji je, kao pristalica Khuenova režima na našem području, sprovodio njegovu politiku. Utjecaj mađarizacije u gradu je prevladavao sve do izbora 1906. godine kada je pobijedila Narodna stranka, a Rubido prisiljen da se povuče.
+Gospodarske prilike tijekom 19. stoljeća daju novi polet gradu. Kralj Franjo I. 1811. godine potvrđuje novu trgovačku organizaciju, no već 1836.godine trgovački stalež dobiva posebno potvrđena pravila od kralja Ferdinanda V.
+U Varaždin prodiru nova umjetnička strujanja i tehnička dostignuća.</t>
+  </si>
+  <si>
+    <t>46.13</t>
+  </si>
+  <si>
+    <t>16.33</t>
+  </si>
+  <si>
+    <t>16.83</t>
+  </si>
+  <si>
+    <t>48000 Koprivnica</t>
+  </si>
+  <si>
+    <t>KC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pretpostavlja se da su jezgru koprivničkog gradskog naselja činili starosjedilačko slavensko naselje (gradište) i naseobina kolonista (hospita). Koprivnica je svoj nastanak te razvoj i jačanje regionalnih funkcija temeljila na gospodarski i politički atraktivnom prometnom položaju. Koprivnica je iskoristila prednosti svojeg položaja i razvila niz funkcija za širu okolicu (prvenstveno obrt, trgovinu, upravu, vjerski život – župa sv. Nikole), pa se još u tijeku 13. stoljeća razvila u gradsko naselje.
+Vrlo je vjerojatno da je uspon koprivničkog gradskog naselja tijekom 14. stoljeća moguće tražiti u jačanju trgovinskog prometa uzduž podravske magistrale pod utjecajem napredovanja grada Varaždina, pri čemu je Koprivnica imala prednost lokacije na transverzalnom odvojku prema jugu, tj. prema Zagrebu i dalje prema Jadranskom moru, ali i na sjever prema Ugarskoj.
+Koprivnica je dobila ime po potoku Koprivnici koja se prvi puta spominje 1207. godine. Građani slobodnih kraljevskih gradova imali su pravo na izbor vlastitog suca te pravo slobode trgovine. Koprivnica koja je prve privilegije gradskog naselja dobila 1338. godine, a povlastice slobodnog i herceškog grada 1353. godine. Te je povlastice potvrdio kralj Ludovik I. Anžuvinac 4. studenog 1356. godine čime je Koprivnica postala slobodni, kraljevski i glavni grad.
+Početkom 15. stoljeća grad je došao u privatne ruke, a oko 1547. Koprivnica se zahvaljujući Ferdinandu I. Habsburg u vraća u kraljevske ruke Koprivnica je u 16. i 17. stoljeću zadržala status slobodnog kraljevskog grada, a istovremeno je nakon izgradnje moderne utvrde (u drugoj polovici 16. stoljeća) postala središte vojnokrajiške kapetanije. Položaj u blizini granice između Habsburškog i Osmanskog Carstva utjecao je na gospodarske, društvene i demografske promjene te svakodnevni život. 
+U drugoj polovici 16. stoljeća Koprivnica je bilo sjedište zapovjednika Slavonske vojne krajine, a od 1595. gubi tu važnu središnju funkciju jer tada general svoje sjedište formira u obližnjem Varaždinu, a Slavonska vojna krajina se pretvara u Varaždinski generalat. No, iako je sjedište generala bilo u Varaždinu, Koprivnica je tijekom cijelog 17. stoljeća ostala najveća i strateški najvažnija utvrda Varaždinskog generalata s najbrojnijom vojnom posadom. 
+Krajem 16. stoljeća Koprivnica je imala oko pet stotina stanovnika (zajedno s vojnom posadom). Nakon Žitvanskog mira (1606.) došlo je do procesa intenzivnog useljavanja u grad. Novom izgradnjom se popunjava slobodni prostor u utvrdi. Početkom 17. stoljeća je bilo samo dvadeset civilnih kuća, da bi sredinom istog stoljeća taj broj narastao na 80 kuća. Pokazatelji gospodarskog uspona grada su izgradnja i širenje grada. Popunjavanjem slobodnog prostora za izgradnju u utvrdi došlo je do naseljavanja sjeverno od utvrde. U drugoj polovici 17. stoljeća u podgrađu je bilo 14 ulica u kojima je živjelo 447 obitelji, dok je u gradu Koprivnici živjelo oko 2500 stanovnika.
+Koprivnica je od tada pa sve do 19. stoljeća bila po broju stanovnika na trećem mjestu među hrvatsko-slavonskim slobodnim kraljevskim gradovima. Poboljšanje kvalitete življenja u gradu se vidi po organiziranoj liječničkoj službi od sredine 17. stoljeća te primalja krajem stoljeća. U gradu je bio organiziran hospital kao ustanova koja je objedinjavala brigu za bolesne s funkcijom sirotišta. Sredinom 17. stoljeća gradi katolička župna crkva Sv. Nikole, koja je i danas u funkciji.
+Nekoliko godina kasnije su se franjevci trajno naselili u gradu, a 1675. izgradili samostan i crkvu sv. Antuna Padovanskog. Širenje grada u svim smjerovima oko utvrde ilustrira izgradnja katoličkih kapela: Sv. Emerika (prije 1634.), Sv. Marije Magdalene (1649.), Sv. Ladislava (1658.), Kapela Svetog Vida kraj Koprivnice (1671.), Sv. Andrije (1671.) na jugu, Sv. Lucije (1650.), Sv. Ivana Krstitelja (1671.), Sv. Roka (1671.) na istoku, Sv. Duha (1659.) na sjeveru, te kapela Blažene Djevice Marije (1659.) i Sv. Triju Kraljeva (1671.) na zapadu. Smirivanjem stanja na granici Habsburškog i Osmanskog Carstva dolazi do obnove trgovine i gospodarskog jačanja Koprivnice. 
+Gospodarski uspon je jasno vidljiv od 1607. godine kada pouzdano znamo da u gradu djeluje ceh kovača, bravara, mačara, remenara, sedlara i zlatara. Zanimljivo je pratiti daljnju gospodarsku obnovu koja je u prvim desetljećima bila spora tako da je grad tek 1638. dobio pravo održavanja dva godišnja sajma. U Koprivnici je 1651. utemeljena malta (mitnica), a 1652. grad je dobio pravo trećeg godišnjeg sajma. U blizini grada, u susjednom trgovištu Drnju je 1660. osnovana tridesetnica (carinarnica), što govori o intenzitetu prometa i trgovine. Daljnje jačanje gospodarstva se vidi osnivanjem novih cehova: čizmarskog ceha 1673. i mesarskog ceha 1697. godine. Time su napravljeni preduvjeti kasnije potpune dominacije cehova u proizvodnji tijekom 18. i dijela 19. stoljeću. U 17. stoljeću dolazi do pojačanog razvitka prosvjete i kulture, što je pokazatelj obnove i sveukupnog jačanja grada. Od kraja 16. stoljeća djeluje župna škola.
+Katolička župna knjižnica djeluje prve polovice 17. stoljeća, a 1650. je u njoj zabilježeno 59 knjiga većim dijelom na latinskom, a manjim na njemačkom jeziku. Po broju knjiga u ondašnjem mjerilu spadala je među veće knjižnice. Pokazatelj gospodarske obnove grada može biti veći broj gimnazijalaca i studenata. Koprivničanci su polazili gimnazije Ruše kod Maribora, Győru i Trnavi, a sveučilišta u Grazu, Trnavi, Beču, Salzburgu i Padovi. Iako je u razdoblju od 1731. do 1765. Koprivnica ponovo bila sjedište generalata, vojna je uprava (Vojna krajina) sputavala razvoj grada sve do preseljenja generala u novoizgrađeni Bjelovar 1765. godine. Nakon toga u stotinjak se godina udvostručava ukupni broj stanovnika od 2589 žitelja popisanih 1769. godine na 5684 stanovnika 1869. godine.
+Početkom 20. stoljeća gradi se nova pruga prema Đurđevcu i Virovitici, a željeznička prometna povezanost je završena 1937. godine kada je Koprivnica željeznički povezana s Ludbregom i Varaždinom. Bolja prometna povezanost omogućila je ubrzani razvitak trgovine, gostioničarstva i hotelijerstva. Grad je imao razvijene i dobro regulirane sajmove na kojima su gradski i vanjski majstori nudili proizvode. Cehovi su bili važna gospodarska značajka Koprivnice od kasnoga srednjega vijeka do druge polovice 19. stoljeća, a primjerice 1846. godine bilo je u gradu evidentirano 130 majstora, koji su uglavnom bili smješteni izvan utvrde. Uz cehove u gradu i predgrađima se razvijaju pivovara, svilogojstvo, mlinarstvo, komunalna klaonica, solana, proizvodnja cigle i crijepa, rudarstvo i bankarstvo, što potvrđuje postupni razvitak manufaktura, rane industrije, rudarstva i bankarstva u gradu. Gospodarski razvitak, znatan porast stanovništva, bolji uvjeti života i drugi čimbenici utjecali su da je u gradu bio razvijen društveni život.
+U 19. stoljeću se osniva Purgerski kor (prvi se puta spominje 1809.), kazališno društvo (1837.), limena glazba (1841.) kasino (1846.), narodna čitaonica (1867.) te nakon toga brojne druge udruge.Godine 1856. organizira se prva muzejska izložba, a više je Koprivničana članovima, suradnicima ili povjerenicima Hrvatskog arheološkog društva i Hrvatskog narodnog muzeja u Zagrebu, te drugih institucija. Muzej grada Koprivnice počeo je s radom 1951. godine. Osim toga u gradu djeluje od prije pošta, ljekarnica, te razvijena zdravstvena služba, prvobitno smještena u hospitalu kraj župne crkve, a od 1875. godine u bolnici koja je i danas u funkciji. Tijekom 1980-ih uz staru je bolnicu izgrađena nova. Škola je isprva djelovala u jednoj privatnoj kući u utvrdi, pa u oružani, u staroj gradskoj vijećnici, zatim u jednoj građanskoj kući, te na još nekim lokacijama, da bi se 1856. godine preselila u novu zgradu (današnja gradska vijećnica) kojoj je kamen temeljac postavio osobno ban Josip Jelačić. U obrazovanju je bila velika uloga Franjevaca koji su od početka 18. i tijekom dijela 19. stoljeća organizirali studije filozofije, moralne teologije i govorništva.
+Koprivničko svjetovno školstvo se najbrže razvijalo na prijelazu iz 19. u 20. stoljeće. Prvo je osnovana šegrtska (obrtnička) stručna škola 1886. godine. Godine 1892. otvara se suvremena školska zgrada, a škola se proširuje na pet razreda. Višu dječačku i djevojačku pučku školu, odnosno peti i šesti razred, Koprivnica dobiva 1902. godine. Nekoliko godina kasnije, 1906. godine formirana je u Koprivnici realna gimnazija, dok je suvremena gimnazijska zgrada bila izgrađena 1908. godine (u srednjoškolskoj funkciji je bila do 1975. godine kada je izgrađen srednjoškolski centar koji se i danas koristi u nastavi). Koprivnica u 20. stoljeće ulazi s razvijenim društvenim i gospodarskim životom. Do stagnacije gospodarskih funkcija je došlo nakon prvoga svjetskog rata. Kriza je posebno bila vidljiva 1930-ih godina kada je propao veći dio koprivničke industrije (Tvornica ulja, Tvornica Danica itd.). Potres na Bilogori 1938. pogodio je okolicu Koprivnice. Bilo je i oštećenja u gradu.
+U vrijeme Drugoga svjetskog rata u Koprivnici je na mjestu nekadašnje tvornice Danica osnovan prvi koncentracijski logor u Nezavisnoj Državi Hrvatskoj. Koprivnicu su 7. studenog 1943. godine oslobodili partizani. Grad je bio dio slobodnog teritorija do 9. veljače 1944.,[8] kada su ga ponovno zauzele njemačko-ustaške snage. Jedna od najžešćih bitaka u Drugom Svjetskom ratu u Jugoslaviji zbila se upravo kod Koprivnice u listopadu 1944. godine. Partizani su napali s dva korpusa, dok su ustaše i Hrvatski domobrani branili grad. Bitka je trajala do 17. listopada kada je pobjedu odnijela vojska NDH.Nakon drugog svjetskog rata dolazi do daljnjih procesa modernizacije i ubrzane industrijalizacije. U to vrijeme osnovana su velika industrijska postrojenja sa značajnim brojem zaposlenika (Podravka, Bilokalnik, Belupo itd.) i financijske ustanove s kasnijom značajnom gospodarskom snagom (npr. Podravska banka itd.) na kojima počiva i današnji gospodarski razvoj Koprivnice.
+Koprivnica je dala veliki doprinos u Domovinskom ratu, kako policijskim i vojnim postrojbama u akcijama obrane od 1991. tako i u oslobađajućim vojno-redarstvenim akcijama Bljesak i Oluja 1995. godine. U samostalnoj Hrvatskoj Koprivnica je postala sjedištem novoosnovane Koprivničko-križevačke županije (od 1993.), a u posljednjem desetljeću dolazi do ubrzanog infrastrukutralnog, gospodarskog, društvenog i kulturnog razvitka grada. 
+Koprivnica je u 17. i 18. stoljeća bila na trećem mjestu po broju stanovnika, obitelji i kuća u civilnoj Hrvatskoj i Slavoniji. Više stanovnika su imali jedino Rijeka i Varaždin, a manje Gradec, Zagreb, Bakar, Karlovac, Križevci i Požega. Grad Koprivnica se sastojao od utvrde, podgrađa i ruralnih predgrađa Banovec, Brežanec, Dubovec, Miklinovec, Koprivnički Bregi, Herešin, Vinica, itd. Od 17. stoljeća dolazi do kontinuiranog ispunjavanja slobodnog gradskog prostora, ali i do gradnje prvih javnih zgrada izvan utvrde. Podgrađe na kojem se formirao novi trg je od 17. stoljeća počelo postupno preuzimati funkciju novog središta grada od stare utvrde.
+Nakon podizanja prvih objekata javne namjene u izvantvrđavnom prostoru dolazi do brze smjene građevina u tom dijelu grada. Stariji, skromniji barokni stambeni i trgovački objekti se ruše, a zamjenjuje ih historicistička arhitektura kada novo središte grada poprima današnji izgled. Od godine 1862. započelo je raskopavanje gradskih bedema, koje nikad nije do kraja dovršeno. Godine 1863. zasađen je najstariji dio budućeg gradskog parka na prostoru dijela bivših opkopa oko utvrde. Upravo je rušenje starih bedema uz izgradnju željezničke pruge bilo odlučujući faktor u prostornom razvitku grada. Tadašnja prvobitna rasvjeta je bila petrolejska, a kasnije je zamijenjena plinskom, a sve je to utjecalo na promjenu načina života u gradu. Za prometno povezivanje je bilo najznačajnije dovođenje željeznice (Budimpešta – Zagreb) do grada 1869./1870. godine. </t>
+  </si>
+  <si>
+    <t>45.91</t>
+  </si>
+  <si>
+    <t>16.84</t>
+  </si>
+  <si>
+    <t>43000 Bjelovar</t>
+  </si>
+  <si>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>Grad Bjelovar, smješten na visoravni podno jugozapadnih obronaka Bilogore, danas je sjedište Bjelovarsko-bilogorske županije i političko, gospodarsko i kulturno središte toga kraja.
+Iako je uvriježeno mišljenje kako povijest Bjelovara počinje s 1756. godinom, odnosno s osnutkom grada, na tom se području očituje kontinuirana naseljenost od najstarijih vremena. Na širem bjelovarskom području pronađeni su ostaci starčevačke, korenovske, sopotske, lasinjske, vučedolske kulture te kulture brončanog i željeznog doba. Intenzivniji razvoj tog područja započinje dolaskom Rimljana koji prvi put dolaze na područje između Save i Drave 229. godine pr. Kr. Upravo se na mjestu na kojem se razvio današnji Bjelovar nalazilo križište dviju rimskih cesta i u njegovoj neposrednoj blizini vojni logor ili postaja. Stabilizacijom sjeverne granice Rimskog Carstva vjerojatno se ovdje razvilo naselje u razdoblju od II. do IV. stoljeća, nezabilježeno na rimskim itinerarima, ali posvjedočeno arheološkim ostacima na današnjem Matoševom trgu, Trgu Stjepana Radića te nalazima na širem gradskom području. Najznačajniji rimski nalaz s bjelovarskog područja, kameni reljef s prikazom mitološke scene Ifigenije na Tauridi, danas nije vidljiv jer je prilikom obnove u 19. stoljeću ugrađen u portal današnje katedrale Sv. Terezije Avilske. Padom Zapadnog Rimskog Carstva propada i područje antičkog Bjelovara i u povijesnim izvorima ostaje nezabilježeno do XIII. stoljeća. 
+Srednjovjekovni izvori uglavnom spominju samo naselja i desetak župa na širem prostoru oko današnjeg Bjelovara. Istovremeno se sredinom XIV. stoljeća prvi put spominje naselje Jakobove Sredice koje odgovara području današnjih ulica Velike i Male Sredice, a u neposrednoj blizini bjelovarskog gradskog središta. Pretpostavka je da se radilo o rudimentarnom obliku urbane jezgre, a s obzirom na to da ime naselja upućuje na dan u tjednu, moguće je da se radilo o mjestu gdje su se srijedom održavali trgovački sajmovi. 
+Prodorom Turaka u XVI. stoljeću u ove krajeve opstala su samo ona utvrđena naselja pod posebnom ingerencijom bečkog dvora u koja se sklanja lokalno stanovništvo. Tek će se uspostavom administrativnog i vojnog sustava obrane protiv Turaka, poznatijeg kao Vojna krajina, unutar kojeg se nalazilo i bjelovarsko područje, potaknuti razvoj naselja. Bjelovar se od prve polovice XVII. stoljeća na vojnim kartama spominje kao vojna stražarnica što govori da je već tada ušao u krajiški obrambeni sustav. Stabilizacija habsburško-osmanske granice na Savi i nove okolnosti u vojnokrajiškom društvu u prvoj polovici XVIII. stoljeća uvjetovale su teritorijalnu i upravnu reorganizaciju Varaždinskog generalata.
+Severinska buna, koja se odvijala 1755. godine u neposrednoj blizini budućeg grada, ukazala je na potrebu za novim središtem iz kojeg bi se provodila bolja kontrola krajišnika. Bečki su vojni stratezi donijeli odluku o osnivanju novoga naselja koje bi preuzelo funkciju sjedišta pukovnijskih uprava. Tražeći najpogodnije rješenje izabrana je lokacija u središtu generalata, na crti razgraničenja Križevačke i Đurđevačke pukovnije. 
+Osnutak i početak izgradnje Bjelovara smješta se u 1756. godinu kada je otkupljeno zemljište i izdana dozvola za nabavu građevnog materijala, a izgradnju je vodio barun Philipp Lewin von Beck. Grad je od samih početaka zamišljen kao središte pukovnija Varaždinskog generalata i u skladu s vojnom funkcijom prvo se otpočelo s gradnjom vojnih objekata i naseljavanja vojnog stanovništva. Izuzetak čini blok na trgu u kojem se od 1765. godine gradi župna crkva sv. Terezije Avilske te pijaristički samostan i škola. Naime, odlukom Marije Terezije za potrebe školstva u Bjelovar 1761. godine dolaze dva redovnika pijarista, braća Hubert i Ignac Diviš. Iste su godine otvorili prvu pučku školu na đurđevačkoj strani grada. Odlukom Marije Terezije o gradnji nove crkve koja je završena 1772. godine osnovana je i bjelovarska crkvena župa kojom su do 1790. godine upravljali pijaristi. Godine 1771. carica Marija Terezija potvrdila je Bjelovaru status povlaštenog krajiškog grada, tj. Vojnog komuniteta što je za posljedicu imalo demografski i značajan gospodarski rast. Taj se trend nastavio i na početku XIX. stoljeća kada se grad počinje širiti van prvotnih granica. 
+Razvojačenjem Vojne krajine i Varaždinskog generalata 1871. godine formira se nova županija sa sjedištem u Bjelovaru. Već 1874. godine, kao dvanaesti grad u Hrvatskoj, Bjelovar dobiva status Slobodnog kraljevskog grad. Preustrojem županija i uprava, od 1886. Bjelovar postaje i središte objedinjene Bjelovarsko-križevačke županije. Zahvaljujući novom upravno-teritorijalnom ustroju Bjelovar će dobiti niz novih funkcija koje će biti značajni poticaj razvoju grada. Od 1872. godine djeluje Kraljevski županijski sudbeni stol, a svoje su urede imali i župan, županijski tajnik, županijski i kotarski školski nadzornici, liječnici, veterinari, nadšumar te kotarski inženjerski pristav. Broj stanovnika od službenog ukinuća Vojne krajine do kraja stoljeća gotovo se udvostručio. Dodatni polet razvoju grada dat će i izgradnja prometne infrastrukture, prvenstveno željeznice krajem stoljeća što će rezultirati intenzivnim razvojem na prijelomu XIX. i XX. stoljeća. Izgradnjom željeznice Bjelovar će doživjeti gospodarski uzlet koji će se nastaviti sve do Prvog svjetskog rata. 
+Prvi industrijski pogon u gradu, Paromlin, otvoren je 1894. godine, u godini dolaska željeznice. Osim Paromlina u to vrijeme djeluju već i pekara Dragutina Wolfa, koja će se razviti u današnji Koestlin, bjelovarska podružnica tvornice kavinih surogata ,,Hinko Franck i sinovi“ te radionica za preradu mesa Josipa Svobode. O gospodarskoj snazi svjedoče i izvještaji Trgovačko-obrtne komore u Zagrebu iz 1906. kada je u Bjelovaru registrirano 118 trgovačkih i 313 obrtnih poduzeća po čemu se Bjelovar smjestio odmah iza Zagreba, Karlovca i Varaždina.
+Miran život i gospodarski uzlet prekinuo je početak Prvog svjetskog rata. Kao važan vojni grad, Bjelovar je svoj doprinos dao regrutacijom muškog stanovništva, prenamjenom javnih zgrada u bolnice, korištenjem željeznice za prijevoz vojnika i ranjenika. Posljedično je nestašica ljudstva i prirodnih resursa dovelo do teške gospodarske situacije i opće nestašice hrane. S krajem rata proglašena je Kraljevina Srba, Hrvata i Slovenaca i Bjelovar je u početku zadržao mjesto upravnog središta Bjelovarsko-križevačke županije. Vidovdanskim ustavom iz 1921. godine, a na temelju Zakona o oblasnoj i sreskoj samoupravi (1922.) Kraljevina SHS je podijeljena na 33 okruga, a Bjelovar je time izgubio status županijskog centra i našao se u Osječkom okrugu sa statusom kotara i grada. Zahvaljujući gospodarskim osnovama, stvorenim u prethodnom razdoblju, a temeljenima na trgovini, obrtništvu i industriji nastavit će se pozitivan gospodarski trend koji će se održati sve do Velike gospodarske krize 1929. godine, kada će biti zabilježen rast registriranih trgovaca, obrtnika i industrijalaca, ali s manjim prihodima. U međuratnom razdoblju grad dobiva i neke nove sadržaje. Na Logorištu je uređeno nogometno igralište Bjelovarskog akademskog športskog kluba. Od 1914. do 1921. godine u gradu je bio otvoren i prvi plivački bazen na zemljištu cikorije Franck. Godine 1932. javila se inicijativa o gradnji novog gradskog kupališta koje je naposljetku izgrađeno i otvoreno u kolovozu iste godine iza prostora starog sajmišta, na posjedu Rudolfa Berghofera, na lokaciji na kojoj se nalazi i danas. Otvorenjem kupališta pristupilo se i hortikulturnom uređenju prostora staroga sajmišta, tj. Trga Stjepana Radića. Izgled koji je tada dobio u velikoj je mjeri sačuvan do danas. 
+Kratkotrajno razdoblje Nezavisne Države Hrvatske za Drugog svjetskog rata zaustavilo je razvoj grada na svim područjima. Dva dana prije službena proglašenja u Zagrebu, 8. travnja 1941. godine, s balkona gradske vijećnice (danas zgrada Gradskog muzeja Bjelovar) gradonačelnik dr. Julije Makanec proglasio je Nezavisnu Državu Hrvatsku. Kroz dva mjeseca uslijedila je i nova teritorijalno-administrativna podjela države na 22 župe. Time je grad Bjelovar nakon 17 godina opet postao regionalno središte, sada novoosnovane Velike župe Bilo Gora. Tijekom rata, za razliku od sela u bjelovarskoj neposrednoj blizini, grad nije doživio teža materijalna razaranja. U više je navrata bombardirana samo pruga kao glavna komunikacija putem koje su se opskrbljivale okupacijske snage te vojarna na Vojnoviću.
+S krajem rata i dolaskom nove socijalističke vlasti od samih se početaka pokazuju tendencije modernizacije države te obnova posrnule industrije i komunalne infrastrukture. Intenzivirana je stanogradnja uglavnom u sjevernom dijelu grada jer dotadašnji stambeni kapaciteti nisu udovoljavali potrebama rastućeg stanovništva. U južnome se dijelu gradske jezgre krajem 50-ih godina intenzivnom gradnjom narušava ambijent povijesne jezgre; 1959. godine podiže se na uglu Matičine i Kačićeve ulice modernistička stambena trokatnica, u Ulici Ivana Viteza Trnskog velika stambena zgrada, a na mjestu zgrade stare pošte 1960. godine podiže se nova zgrada pošte, također modernističkih oblika i neprimjereno velika volumena negirajući pritom oblike historijske osnove grada. U Ulici Petra Preradovića tijekom 1962. i 1963. godine ruše se autentične prizemnice povijesne vrijednosti i grade trokatni objekti duž zapadne strane te ulice te neboder visine jedanaest katova na uglu Preradovićeve i Matičine ulice. Unatoč tome, 1962. godine povijesna jezgra Bjelovara stavljena je u registar nepokretne spomeničke baštine pod zaštitom konzervatora. 
+Razvoj grada zahtijevao je i izgradnju novih zgrada gospodarske i javne namjene. Na Matoševom trgu podiže se 1959. godine zgrada uprave Elektre, 1960. godine dovršen je Dječji odjel bjelovarske bolnice, a 1964. dovršena je i nova zgrada III. osnovne škole. U tom se razdoblju formirala industrijska gradska zona u mjeri u kojoj je poznata i danas. Postrojenje Koestlina se 1955. preselilo iz stroge gradske jezgre u industrijsku zonu južno od pruge prema Kloštru. Uz Koestlin i već postojeće tvornice Tome Vinkovića, na tom su se području od 60-ih godina izgradila i postrojenja Česme, Sjedinjenih paromlina (kasnije preimenovano u 5. maj), Tehnogradnje i Elektrometala. Zbog širenja grada i povećanja populacije, na njegovu sjevernom dijelu gradi se i nova Osnovna škola „Maršal Tito“ te Školsko-sportska dvorana prema projektima Miljenka Smoljanovića. Radi bolje prometne povezanosti gradi se i autobusni kolodvor, na lokaciji pokraj željezničkog kolodvora. Također se pristupilo proširenju Medicinskog centra. Od 1976. do 1982. godine gradi se nova zgrada u Franjevačkoj ulici od 12 tisuća četvornih metara, s 200 kreveta i novim specijalističkim odjelima. Uz demografski i gospodarski rast i spomenuta izgrađena infrastruktura doprinijela je jačanju svih funkcija čime se Bjelovar prometnuo u jedan od najznačajnijih centara sjeverozapadne Hrvatske.
+Nakon prvih višestranačkih demokratskih izbora u SR Hrvatskoj održanih 22. i 23. travnja 1990. godine, novoosnovana Hrvatska demokratska zajednica osvojila je vlast i u Bjelovaru. Nakon referenduma i proglašenja samostalnosti došlo je do zaoštravanja krize i početka ratnih sukoba. Zbog toga je predsjednik Republike Hrvatske dr. Franjo Tuđman 12. rujna donio odluku o blokiranju svih vojarni JNA u Hrvatskoj i obustavu opskrbe tih vojarni strujom, vodom i hranom. Nakon niza neuspješnih pokušaja da vojska JNA mirno napusti vojarne smještene u gradu ili u njegovoj neposrednoj okolini, a riječ je o vojarnama ili vojnim objektima na Logoru, Vojnoviću, Zvijercima, u Bedeniku te vojarni Preradović na glavnom gradskom trgu, ujutro 29. rujna 1991. godine policija i Zbor narodne garde napali su vojarnu na Vojnoviću. Na grad je iz vojarne, do istog dana u 19.00 sati kada su se pripadnici JNA predali, ispaljeno više desetaka raznih projektila. Osim ljudskih žrtava, grad je doživio teška razaranja i oštećenja objekata u povijesnoj jezgri. Među spomenicima kulture oštećeni su vojarna na glavnom gradskom trgu, zgrade na sjevernoj i južnoj strani glavnoga trga, pravoslavna crkva Sv. Trojice te katolička crkva Sv. Terezije Avilske. Od ostalih objekata oštećene su zgrade bolnice, policije, doma umirovljenika, pošte te silosi Prerade. Sveukupno je u tom jednom danu oštećeno 437 stambenih objekata, 169 gospodarskih zgrada i 25 zgrada javne namjene. Istog je dana, u neposrednoj blizini grada, u šumi Bedenik (danas spomen-područje Barutana) eksplodiralo skladište streljiva pri čemu je poginulo jedanaest hrvatskih vojnika.
+Taj 29. rujna 1991. godine postao je jedan od važnijih datuma u novijoj hrvatskoj povijesti Bjelovara Gradsko vijeće Grada Bjelovara 1997. godine donijelo je odluku o proglašenju tog datuma Danom Grada Bjelovara. Od 2007. godine 29. rujna obilježava se i kao Dan bjelovarskih branitelja, kao zahvala svim našim braniteljima koji su stali u obranu svoga grada i domovine te sjećanje na sve one koji danas, nažalost, više nisu s nama, a pridonijeli su hrvatskoj slobodi i neovisnosti.</t>
+  </si>
+  <si>
+    <t>45.33</t>
+  </si>
+  <si>
+    <t>14.44</t>
+  </si>
+  <si>
+    <t>51000 Rijeka</t>
+  </si>
+  <si>
+    <t>Najstariji tragovi ljudske prisutnosti na današnjem području Rijeke potječu još iz doba paleolitika i neolitika, a ostaci pretpovijesnih gradina (Solin iznad Martinšćice, Trsatski brijeg i Veli vrh – Gradišće iznad Rječine) iz brončanog i željeznog doba.
+Takvo je naselje dominiralo Riječkim zaljevom te osiguravalo luku i u doba života Ilira (Liburna).
+Rimljani pomiču centar života bliže moru, na desnu stranu utoka Rječine u Jadran, na mjestu današnjeg Starog grada. O urbanoj razini rimske Tarsatice svjedoče brojni arheološki nalazi (temelji rimskih bedema, zidova zgrada, ostaci termi, rimskog vojnog zapovjedništva).
+Takvim smještajem na blago položenoj padini, s uskim obalnim pojasom, izdašnim izvorima pitke vode, zaklonjenim zaljevom s prirodnim obilježjem luke, ovaj je grad imao sve predispozicije da se razvije u važnu luku i trgovački grad.
+To je potaklo novodoseljeno slavensko stanovništvo, Hrvate, da zauzmu Tarsaticu i otpočnu formirati novo naselje. Prva izvorna vijest o srednjevjekovnom naselju potječe iz prve polovine XIII. st., no tada se u povijesnim izvorima pojavljuju dva naselja:
+    Trsat, na brijegu na lijevoj strani Rječine, na mjestu liburnskog naselja Tarsate i
+    Rijeka, na obali, na mjestu rimske Tarsatice.
+Tadašnja je Rijeka utvrđeni gradić, zbijen unutar zidina s nekoliko obrambenih kula podijeljen na dva dijela: u gornjem je srednjovjekovni kaštel i crkva Sv. Vida (otuda naziv Flumen Sancti Viti) i donje pučko, trgovačko i obrtničko naselje među čijim je žiteljima uobičajen naziv Rika ili Rijeka.
+Na početku i potkraj XIV. st. Rijeka je u posjedu Devinske gospode, knezova Krčkih (potonji Frankopani), nakon toga u posjedu obitelji Walsee, a od 1466. Habsburgovaca. Tada je Rijeka imala oko 3000 stanovnika.
+Znatan ekonomski procvat počeo je u XVI. st. uz trgovinu željezom, uljem, drvom, vunom, stokom i kožom. U XVI. st. u gradu djeluje i tiskara s hrvatskim pismom – glagoljicom.
+Tada na lijevoj obali Rječine ispod naselja Trsat još nema naselja (Sušak), ono se formira tek u XVIII. stoljeću.
+Zlatno doba riječke trgovine naglo slabi u drugoj polovici XV. st.
+Česte turske provale prekidaju prometne putove, kao i ratovi pretendenata na mađarsko prijestolje, te dugotrajni sukobi uskoka s Mlečanima.
+Smirivanje ratnih prilika započinje u drugoj polovici XVII. st.
+Dolazakisusovaca u Rijeku, te osnivanje njihove gimnazije znatno unapređuje prosvjetno-kulturni život uz jačanje romanstva na uštrb hrvatskog jezika i glagoljice.
+Značajnu prednost riječka privreda počinje stjecati u XVIII. st. Tada je car Karlo VI. proglasio Rijeku slobodnom lukom, ali uskoro ojačala Mađarska kao dio Habsburške Monarhije počinje na Rijeku gledati kao svoj izlaz u svijet.
+Na prijelazu iz XVIII. i XIX. st. Rijeka je pod francuskom upravom, a nakon toga opet pod Austrijom.
+U građanskoj revolucionarnoj 1848. grad je uključen u Bansku Hrvatsku te ban Josip Jelačić postaje guvernerom Rijeke. Borba za Rijeku između Hrvatske i Mađarske sve se više zaoštrava, a Hrvatsko-ugarskom nagodbom 1868. tzv. “riječkom krpicom” utvrđen je provizorij prema kojemu Rijeka dolazi pod neposrednu upravu. Ona ju ubrzano razvija u svoj najveći pomorsko-lučki emporij.
+Nakon raspada Austro-Ugarske 1918. godine, Rijeka i Sušak su dio Države SHS sa sjedištem u Zagrebu, ali je ubrzo okupirana od Kraljevine Italije.
+S obzirom da Italija ranije nije tražila Rijeku, već ju je prepuštala Hrvatskoj, nastupa prijelazno razdoblje: okupacija Gabriela D’annunzia 1919. te Slobodna Država Rijeka 1920., da bi 1924. ipak pripala Italiji.
+Rijeka ubrzano gospodarski propada i postaje periferni gradić. Sušak je uključen u sastav Kraljevine SHS sa sjedištem u Beogradu i ubrzano raste s osloncem na široko zaleđe.
+Rijeka je, uz susjednu Istru, prva u svijetu pružila otpor fašizmu te je u Drugom svjetskom ratu dio antifašističke fronte.
+Nakon talijanske kapitulacije 1943. godine Rijeku i Sušak okupiraju Nijemci i drže do 3. svibnja 1945. kad je grad oslobođen.
+Zaključcima mirovne konferencije u Parizu 1947. godine, Rijeka je ponovo vraćena matici zemlji Hrvatskoj u okviru države Jugoslavije. Godine 1948. gradovi Rijeka i Sušak su udruženi u grad Rijeku, koji se ubrzano razvija u raznim područjima.
+Nakon obnove, Rijeka je preuzela funkciju glavne luke socijalističke Jugoslavije.
+U industrijskoj strukturi obnavljaju se tradicionalne riječke industrije: brodogradnja, tvornica papira, rafinerija nafte, proizvodnja brodskih uređaja i motora, koksara, industrija odjeće, hidroelektrane i termoelektrane. Tu je razvoj brodarskih poduzeća, a sjecište pet magistralnih cestovnih prometnih pravaca prema Zagrebu, Ljubljani, Trstu, Puli i Zadru te željezničke pruge osiguravaju Rijeci razvoj tercijarnog sektora.
+Ekspanzivan društveno-ekonomski razvoj povećao je i broj stanovnika. Tada Rijeka s okolicom ima oko 200.000 stanovnika. Paralelno s industrijskim razvojem, Rijeka je postala središte Zapadne Hrvatske (Istra, Hrvatsko primorje i Gorski kotar). Od početka šezdesetih godina izgrađuju se nove gradske četvrti, jačaju prigradska naselja.
+Ukratko, krajem XX. st. Rijeka je razvijeno urbano i industrijsko središte kao i središte raznih razvojnih inicijativa koje igraju važnu ulogu u ukupnom razvoju Republike Hrvatske. Postaje sjedište novoosnovane Riječko-senjske nadbiskupije i metropolije te sveučilišta.
+Hrvatske težnje za brzim približavanjem demokratskom i liberalnom obzoru zapadnog svijeta dovele su i do temeljitih promjena državnog i društvenog sustava.
+Iako u Rijeci nije bilo oružanih okršaja kao dijela Domovinskog rata, posljedica rata je stagnacija gospodarstva, preusmjeravanje na ratnu proizvodnju, pomoć u opskrbi bojišta širom Hrvatske.
+Mnoštvo je riječkih dragovoljaca na hrvatskim bojišnicama. Rijeka smješta i brine o mnoštvu prognanih iz ostalih dijelova Hrvatske.
+Demokratske promjene i okretanje tržišnom gospodarstvu dovode do znatnih promjena – buja političko-stranački život, započinju ulaganja privatnog kapitala u razvoj gospodarstva, u tijeku je pretvorba društvene imovine, što je rezultiralo i velikim brojem nezaposlenih, a Rijeka postaje središte Županije primorsko-goranske.
+Od 1993. godine, nakon donošenja Zakona o područjima županija, gradova i općina u Republici Hrvatskoj, ukinuta je općina Rijeka, a umjesto nje nastali su gradovi Rijeka, Kastav, Bakar i Kraljevica te općine Viškovo, Kostrena, Čavle, Jelenje i Klana.
+Time administrativne granice Grada Rijeke obuhvaćaju površinu od 44 km², a prema posljednjem popisu stanovništva iz 2011. godine, Rijeka ima 128.384 stanovnika.
+Rijeci je 24. ožujka 2016. dodijeljena prestižna titula Europske prijestolnice kulture 2020., i to za program “Luka različitosti”, čiji je cilj stvoriti grad kulture i kreativnosti za Europu i budućnost.</t>
+  </si>
+  <si>
+    <t>O postanku imena grada Zagreba postoje različite teorije. Po jednima se izvodi od glagola zagrepsti, odnosno, ukopati.[5] Po drugima se dovodi u svezu sa starim hrvatskim imenom za obalu „b(e)reg” koju i danas koriste u krašićkom kraju gdje Zagreb nazivaju Zabreg.
+Većina povjesničara danas smatra da ime Zagreb ima svoj korijen u složenici „zagrebb”, tj. „mjesto za utvrdom” ili pak „za brdom”. U novije vrijeme sve je prihvaćenija i teorija o tome da je prije osnivanja zagrebačke biskupije i naselja na kaptolskom brdu ondje postojao samostan posvećen sv. Gabrijelu (San Gabriel, „Za'Gabriel”) od kojega je u konačnici i Zagreb dobio ime.
+Iako je vremenom naziv Zagreb postao sinonimom za sva naselja na prostoru okolo i na gradečkomu i kaptolskomu brežuljku, a nakon spajanja naselja 1850. godine i službeni naziv za novi grad, to nije oduvijek bilo tako. Naime, naziv Zagreb u početku se odnosio na kaptolski brežuljak, točnije na jedno od naselja na njemu. Iako Felicijanova isprava svjedoči da se biskupija osnovana sa središtem na Kaptolu nazivala zagrebačka (lat. zagrabiensem episcopatum), prvi spomen naziva Zagreb dolazi s popisa biskupskih posjeda iz 1201. godine u latinskomu obliku Zagrabia i odnosi se na naselje na prostoru današnje Opatovine, koje se 40 godina kasnije ponovno javlja kao villa zagrabiensis. Da se naziv Zagreb u početku nije odnosio na naselje smješteno na susjednomu brdu svjedoči jedan od najranijih spomena zagrebačkoga Gradeca. Naime, nešto više od desetak godina nakon što je 1242. godine Zlatnom bulom Bele IV. osnovan Gradec uz uvjet podizanja zidina, godine 1261. spominje se naselje kao „utvrda Grič kraj Zagreba”. Svega pet godina kasnije, 1266. godine, naselje se ponovno spominje u jednoj od isprava Bele IV. u kojoj Bela IV. navodi „odredili smo da se sagradi utvrda na brdu Gradec kraj Zagreba”. Od slavenskoga naziva Gradec razvio se i njemački oblik Grez ili Grech, a u 13. stoljeću prvi se puta javlja i poznati njemački naziv za Zagreb (Agram) u obliku Agrim.
+O nastanku imena grada govori poznata legenda, u kojoj stari drevni ban, umoran i žedan, naredi djevojci Mandi da donese vode s izvora. Ban reče: "Mando, dušo, zagrabi"!
+Prvi pisani spomen Zagreba datira iz 1094. godine kada je na Kaptolu osnovana biskupija, što govori da je tu i ranije postojalo naselje.
+Stara jezgra današnje Gradske četvrt Gornji grad - Medveščak, ujedno i jezgra Zagreba, svoj gotovo tisućljetni razvoj započela je na dva brežuljka koja je razdvajao potok Medveščak što je s podnožja Medvednice tekao prema Savi koritom na kojem su smještene današnje ulice - Medvedgradska i Tkalčićeva. Na istočnom je brežuljku niknuo biskupski Kaptol, a na zapadnom naselje Gradec - Grič.
+Zagrebačku biskupiju je na Kaptolu utemeljio ugarski kralj Ladislav 1094. izgradnjom prvostolnice - crkve sv. Stjepana, a koja je dovršena tek nakon 123 godine, odnosno 1217. Otad je, što zbog potresa ili požara, više puta obnavljana, preuređivana i dograđivana. Svoj današnji izgled je dobila tek 1895. nakon obnove i preoblikovanja, a kojima se trebalo pristupiti zbog jakog potresa iz 1880., prema projektu arhitekata Bollea i Schmidta. U drugoj polovini 15. i na početku 16. st., u vrijeme najjačih prijetnji turskih osvajača, oko Kaptola su podignuti obrambeni zidovi i kule, a što je u velikom dijelu sačuvano do danas. Zagrebački kanonici 1334. naseljavaju kaptolske kmetove u blizini svojih domova, sjeverno od Kaptola. Tako nastaje naselje, današnja Nova Ves koje je s Vlaškom Vesi, također današnjom ulicom, smještenom podno južnih kaptolskih bedema, pod jurisdikcijom Kaptola.
+Gradec je 1242. Darovnicom kralja Bele IV. proglašen “slobodnim i kraljevskim gradom na brdu Gradecu zagrebačkom”. Grad je tim aktom dobio položaj feudalca koji je odgovoran izravno kralju. Građani su, među ostalim, stekli pravo svake godine birati “gradskog suca” (gradonačelnika) i upravljati gradskim životom. Pritom su preuzeli i određene obveze pa su, izvršavajući jednu od njih, u razdoblju od 1242. do 1266. utvrdili grad bedemima i kulama. Gradnjom zidina, Gradec je dobio urbanistički lik po kojem i danas prepoznajemo Gornji grad. Prateći oblik brežuljka, bedemi opasuju grad u formi nepravilnoga istokračnog trokuta s vrhom kod Popova tornja na sjeveru te s osnovicom na Strossmayerovu trgu na jugu. U grad se ulazilo na četvera glavna vrata - Mesnička na zapadu, Nova, kasnije nazvana Opatička na sjeveru, Dverce na jugu i Kamenita na istoku. Jedino su Kamenita vrata sačuvana do danas. Već u 13. st. je na središnjem gornjogradskom trgu stajala crkva sv. Marka, nešto manja negoli je današnja, a koja je nanovo podignuta ili temeljito pregrađena sredinom 14. ili početkom 15. st. Najvrjednija starina Markove crkve je njezin južni gotički portal. Na uglu Markova trga, na ulazu u današnju Ćirilometodsku ulicu, već je u srednjem vijeku stajala Gradska vijećnica, sjedište Gradske uprave, a koja je kasnije dograđivana, rušena, ponovo građena i pregrađivana. Formiranje današnjega središnjeg zagrebačkog trga - Trga bana Josipa Jelačića je započelo 1641. s otvaranjem novog sajmišta u nizini podno Gradeca i Kaptola, gdje se nalazio veći izvor Manduševec i po kojem je Trg dobio i svoje prvo ime. Oko tog okupljališta tadašnjeg “poslovnog svijeta” Zagreba i drugih krajeva, kasnije nazvan Harmicom, postupno se zahuktala gradnja kuća i pristupnih putova pa se npr. današnja Petrinjska ulica u 18. st. zvala Med grabami, što odlično ilustrira njezin tadašnji izgled i okoliš u kojem je nastajala.
+Sjedinjavanje nekad oštro razdvojenih, nerijetko i žestoko zavađenih naselja na susjednim brežuljcima i onih u njihovu podnožju, u formalnom je smislu započelo objavom Privremenog obćinskog reda za kraljevski grad Zagreb 7. rujna 1850. Tim je aktom određen pojam Zagreba. Umjesto malih starih općina, konstituiran je jedinstveni grad koji je obuhvatio Gradec, Kaptol s Vlaškom ulicom i općinu Horvati. Ukinute su stare feudalne pravice, propisane još u Zlatnoj buli, a uveden je demokratski ustroj i rukovođenje gradom u kojem sudjeluju širi slojevi zagrebačkoga građanstva. Gradska je uprava otad mogla pa i morala upravljati na moderniji način.
+Prostor Gornjega grada - Medveščaka već je stoljećima središnja pozornica zagrebačke i hrvatske povijesti. Zahvaljujući tomu, svaka stopa toga dijela Zagreba ima svoje povijesno-spomeničko i simboličko značenje, osobito tri tamošnja najpoznatija trga - Trg bana Josipa Jelačića, Kaptol i Markov trg.
+U razdoblju od 1945. do 1952., područje današnje gradske četvrti Gornji grad - Medveščak pripadalo je I. i II. gradskom rajonu (Centar i Medveščak). Rajoni su 1952. ukinuti pa uže gradsko područje prelazi u upravnu nadležnost Narodnog odbora Grada. Samo godinu dana kasnije se osnivaju općine na užem gradskom području. Prostor današnjega Gornjega grada - Medveščaka ulazi u okvir dviju općina: Gornji grad i Medveščak. Spajanjem dotadašnjih općina Gornji i Donji grad, 1955. nastaje Općina Centar. Od 1967. do 1974. Grad Zagreb funkcionira kao jedinstvena općina. Ponovnim osnivanjem općina 1974., dijelovi Gornjega grada - Medveščaka pripadaju općinama Centar i Medveščak, a koje djeluju do 31. prosinca 1990. U veljači 2009. je na području Gradske četvrti Gornji grad - Medveščak osnovano 13 mjesnih odbora.</t>
+  </si>
+  <si>
+    <t>Krapina, glavni grad Krapinsko-zagorske županije koji krase ne samo prirodne ljepote nego i bogato kulturno naslijeđe. Starodrevni hrvatski grad Krapina prvi put se spominje u pisanim povijesnim vrelima krajem 12. stoljeća, a razvijeno gradsko naselje koje je nosilo isto ime od sredine 14. stoljeća. Sam je grad postojao i ranije, a to potvrđuju brojni arheološki nalazi ne samo iz razdoblja vladavine Rimljana nego i iz ranijih razdoblja kamenog doba. Naime, Dragutin Gorjanović Kramberger otkrio je ostatke krapinskog diluvijalnog čovjeka na brdašcu blizu samog centra Krapine, Hušnjakovom, te je utvrdio kako je to nalazište staro oko 130 tisuća godina.
+ Što se tiče pisanih povijesnih dokumenata vraćamo se u 1193. godinu kada je Krapina prvi puta spomenuta u povelji kojom je pečuški biskup Kalan, a ujedno i upravitelj Kraljevine Dalmacije i Hrvatske dopustio zagrebačkom biskupu Dominiku i njegovim nasljednicima pravo ubiranja desetine od uroda žitarica i vina u Krapini, Okiću i Podgorju. Uz mjesto Krapina spominje se 1225. godine i kraljevska utvrda, tkz. burg u kojem je 2. lipnja spomenute godine boravio hrvatsko-ugarski Bela IV. Arpadović. 
+ Najstariji pisani spomenici, u smislu izvorne arhivske građe, potječu dakle s kraja 12. stoljeća, a nastavljaju se, u obliku kraljevskih povlastica, od početka 13. pa sve do sredine 19. stoljeća. Sama povijest grada najviše se čuva upravo u tim povlasticama preko kojih saznajemo o brojnim zanimljivostima o životu i radu građana Krapine. 1347. godine kralj Ludovik I. Anžuvinac dodijelio je Krapini privilegij slobodnog kraljevskog grada i time Krapincima omogućio znatnu autonomiju. Nakon njegove smrti, krapinsku utvrdu i pravo izravnog vladanja u Krapini naslijedio je novi hrvatsko-ugarski kralj – Žigmund Luksemburški koji je vladao od 1387. do 1437. godine. Kroz povijest krapinska je utvrda često mijenjala vlasnike, bilo da se radilo o kupnji, ženidbi ili darivanju i tako su tamo stolovali kneževi Celjski (nakon što su dobili „Stari grad“ od kralja Žigmunda dobivaju i titulu grofovi Zagorski), obitelj Keglević, obitelj Drašković, grof Wojkffy, a posljednji gospodari grada bile su obitelji Lichtenberg i Ottenfels. 
+Prirodni položaj Krapine i okolnih mjesta našao se i na meti renesansnih kartografa svjetskoga glasa. Radi se o najstarijim hrvatskim kartografima – Trogiraninu Ivanu Lučiću i Varaždincu Stjepanu Glavaču koji su u svojim zemljopisnim kartama, tiskanima u srednjoeuropskim gradovima već od 16. stoljeća, pažljivo zabilježili Krapinu i njenu okolicu. 
+Kolika je bila važnost Krapine svjedoči i činjenica da je za vrijeme najtežih turskih navala na Hrvatsku, krajem 16. i početkom 17. stoljeća, u krapinskoj utvrdi održano čak pet hrvatskih Sabora (1598., 1599., 1600., 1605. i 1607. godine). Na to je utjecao status samog grada u kojem su cvjetali trgovački i obrtnički poslovi, redovito se održavali godišnji i kraljevski sajmovi na kojima su sudjelovali i strani građani što je ujedno i doprinijelo razvoju školstva, urbanizacije, uprave i sudstva.
+Razvoj grada na temelju kraljevskih privilegija prestaje u doba hrvatskog narodnog preporoda koji je započeo krajem 18. stoljeća, a sam vrhunac doživio sredinom 19. stoljeća, točnije 1848. godine, kada je Josip Jelačić imenovan hrvatsko-slavonsko-dalmatinskim banom. Te je iste godine ukinuo feudalni poredak i o tome obavijestio sve općine i gradove posebnim Banskim pismom, pa tako i Krapinu. Na taj je način Krapina zakoračila u novo doba – doba moderne Krapine, moderne gradske uprave, modernog građanskog društva.
+Otac hrvatskog narodnog preporoda, Ljudevit Gaj, rodom iz Krapine, pokrenuo je zajedno s ostalim hrvatskim preporoditeljima, osnivanje modernih preporodnih ustanova, najprije u Zagrebu, a ubrzo i u Krapini. Otvaraju se podružnice Matice hrvatske, Hrvatsko-slavonskog gospodarskog društva, Narodnog kazališta, Narodnog muzeja i naravno, čitaonice (1845. godine) kao „žarišta preporoda“. Osim kulturnog zamaha, preporod je donio i određene gospodarske pomake – dojučerašnji je kmet nakon 1848. godine postao slobodni građanin s pravom sudjelovanja u cjelokupnom javnom životu, došlo je do osnivanja modernih trgovačkih poduzeća i obrtničkih radionica kao i organizacija gospodarskih izložbi od kojih su neke imale i međunarodno značenje, a njima sudjeluju i gospodarstvenici iz Krapine.
+Modernizacijski procesi u gradu nastavljaju se i tijekom druge polovice 19. stoljeća pa sve do izbijanja Prvog svjetskog rata. Grad dobiva modernu upravu i sudstvo, a i mijenja se socijalna struktura stanovništva - prisutno je povećanje pučanstva, stvaranje novih društvenih struktura, u javni život polako ulaze i žene, povećava se pismenost. Veliku ulogu u svemu tome imala je i gradnja „Zagorske željeznice“ koja je prvi put protutnjila ovim krajem 1886. godine i zbog svoje važnosti prozvana je „žilom kucavicom“ Hrvatskog zagorja. Daljnji razvoj Krapine vidljiv je u otvaranju brojnih kulturnih i prosvjetnih ustanova od javnoga značenja - osim pučke i srednje škole, tu su i Društvo čitaonice, Pjevačko društvo, Društvo Crvenoga križa, Vatrogasno društvo i različita dobrotvorna društva. Brojne se obrtničke zadruge također nastoje modernizirati. Neke od njih postupno se uređuju u moderna industrijska postrojenja i zapošljavaju veći broj radnika, kao npr. glasovita tvornica kamenine („Krapinske kamenine“) u krapinskoj kuriji sačuvanoj sve do danas na uglu Magistratske ulice i Ulice D. G. Krambergera, a njihov se položaj krajem 19. stoljeća sve više regulira prema zahtjevima prvoga hrvatskog Obrtnog zakona. Sve to stavlja Krapinu u klasu s razvijenijim hrvatskim gradovima toga vremena.
+Kada govorimo o Krapini, moramo staviti naglasak i na vjerski život grada u kojem je već od sredine 13. stoljeća katolička župa, a župna crkva sv. Nikole spominje se već početkom 14. stoljeća. Uz crkvu su djelovali brojni zaslužni župnici i svećenici, a tijekom druge polovice 18. stoljeća posebno svečano i važno mjesto u gradu zauzima crkva Majke Božje Jeruzalemske na Trškom Vrhu koja ubrzo postaje naširoko poznato proštenište. Istovremeno su u gradu djelovale i brojne kršćanske bratovštine kulturno-prosvjetnog i humanitarnog značenja. Župna crkva sv. Nikole i pripadajuće kapele te kasnije crkva i samostan franjevaca s bogatom knjižnicom od 8000 naslova, bili su i ostali simbolima Krapine, ali i središnja urbana jezgra grada. Kako su godine, desetljeća odmicala tako su oko njih nastajale gradska vijećnica, škole, kurije velikaša, razvijale se gradske prometnice, trgovi, zelene površine, postavljali se javni gradski spomenici... 
+Sastavni dio opće kulture građana potvrđuje se i u njegovanju zdravstvene kulture, koja je na različite načine i u skladu s razvojem medicinske znanosti, prisutna u Krapini već u razdoblju srednjovjekovlja. Modernija zdravstvena kultura razvija se od sredine 18. stoljeća kada na području Krapine nalazimo više stručnih ranarnika, ljekarnika i liječnika. Početkom 20. stoljeća, točnije 1903. otvoreno je glasovito Kneippovo lječilište tkz. krapinske mrzlice, a potom i moderni Dom zdravlja koji djeluje i danas.
+Krapina je danas kulturno, upravno i političko središte županije Krapinsko-zagorske te grad koji je izrazito ponosan na svoju povijesnu baštinu, dugu tradiciju školstva i obrtništva.</t>
+  </si>
+  <si>
+    <t>53000 Gospić</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>44.54</t>
+  </si>
+  <si>
+    <t>15.37</t>
+  </si>
+  <si>
+    <t>Područje Gospića i njegove okolice naseljeno je od pretpovijesti (u starije kameno doba, te u kontinuitetu u brončano i željezno doba). Dokaz tomu su brojni arheološki nalazi, što se posebice odnosi na željeznodobno pleme Japoda. Lika obliluje kamenom i drvo pa su se od toga radile kuće, a stanovništvo se stoljećima bavilo stočarstvom, jer nije bilo uvjeta za zemljoradnju. 
+U antičko doba, ovaj je prostor obilježen jednom od najznačajnijih prometnih komunikacija što je iz unutrašnjosti (Siscia), kontinentalnim pravcem vodila prema jugu i morskoj obali (Salona). Na ovom području i prije dolaska Hrvata živjelo je autohtono domorodačko stanovništvo kojeg su činili potomci Japoda i rimski doseljenici, koji su vladali Likom, koja je bila u sklopu Rimskog Carstva. Rimljani su gradili puteve, postaje, širili svoju kulturu i običaje. 
+Pokazatelji o razdoblju hrvatskih narodnih vladara i stvaranju hrvatske države su ulomci starohrvatskog pletera, pronađeni u nekoliko stilskih i vremenskih odrednica na nekoliko lokaliteta u neposrednoj blizini Gospića. Oni nas ujedno upućuju i na brojne sakralne građevine i kršćansku pripadnost stanovništva ovog prostora u srednjem vijeku. 
+Od 11. stoljeća jačaju plemenitaške obitelji, koje uz gospodarski razvitak, grade svoje dobro utvrđene gradove – burgove, te u njima razvijaju kulturne i duhovne tekovine ondašnjeg doba. Obitelji su to Tolimirovića, Mogorovića, Tugomirića, Disislavića i drugih. 
+Začetke naselja današnjeg grada otkrivamo u ispravi iz 1263. godine, u kojoj kralj ugovara zamjenu posjeda s ličkim županom Petrom Tolimirovićem, u kojoj se između ostalih, spominje i naselje Kaseg, a kasnije Kasezi, na lijevoj obali rijeke Like, pored potoka Novčice. Poznato je da je kralj Bela IV., s ličkim županom Petrom Tolimirovićem ugovorio zamjenu toga grada. Kralj je za Počitelj dao ličkom županu sela Kaseg (današnji grad Gospić), Sičevo, Grebenar i Brotnjan. Iz nešto kasnijih isprava doznajemo da su u Kasegu živjeli lički rodovi Mogorovići, Korini, Vidasi, Prohočići, Ljutčid i Lukšići. 
+U vrijeme turskih prodora Kasezi se raseljavaju, te nanovo naseljavaju, sudeći po riječima putopisca koncem 18. stoljeća koji spominjući Gospić, govore o gradu koji "bijaše prije kukavni turski grad", u kojem "Grci" imaju malu crkvu s kipom Gospe, a po čemu je Gospić dobio ime.
+Brojne su legende o nastanku naziva Gospić. Jedna je priča o dvije kneginje od kojih je jedna Gospava osnovala ovdje grad, do teorije da naziv dobiva po hospitiumu u Kaniži kojeg su osnovali karlobaški kapucini (1721. g.), no tada je poznati naziv već ustaljen.
+U prvom popisu na području današnjeg grada ili sasvim blizu njega, nalazi se selo Gospojina u nahiji (kotaru) Novi, a 1604. godine kao naselje Gospić.
+Temelj današnjeg grada, udaraju dvije turske kule – kula age Senkovića na prijelazu preko rijeke Novčice (danas najstarija kuća u gradu), te kula age Alića, na kojoj se i danas vide ostatci kružnog tlocrta na lokaciji Kulina (poznat kao Rajčić-grad). Od 1527. do 1689. bio je pod vlašću Turaka.
+Prije dolaska Turaka, u Lici su živjeli uglavnom Hrvati. Iako je na području Like bilo mnogo utvrđenih gradova, nije bilo vojske ni stanovništva koji bi ih branili od Turaka u vrijeme napada. Zbog opasnosti od Turaka i mnogobrojnih upada, mnogobrojno stanovništvo se povuklo u sigurnije krajeve pa su Turci osvojili cijelu Liku. Opustjelu Liku, Turci su naseljavali Vlasima, koji su većinom ostali i nakon odlaska Turaka. Središte Ličkog sandžaka bilo je u Širokoj Kuli kraj Gospića.
+Nakon izgona Turaka iz Like 1689. godine pod zapovjedništvom generala Herbersteina, od konca 17., tijekom 18., a posebice u 19. stoljeću, Gospić dobiva prepoznatljive urbanističke odrednice kao upravno, administrativno, političko, vojno i kulturno središte ličkog prostora. Hrvati koji su napustili Liku dolaskom Turaka, nisu se više vraćali, nego su u Liku doselili novi Hrvati uglavnom iz Gorskog kotara, Dalmacije i Primorja. 
+To je vrijeme izgradnje današnje katedralne crkve Navještenja Blažene Djevice Marije (1781. – 1783.), gradske kapelice Sv. Ivana Nepomuka, premda je ona već postojala prije 1756. godine (spominje se u gospićkoj Matici umrlih 1759. godine), a na toj lokaciji pored kapelice bilo je i groblje. 
+Širenjem gradske jezgre i populacije, osjeća se potreba za novim prostorom gradskog groblja, te se ono premješta na današnju lokaciju i gradi kapelica posvećena Sv. Mariji Magdaleni (1856.), ujedno zaštitnici Grada. 
+Od 1729. g. Gospić je sjedište Ličke i Otočke pukovnije, ali i stožerno mjesto, pa je intenzivirana izgradnja za vojne, časničke potrebe – zgrada generala brigadira (1767.), general pukovnika (1798. g.), zgrada za liječnike. 
+Godine 1729. osniva se i prva pučka škola, 1766. njemačka škola, 1799. "normalka", 1823. matematička škola za obrazovanje dočasnika, Djevojačka škola, pa zatim Viša domaćinska škola. 
+U doba napoleonove vladavine, Lika je bila jedno vrijeme do 1814. pod vlašću Francuza. Sagrađene su nove ceste, škole i upravne zgrade. Dio stanovnika se iselio, jer nisu htjeli služiti u francuskoj vojski. Nakon pada Napoleona, Lika je ponovno pod austrijskom vlašću. Gospić je središte Ličko-krbavske županije od 1886. do 1924. godine. Površina je bila slična današnjoj Ličko-senjskoj županiji, ali s područjem Gračaca. Županija je imala 204 710 stanovnika 1910. godine. Prema popisu stanovnika 2011. godine, Ličko-senjska županija imala je 50 927 stanovnika. 
+U 19. stoljeću grade se i novi gradski mostovi: preko Novčice 1804. g. i preko Bogdanice 1845. godine U okolici Gospića rođena su dva velikana u 19. stoljeću. Ante Starčević rođen je 1823. godine u mjestu Veliki Žitnik.[12] Pučku školu pohađao je u Klancu.[13] Nikola Tesla rođen je 9./10. srpnja 1856. godine u mjestu Smiljan. Već s pet godina Nikola se šetao po Velebitu koji se nadvijao iznad njegova rodnog sela. Budući izumitelj svjetske slave pohađao je njemačku osnovnu školu u Smiljanu, a istu je završio u Gospiću. Za vrijeme vatrogasne vježbe na rijeci u Gospiću, dogodio se kvar, a popravio ga je Tesla. Skočio je u vodu gdje se nalazio drugi kraj vatrogasne cijevi, koji je bio začepljen. Nikola je cijev vrlo brzo odčepio, pa je voda iz pumpe suknula po okupljenim građanima. Bio je iznesen na ramenima i postao heroj dana.[14] Gimnaziju je pohađao u Gospiću, potom u Rakovcu kraj Karlovca, gdje je maturirao. Uredio je gospićku knjižnicu. U školi je bio dobar đak, jedino mu slobodno crtanje nije polazilo za rukom. Najdraži predmet bila mu je matematika. Kad je završio treći razred niže realne gimnazije u Gospiću, teško se razbolio i čak je izgledalo da će umrijeti. 
+Gradsku jezgru krasi i brončani kip Vodarice Marte nepoznatog autora, postavljen u čast dovršenja gradskog vodovoda Brušane – Gospić 31. prosinca 1893. g. (pušten u rad 1. siječnja 1894. godine). 
+Željeznička pruga prolazi 1920., a prvi vlak 1921. godine.
+Razdoblje austro-ugarske vlasti, odnosno Vojne krajine, ostavilo je povijesnu jezgru grada, koja je tijekom francuskih prodora i iste, kratkotrajne vladavine (brončani reljef Roberta Frangeša-Mihanovića u spomen na Bilajsku bitku 1809., na pročelju Katedrale), zatim ratna razaranja tijekom I. i II. svjetskog rata, te Domovinskog rata, ali i urbanističkih rješenja u ime razvitka 70-ih godina 20. stoljeća, doživljavaju brojne devastacije i preinake.
+Od kraja 19. stoljeća, pa do 1940. godine, Gospić živi intenzivnim životom manje metropole.
+Polovicom 19. stoljeća sjedištem je Ličke pukovnije (Lička krajiška pješačka pukovnija cara Franje Josipa br. 1., nje. Kaiser Franz Josef Likaner 1 grenz Regiment).
+Kulturne ustanove su vrlo aktivne, osnutak Matice hrvatske, Hrvatskog sokolskog društva, razvijaju se brojne sportske udruge, građani se angažiraju u osnivanju i radu različitih udruga i društava (Gospićko pjevačko društvo "Hrvat", Dobrovoljno vatrogasno društvo i dr.).
+Godine 1900. u gospićkoj park šumi Jasikovac bilo je tenisko igralište, prvo u ovom dijelu Europe.
+No, u političkom svijetu, Gospić proživljava svoju kalvariju. Težak život i gušenje nacionalne pripadnosti u Kraljevini Jugoslaviji pod žandarmerijskim terorom velikosrpskih hegemonista, rezultira Velebitskim, odnosno Brušanskim ustankom 1932. godine. Gospić je prije Drugog svjetskog rata bio grad obrtnika i službenika. Hrvati, iako većina, bili su obespravljeni i izvrgnuti nasilju srpske manjine.
+Gospić je prije i tijekom Drugog svjetskog rata bio poznat po jakoj ustaškoj organizaciji. Za vrijeme Drugog svjetskog rata, Gospić je bio u sastavu NDH-a, sve do 4. travnja 1945. Vlast NDH-a u Lici neprestano je funkcionirala tijekom Drugog svjetskog rata jedino u Gospiću. U Gospiću je već ranije djelovala skupina istaknutijih Pavelićevih pristalica, uglavnom intelektualaca, npr. Andrija Artuković, Jozo Dumandžić, Jurica i Mate Frković. Jozo Dumandžić imao je odvjetničku pisarnu zajedno s Andrijom Artukovićem u Gospiću prije rata. Logor Jadovno bio je sabirni logor u dolini Velebita, zapadno od Gospića, koji je 1941. vodila Ustaška obrana tijekom NDH. Djelovao je od 11. travnja do 25. kolovoza 1941. godine po nalogu Eugena Dide Kvaternika. Logorski sustav sačinjavali su tadašnji zatvor u Gospiću, logor na Velebitu i logor Slano na otoku Pagu. U logoru, koji je izradilo nekoliko stotina mladih Židova iz Zagreba, završili su brojni konvoji koji su vlakovima stizali iz cijele Hrvatske i dalje pješice na Velebit.
+Kada su nakon uzaludnih pokušaja tijekom rata, 4. travnja 1945. partizani ušli u Gospić dogodile su se brojne likvidacije. Najprije su prvih 48 sati ubijali Gospićane koje su ranije popisali za odstrjel. Među više partizanskih zatvora u Gospiću isticale su se kaznionica u gradskom središtu i zgrada u kojoj je do dolaska partizana bila financija na Tratini blizu Kaniškoga mosta na rijeci Bogdanici.  Brojni građani odvođeni su na stratište, te im se ni danas ne zna posljednje počivalište. Jedno od takvih mjesta je pored današnjeg gradskog groblja Sv. Marije Magdalene, kojem uskoro predstoji civilizirano obilježavanje dostojno žrtve. Među ubijenima su i svećenik i pisac Dragutin Kukalj te redovnica i medicinska sestra Žarka Ivasić, mučenica, za koju je pokrenut biskupijski postupak za proglašenje blaženom. Tijela pobijenih Hrvata nalaze se po neobilježenim i neistraženim stratištima i skupnim grobištima koja su danas zarasla pod šumom i šikarom, a nalaze se u obližnjim mjestima i predjelima Divoselo, Imovina, Jasikovac, Korenica, Ljubovo, Smiljan, Široka Kula, pa čak i u Karlobagu. 
+U doba Jugoslavije, Gospić se relativno slabo razvijao u odnosu na druga područja, dijelom iz geografskih, dijelom iz ekonomskih, a najvećim dijelom iz političkih razloga. Tome je pridonijela i ekonomska migracija u druge dijelove Hrvatske, a od 1960-ih i zemlje Zapadne Europe i Kanadu. Time je nastavljen demografski trend depopulacije Like koji traje do današnjih dana. Unatoč tome bilo je industrijalizacije. Godine 1950. godine osnovana je u Ličkom Osiku tvrtka "Ivan Gošnjak", koja je 1954. godine primijenila naziv u Radna organizacija „Marko Orešković“ Lika (skraćeno MOL). Do početka 1990-ih godina tvornica MOL bila je najznačajnije poduzeće metalne industrije Like s oko 1500 zaposlenika, za koje je sagrađeno novo naselje u Ličkom Osiku, koje je rijedak primjer novoplaniranog grada nastalog u Hrvatskoj u drugoj polovici 20. stoljeća.
+Težnju hrvatskog čovjeka za svojom državnošću i stvaranje moderne države Hrvatske, Gospić je dočekao 1990. godine, no već se iduće godine našao u ratnom vihoru kojem se herojski usprotivljuje i nakon niza vojno-redarstvenih akcija kojima brani svoj teritorij i završetka Domovinskog rata, 1995. godine pristupa obnovi razrušenog grada, izgrađujući danas moderno županijsko središte. Na prvim demokratskim izborima 1990. godine, s obzirom na svoju hrvatsku većinu, Gospić se opredijelio za Hrvatsku demokratsku zajednicu. Ubrzo nakon toga, područja Gospića sa srpskom manjinom priključila su se nacionalističkom pokretu koji će dovesti do stvaranja Republike Srpske Krajine. Dio Srba ostao je na hrvatskoj strani.
+Grad je bio jednim od važnih strateških i psiholoških ciljeva velikosrpskim snagama. Prvo značajnije uznemirenje situacije je bilo u lipnju 1991., a u rujnu su se bile vodile žestoke bitke za grad. Prijetila je opasnost da će ga velikosrbi zauzeti i situacije je bila vrlo neizvjesna.
+Gospićani su prvih dana uspjeli zaustaviti napredovanje četničkih bandi. Policija, ZNG i građani zauzeli su crtu bojišta koja nikada nije probijena.
+Već 4. rujna osnovana je proslavljena 118. brigada HV s prvim zapovjednikom Mirkom Norcem. Najžešće pješačke borbe vođene su od novog mosta na Novčici do Alarovog brda 10. rujna 1991. godine kada su tenkovi gotovo ušli u grad. Nakon pada perušićke vojarne 14. rujna, potom 18. rujna vojarne u Gospiću, hrvatske su se postrojbe imale s čime braniti. Međutim, na okupiranim područjima nastavljeni su masakri nad hrvatskim civilima, ubijani su civili u Lovincu, Perušićkoj Kosi, Širokoj Kuli, Urijama, Ličkom Osiku...
+Napadi na Gospić i okolna mjesta nisu jenjavali. U znak odmazde za uspješnu akciju hrvatskih snaga u Divoselu koja je izvedena 16. listopada, četničko je topništvo 19. listopada 1991. punih 10 sati bez prestanka tuklo po Gospiću. 
+U tim najtežim napadima grad je gorio na dvadesetak mjesta. Prema grubim procjenama, samo toga dana na Gospić je palo više od tisuću projektila, po nekim izvorima znatno više.
+Između 16. i 18. listopada 1991. u Gospiću su hrvatski vojnici ubili između 23 i 50 lokalnih civila, većinom srpske nacionalnosti. Masakr se dogodio samo tri dana nakon što su srpski vojnici počinili pokolj nad Hrvatima u Širokoj Kuli. Hrvatski vojni sud kasnije je utvrdio brojku od 50 ubijenih civila; polovica (24) su bili Srbi. Zapovjednik akcije, general Mirko Norac, osuđen je 2003., zajedno s četvoricom ostalih, za odgovornost. Osuđeni su i Tihomir Orešković na 15 godina zatvora i Stjepan Grandić »Štef« na 10 godina zatvora.
+Dana 1. studenoga 1992. godine osnovana je 6. (kasnije 9.) gardijska brigada HV. U prvoj većoj osloboditeljskoj akciji HV-a, u siječnju 1993. godine na Maslenici je sudjelovala i gospićka 9. gardijska brigada. Bez ijednog izgubljenog vojnika, deveta je iz Rovanjske silovito potisnula brojčano i tehnički nadmoćnijeg neprijatelja i zauzela visove kod Tulovih greda. Na tim položajima zamjenu je obavila 118. brigada HV koja je uz ljudske žrtve u travnju odbila siloviti napad "Niških specijalaca", zrakoplova i topništva tzv. "vojske Krajine". U međuvremenu napadi na Gospić bili su gotovo svakodnevni i pala je odluka da se zauvijek ušutkaju četnički topovi u Divoselu i Čitluku.
+Ove dvije brigade HV su uz pomoć policije sudjelovale u oslobađanju područja "Medačkog džepa". Akcija je provedena 9. rujna 1993. godine, a broj topničkih napada na Gospić nakon tog datuma je prepolovljen. Zbog ubojstava civila i ratnih zarobljenika u akciji, na višegodišnju zatvorsku kaznu je osuđen (po zapovjednoj odgovornosti) general Mirko Norac, jedan od zapovjednika akcije.
+U veljači 1994. godine četnici su na obroncima Ljubova nastojali osvojiti položaje Hrvatske vojske kod kote "Repetitor". Nakon četverodnevnih borbi, četnici su uz jake gubitke uzmakli. Tijekom borbi, Gospić i Perušić nemilice su granatirani. 
+Dana 4. kolovoza 1995. godine u 6.00 sati pokrenuta je operacija Oluja.
+Združene snage pričuve i profesionalnaca krenule se na svim položajima.
+Nesavladivo "gvozdeno Ljubovo", kako su ga zvali Martićevci, popustilo je već prvog dana, da bi 5. kolovoza hrvatske snage ušle u Lički Osik, Bunić, Svračkovo Selo, Podlapaču, Medak. Brojni civili koji su zatečeni u oslobađanju izjavili su kako su paravojne postrojbe bježale pred civilima, ostavljajući ih bez prijevoza i zaliha hrane. Susretom sa snagama Armije BiH na rijeci Uni, na ovim je prostorima rat završio jer su Srbi pobjegli u Republiku Srpsku i SR Jugoslaviju.
+Neprijeporna je istina da je Gospić nakon Vukovara najrazrušeniji hrvatski grad, za čiju je slobodu živote položilo više stotina vojnika, policajaca i civila. 
+U usporedbi s 1991. godinom, broj Hrvata je porastao s 5015 na 11 860 2011. godine, a broj Srba je pao s 3243 1991. godine na 609 stanovnika 2011. Nakon završetka Domovinskog rata, Gospić se s obzirom na velika ratna razaranja, teško oporavljao, a od 2000. godine dodatni problem su predstavljale političke napetosti s novom vladom lijevog centra. U kolovozu 2000., u Gospiću je ubijen Milan Levar, hrvatski branitelj i zaštićeni haaški svjedok.[27] Nakon toga, provedene su policijske istrage i suđenja te sudske presude za ratne zločine na koje je Levar ukazivao. Nakon rata ostale su brojne mine u okolici Gospića. 
+Dana 25. svibnja 2000. godine papa Ivan Pavao II. izdao je bulu kojom dijeli dosadašnju Riječko-senjsku nadbiskupiju na dvije crkvene jedinice: Riječku nadbiskupiju i Gospićko-senjsku biskupiju. Novoj biskupiji pripali su dekanati: gospićki, ogulinski, otočki, senjski i slunjski. Za prvog biskupa imenovan je Mile Bogović, sa sjedištem u Gospiću.
+Gospodarski poticaj napretku Gospića dala je izgradnja autoceste A1, koja prolazi kroz Gospić i Liku, otvorene 26. lipnja 2005. U Lici i Gorskom kotaru povoljan utjecaj nove prometnice na razvoj bio je primjetan i prije njezina dovršetka.[28]
+Prigodom 150. godišnjice rođenja Nikole Tesle, 10. srpnja 2006. u Smiljanu je otvoren Memorijalni centar »Nikola Tesla«.
+U Smiljanskom je polju početkom srpnja 2021. otvorena energana na biomasu za proizvodnju električne i toplinske energije.
+U organizaciji Ličko-senjske županije, Grada Gospića i Gospićko-senjske biskupije te uz potporu Ministarstva hrvatskih branitelja, u Gospiću je 3. travnja 2024. održan posljednji ispraćaj i pokop 253 žrtve Drugoga svjetskog rata i poslijeratnog razdoblja, ekshumirane na predjelu ispred gospićkoga groblja sv. Marije Magdalene.
+Dana 4. svibnja u Gospiću se okupilo deset tisuća mladih iz raznih dijelova Hrvatske i iseljeništva na XII. Susretu hrvatske katoličke mladeži.</t>
+  </si>
+  <si>
+    <t>45.84</t>
+  </si>
+  <si>
+    <t>17.40</t>
+  </si>
+  <si>
+    <t>170,7 </t>
+  </si>
+  <si>
+    <t>33000 Virovitica</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>Najstarije naseobine ljudi na području današnje Virovitice nalazimo u obližnjem brdskom zaleđu Bilogore. Prema tim pokazateljima tu su obitavali najstariji paleolitski ljudi. Bili su lovci, sakupljači hrane, a kretali su se širokim prostranstvima između Bilogore i rijeke Drave. Oko današnje Virovitice u pretpovijesno vrijeme živjela su ilirsko panonska plemena. O tim se plemenima ima spoznaje samo preko arheoloških nalaza.[4] Pouzdanije podatke o plemenima i naseljima iz ovog kraja se ima od antičkih zemljopisaca. Biocenoze koje su dominirale ovim krajem bile su velike hrastove šume koje su zauzimale velike površine te močvare kroz koje je ljudima bilo gotovo nemoguće prolaziti. Od šestog stoljeća bilježi se dolazak Slavena i Avara te pobjedu Hrvata nad Avarima. Od tog događaja na prostoru između Save i Drave dominiraju Slaveni.
+Godina „rođenja“ Virovitice je 1234. godina. Tada je slavonski herceg Koloman, sin kralja Andrije II. i brat Bele IV., Virovitici izdao povelju kojom je tadašnje naselje dobilo status povlaštenog trgovišta s odgovarajućim slobodama, odnosno, virovitičkim došljacima podaren je status građana slobodnog grada. Povelja je bila iznimno značajna u dobivanju punopravnog statusa srednjovjekovnoga grada, u vrijeme kada slična prava nisu imala mnoga mjesta u Slavoniji. U tom je vremenu Virovitica uživala iznimno značajan položaj pa su je često za posjećivanje, čime se potkrepljuje već navedena tvrdnja, koristili kraljevi iz kuće Arpadovića koji su tu imali i svoj sezonski dvorac. Istodobno, u Virovitici i oko nje, Koloman II. imao je svoje velike posjede. Današnji Zagreb, povijesno Gradec, „papirnato“ je zaživio u Virovitici. Povijest bilježi da je kralj Bela IV. bježeći pred Mongolima prema Trogiru preko Gradeca, izbjegao tragediju. Vraćajući se iz Trogira prema Slavoniji, Bela IV. zastao je u Virovitici gdje je tadašnjem Gradecu, današnjem Zagrebu, dodijelio status slobodnog grada, odnosno „Zlatnu bulu“. Bilo je to 16. studenog 1242. godine. 
+Povijest bilježi da je novo razdoblje za Viroviticu započelo 1429. godine kada je kralj Sigismund založio svoj kraljevski posjed za 10.000 forinti Emeriku Marczalyu. Tako je Virovitica postala privatni posjed te su Emerik i Ivan Marczaly dobili Viroviticu u trajno vlasništvo. Grad je nakon toga mijenjao vladare. Povijest Virovitice bilježi i pobunu seljaka u Donjoj Bukovici, 1479. godine, kada su se pobunili protiv pavlinskog samostana u koji su provalili, razbili brave te pretukli redovnike. Godinu dana kasnije pavlini i "svetogrdnici" su se izmirili jer su se pavlini odrekli naknade za štetu, a seljaci su odustali od potraživanja prema samostanu. Godine 1552. Turci i njihov Ulama Paša osvojili su Viroviticu koja je tada bila posjed Stjepana Banffya. Zadnji zapovjednik Virovitice Juraj Brodjanin i njegovih 50 haramija bili su bespomoćni pred naletom višestruko nadmoćnijeg neprijatelja te su se predali. Virovitica je pripala Požeškom sandžaku. Virovitica postaje snažno tursko središte. Imala je posadu od 300 konjanika i 300 pješaka. Pod turskom vladavinom postala je čvrst grad, okružen zidovima s jednom utvrdom u kojoj je smješteno topništvo s oko 300 kuća i 400 ljudi sposobnih za oružje, a u njoj stalno borave kapetan i turske age. Nalazila se u šumi medu drvećem i bila je četverokutnog oblika. 
+Kraj turske vladavine stigao je 1684. godine kada je carski general Leslea natjerao kapetana Alibega Muftiju na predaju. Iz Virovitice je tada otišlo 300 članova posade i oko 1000 turskih građana. Virovitica je potom pripojena Đurđevačkoj kapetaniji, a do kraja ljeta grad i njegova okolica zauvijek su oslobođeni od Osmanlija. Od tada započinje novo, mnogo povoljnije, razdoblje u razvoju Virovitice i cijelog tog kraja. Čitavo je virovitičko imanje 1753. darovnicom Marije Terezije dodijeljeno obitelji Pejačević, i to barunu Marku III. Aleksandru Pejačeviću, prvom srijemskom županu, i njegovim rođacima Josipu, Henriku i Ignjatu, kao naknada za imanje Mitrovicu, koje je pripojeno Vojnoj krajini. Nešto kasnije barunska obitelj dobiva grofovstvo i uzima naslov Pejačevići Virovitički. Na mjestu srednjovjekovne tvrđave koja je srušena na prijelazu iz 18. u 19. stoljeće, grof Antun Pejačević daje izgraditi dvorac, čija je gradnja trajala od 1800. do 1804. godine, prema projektu austrijskog arhitekta N. Rotha.
+U 19. stoljeću virovitički ogranak Pejačevića dolazi u financijske poteškoće te prodaje dvorac i pripadajuće vlastelinstvo, koje dolazi u ruke knezova Schaumburg-Lippe te doživljava novi gospodarski uspon. Danas se u dvorcu nalazi Gradski muzej. Oko dvorca je njegovani perivoj, djelomično devastiran izgradnjom gradskog bazena. 
+Virovitica se najviše počela razvijati u 20. stoljeću. Tako je 1902. godine otvorena Opća javna bolnica. Imala je 59 kreveta, jednog liječnika, pet časnih sestara, zavodskog slugu i dnevničara. Bilježi se razvoj trgovine jer je Virovitica oduvijek bila sajamski grad te razvoj drvne industrije. Tome je pridonijela i odluka Općinskog zastupstva da se Virovitica osvijetli električnom rasvjetom. Virovitička pošta dobila je telefonsku centralu, ukopčanu u promet s Bečom, a potom i s Trstom. Virovitica polako počinje dobivati današnje konture. Otvara se kinematograf, a nakon I. svjetskog rata otvorena su četiri razreda virovitičke Realne gimnazije. Napokon, 1921. godine Virovitica je proglašena gradom. U drugoj polovici 20. stoljeća bilježi se novi gospodarski zamah, a pritom se otvaraju mnogobrojna poduzeća i obrti. Virovitica se kontinuirano razvija do današnjeg dana kada je postala iznimno važno i jako regionalno središte. 
+U novijoj hrvatskoj povijesti Virovitica ima veliku, iznimno značajnu ulogu u Domovinskom ratu, posebice jer je Virovitica bila izraz stremljenja velikosrpske čežnje. Povijesne činjenice predstavljaju osobnu kartu identiteta svakog područja, grada, naroda i države pa je doprinos Virovitice u Domovinskom ratu i u obrani Hrvatske od srpskog agresora i agresije bivše JNA na Hrvatsku važan element povijesne istine o ulozi i značaju Virovitice u Domovinskom ratu i obrani Hrvatske. U toj cjelini vrlo važno mjesto ima suđenje Virovitičanima koji su zarobljeni u siječnju 1991. godine, a suđeno im je na Vojnom sudu u Zagrebu u prvoj polovici iste godine. Virovitica je bila prvi oslobođeni grad u Hrvatskoj jer je 17. rujna 1991. godine, u 11 sati i 20 minuta, zauzeta vojarna bivše vojske. Nekoliko dana prije toga zauzeta je i karaula i granični prijelaz Terezino Polje čime je Republika Hrvatska dobila svoju međunarodnu granicu. Akciji oslobađanja vojarne, uz jednu žrtvu, Vladu Vampovca, sudjelovalo je oko 400 pripadnika 50. samostalnog bataljuna Zbora narodne garde, MUP-a i rezervnog sastava policije. Iz 50. samostalnog bataljuna ZNG Virovitica, koji je osnovan po zapovijedi tadašnjeg ministra obrane generala Martina Špegelja, proizišla je 127. brigada ZNG Virovitica, jedna od najjačih brigada u Hrvatskoj, u kojoj je bilo aktivirano preko 4000 ljudi. Ratni zapovjednik 127. brigade bio je general pukovnik Đuro Dečak. Nakon formiranja 127. brigade prva ratna operacija širih razmjera bila je akcija "Otkos 10" u kojoj je na Bilogori, oko Grubišnog Polja, oslobođeno oko 3000 kilometara teritorija. Slijedilo je oslobođenje Zapadne Slavonije i ostala hrvatska ratišta sve do Oluje i potpunog oslobođenja Hrvatske. U svim važnijim akcijama, ne samo oslobađanja virovitičke vojarne već i u ostalim akcijama, virovitički su borci svojim junaštvom ostavili neizbrisiv trag u stvaranju novije hrvatske povijesti. Premda nije bila pod takvom ugrozom kao neka druga mjesta u Hrvatskoj, neprijateljski napadi nisu mimoišli Viroviticu. 7. studenoga 1991. četnička diverzantska skupina iz zasjede je ubila šestoricu pripadnika 127. brigade HV u okolici Virovitice.</t>
+  </si>
+  <si>
+    <t>17.67</t>
+  </si>
+  <si>
+    <t>133,8 </t>
+  </si>
+  <si>
+    <t>34000 Požega</t>
+  </si>
+  <si>
+    <t>PŽ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korijeni nastanka grada nisu jasni. Kukuljević je pretpostavio da se rimski grad Incerum nalazio na mjestu Požege. Arheološka istraživanja Dubravke Sokač-Štimac kod Tekića, u središnjem dijelu Požeškog polja južno od Vetova, potakla su većinsko mišljenje da se Incerum nalazio na tom položaju, no dokazi za to još nisu pronađeni. Manji, uglavnom usputni nalazi na tlu grada ipak su dovoljni da se postojanje jednog antičkog naselja, a također i utvrde na mjestu kasnijeg srednjovjekovnog županijskog požeškog Castruma, može smatrati izvjesnim i na mjestu Požege. Nalazi pretpovijesne keramike, ali prije svega opći vrlo povoljni uvjeti položaja za nastanak naselja ukazuju na nesumnjivi kontinuitet naseljavanja, međutim ostaje pitanje o važnosti i veličini naselja prije i u vrijeme antike.
+Požega kakvu poznajemo danas, počinje se oblikovati u srednjem vijeku. Stari požeški burg izgrađen je vjerojatno u 11. stoljeću. Radilo se o šesterokutnoj utvrdi smještenoj na brijegu u središtu grada. 
+Danas to brdo Požežani zovu Stari grad. Požega je tada bila rezidencija hrvatsko-ugarskih kraljica, te kao takva izuzeta od nadležnosti bana i župana. Iako iz tog doba potvrda o dobivanju statusa slobodnog kraljevskog grada nije očuvana, građani civitasa uživali su povlastice jednake onima u slobodnim kraljevskim gradovima. Službeno status slobodnog kraljevskog grada Požega dobiva 1765.
+Neimenovani notar Bele III. (1172. – 1196.), hrvatsko-ugarskog vladara, u svom djelu Gestae Hungarorum, opisu najranije povijesti Mađara, govori o osvajanju tri utvrde pri prelasku preko Drave: Zagrab, Vlco i Posega. To su tada bila središta urbanizacije i najrazvijeniji gradovi u Slavoniji (koja je tada obuhvaćala prostor od Sutle do Dunava).
+Požega je do danas zadržala svoj srednjovjekovni raspored ulica, s dominantnim srednjovjekovnim trgom nastalim u križištu četiri pristupna pravca (najvećim srednjovjekovnim trgom u Hrvatskoj), smještenom neposredno u sjevernom podnožju obronaka Požeške gore. Sjeverno od trga do nekadašnjih Kamenitih vrata (srušenih u 19. st). vodile su tri karakteristične međusobno usporedne ulice od kojih je ostala središnja (Cehovska – Sv. Florijana) i zapadna (Županijska) te dio istočne uz barokni Trg sv. Terezije.
+Požeška županija spominje se 1210. godine, a grad je 1227. spomenut kao Castrum de Posega.
+Od srednjovjekovnih spomenika očuvane su dvije redovničke samostanske crkve, crkva sv. Lovre, izvorno dominikanska posvećena Blaženoj Djevici Mariji iz druge polovice 13. st. s gotičkim freskama, te crkva sv. Duha, izvorno sv. Dimitrija, izgrađena oko 1235., kasnije franjevačka (od 1573. do 1688. služila kao džamija), dok je župna sv.Pavla porušena u opsadi grada 1536. Županijski Castrum, smješten na osamljenoj kamenoj uzvisini porušen je do temelja početkom 19. st., ali očuvan je dio gradskih srednjovjekovnih kamenih zidina.
+Godine 1537. Požega je osvojena opsadom u korist Osmanskog Carstva. Grad postaje središte Požeškog sandžakata, upravni i vojni centar Slavonije. Dva glavna osvajača grada Mehmed-paša Jahjaoglu, smederevski beglerbeg i Gazi Husrev-beg bosanski grade na dotadašnjem središnjem gradskom trgu najvažnije građevine kao svoje zaklade, Mehmed paša trgovačku čaršiju sa 70 dućana, a Gazi Husrev-beg hamam, karavan-saraj i nekoliko dućana za uzdržavanje medrese u Sarajevu. Grad u 16. st. dobiva vodovod, prvi u Hrvatskoj nakon dubrovačkog.
+Nakon bitke kod Haršanja 1687. Požega je oslobođena iduće 1689. (fra Luka Ibrišimović Sokol), a zatim konačno 1691. godine. U ovom razdoblju razvija se Požega kakvu je danas poznajemo. Grad dolazi pod vlast Habsburgovaca. Srednjovjekovnoj gradskoj osnovi dodaje se bogat barokni izgled.
+Obnavlja se Požeška županija, isusovci osnivaju gimnaziju (1699.), petu najstariju u Hrvatskoj, i najstariju u današnjoj Slavoniji. Franjevci 1708. g. pristupaju obnavljanju samostana iz srednjeg vijeka porušenog od strane Turaka, i dovršavaju ga 1724., te je smješten uz crkvu sv.Duha. Samostan sadrži knjižnicu s oko 15 tisuća svezaka s inkunabulama iz 16. stoljeća. Unatoč požaru u 19. stoljeću koji je uništio velik dio građe, knjižnica spada u nultu kategoriju i među vrjednijima je u Hrvatskoj. Stanovništvo je 1739. g. pogodila kuga. 1749. g., u spomen na 798 umrlih Požežana podignut je barokni spomenik Svetog Trojstva, koji i danas krasi središnji Trg u Požegi. Gradi se kazališna dvorana 1727., prva ljekarna u gradu 1740.
+Požega je u to vrijeme, uz Zagreb, jedini centar višeg obrazovanja u Hrvatskoj. Postojao je filozofski studij za mlade franjevce i Academia Posegana. 1763. sagrađena je i današnja Katedrala sv. Terezije Avilske.
+Svoj doprinos katedrali svojim zidnim slikama dali su i glasoviti slikari Celestin Medović i Oton Iveković. Zbog mnoštva znanstvenika i književnika koje je Požega podarila Hrvatskoj, i zbog niza kulturnih ustanova i spomenika, Požega je prozvana slavonska Atena. Osobito plodno bilo je XVIII. i XIX. stoljeće. Glasoviti slikar i književnik Matko Peić je rekao kako Požega ima toliko književnih i kulturnih ličnosti da se može govoriti o požeškoj književnosti.
+U 19. st. važnost Požege opada u korist Osijeka i Slavonskog Broda smještenih na povoljnijih prometnim položajima uz Savu i Dravu, u ono vrijeme presudnih čimbenika zbog gradnje prvih željeznica.
+Od 1921. do 1991. grad nosi naziv Slavonska Požega kako bi se razlikovao od Požege u Srbiji. 1993. nakon obnove županijskog sustava obnavlja se Požeška županija (pod imenom Požeško-slavonska županija), ali bez svog nekadašnjeg posavskog dijela, te sa znatno smanjenim područjem na zapadu, ali zato u početku obuhvaćajući Našice i pripadajuća mjesta, a nakon pripajanja Našica Osječko-baranjskoj županiji oblikuje se u današnjim okvirima. </t>
+  </si>
+  <si>
+    <t>45.16</t>
+  </si>
+  <si>
+    <t>18.00</t>
+  </si>
+  <si>
+    <t>35000 Slavonski Brod</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naselja su na ovom dijelu Hrvatske postojala još u prapovijesno doba što je uvjetovano povoljnim geografskim položajem, ugodnom kontinentalnom klimom, plodnim tlom i blizinom rijeke. Grad je dobio ime Brod koje je isprve simboliziralo mjesto na kojem se dala pregaziti rijeka, a poslije i sredstvo za ostvarivanje istog.
+Na sjeveroistočnom dijelu grada, na lokalitetu Galovo relativno nedavno otkriveno je bogato nalazište starčevačke kulture iz ranoga kamenog doba. Osim činjenice, da se radi o najvećem nalazištu iz kamenog doba na području Sjeverne Hrvatske, iznimno je bitno naglasiti da pronađeni materijalni ostaci potvrđuju 8000 godina staro naseljavanje Broda.
+Znanstvenici procjenjuju da je riječ, ne samo o najstarijim dokazima naseljavanja grada, nego, općenito, i o tragovima najstarijeg naselja u cjelokupnoj Hrvatskoj. Nalazište karakterizira više osobitosti, zbog kojih privlaći pažnju stručnjaka. Jedna od njih je i prvi put u Europi pronađena zemunica za ukop, posebno sagrađena. Ona je ograđena drvenom ogradom sa žrtvenikom i preko 20 kamenih sjekira. Zanimljivi su i ostaci ovdje pronađenih kostura, gdje je jedan pokopan bez glave, dok kod drugog na lubanji nedostaje lice, što znanstvenike upućuje na postojanje kulta lubanje i žrtvene obrede. Prema nalazima s još nekih lokaliteta, stručnjaci smatraju da se na gradskom području vjerojatno nalazilo dosta veliko prapovijesno naselje.
+Kroz povijest je lokacija grada Slavonskog Broda bila dobro nastanjena, a prva povijesna naseobina na tom mjestu datira iz rimskih vremena, o čemu svjedoče arheološki nalazi iz tog doba, po imenu Marsonia. Do danas nije utvrđeno da li je Marsonija bila samo poštanska stanica i prenoćište, ili i čitava naseobina.
+Na poznatoj Peutingerovoj tabli je Marsonija označena kao Marsonie, a u djelu Notitia dignitatum zapisana je kao Auxilia Ascaria Tauruno sive Marsonia.
+S problematikom ubikacije Marsonije bavili su se već izdavači Ptolomejeve Geografije u 16. stoljeću. U tom pogledu bilo je različitih mišljenja. Prvi geograf iz 16. stoljeća koji je odredio položaj Marsonie na lokalitetu Broda bio je Abraham Ortelius, koji je u svom atlasu Theatrum orbis terrarum (Antwerpen 1590) objavio kartu na kojoj je pokušao rekonstruirati i ubicirati sve antičke nazive panonskih i ilirskih naselja. On je Marsoniju smjestio na Savi upravo tamo gdje se danas nalazi Brod.
+Na već spomenutoj Peutingerovoj tabli se najbolje vidi da je Marsonija ležala neposredno uz rijeku Savu, na mjestu gdje je rimska cesta prelazila preko spomenute rijeke. Od naših stručnjaka prvi koji je utvrdio da je Marsonija (originalno MARSVNNIA) bila na lokaciji Broda bio Matija Petar Katančić. Nakon toga, ova je činjenica opće prihvaćena u znanosti.
+Nakon Marsonije na lokacija grada su se nastanili Slaveni u 6. stoljeću nove ere. Samo ime grada se prvi puta spominje u povelji ugarsko-hrvatskog kralja Bele IV. 1224. godine. Kroz kasni srednji vijek i glavninu novog vijeka Slavonski Brod je bio važna utvrda u Vojnoj Krajini, seriji utvrđenja na granici Austrije s Turskim carstvom. Utjecaj Turaka na ovom prostoru je dominantan sve do kraja 17. stoljeća kada se situacija mijenja osvajanjem teritorija od strane Austro-Ugarske monarhije. Osim obrambene uloge, u gradu se u to vrijem razvijaju i sitni obrt i trgovina, a od najranijeg doba duhovnu službu vrše Franjevci pod čijim utjecajem se razvijaju prosvjeta i kultura. U 20. stoljeću Slavonski Brod je iskusio nekoliko perioda brzog rasta, kao prometni i industrijski centar. Zbog naglog gospodarskog razvitka dvadesete godine prošlog stoljeća se nazivaju zlatnim dobom Broda. Za vrijeme Kraljevine Jugoslavije grad mijenja ime iz Brod na Savi u Slavonski Brod. 
+Slavonski Brod teško stradava u Drugom svjetskom ratu. Dio građana nije podržavao ustašku vlast već je prešao u antifašistički partizanski pokret. Grad je teško stradao u nemilosrdnim savezničkim razaranjima 1945. godine. Slavonski Brod (za NDH se zvao Brod na Savi) je bio vrlo važan kao strateško i prometno mjesto za NDH i Osovinske sile. Od hrvatskih gradova samo je Zadar toliko stradao u završnim akcijama Saveznika. Više od 80% građevina je bilo uništeno u savezničkim bombardiranjima pri čemu su uništene i građevine iz vremena Austro-Ugarske od iznimne kulturno – povijesne i urbanističke vrijednosti.
+Teška ga je sudbina zadesila za vrijeme Domovinskog rata za osamostaljenje Republike Hrvatske, kada je pretrpio strahovita razaranja iz susjedne Bosne i Hercegovine od strane JNA. Slavonski Brod je bio vrlo važan i srpskom agresoru zbog svog geopolitičkog položaja. Po nekim stručnjacima Brod je drugi najteže stradali hrvatski grad poslije Vukovara. U prosjeku je dnevno samo u Slavonskom Brodu kao posljedica velikosrpske agresije ginulo petero ljudi. U napadima je ukupno ubijeno 29-ero djece. Poznat je velikosrpski teroristički topnički napad od 16. srpnja 1991., kad su bosanski Srbi granatom pogodili slavonskobrodski izbjeglički centar, pri čemu su ubili 12 osoba, a 60-ak ranili.
+Pri gotovo svakodnevnom granatiranju Slavonskog Broda od neprijateljskih granata stradale su 182 osobe od kojih je 28-ro djece. Od svibnja 1992. do 1995. ranjeno je 969 hrvatske djece. Uglavnom su uzroci ranjavanja bile eksplozije ili prostrijeli za vrijeme topničkog ili zračnog napada. Među djecom ima 90 teških invalida.
+Zanimljivo je da je rat u Slavonskom Brodu trajao u vrijeme kada nisu postojale vojne akcije JNA u drugim gradovima istočne Hrvatske. Grad se tijekom poratnih '90-ih postupno oporavljao i obnavljao te nastojao dobro povezati, gospodarski i prometno s ostalim dijelovima Hrvatske što je uvijek bilo primarno za Brod, a i radilo se na obnavljanju industrijskih pogona, koji su svojevremeno zapošljavali većinu stanovnika.
+Slavonski Brod i okolica su dali obol u obrani i oslobađanju i drugih dijelova Hrvatske. U operaciji Maslenica su podnijeli veliki teret, braneći tek oslobođeni Kašić, ključno mjesto za obranu Zadra. U samo jednoj noći (1. na 2. veljače) su u području sela Kašića ili njegove okolice poginula 23 pripadnika brodske 3. bojne Kobre iz sastava 3. gardijske brigade Kune.
+Danas je Slavonski Brod prometni grad na auto-cesti koja povezuje Središnju Europu s Malom Azijom. Kao administrativni centar Županije i industrijski centar, Slavonski Brod i dalje raste i razvija se, pogotovo u posljednjih desetak godina.Iako se naglasak razvitka u posljednje vrijeme stavlja u razvijanje turizma i uslužnih djelatnosti,Brod je uvijek bio i uvijek će biti industrijski grad i njegova budućnost je upravo u tom sektoru te je potrebna daljna modernizacija brodskih tvornica i industrije. </t>
+  </si>
+  <si>
+    <t>44.12</t>
+  </si>
+  <si>
+    <t>15.24</t>
+  </si>
+  <si>
+    <t>23000 Zadar</t>
+  </si>
+  <si>
+    <t>ZD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Područje današnjeg Zadra najranije dokaze o ljudskome životu vuče iz mlađega kamenoga doba. Zadar svoje podrijetlo vuče od 9. st. pr. Kr. kao naselje ilirskoga plemena Liburna nazvan Iader. Godine 59. pr. Kr. preimenovan je u Iadera kada je postao rimski municipij. Godine 48. pr. Kr. postao je rimska kolonija. Za vrijeme rimske vladavine Zadar dobiva obilježja tradicijskoga starorimskoga grada s pravilnom cestovnom mrežom, javnim trgom (forumom) i povišenim kapitolijem s hramom. Nakon pada Zapadnoga Rimskoga Carstva 476., Zadar postaje prijestolnica bizantske teme Dalmacije. Početkom 9. stoljeća Zadar je nakratko došao pod franačku vlast. Prvi hrvatski vladari nakratko su stekli vlast nad gradom u 10. stoljeću. Godine 998. Zadar je prisegnuo na vjernost duždu Pietru Orseolu II. i postao vazal Mletačke Republike. Godine 1186. stavlja se pod zaštitu ugarsko-hrvatskog kralja Bele III.
+Godine 1202. Mlečani su uz pomoć križara ponovno osvojili i opljačkali Zadar. Ugarska je ponovno preuzela kontrolu nad gradom 1358., kada ga je dobio ugarski kralj Ludovik I. Kralj Ladislav Napuljski je 1409. prodao Dalmaciju Mlečanima. Kada je Osmansko Carstvo početkom 16. stoljeća osvojilo zadarsko zaleđe, grad je postao važno uporište koje je osiguravalo mletačku trgovinu na Jadranu, administrativno i kulturno središte mletačkih posjeda u Dalmaciji. To je potaknulo okruženje u kojem su umjetnost i književnost mogle cvjetati, a između 15. i 17. stoljeća Zadar je došao pod utjecaj renesanse, iznjedrivši mnoge važne talijanske renesansne osobe kao što su Giorgio Ventura i Giovanni Francesco Fortunio, koji su napisali prvu talijansku gramatiku, te mnogi hrvatski književnici, kao što su Petar Zoranić, Brne Krnarutić, Juraj Baraković i Šime Budinić, koji su pisali na hrvatskom jeziku. Nakon pada Venecije 1797. godine, Zadar je do 1918. godine, osim u razdoblju kratkotrajne francuske vladavine i Ilirskih pokrajina (1805. – 1813.), ostao pod austrijskom vlašću, i dalje glavni grad Dalmacije. Za vrijeme francuske vladavine u Zadru su izlazile prve novine na hrvatskom jeziku Il Regio Dalmata – Kraglski Dalmatin (1806. – 1810.). Tijekom 19. stoljeća Zadar je funkcionirao kao središte hrvatskog pokreta za hrvatski kulturni i nacionalni preporod u kontekstu sve veće polarizacije i politizacije etničkih identiteta između Hrvata i dalmatinskih Talijana.
+Rapalskim ugovorom 1920. Zadar je pripao Kraljevini Italiji. Tijekom Drugog svjetskog rata bombardirali su ga saveznici i svjedočio je evakuaciji etničkih Talijana. Partizani su oslobodili grad 1. studenoga 1944., a 1947. službeno je ušao u sastav SR Hrvatske (federalnog sastava SFR Jugoslavije) čije su ga oružane snage obranile u listopadu 1991. od srpskih snaga koje su je namjeravale zauzeti.
+Zbog svoje bogate baštine Zadar je danas jedno od najpopularnijih hrvatskih turističkih odredišta, koje je The Times nazvao „zabavnim središtem Jadrana”, a The Guardian „novom hrvatskom prijestolnicom cool-a”. UNESCO-ov popis svjetske baštine uključio je utvrđeni grad Zadar kao dio venecijanskih obrambenih djela između 15. i 17. stoljeća: Stato da Terra – zapadni Stato da Mar 2017. godine. </t>
+  </si>
+  <si>
+    <t>45.55</t>
+  </si>
+  <si>
+    <t>18.69</t>
+  </si>
+  <si>
+    <t>31000 Osijek</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Na tlu današnjeg grada bilo je više ilirskih i andizetskih naselja, a najveću je važnost imala keltska Mursa. Nalazom, između ostalog, keltskog svetišta iz 2. st. pr. Kr. potvrđeno je da se nalazila na području današnjeg Donjeg Grada. Rimski vojni logor iz vremena osvajanja Panonije potvrđen je nalazom tegula VII Legije. Dvostruki opkopi i očuvani zemljani nasipi bedema logora bili su vidljivi na površini sve do sredine 18. stoljeća. Tada im je položaj na zapadnoj strani zabilježen i u kartografskim prikazima, a nestali su širenjem Donjeg Grada. Standardni pravokutni legijski Castrum imao je prema Dravi utvrđen dodatak koji je štitio luku i most preko Drave. Ostatci njegovih temeljnih kamenih stubova još su uvijek vidljivi za niskog vodostaja rijeke. Na most se s druge strane Drave nastavljao dugačak nasip ili sustav mostova preko močvara, vjerojatno prema Kopačevu. To je svojevrsna preteča kasnijeg slavnog osječkog mosta do Darde sultana Sulejmana.
+U vrijeme cara Hadrijana, rimska Mursa uzdignuta je u status kolonije Colonia Aelia Mursa (124. ili 133. g.), a grad se razvio u velikoj ekstenziji i izvan zidina nekadašnjeg Castruma s njegove zapadne strane. Središnji dio te zapadne ekstenzije kontinuirano i opsežno se istražuje od 2001. pod vodstvom Slavice Filipović (voditeljica antičkog odjela Muzeja Slavonije). Otkrivena je vjerojatno središnja ulica u pravcu istok – zapad (Decumanus Maximus) s kolovozom širokim 3 m te dubokim odvodnim jarcima s obje strane ulice. (s jarcima njena širina narasta na 8 m). Nađeni su i široki trijemovi na obje strane. Brojne baze stupova trijemova kao i kapiteli nađeni su obrušeni u jarcima. Ulica je otkrivena u dužini od oko 150 m, a uz nju s jedne i druge strane iza trijemova i brojne građevine nekadašnjeg gradskog tkiva od kojih se ističu tabernae, veliko svetište boga Silvana s 5 žrtvenika i ostacima zidova i trijema oko njih (dim. 57x34m) i jedne veće građevine (površine 1600 m2) s osobito reprezentativnim pročeljem itd.
+Na temelju navoda grčkog povjesničara Zosima pretpostavlja se postojanje građevine amfiteatra izvan jugozapadnog dijela obrambenih zidina rimske Murse. Također ing. Franjetić spominje jednu depresiju koja se može odčitati na karti iz 18. st. blizu spomenutog ugla Castruma, koja po svoj vjerojatnosti predstavlja indicirani ostatak građevine rimskog amfiteatra.
+Godine 351. odigrala se pred zidinama Murse velika bitka između cara Konstancija II., sina i nasljednika cara Konstantina Velikog i uzurpatora Magnencija, bitka između suprotstavljenih rimskih vojski istočne i zapadne strane Carstva, jedna od najkrvavijih međusobnih sudara rimske vojske u povijesti Rimskog carstva. Nakon pobjede, koju je Konstancije dočekao u molitvi u arijanskoj crkvi sv. Mučenika na groblju izvan zidina Murse, Konstancije je u Mursi podigao i trijumfalni slavoluk (čiji ostaci još nisu pronađeni). U bitci je poginulo preko 40 000 ljudi, a tijela poginulih su se nalazila sve do današnje Trpinje.
+Grad su konačno 441. g. razorili Huni. 
+U hrvatskoj historiografiji postoji tumačenje da su ime Osijek Hrvati naselju dali zbog ponešto povišenog mjesta od okolih voda, mjesto gdje je oseka, te je suho i pogodno za izgradnju nastambi. Takvo tumačenje treba uzeti s dozom opreza, kao i pitanje etničkog identiteta prvih stanovnika, s obzirom na to da o tome nemamo nikakvih pisanih ili arheoloških tragova. U srednjovjekovnim dokumentima pisanim latinskim jezikom pod utjecajem mađarskog jezika javlja se kao Eszek ili Ezeek. Kasnije su varijante, Essegg, njemačka ili Essec, latinska, samo varijante imena Osijek. 
+Najraniji spomen Osijeka u povijesnim izvorima datira iz 1196. godine. Radi se o ispravi kralja Emerika (1196. – 1204.), kojom se cistercitskom cikadorskom samostanu potvrđuje pravo ubiranja pristojbi od carina i trgovine te skelarine preko rijeke pošto je Osijek je bio poznat prijelaz preko rijeke Drave. Taj dokument je vrlo važan jer svjedoči o tome da je Osijek već u 12. stoljeću bio važno trgovačko mjesto na trasi stare rimske ceste koja je povezivala jugoistok Europe s panonskom nizinom. Nažalost, pisani izvori za povijest Osijeka u 13. stoljeću nisu sačuvani, tek gabariti romaničkog sloja temelja, najvjerojatnije, župne crkve Sv. Trojstva mogu svjedočiti ponešto o veličini i značaj grada u to doba. Temelji su pronađeni u dvorištu današnjeg franjevačkog samostana. Kasnijom gotičkom dogradnjom, vjerojatno u 15. stoljeću, Osijek je dobio razmjerno veliku trobrodnu crkvu u kojoj su pokapani i pripadnici plemićke obitelji Korogy, u čijem se vlasništvu duže vrijeme gard nalazio. Znamo da se u Osijeku nalazio i augustinski samostan, što je dodatna potvrda urbanog statusa mjesta.
+Osijek je kroz čitavi kasni srednji vijek bio u vlasništu plemićkih obitelji i crkvenih ustanova. Kakva je feudalna prava imala opatija Cikador, osim ubiranja spomenutih taksi, nije poznato. Međutim, zna se da su u 14. stoljeću vlasnici grada vrlo utjecajna plemićka obitelj Korogy. Oni su ujedno i najzaslužniji za činjenicu da se Osijek razvio u jedno od značajnijih mjesta u donjem međuriječju. U 14. stoljeću spominje se županijski sajam. Budući da su vlastelini nerijetko vršili dužnosti župana i bana Mačve, Osijek je tada imao ulogu i važnog upravnog središta. O razvijenom gradskom životu svjedoči i porezni popis Osijeka i okolice iz 1469. godine iz kojeg se može iščitati i ustrojstvo gradske općine te ekonomska i demografska struktura građana. To je ujedno i jedini dokument gdje se Osijek navodi kao grad (civitas), dok ga ostali izvori spominju kao trgovište (oppidum). Treba reći da je prema ovom izvoru Osijek tipičan srednjovjekovni gradić trgovaca i obrtnika, a prevladava mađarsko stanovništvo. Neki povjesničari misle da je u vrijeme Korođskih Osijek bio opasan bedemima, ali oko toga nema suglasja u literaturi jer se gradske zidine izravno spominju tek u vrelima iz vremena osmanske vlasti. Gotovo je sigurno da su Korođski u gradu podigli mali kaštel koji je bio njihova rezidencija. Nakon što su Korođski izumrli 1472. godine, kralj Matija njihove posjede daruje Ivanu Ungoru i Nikoli Csuporu. Potom se Osijek navodi kao posjed budimskog kaptola Blažene Djevice Marije. Godine 1490. bio je posjed Petra Gereba, a 1517. je ponovo u vlasništvu budimskog kaptola.
+Jedna zanimljivost je da je na samom kraju srednjega vijeka kralj Ludovik II. (1516. – 1526.) odobrio bosanskom biskupu Mihovilu Keserűu i dvorskom komorniku Ivanu Szerecsenyu u Osijeku otvoriti kovnicu novca na godinu dana. 
+Osvajači Osmanskoga Carstva u grad su stigli 14. kolovoza 1526. kad je Osijek predan bez borbe, no kažu da ga je Ibrahim-paša do temelja razorio. Kasnije ga Sulejman Veličanstveni potpuno obnavlja te gradi čuveni pontonski most preko Drave i obližnjih močvara do mjesta Darda u ukupnoj dužini od 8 km. Osijek kasnije opet postaje čuven po obrtu, trgovini i velikim sajmovima.
+Grad je ostao pod Turcima više od 160 godina. Nalazio se u sklopu Požeškoga sandžakata. Snage Svete lige oslobodile su Osijek na Miholjdan, 29. rujna 1687., no, od 1690. Osijek je opet pod turskom opsadom, biva potpuno porušen, ipak ovoga puta ne i osvojen.
+Od 1687. Osijek i istočno područje današnje Hrvatske nalazili su se u okviru Habsburške Monarhije. Zbog strateškog položaja grada, nove su vlasti na obali Drave izgradile vojnu utvrdu, koje čini današnju Tvrđu, (1712. – 1721.). Unutar bedema nastao je grad građanskih kuća u baroknom stilu. Stanovništvo se zbog vojnih razloga naseljavalo zapadno i istočno te su tako nastale nove četvrti. Na zapadu, uzvodno uz Dravu Gornji grad te nizvodno od Tvrđe Donji grad. 
+Početkom 18. stoljeća u Donjem i Gornjem gradu formiraju se zasebni magistrati čime te dvije jedinice počinju funkcionirati kao samostalne gradske općine. Zemljišni gospodar sve tri općine bila je Dvorska komora. Politike dekameralizacije u Slavoniji, reforme i općenito politika Marije Terezije u ovim krajevima dovela je do početka pregovora između tri komorske općine o ujedinjenju, očito s namjerom da se Osijeku, kao i drugim značajnijim centrima u regiji, dodijeli status slobodnog i kraljevskog grada. Međutim, zbog razmirica oko održavanja sajmova do ujedinjena je došlo tek 2. prosinca 1786. godine, ukazom Josipa II. Tijekom 18. stoljeća Osijek se razvio u najznačajnije političko, gospodarsko i kulturno sjedište u Slavoniji, u kome su se djelovali brojni obrtnici, trgovci, knjižnice, kazališta, a već 1729. godine otvorena je isusovačka gimnazija. Godine 1735. Franjevci su osnovali tiskaru, a njihovim je nastojanjima osnovan i studiji filozofije i teologije. Dana 28. kolovoza 1809. godine Osijek je svečano proglašen slobodnim i kraljevskim gradom, a time počinje novo doba grada Osijeka.
+Sredina 19. stoljeća je doba bržeg razvoja Osijeka, osobito Gornjeg grada. U Donjem je gradu 1874. godine sagrađena jedna od najvećih i najljepših bolnica u ovom dijelu Europe. Godine 1846. podignuta je velika županijska palača, a kasnije, 1866., nasuprot županijske palače i Hrvatsko narodno kazalište. Godine 1868. osnovana je Srpska čitaonica u Osijeku.Pod kraj 19. stoljeća otvaraju se srednje škole – obrtna, realna, učiteljska i trgovačka. Na potezu od Tvrđe do Gornjeg grada kasnije se grade vile i druge građevine u secesijskom stilu. 
+Krajem 1918. i raspadom Austro-Ugarske, Osijek s današnjom istočnom Hrvatskom ulazi u Kraljevinu Srba, Hrvata i Slovenaca, koja 1929. mijenja ime u Kraljevina Jugoslavija. U travnju 1941., s početkom Drugog svjetskog rata u Jugoslaviji, Kraljevina Jugoslavija se raspada te Osijek ulazi u sastav NDH. Od 1941. do 1945. hrvatski dio Baranje pripada Mađarskoj te je Osijek pogranični grad. Važno je napomenuti da je Osijek u ratnom periodu bio žrtva Savezničkog bombardiranja civilnih objekata. Nakon sloma fašizma, u travnju 1945., svi dijelovi današnje Hrvatske i Osijek ulaze u sastav Federativne Narodne Republike Jugoslavije (kasnije Socijalističke Federativne Republike Jugoslavije). Sam je grad oslobođen 14. travnja 1945. godine. U Osijeku se osniva više fakulteta i viših škola, a 1975. i sveučilište, koje od osnutka nosi naziv velikog biskupa Đakovačko ili bosansko i srijemske biskupije (1855. – 1905.) i hrvatskoga mecene rođenog Osječanina Josipa Jurja Strossmayera. 
+Tijekom Domovinskog rata (1991.), posebno nakon pada Vukovara u studenom 1991., srpske paravojne snage i Jugoslavenska narodna armija (JNA) prodiru nadomak grada. Grad je bio ratno ugrožen još mnogo prije. 11. srpnja 1991. je osječki MUP RH nakon 10-satne akcije uhitila skupinu srpskih terorista. Pod topništvom JNA i četnika Osijek trpi znatna razaranja, ali se uspijeva održati. Prije rata u Osijeku je na nekoliko lokacija bio smješten garnizon JNA pod imenom 12. proleterska mehanizirana brigada u sklopu 1. vojne oblasti (sa sjedištem u Beogradu) a u sastavu tzv. Tuzlanskog korpusa. Na čelu garnizona (koji se službeno zvao Kasarna Milan Stanivuković – narodni heroj) u Osijeku nalazio se tada pukovnik Bora Ivanović zvani Konj, koji se ne samo tijekom boravka u Osijeku već i nakon izlaska iz grada aktivno uključio u rat protiv Hrvatske. Osječko je Državno odvjetništvo protiv sada umirovljenog generala JNA i Vojske Jugoslavije Bore Ivanovića i još trojice časnika iz tadašnjeg garnizona JNA u Osijeku 2006. podigla optužnicu zbog razaranja grada Osijeka i civilnih objekata. 
+Nakon žestokih borba, velikosrpske postrojbe su zauzele Paulin Dvor 16. prosinca 1991., 11 dana nakon što su okupirale Antunovac,a skoro pola godine otkad su (u lipnju) u osječkoj neposrednoj okolici, u Bijelom Brdu, Tenji i Markušici uspostavljene terorističke baze velikosrpskih ekstremista, odakle su isti napadali Osijek (još 29. lipnja 1991. je bio žestoko napadnut iz Tenje) i kontrolirali prugu i cestu Osijek – Vinkovci (iz Markušice). 
+Osijek je vrlo rano došao u tjeskobno okružje neprestanog granatiranja i opasnosti okupacije koju su JNA i pobunjeni Srbi uspješno izveli u Baranji, zapadnom Srijemu i drugim dijelovima hrvatskog Podunavlja. 
+Napadi su počeli još 29. lipnja 1991. iz Tenje koju su držali pobunjeni Srbi i JNA. JNA i pobunjeni Srbi granatirali su grad i iz inih iz okupiranih naselja. 5. srpnja 1991. dužnosnici Srbije i JNA (Milošević – Jović – Kadijević) dogovorili su razmještaj postrojba JNA u Hrvatskoj na područja koja su Srbi željeli izdvojiti iz Hrvatske,[10] ako već ne uspiju zauzeti cijelu Hrvatsku. Osijek se našao na planskoj ruti udara na Hrvatsku i odsijecanja dijelova Hrvatske: Glavne snage koncentrirati na liniji: Karlovac – Plitvice na zapadu; Baranja, Osijek, Vinovci – Sava na istoku i Neretva na jugu. Na taj način pokriti sve teritorije gde žive Srbi do potpunog raspleta. I kad su te dane (5. – 6. srpnja) hrvatski MUP i ZNG potisnuli četnike iz Stare Tenje, JNA, neusporedivo moćnija od hrv. snaga, otvoreno se je stavila na stranu pobunjenih Srba, napadom na Osijek. 19. kolovoza zrakoplovi JNA bombardirali su Osijek, dvije su žene stradale smrtno, pogođena je osječka katedrala i industrijski pogoni. 21. kolovoza JNA snažno topnički napale Osijek i okolna sela, ranivši mnoštvo civila. Vođa srpskih terorista Željko Ražnatović zahtijevao je predaju grada u roku od 24 sata. 3. rujna srpske su snage zauzele Bilje. Istog su dana unatoč potpisane obustave paljbe, srpske snage topnički napale Osijek, ubivši 18, a ranivši 28 osoba. 6. rujna u napadu JNA je oštetila crkvu sv. Petra u Osijeku. 10. rujna topničkim napadom JNA pogođen dječji vrtić i franjevački samostan. 15. rujna srpske paravojne snage topnički su napale osječku bolnicu i ubile pritom 4 osobe. 16. rujna hrvatski su branitelji u Osijeku uništili 10 tenkova JNA, koja je cijeli dan neprekidno napadala osječku bolnicu. Tog se dana predao Dom JNA u Osijeku hrvatskim snagama. Tijekom rujna JNA je nagomilala oklopno-mehanizirane snage u osječkim predgrađima te u Baranji, tako da se mogao očekivati oubhvatni napad na Osijek sa sjeverne strane. Rujna je JNA izvodila koordinirani udar radi izvlačenja 12. pmbr koja je bila okružena u vojarni u Osijeku. Hrv. su snage pokušale olakšati pritisak na grad manjom napadnom akcijom. 16. rujna na Tenjskoj je cesti JNA srušila nadvožnjak, a tenkovi s poligona C pucali su na Brijest, Retfalu i Dinaru. 17. rujna ZNG zauzeo je borbama poligon C i ine vojarne, no iz svih je tih objekata JNA izvukla kompletno oružje, koje je poslije rabila u napadu na Vukovar. ZNG je napustio položaje u Sarvašu. Opasnost pješačko-tenkovskog napada dugo je visila Osijeku kao mač nad glavom. Vukovar je nakon dugotrajne opsade pao 18. studenoga, vijesti o padanju hrvatskih naselja stizale su odosvuda, a neprijatelj se primicao gradu. 5. prosinca pao je Antunovac. Istog su dana snage JNA i četnici, nakon strahovite topničke pripreme, krenuli u konačno osvajanja grada Osijeka općim oklopno-pješačkim napadom, a hrvatske su snage uz velike žrtve u bitci na šumi Rosinjači na južnom prilazu gradu malim postrojbama zaustavile udar. JNA i pobunjeni Srbi okupirali su Paulin Dvor 16. prosinca 1991. U periodu od 17. i 18. prosinca 1991., hrvatske su snage uspjele olakšati pritisak na Osijek sa sjeverne strane, oslobađanjem 30 km2 u Baranji, operacijom naziva Đavolja Greda[12] te osigurati mostobran za buduće vojnooslobodilačke akcije.
+Tijekom Domovinskog rata je u obrani Osijeka od srpskih paravojnih snaga i Jugoslavenske narodne armije (JNA) poginulo 1260, a ranjeno više od 5000 hrvatskih vojnika i civila. Među žestoke napade spada onaj od 3. travnja 1992. kad je u napadu velikosrpskih snaga poginulo 20 (dvadeset), a ranjeno 100 (ljudi).</t>
+  </si>
+  <si>
+    <t>43.74</t>
+  </si>
+  <si>
+    <t>15.89</t>
+  </si>
+  <si>
+    <t>22000 Šibenik</t>
+  </si>
+  <si>
+    <t>ŠI</t>
+  </si>
+  <si>
+    <t>O najstarijoj povijesti Šibenika ne zna se mnogo. Pretpostavlja se da je bio utemeljen u doba kneza Domagoja u IX. st. Isprva se razvijao kao utvrda (castrum) sa starijim predgrađem (suburbium) na području Dolca i mlađim na istočnoj strani kaštela, gdje je u XII. st. sagrađena crkva sv. Krševana, oko koje se poslije razvila jezgra srednjovjekovnoga grada. Šibenik je pripadao skupini tzv. hrvatskih gradova, a izniknuo je na brijegu 70 m iznad mora (današnja tvrđava sv. Ane), na kojem nije nađen nikakav trag antičke urbane tradicije, ali je bilo nekog života u kasnoantičko doba. 
+Prvi spomen nalazi se u ispravi kralja Petra Krešimira IV. od 25. XII. 1066., kojom je kralj poklonio slobodu benediktinskomu samostanu sv. Marije u Zadru. Upravo u to doba došlo je do jačanja Šibenika, u okviru kraljeva nastojanja da uz pomoć hrvatskih gradova stvori protutežu romanskim gradovima bizantske Dalmacije. Nakon bitke s ugarskom vojskom na Petrovoj gori 1097. i pogibije hrvatskog vladara Petra, Šibenik je 1105. priznao vlast hrvatsko-ugarskoga kralja Kolomana. Od tada su se za prevlast nad Šibenikom neprestano do 1180. borili Venecija, Bizant i Arpadovići. U XII. st. u pravnom je smislu bio utvrđeno naselje (castrum, oppidum), a ne grad (civitas), pa su njegova buduća nastojanja bila usmjerena prema postizanju civiteta, čime bi dostigao druge dalmatinske gradove. Od kraja XII. st. priznavao je vlast hrvatskih knezova, isprva kneza Domalda (1200–26), a zatim knezova Bribirskih (do 1322). Za vladavine potonjih Šibenik je postao biskupskim sjedištem te je stekao civitet, ali je gospodarski zaostajao zbog teških nameta i obveza. Bio je to uzrok izbijanja pobune protiv vlasti Bribirskih; tada se uz potporu Mletačke Republike grad uspio othrvati vlasti Mladina II., ali je na posljetku izgubio autonomiju i pravo slobodnog izbora kneza, kojega su od tada birali Mlečani. Nakon poraza Mletačke Republike u ratu s Ludovikom I. Anžuvincem i potpisivanja mira u Zadru (1358), grad je došao pod anžuvinsku vlast. Od 1390. zajedno s ostalim gradovima Dalmacije (osim Zadra) priznavao je vlast bosanskoga kralja Tvrtka I. Kotromanića, početkom XV. st. bosanskoga vojvode Hrvoja Vukčića Hrvatinića i kralja Ladislava Napuljskoga, a 1412. ponovno je došao pod vlast Mletačke Republike. 
+Nakon polustoljetnoga razdoblja obilježenoga gospodarskim rastom, u drugoj polovici XV. st. Šibenik se našao pod osmanskom prijetnjom, čime je započelo razdoblje njegova gospodarskog zastoja. Pad gradova u zaleđu, Knina i Skradina, pod osmansku vlast 1522., te česte osmanske navale i pustošenja, sljedećih su godina prouzročili znatan pad broja stanovnika i na području Šibenika. Od osmanskih pustošenja i gospodarskog sloma uzrokovanog smanjivanjem prodaje soli Šibenik se počeo oporavljati tek nakon 1581., u doba vladavine kneza Giovannija Antonija Foscarinija (1581–83), koji je dobro organizirao vojsku i obranu grada. Godine 1646., radi obrane grada od Osmanlija, mletački general Christoph Martin von Degenfeld dao je sagraditi utvrdu, koja je prema njemu nazvana Barone Degenfeld (od 1911. Šubićevac), a koja je odigrala važnu ulogu pri slamanju osmanske opsade Šibenika 1647. Ponovni gospodarski oporavak grada, što je uslijedio nakon poraza Osmanlija u Morejskom ratu (1684–99), tekao je vrlo sporo. 
+Nezadovoljstvo dalmatinskog i šibenskoga puka i težaka dosegnulo je vrhunac u bunama koje su trajale 1736–40. Gušenje ustanka za mletačkog providura Cavallija (1739) utjecalo je na porast nesnošljivosti između šibenskih plemića s jedne te pučana i težaka s druge strane. Propašću Mletačke Republike, Šibenik se 1797–1805. nalazio pod habsburškom vlašću, a nakon toga je prema Požunskomu miru (1805) došao pod francusku vlast. Godine 1813–1918. ponovno se nalazio u sastavu Habsburške Monarhije. U tom je razdoblju, nakon sredine stoljeća, u gradu ojačao hrvatski narodni preporod, 1866. bila je osnovana Narodna slavjanska čitaonica, a 1872. narodnjaci su pobijedili na općinskim izborima i sljedeće godine osnovali prvu hrvatsku općinsku upravu. Potkraj XIX. st. u gradu je ojačao pravaški pokret, a 1903. pravaši su (pod vodstvom Mate Drinkovića) zajedno s narodnjacima ušli u općinsko vijeće te su uskoro postali najjača politička stranka na tom području.
+Slomom Austro-Ugarske Monarhije 1918. grad se našao u sastavu područja pod talijanskom upravom, a temeljem Rapalskog ugovora ušao je u sastav Kraljevine SHS (1922). Za II. svjetskoga rata od 1941. bio je pod talijanskom, a od 1943. njemačkom okupacijom. Oslobođen je 3. XI. 1944. Tijekom 1960-ih postao je važnom lukom i gospodarskim središtem, osobito kada je završen Šibenski most (1964/65), jedan od strateških objekata na tada dovršenoj Jadranskoj magistrali. Za Domovinskoga rata grad i njegova okolica bili su izloženi napadima srpskih snaga, kojima je odolio zahvaljujući uspješno organiziranoj obrani.</t>
+  </si>
+  <si>
+    <t>45.35</t>
+  </si>
+  <si>
+    <t>18.99</t>
+  </si>
+  <si>
+    <t>32000 Vukovar</t>
+  </si>
+  <si>
+    <t>VU</t>
+  </si>
+  <si>
+    <t>Naseljenost vukovarskog kraja prati se kroz pet tisuća godina u kontinuiranom slijedu putem brojnih arheoloških lokaliteta.
+Ovdje su značajne kulture mlađeg kamenog doba (neolitik) starčevačka, vinčanska i sopotska. Temeljile su se na sjedilačkom načinu života i izgradnji trajnih nastambi. U upotrebi je polirano kameno oruđe, usavršena je proizvodnja keramike.
+Migracijskim kretanjima i dolaskom novih etničkih skupina indoevropskog porijekla uvode se i nove tehnologije. Počinje razdoblje bakrenog doba (eneolitik) s badenskom, kostolačkom i vučedolskom kulturom. Nastaju novi oblici proizvodnje, sahranjivanja i vjerovanja i složeniji društveni odnosi medu ljudima. Način gradnje kuća i kultni predmeti svjedoče o povezanosti s mediteranskim kulturnim krugom.
+Vučedolska kultura posebno je značajna za vukovarski kraj. Ime je dobila po lokalitetu Vučedol, pet kilometara od Vukovara nizvodno na Dunavu. Lokalitet je sustavno istražen, otkrivene su radionice za preradu bakra, karakteristične kuće (megaron) i prekrasna keramika, koju naročito karakteriziraju bijeli stilizirani ukrasi na crnoj podlozi.
+U vukovarskom kraju brojna su arheološka nalazišta iz brončanog, starijeg i mlađeg željeznog doba, koja svjedoče o životu Ilira i Kelta. Nekropola ilirskih grobova na Lijevoj bari u Vukovaru dokazuje da je ovdje bilo i veliko naselje.
+Rimljani su u osvajačkim pohodima u posljednjim desetljećima prije Krista izbili na Dunav. Izgradili su brojna utvrđenja, kao granicu ( limes ) prema barbarskim plemenima. U vukovarskom kraju značajni su rimski lokaliteti Cornacum (Sotin), Cuccium (Ilok) i Ulmo (Tovarnik). Uz Dunav je vodila i važna rimska cesta. Rimska civilizacija u ovim krajevima utjecala je na unapređivanje gospodarstva, isušivane su močvare i zasađeni prvi vinogradi.
+Propast rimske civilizacije, velika seoba naroda i avarsko-slavenska ekspanzija od šestog stoljeća dalje dovela je do velikih promjena. Međuriječje Dunava i Save poprište je velikih sukoba i interesa moćnih država toga vremena. U to vrijeme se ovdje naseljavaju Hrvati.
+Početke današnjeg Vukovara treba tražiti vrlo rano, sto potvrđuju i arheološki podaci. Izuzetan topografski položaj visoke obale Dunava kod ušća Vuke bio je važna obrambena točka. Ovdje je srediste cijelog kraja u vrijeme kada knez Pribina, kao franački vazal, dobija stotinu sela uz rijeku Vuku sredinom 9. stoljeća. U prvoj polovici 10. stoljeća zabilježeno je da su Mađari opljačkali tvrđavu Vukovo. Na Lijevoj bari u Vukovaru istraženo je veliko groblje s brojnim nalazima koji pripadaju bjelobrdskoj kulturi. Datiranje ovih nalaza u 10. ili 11. stoljeće najbolje potvrđuje da je u susjedstvu bilo veliko naselje. To je vrijeme hrvatskih narodnih vladara, kada su, posebno, za kraljeva Tomislava i Petra Krešimira IV., sjedinjene sve hrvatske zemlje od Drave do mora.
+U sačuvanim pisanim dokumentima Vukovar se spominje već početkom 13. stoljeća kao Volko, Walk, Wolkov, odnosno hrvatski Vukovo. Od 14. stoljeća sve je više u upotrebi pomađareni naziv Vukovar. U to je vrijeme Hrvatska u državnopravnoj zajednici s Ugarskom. Vukovar, kao i susjedni Ilok, u tom su razdoblju čuvari hrvatskog identiteta u dunavsko-savskom međuriječju.
+Vukovarska tvrđava bila je čvrsto zidana na visokoj dunavskoj obali. U gradu su stanovali obrtnici, trgovci i seljaci. Već 1231. godine, medu prvima u hrvatskim zemljama Vukovar je dobio status slobodnog kraljevskog grada. Poveljom hercega Kolomana potvrđene su povlastice, koje su štitile vukovarske stanovnike.
+U Vukovaru je tada sjedište velike Vukovske županije, koja se protezala između Dunava i Save. Vukovarski kraj je tada gusto naseljen, brojne su utvrde i kmetska sela. U crkvenom pogledu Vukovska županija je pod katoličkom nad-biskupijom u Pečuhu. Nekoliko crkvenih redova ima ovdje svoje samostane, a najutjecajniji je franjevački red.
+U 14. i 15. stoljeću vukovarskim krajem vladaju brojne velikaške porodice. Pred kraj ovog razdoblja najutjecajniji su Iločki, kada je Nikola proglašen naslovnim kraljem Bosne i kuje svoj novac. Ilok je u to vrijeme značajno naselje i tvrđava, od 1525. godine ima svoj gradski statut i grb.
+Sto pedeset godina turske vladavine donijele su vukovarskom kraju velike promjene. Turci su na svom pohodu 1526. godine, pod vodstvom sultana Sulejmana Veličanstvenog zauzeli sve utvrde uz Dunav, pa tako i Ilok i Vukovar, te su potom izvojevali veliku pobjedu na Mohačkom polju. Vukovar je izgubio strateško značenje, ali je ostao značajno trgovačko-obrtničko mjesto na važnom prometnom pravcu. Imao je nekoliko gradskih četvrti, bogomolje, kupatila, prenoćišta i škole. Pred kraj turske vlasti imao je do 3.000 stanovnika.
+U isto vrijeme Ilok je značajno tursko upravno i vojno središte. Pretežito je naseljen muslimanima.
+Tada je starosjedilačko katoličko hrvatsko i madžarsko pučanstvo teško stradalo, povuklo se u šume ili je pobijeno. Za turske vladavine ovdje djeluju franjevci okupljajući katolički puk. Na opustjelo područje kao pomoćne turske čete dolaze pravoslavni Vlasi, ali će se povući zajedno s turskom vojskom. Vukovar je oslobođen 1687. a Ilok 1688. godine.
+U Vukovaru je ostalo naseljeno pedesetak kuća. U opustošeni vukovarski kraj vraća se starosjedilačko i novodoseljeno hrvatsko pučanstvo. U neka opustjela mjesta naseljavaju se pravoslavni Srbi, koje iz potrebe za radnom snagom prihvaća bečki dvor. U 18. 1 19. stoljeću naseljava se i znatan broj Nijemaca, Mađara, židova, Rusina, Slovaka i Ukrajinaca. Tako ovo hrvatsko područje postaje višenacionalno. Hrvatske zemlje su sada u sastavu habzburškog carstva. Carica Marija Terezija obnovila je 1745. godine slavonske županije, koje su pod upravom Hrvatskog sabora i bana, ali pod pritiskom Mađara.
+Vukovar je sjedište velike Srijemske županije, koja se protezala između Dunava i Save, na istoku sve do Zemuna, na zapadu do Osijeka, osim područja Vojne krajine.
+Velike posjede u Slavoniji dobijaju ili kupuju feudalci. Grofovi Eltz, koji se ubrajaju u njemačko praplemstvo, dolaze u posjed vukovarskog vlastelinstva. Filip Karlo Eltz nadbiskup u Mainzu i njemački knez izbornik 1736. godine kupuje ovaj ogroman posjed s 35 naseljenih mjesta. Tijekom narednih stoljeća zemljišne površine su smanjene agrarnim reformama. Cijeli razvoj vukovarskog kraja sve do 1945. godine tijesno je vezan uz vukovarsko vlastelinstvo grofova Eltz.
+U isto vrijeme iločko vlastelinstvo drže kneževi Odescalchi. U 18. i 19. stoljeću Vukovar je imao značajke administrativnog, gospodarskog, prometnog i kulturnog središta. Suvremenici ga smatraju "prijestolnicom Srijema".
+Već na početku ovog razdoblja polovicu stanovnika Vukovara čine obrtnici i trgovci. Pučanstvo je izuzetno radino cvjeta obrt, trgovina, svilarstvo, brodogradnja. Roba se lađama otprema u podunavske zemlje. Rano su osnovane brojne cehovske organizacije koje štite obrtnike. U Vukovaru je središte trgovine za cijeli zapadni Srijem.
+Vukovarski kraj ima izvanredne uvjete za agrarnu proizvodnju. Još krajem 19. stoljeća gotovo 80% pučanstva živi od zemljoradnje. Vlastelinstvo grofova Eltz uznapreduje proizvodnju, sto utječe i na mala seoska gospodarstva. Pored osnovne proizvodnje žitarica vinogradarstvo je važna gospodarska grana. Vukovarska i iločka kvalitetna vina priznata su na svjetskim gospodarskim izložbama. U govedarstvo se uvode najbolje mliječne pasmine, a ovdje su i čuvene ergele konja poznate u svjetskim razmjerima.
+Od 1840. godine Vukovar je uključen u stalni parobrodarski promet na Dunavu. Od 1878. godine priključen Je na željeznički promet. Vukovarska luka je najveća pretovarna luka u hrvatskim krajevima. Kao i u drugim hrvatskim, posebno slavonskim krajevima, u Vukovaru se sporo razvijala industrija. Intenzivnija primjena parnih strojeva je u drugoj polovici 19. stoljeća i to više u zemljoradnji nego u industriji. Na spori razvoj industrije utječe nedostatak kapitala. štedionica u Vukovaru osnovana je 1861. godine. Prvo veliko industrijsko poduzeće Vukovarska kudjeljara proradilo je tek 1905. godine. Iz ovih pogona Vukovar dobija električnu energiju od 1909. godine.
+Spori razvoj industrije utječe na mali porast stanovništva grada. Prema popisu pučanstva 1900. godine u Vukovaru živi 1/4 stanovništva vukovarskog kotara. Vukovar tada ima 10.400 stanovnika, od toga po nacionalnosti: preko 4.000 Hrvata, 3.500 Nijemaca, oko 1.600 Srba, 950 Mađara, itd.
+Značajniji industrijski objekti osnova su u razdoblju između dva svjetska rata. Tvornica »Bata« u obućarsko-gumarskoj grani proizvodnje osnovana je 1931. godine. U isto vrijeme počinju raditi u Vukovaru značajni pogoni tekstilne industrije.
+Industrijalizacija je utjecala na porast gradskog stanovništva, tako da Vukovar ima prema popisu pučanstva 1948. godine preko 17000 stanovnika.
+U skladu sa svojim položajem u gospodarskom i administrativnom pogledu Vukovar se razvio u prosvjetno, kulturno i zdravstveno središte. U Vukovaru se u 18. i 19. stoljeću živjelo na europski način.
+U 18. stoljeću u Vukovaru već djeluju ranarnici, a liječenjem se bave i neki franjevci. Prvi diplomirani liječnik djeluje od 1763. godine, a ljekarna je otvorena 1791. godine. Krajem 18. stoljeća vladala je ovdje velika srijemska kuga. Prva mala bolnica otvorena je tek 1857. godine.
+Već od 1730. godine Vukovar ima razvijeno pučko školstvo. Iz franjevačke škole razvila se pučka škola u Starom Vukovaru. Novi Vukovar ima svoju školu. Djelovale su i konfesionalne škole za djecu pravoslavne i židovske vjere, te škole na njemačkom i mađarskom jeziku. šegrtska škola osnovana je 1886. a gimnazija 1891. godine.
+U Vukovaru je osnovana tiskara 1867. godine i izdavala je prve vukovarske novine na njemačkom jeziku »Der Syrmier Bote«. Kasnije je radilo više tiskara, a od brojnih novina isticale su se "Sriemski Hrvat« i »Sriemske novine«, koje su izlazile gotovo tri desetljeća na prijelazu u 20. stoljeće.
+Najstarija književna djela ovoga područja potječu iz pera vukovarskih i iločkih franjevaca. Najpoznatiji književnici iz ovog kraja su Nikola Andrić, Julije Benešić i Antun Gustav Matoš.
+U Vukovaru su djelovali brojni likovni stvaraoci. Od starijih su poznati J. F. Mucke, F. K. Giffinger, a u 20. stoljeću gimnazijski profesori Dragan Melkus, Dragutin Renarić, Marijan Detoni, i drugi.
+Vukovar ima svog nobelovca Lavoslava Ruzičku. Rođen je u Vukovaru 1887. godine, a Nobelovu nagradu za kemiju dobio je 1939. godine.
+Vukovar je imao razvijen društveni život po uzoru na europska shvaćanja. Samo u razdoblju do prvog svjetskog rata djelovalo je 30-tak društava. Pjevačka, čitalačka, športska i potpomagajuća društva imala su svoje čitaonice, organizirala koncerte i zabave. Društva su često bila organizirana na nacionalnoj osnovi. Prva predstava na hrvatskom jeziku održana je 1821. godine, bilo je to dramsko djelo gvardijana franjevačkog samostana Grge Čevapovića. Najutjecajnije hrvatsko društvo je pjevačko društvo »Dunav«. U Vukovaru je 1922. godine otvoren Hrvatski dom, stjecište svih kulturnih zbivanja.
+U razdoblju između dva svjetska rata, u okvirima jugoslavenske države, vukovarsko područje, kao i ostali hrvatski krajevi, nalazilo se pod izrazitim velikosrpskim pritiskom. Teritorijalnim podjelama na oblasti i banovine hrvatsko područje namjerno je cijepano. Intervencijama jugoslavenske državne vlasti se mijenjala sastav stanovništva. Površine dobijene agrarnom reformom dijele se solunskim doborovoljcima i općenito stanovništvu iz srpskih krajeva. Čak se i zapošljavanje u tvornicama vješto koristilo da se mijenja hrvatski značaj vukovarskog kraja.
+Na početku ovog razdoblja u Vukovaru je vrlo snažan radnički pokret, koji svoje uporište nalazi u neriješenom socijalnom i nacionalnom pitanju u tadašnjoj jugoslavenskoj državi.
+Pored svih pritisaka velikosrpske politike toga doba u Vukovaru je sačuvana snažna hrvatska nacionalna svijest i s olakšanjem je dočekano osnivanje Banovine Hrvatske 1939. godine.
+Na žalost, slijede tragični događaji drugog svjetskog rata. Međunacionalni sukobi izazvani ranije sada se zaoštravaju i u Vukovaru. Grad nije pretrpio veća razaranja. Sastav stanovništva znatno se promijenio, posebno progonima židova, Srba i antifašistički orijentiranih Hrvata i iseljavanjem Nijemaca pred kraj i poslije rata.
+Poslije 1945. godine u novoj jugoslavenskoj državi cijeli Srijem je odvojen od hrvatskih zemalja. Vukovarsko-iločki kraj, ostao je u sastavu Hrvatske u administrativnom pogledu činio je općinu Vukovar.
+U skladu sa socijalističkim sustavom izvršena je nacionalizacija većine dobara i pretvorena u državno ili kasnije u tzv. društveno vlasništvo. U vukovarskom kraju dolazi do brze industrijalizacije, iznad prosjeka u odnosu na ostale dijelove Hrvatske. Na žalost industrija je usko specijalizirana, neatraktivna s masovnim zapošljavanjem radne snage. U isto vrijeme agrarna proizvodnja je autarhična. Godine 1990. od ukupno zaposlenih u gospodarstvu vukovarskog kraja oko 60% radi u industriji a samo 12% u poljoprivredi, u tzv. društvenom sektoru.
+Vlast se u socijalističkoj Jugoslavenskoj državi krila iza komunističke ideje i parole »bratstva i jedinstva«. Ustvari to je bila unitaristička i velikosrpska vladavina. Na svim važnijim položajima u gospodarstvu, politici i upravi bili su uglavnom Srbi. Isticanje hrvatske ideje ili odlazak u crkvu donosili su progone. Hrvatski dom u Vukovaru djelomice je srušen i pretvoren u dom kulture, da mu se zametne trag. U hrvatskom gradu Vukovaru Hrvati su zapravo bili stanovnici drugog reda.</t>
+  </si>
+  <si>
+    <t>43.51</t>
+  </si>
+  <si>
+    <t>16.45</t>
+  </si>
+  <si>
+    <t>21000 Split</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>Povijesnu jezgru grada Splita tvori Dioklecijanova palača i dio grada unutar mletačkih obrambenih zidova iz XVII. st. (od 1979. na UNESCO-ovu popisu svjetske kulturne baštine).
+Najstariji nalaz na splitskom poluotoku bakrenodobna je ostava zlatnoga nakita i bakrenih sjekira na Gripama. Arheološki ostatci villa rustica, akvedukta i nekropola (Meje, Manuš, Gripe, Poljud, Špinut, Sustipan) svjedoče o postojanju naselja prije Dioklecijanove odluke da ondje podigne svoju palaču. Izgradnjom palače uništene su neke starije građevine kojih se ostatci nalaze unutar podzemnih prostorija palače. Istraživanja iz 2006–07. otkrila su ostatke drvenih pristaništa i kamenih gatova luke preddioklecijanovskoga Spalatuma kao i dijelove monumentalne Dioklecijanove obale. Na lokalitetu Ad basilicas pictas na ostatcima antičkoga odeona (?) podignut je u V. st. ranokršćanski bazilikalni sklop s krstionicom. Prema izvješću Tome Arhiđakona, na istom je mjestu u XII. st., u tadašnjoj crkvi sv. Andrije, bila održana važna crkvena sinoda. Crkva sv. Frane pokraj luke također je kasnoantičkoga postanka i bila je posvećena sv. Feliksu. U njezinoj je poligonalnoj krstionici pronađen sarkofag s prikazom prelaska Izraelaca preko Crvenoga mora. Na Sustipanu je bilo ranokršćansko groblje, vjerojatno i crkva na mjestu koje je u XI. st. bila izgrađena srednjovjekovna crkva i samostan sv. Stjepana.
+U ranome srednjem vijeku svi glavni dijelovi Dioklecijanove palače preuzeli su funkciju novoga grada. Zidine i vrata postali su dio gradskoga obrambenoga sustava; zapadna vrata palače postala su glavni ulaz u grad, iznad kojega je bio otklesan reljef antičke božice pobjede, a na njegovo je mjesto uklesan križ. Dioklecijanov mauzolej bio je pretvoren u katedralu (isprva posvećenu sv. Mariji, potom zaštitniku grada sv. Dujmu), Jupiterov hram postao je krstionica. U njoj je krsni zdenac opločen pločama s pleternim ukrasom i reljefom hrvatskoga vladara na prijestolju, prenesenima iz neke druge građevine. Dijelovi palače, osobito hodnici, bili su pretvoreni u predromaničke crkvice (Sv. Martin s cjelovitom oltarnom pregradom, XI. st.; Gospa od zvonika, kraj XI. st.). Širenje grada u ranome srednjem vijeku započelo je izgradnjom predgrađa. S vanjske strane sjevernoga zida palače podignuta je trobrodna crkva sv. Eufemije, uz koju je u XI. st. bio sagrađen samostan benediktinki. U Velom Varošu sačuvala se najstarija predromanička crkva sv. Mikule u obliku križa u pravokutnom tijelu, nastala pod bizantskim utjecajem. Na Poljudu se nalazila crkva sv. Marije, a nedaleko od nje šesterolisna crkva sv. Trojice, najbolje očuvana građevina oktogonalnoga tipa u Dalmaciji (VIII–IX. st.). Od većine ranosrednjovjekovnih crkava sačuvani su tek pojedini građevni dijelovi ili dijelovi crkvenoga namještaja, često uklopljeni u mlađe građevine. Iz toga je razdoblja mnogobrojna i raznovrsna pleterna ornamentika (krsni zdenac hrvatskoga kralja Krešimira IV. iz XI. st.) i sarkofazi (nadbiskupa Ivana II. iz X. st.) te iluminacije. (→ splitski evanđelistar)
+Iz doba romanike sačuvan je velik broj stambenih zgrada omanjih dimenzija i nekoliko palača (Ciprianis, 1394), a najistaknutiji je spomenik zvonik katedrale (započet u XII. st., potkraj XV. i početkom XVI. st. povišen i završen gotičko-renesansnim gornjim katom). Romaničkoga su stila skulpture na zvoniku (majstor Otto, XIII. st., i trogirski majstori Radovanova kruga, druga polovica XIII. st.), propovjedaonica u unutrašnjosti katedrale, drvene vratnice majstora Buvine (1214), korska sjedala (druga polovica XIII. st.) i crkveni liturgijski predmeti, relikvijari mjesnih svetaca i dr. Romaničko slikarstvo zastupljeno je ikonama i raspelima splitske slikarske škole (Gospa od zvonika, druga polovica XIII. st.).
+Gotika se pojavila u XIV. st. (Hrvojev misal, izrađen za crkvu sv. Mihovila, 1403–04), a vrhunac je dosegnula nakon mletačkoga osvojenja grada 1420. u gradskim palačama, koje nose oznake venecijanskoga tzv. cvjetnoga stila. Podižu se i plemićke palače s unutarnjim dvorištem, a neke od njih gradio je ili pregradio Juraj Dalmatinac (Papalićeva palača, danas Muzej grada Splita; tzv. Mala Papalićeva palača). Kasnogotička skulptura zastupljena je u katedrali dvama bočnim oltarima: sv. Dujma, rad Bonina iz Milana (1427), i sv. Staša Jurja Dalmatinca (1448). U slikarstvu su prevladavali domaći majstori (Dujam Marinov Vušković i Ivan Petrov iz Milana rade freske u katedrali), a neko je vrijeme u Splitu djelovao Blaž Jurjev Trogiranin (slikano raspelo u crkvi sv. Frane).
+U XVI. st. pojavile su se prve kuće i palače u renesansnome stilu (kuća Karepić na Narodnome trgu; palača Grisogono-Cipci na Peristilu), a istih su značajki reljefi Andrije Alešija i radovi iz kruga Nikole Firentinca (Majka Božja s djetetom na sjevernim gradskim zidinama, 1503) te nadgrobne ploče samostana u Poljudu.
+U XVII. st. izgrađen je novi sustav poligonalnih utvrda oko grada, a u njem nove palače barokno raščlanjenih pročelja (Cindro u Krešimirovoj ulici, Milesi na Voćnom trgu). Talijanski graditelj Francesco Melchiori izgradio je crkvu sv. Filipa (1725–35), a najveće predgrađe Veli Varoš razvija se oko barokne crkve sv. Križa. U slikarstvu su očuvana djela talijanskih (Jacopa Palme ml.) i domaćih autora (Mateja Ponzonija).
+Pod kratkom francuskom vlašću početkom XIX. st. izvedeni su krupni komunalni zahvati (djelomično rušenje zidina, gradnja cesta, obale i perivoja), a prostorni se rast nastavio i nakon 1813., u razdoblju austrijske uprave, gradnjom luke i spajanjem predgrađa sa starom gradskom jezgrom. Potkraj toga razdoblja, 1914. izrađen je prvi poznati urbanistički plan grada.
+U XIX. st. u široj gradskoj jezgri podižu se zgrade u povijesnim stilovima (Bajamontijeva palača, 1858; Prokurative, 1863–67. i 1909–28; Kazalište, 1893., danas Hrvatsko narodno kazalište), a početkom XX. st. i niz reprezentativnih secesijskih ostvarenja (Palača Nakić na Narodnome trgu, Špiro Nakić, 1902; Sumporno kupalište, Kamilo Tončić, 1903).
+Nakon I. svjetskoga rata grad se sve više širi izvan stare jezgre. Nastaje niz zgrada novoga modernističkog izraza poput Osnovne škole Manuš-Dobri (danas Osnovna škola Dobri, Josip Kodl, 1930) i hotela Ambasador na rivi (J. Kodl, 1937), Biološko-oceanografskoga instituta na Marjanu (danas Institut za oceanografiju i ribarstvo, Fabijan Kaliterna, 1933), Palače Bratimske blagajne na Bačvicama (Emil Ciciliani, 1939) i dr.
+Split je tada bio druga rezidencija Ivana Meštrovića, koji je po vlastitoj zamisli dao sagraditi svoju palaču na Mejama (1931–39., danas Galerija Meštrović). Na kraju zapadne obale 1940. podignuta je zgrada Primorske banovine (danas Gradska uprava), djelo zagrebačkoga tima, Vladimira Turine, Nikole Despota i Vida Vrbanića.
+Ubrzani razvoj gospodarstva nakon II. svjetskoga rata, a time i velik priljev stanovništva, potaknuo je masovnu stambenu gradnju. Grad se širi isprva prema sjeveru; 1949. uz splitsko brodogradilište nastaje prvo naselje kolektivnoga stanovanja (Zlatibor Lukšić i Dinko Vesanović), a potom se definiraju nove gradske četvrti te nastaju naselja poput Poljuda i Spinuta (stambene zgrade Ive Radića, 1968; tzv. Kineski zid Frane Gotovca, 1970–71). Prema istoku se u blizini Gripa ekonomičnim, tipskim višekatnicama gradi Split II (Josip Vojnović i Lovro Perković, 1962) i još istočnije Split III, vrhunsko urbanističko-arhitektonsko ostvarenje (više autora, 1973–82; predviđena izgradnja 14 000 stanova), te naselje Žnjan (Neno Kezić, Emil Šverko i dr., 1990–2006) i dr. Istodobno nastaju i novi gradski orijentiri; u širem središtu podižu se javne zgrade modernističkoga izraza (zgrada Oblasnoga narodnog odbora, danas Ured državne uprave u Splitsko-dalmatinskoj županiji, područni ured Porezne uprave i Prekršajni sud, Marko Markovina, 1951; Palača pravde, Stanko Fabris, 1965. i 1973), poslovni neboderi (Slobodne Dalmacije, Z. Lukšić 1963; Koteksa, L. Perković, 1964) i robne kuće Prima (Antun Šatara, 1966) i Dalma (Vuko Bombardelli, 1975) te u novome istočnom djelu grada Prima 3 (Ante Svarčić, 1981). Na zapadnoj obali nastaje modernistički hotel Marjan (L. Perković, 1963) i zgrada Pomorske privrede (Neven Šegvić, 1964), a na Gripama ekspresionistički oblikovan sportsko-poslovni kompleks (Slaven Rožić, 1979., 1981), novo žarište grada.
+Početkom XXI. st. u istočnome dijelu grada podignut je studentski kampus; uz Srednjoškolski centar na Visokoj (1992) i Ekonomski fakultet (2001) Dinka Kovačića izgrađena je i nova Sveučilišna knjižica (više autora, 2009) te nekoliko fakulteta i studenski domovi. Uz splitske, u izgradnji prepoznatljivih gradskih ostvarenja sudjelovali su i zagrebački arhitekti (Muzej hrvatskih arheoloških spomenika, Mladen Kauzlarić, 1976; Gradski stadion u Poljudu, Boris Magaš, 1979; Spaladium arena, Studio 3LHD, 2008).</t>
+  </si>
+  <si>
+    <t>45.24</t>
+  </si>
+  <si>
+    <t>13.94</t>
+  </si>
+  <si>
+    <t>PU</t>
+  </si>
+  <si>
+    <t>52000 Pazin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grad Pazin prvi se put spominje 983. kao tzv. Pazinska utvrda (lat. castrum Pisinum). Od 12. stoljeća Pazin je središte Pazinske knežije, nad kojom su 1374. preuzeli vlast Habsburgovci. 1822. Austrija je Pazin učinila upravnim središtem Istarskog okruga. 
+Pazinski je kraj u 19. st. bio većinski hrvatski, no vlast su držali Talijani i talijanaši. Hrvati su bili mahom težaci i koloni, a Talijani i talijanaši su bili među trgovcima, veleposjednicima i razni pripadnici slobodnih profesija. Koloni u Pazinu su bili u gorem položaju od inih kolona s poluotoka, jer je uglavnom bio slučaj da nisu imali ni kuću ni zemlju. Od 4400 posjednika, pravu su moć imalo njih sedmero iz talijanaško-talijanskih redova. Posjedi su se često prodavali, a zemljišta su posebice kupovali doseljenici iz Furlanije.
+Zadnja desetljeća 19. stoljeća podižu bitnost grada Pazina, zbog čega hrvatski, talijanaški i talijanski pokret svoje središte prebacuju u taj gradić. Tome je pridonijela činjenica da koju su sve strane shvatile, da tko pobijedi na središnjem dijelu Istre, koji je bio uglavnom naseljen Hrvatima, vrlo će vjerojatno pobijediti u cijeloj pokrajini. Stoga su usredotočili svoje političke i gospodarske resurse prema Pazinu, pa su i same vlasti 1880-ih onamo namjeravale preseliti sjedište Istarskoga sabora iz Poreča. Okolnosti su bile takve da je markgrofovija Istra bila izrazito nepismena, izuzevši Krk i Kastavštinu, sve kao posljedica dotadašnje talijanaško-talijanske politike. Tako nepismeni predjeli nisu ni mogli dati kvalitetnih kadrova koji bi vodili nacionalni preporod, stoga se poslalo preporoditelje iz pismenijih dijelova markgrofovije, s Kastavštine i s Krka. Borba je bila vrlo teška - primjerice, pazinski načelnik Ante Dukić iz Kastavštine je umro zbog iscrpljenosti. Na njegovo je mjesto došao doktor prava Dinko Trinajstić, koji je udovoljio uvjetima za kandidata: iznimno jako zdravlje i natprosječna fizička snaga. Trinajstić je energično vladao, prekinuvši praksu ponizna nastupa pred zelenašima (kreditno-špekulantska mreža[5]), a mahom su bili iz talijanaško-talijanske koja je do tada vladala. U tome su pravcu utemeljene podružnice narodnjačke Istarske posujilnice radi uništavanja posla zelenašima. Time zelenaši i talijanaši više nisu mogli za sušnih godina manipulirati siromašnim pazinskim težacima, mahom Hrvatima. Hrvatski je književnik Vladimir Nazor koji je tih godina službovao u pazinskoj gimnaziji, opisao je grad Pazin iz vremena Trinajstićeva načelnikovanja Pazinom kao "srcem srca Istre". Trinajstić je tako dobro vodio općinu da je na svoju stranu privukao one koji su do tada bili neodlučni ili ovisni. Stvorivši takvu većinu, načelnik koji je došao iza njega, Šime Kurelić iz Pićna imao je tako veliku bazu da je bio načelnikom dva desetljeća sve dok Italija nije 1918. okupirala taj kraj, a Kurelića zatočila.
+Tako je u drugoj polovini 19. stoljeća Pazin postao jednim od središta hrvatskog kulturnog preporoda, te su osnovane Čitaonica, Hrvatska gimnazija i Narodni dom. Sve te institucije ukinute su kada je nakon Prvog svjetskog rata Pazin 1918. okupirala, a potom anektirala Italija. Ipak, preporoditeljski rad je urodio plodom. Učinci su talijanizacije uvelike neutralizirani i poništeni. Doseljeni Talijani i talijanaši su nakon desetljeća odbijanja shvaćanja povijesne zbilje shvatili stvarne okolnosti; rashrvaćivanje i talijanizacija je vremenom oslabilo te je tako od 1880. do 1910. broj osoba koje su službeno izjasnile kao Talijani skoro prepolovio.
+Za vrijeme Drugog svjetskog rata, nakon što je Italija kapitulirala, Pazin su u rujnu 1943. zauzeli istarski partizani. U tom je gradu Pokrajinski NOO za Istru donio odluku kojom se Istra sjedinjuje s maticom Hrvatskom. Ta je odluka godine 1947. potvrđena Pariškim mirovnim ugovorom. 
+Nakon što je Hrvatska 1991. godine postala neovisna, Pazin, iako je po ekonomskoj snazi zaostajao za Pulom, određen je kao sjedište Istarske županije uglavnom iz povijesnih razloga. </t>
+  </si>
+  <si>
+    <t>42.66</t>
+  </si>
+  <si>
+    <t>20000 Dubrovnik</t>
+  </si>
+  <si>
+    <t>DU</t>
+  </si>
+  <si>
+    <t>Na ulasku u Jadransko more to je prva otocima zaštićena točka na pomorskom putu od istoka prema zapadu, a dolinom Neretve najbrže je povezan s unutrašnjošću. Novija arheološka istraživanja utvrdila su da je naselje na mjestu današnjeg grada postojalo u 6. stoljeću, a vjerojatno i prije. Širi se dolaskom Hrvata, nakon napuštanja antičkog Epidaura (današnji Cavtat) u 7. stoljeću.
+Pojačani promet između istoka i zapada, za vrijeme i nakon križarskih ratova, potaknuli su u 12. i 13. stoljeću razvoj pomorsko-trgovačkih središta na Mediteranu i Jadranu, među njima i Dubrovnika. Oslobađanje od mletačkog utjecaja, koje je Dubrovnik ishodio Zadarskim mirom 1358., presudno je za njegov daljnji uspješan razvoj. Ostalim dalmatinskim gradovima to nije uspjelo pa su 1420. g. definitivno potpali pod vlast Mletačke Republike. Već tijekom 14. i u 15. stoljeću Dubrovnik je, uz Veneciju i Anconu, najznačajnije pomorsko-trgovačko središte na Jadranu. Ugovorima i kupnjom Dubrovčani proširuju svoj teritorij od Kleka na sjeveru do Sutorine na ulazu u Bokokotorski zaljev, zajedno s otocima Mljetom, Lastovom, Elafitima i Lokrumom.
+U 15. stoljeću potpuno je izgrađen državnopravni položaj Dubrovačke Republike, što znači samostalno biranje kneza i vijećnika, kovanje novca i državna zastava s likom sv. Vlaha, samostalno zakonodavstvo i pravo otvaranja konzulata u inozemstvu. Prema aristokratskom ustavu, temelj državne vlasti činilo je Veliko vijeće dubrovačke vlastele koje bira Vijeće umoljenih i Malo vijeće kao izvršni organ Velikog vijeća. Knez se birao svaki mjesec kao nominalni simbol vlasti.
+Dubrovčani su već u 15. stoljeću dobro organizirali tranzitnu trgovinu s balkanskim zaleđem. Zbog sve jače osvajačke politike Turske na Balkanu, Dubrovačka Republika je 1525. prihvatila tursko pokroviteljstvo i plaćanje tributa, ali su od njih ishodili slobodu trgovanja po čitavom turskom carstvu, uz carinu od samo 2 %. Malena država, bez vlastite vojske, dovela je do savršenstva svoj obrambeni sustav vještom diplomatskom službom i razgranatom konzularnom djelatnošću. Ustrajavanje na neutralnosti u međunarodnim sukobima i pokroviteljstvu moćnih država, poglavito Španjolske i Vatikana, omogućuju joj očuvanje nezavisnosti. Jedini stalni konkurent i neprijatelj bila joj je Mletačka Republika.
+Zlatno doba Dubrovačke Republike nastupa u 16. stoljeću kada sjaj i moć Mletačke Republike jenjava. Temelj prosperiteta čini pomorska trgovina. Dubrovačka trgovačka mornarica u 16. stoljeću svojom kvalitetom i brojem od 180 do 200 brodova dostiže svjetsku razinu. Grade se sve veći brodovi tipa galijuna, karaka i nava, koji poduzimaju sve duža i opasnija putovanja po cijelom Mediteranu, Crnom moru i oceanom do sjevernih luka Engleske i Njemačke, a plovili su i do Indije i Amerike. Dubrovčani postaju svjetski poznati i traženi prijevoznici tereta, s vrlo razgranatim pomorsko-trgovačkim poslovanjem.
+Materijalno blagostanje, osjećaj sigurnosti i slobode, formiralo je kulturu življenja u humanističkom duhu i potaklo kreativan stvaralački polet. Dubrovnik doseže blistave domete u svom urbanističkom i graditeljskom razvoju koji se zadržao do danas u književnosti i pjesništvu (Marin Držić, Ivan Gundulić), znanosti (Ruđer Bošković) i mnogim drugim vidovima umjetnosti i kulture.
+Opća kriza pomorstva na Mediteranu u 17. stoljeću pogodila je i dubrovačku pomorsku trgovinu. Katastrofalni potres 1667. doveo je Dubrovačku Republiku u kritično razdoblje borbe za opstanak i političkog očuvanja nezavisnosti. 18. stoljeće donosi Dubrovniku priliku za gospodarskom obnovom u pomorskoj trgovini pod neutralnom zastavom i tako dočekuje Napoleonovo ukinuće Dubrovačke Republike 1808.
+Bečkim kongresom 1815. dubrovačka regija je pripojena ostalom dijelu Dalmacije i Hrvatske i od tada dijele zajedničku političku sudbinu.
+Nakon proglašenja neovisnosti Republike Hrvatske i srpske agresije na Hrvatsku, Dubrovnik je bio napadnut u listopadu 1991. neviđenom uništavajućom silom Srba i Crnogoraca, u nakani da čitav kraj osvoje i unište. Dubrovački kraj je bio okupiran i znatno porušen, a sam grad u osmomjesečnom potpunom okruženju više puta bombardiran i najbrutalnije razaran, posebno 6. prosinca 1991. g.</t>
+  </si>
+  <si>
+    <t>46.39</t>
+  </si>
+  <si>
+    <t>16.42</t>
+  </si>
+  <si>
+    <t>40000 Čakovec</t>
+  </si>
+  <si>
+    <t>ČK</t>
+  </si>
+  <si>
+    <t>Prema dosad poznatim podacima, prvo naselje na današnjem području Čakovca podigli su Rimljani pod nazivom Aquama, kao utvrdu za vojne potrebe. Čakovec je ime dobio po grofu Dimitriju Csakyju (Čakiju), koji je početkom 13. stoljeća podigao drvenu utvrdu nazvanu “Čakov turen”. Prvi puta izrijekom se Čakovec, kao utvrđeni grad, spominje 1333. godine u ispravi kralja Roberta. Kroz svoju burnu povijest Čakovec je, kao i Međimurje, često mijenjao gospodare. Najznačajnije razdoblje je svakako 16. i 17. stoljeće, kada su u Čakovcu stolovali hrvatski banovi i vojskovođe iz obitelji Zrinski. Kroz više generacija obitelj Zrinski je od čakovečke utvrde stvorila jedan od najraskošnijih hrvatskih i europskih dvoraca toga doba.
+U to vrijeme grad je bio oaza civilizacije i kulture na vječno nemirnoj turskoj granici i mjesto na kojem su se donosile odluke od bitnog značaja kako za Hrvatsku i njeno srednjoeuropsko okruženje. U Čakovcu su održane banske konferencije za Nikole Zrinskog -Čakovečkog (1620.-1664.).
+Poveljom Jurja IV. Zrinskog, od 29. svibnja 1579. godine, stanovnicima podgrađa čakovečke utvrde daje se status slobodnog trgovišta, čime je naselje dobilo osnovne atribute grada.
+1848. godine Čakovec je proglašen slobodnim kraljevskim gradom. Izabrano je gradsko vijeće od 30 članova, njegov izvršni organ – Savjet Grada Čakovca od 10 članova te prvi gradonačelnik. Snažan gospodarski i društveni polet Čakovec doživljava u drugoj polovici 19. stoljeća izgradnjom željezničke pruge, jedne od prvih na ovim prostorima.
+Ustrojavanjem jedinica lokalne uprave i samouprave, čime je Republika Hrvatska podijeljena na županije, te gradove i općine, Čakovec 1993. godine ponovo dobiva status grada.</t>
+  </si>
+  <si>
+    <t>ZG</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>49000 Krapina</t>
+  </si>
+  <si>
+    <t>47000 Karlovac</t>
+  </si>
+  <si>
+    <t>385 (0)49</t>
+  </si>
+  <si>
+    <t>385 (0)1</t>
+  </si>
+  <si>
+    <t>385 (0)44</t>
+  </si>
+  <si>
+    <t>385 (0)47</t>
+  </si>
+  <si>
+    <t>385 (0)42</t>
+  </si>
+  <si>
+    <t>385 (0)48</t>
+  </si>
+  <si>
+    <t>385 (0)43</t>
+  </si>
+  <si>
+    <t>385 (0)51</t>
+  </si>
+  <si>
+    <t>385 (0)53</t>
+  </si>
+  <si>
+    <t>385 (0)33</t>
+  </si>
+  <si>
+    <t>385 (0)34</t>
+  </si>
+  <si>
+    <t>385 (0)35</t>
+  </si>
+  <si>
+    <t>385 (0)23</t>
+  </si>
+  <si>
+    <t>385 (0)31</t>
+  </si>
+  <si>
+    <t>385 (0)22</t>
+  </si>
+  <si>
+    <t>385 (0)32</t>
+  </si>
+  <si>
+    <t>385 (0)21</t>
+  </si>
+  <si>
+    <t>385 (0)52</t>
+  </si>
+  <si>
+    <t>385 (0)20</t>
+  </si>
+  <si>
+    <t>385 (0)40</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -370,12 +1184,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1589,8 +2412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C803E9B5-3D36-F741-9558-D084333C0D41}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1730,4 +2553,1903 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B507D620-4341-924E-8188-4E502D276425}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView topLeftCell="M1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="114.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="55.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="67.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="82.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E265F14-DFAD-2341-A15B-FDB6F5CC7122}">
+  <dimension ref="A1:AA21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="27" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1196</v>
+      </c>
+      <c r="D2">
+        <v>641.20000000000005</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2">
+        <v>48266</v>
+      </c>
+      <c r="L2">
+        <v>54761</v>
+      </c>
+      <c r="M2">
+        <v>67188</v>
+      </c>
+      <c r="N2">
+        <v>82848</v>
+      </c>
+      <c r="O2">
+        <v>111565</v>
+      </c>
+      <c r="P2">
+        <v>136351</v>
+      </c>
+      <c r="Q2">
+        <v>167765</v>
+      </c>
+      <c r="R2">
+        <v>258024</v>
+      </c>
+      <c r="S2">
+        <v>356529</v>
+      </c>
+      <c r="T2">
+        <v>393919</v>
+      </c>
+      <c r="U2">
+        <v>478076</v>
+      </c>
+      <c r="V2">
+        <v>629896</v>
+      </c>
+      <c r="W2">
+        <v>723065</v>
+      </c>
+      <c r="X2">
+        <v>777826</v>
+      </c>
+      <c r="Y2">
+        <v>779145</v>
+      </c>
+      <c r="Z2">
+        <v>790017</v>
+      </c>
+      <c r="AA2">
+        <v>767131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>242</v>
+      </c>
+      <c r="D3">
+        <v>47.7</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K3">
+        <v>5457</v>
+      </c>
+      <c r="L3">
+        <v>6060</v>
+      </c>
+      <c r="M3">
+        <v>6435</v>
+      </c>
+      <c r="N3">
+        <v>7007</v>
+      </c>
+      <c r="O3">
+        <v>7538</v>
+      </c>
+      <c r="P3">
+        <v>8141</v>
+      </c>
+      <c r="Q3">
+        <v>7884</v>
+      </c>
+      <c r="R3">
+        <v>8224</v>
+      </c>
+      <c r="S3">
+        <v>9222</v>
+      </c>
+      <c r="T3">
+        <v>9473</v>
+      </c>
+      <c r="U3">
+        <v>10384</v>
+      </c>
+      <c r="V3">
+        <v>11533</v>
+      </c>
+      <c r="W3">
+        <v>12540</v>
+      </c>
+      <c r="X3">
+        <v>12938</v>
+      </c>
+      <c r="Y3">
+        <v>12950</v>
+      </c>
+      <c r="Z3">
+        <v>12480</v>
+      </c>
+      <c r="AA3">
+        <v>11530</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="288" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5">
+        <v>95</v>
+      </c>
+      <c r="D4">
+        <v>421.4</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" t="s">
+        <v>148</v>
+      </c>
+      <c r="J4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K4">
+        <v>15738</v>
+      </c>
+      <c r="L4">
+        <v>18669</v>
+      </c>
+      <c r="M4">
+        <v>20433</v>
+      </c>
+      <c r="N4">
+        <v>22829</v>
+      </c>
+      <c r="O4">
+        <v>24277</v>
+      </c>
+      <c r="P4">
+        <v>26014</v>
+      </c>
+      <c r="Q4">
+        <v>26234</v>
+      </c>
+      <c r="R4">
+        <v>28799</v>
+      </c>
+      <c r="S4">
+        <v>28893</v>
+      </c>
+      <c r="T4">
+        <v>34776</v>
+      </c>
+      <c r="U4">
+        <v>43382</v>
+      </c>
+      <c r="V4">
+        <v>55095</v>
+      </c>
+      <c r="W4">
+        <v>59812</v>
+      </c>
+      <c r="X4">
+        <v>61413</v>
+      </c>
+      <c r="Y4">
+        <v>52236</v>
+      </c>
+      <c r="Z4">
+        <v>47768</v>
+      </c>
+      <c r="AA4">
+        <v>40121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="208" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>123</v>
+      </c>
+      <c r="D5">
+        <v>401.4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G5" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J5" t="s">
+        <v>152</v>
+      </c>
+      <c r="K5">
+        <v>24865</v>
+      </c>
+      <c r="L5">
+        <v>26964</v>
+      </c>
+      <c r="M5">
+        <v>26947</v>
+      </c>
+      <c r="N5">
+        <v>30339</v>
+      </c>
+      <c r="O5">
+        <v>32608</v>
+      </c>
+      <c r="P5">
+        <v>34713</v>
+      </c>
+      <c r="Q5">
+        <v>35171</v>
+      </c>
+      <c r="R5">
+        <v>41120</v>
+      </c>
+      <c r="S5">
+        <v>44974</v>
+      </c>
+      <c r="T5">
+        <v>50342</v>
+      </c>
+      <c r="U5">
+        <v>58013</v>
+      </c>
+      <c r="V5">
+        <v>63887</v>
+      </c>
+      <c r="W5">
+        <v>69622</v>
+      </c>
+      <c r="X5">
+        <v>73426</v>
+      </c>
+      <c r="Y5">
+        <v>59395</v>
+      </c>
+      <c r="Z5">
+        <v>55705</v>
+      </c>
+      <c r="AA5">
+        <v>49377</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5">
+        <v>731</v>
+      </c>
+      <c r="D6">
+        <v>59.9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="G6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="I6" t="s">
+        <v>157</v>
+      </c>
+      <c r="J6" t="s">
+        <v>158</v>
+      </c>
+      <c r="K6">
+        <v>11560</v>
+      </c>
+      <c r="L6">
+        <v>12188</v>
+      </c>
+      <c r="M6">
+        <v>12116</v>
+      </c>
+      <c r="N6">
+        <v>13021</v>
+      </c>
+      <c r="O6">
+        <v>14931</v>
+      </c>
+      <c r="P6">
+        <v>16925</v>
+      </c>
+      <c r="Q6">
+        <v>17441</v>
+      </c>
+      <c r="R6">
+        <v>17112</v>
+      </c>
+      <c r="S6">
+        <v>21602</v>
+      </c>
+      <c r="T6">
+        <v>23743</v>
+      </c>
+      <c r="U6">
+        <v>31243</v>
+      </c>
+      <c r="V6">
+        <v>39383</v>
+      </c>
+      <c r="W6">
+        <v>45844</v>
+      </c>
+      <c r="X6">
+        <v>48834</v>
+      </c>
+      <c r="Y6">
+        <v>49075</v>
+      </c>
+      <c r="Z6">
+        <v>46946</v>
+      </c>
+      <c r="AA6">
+        <v>43782</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5">
+        <v>311</v>
+      </c>
+      <c r="D7">
+        <v>91.8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J7" t="s">
+        <v>159</v>
+      </c>
+      <c r="K7">
+        <v>4554</v>
+      </c>
+      <c r="L7">
+        <v>5823</v>
+      </c>
+      <c r="M7">
+        <v>6582</v>
+      </c>
+      <c r="N7">
+        <v>7574</v>
+      </c>
+      <c r="O7">
+        <v>8544</v>
+      </c>
+      <c r="P7">
+        <v>11552</v>
+      </c>
+      <c r="Q7">
+        <v>11536</v>
+      </c>
+      <c r="R7">
+        <v>11932</v>
+      </c>
+      <c r="S7">
+        <v>12864</v>
+      </c>
+      <c r="T7">
+        <v>14139</v>
+      </c>
+      <c r="U7">
+        <v>16582</v>
+      </c>
+      <c r="V7">
+        <v>21104</v>
+      </c>
+      <c r="W7">
+        <v>25941</v>
+      </c>
+      <c r="X7">
+        <v>29706</v>
+      </c>
+      <c r="Y7">
+        <v>30994</v>
+      </c>
+      <c r="Z7">
+        <v>30854</v>
+      </c>
+      <c r="AA7">
+        <v>28580</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5">
+        <v>198</v>
+      </c>
+      <c r="D8">
+        <v>187.9</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="G8" t="s">
+        <v>166</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I8" t="s">
+        <v>163</v>
+      </c>
+      <c r="J8" t="s">
+        <v>164</v>
+      </c>
+      <c r="K8">
+        <v>10128</v>
+      </c>
+      <c r="L8">
+        <v>11763</v>
+      </c>
+      <c r="M8">
+        <v>12942</v>
+      </c>
+      <c r="N8">
+        <v>16123</v>
+      </c>
+      <c r="O8">
+        <v>19652</v>
+      </c>
+      <c r="P8">
+        <v>21974</v>
+      </c>
+      <c r="Q8">
+        <v>22990</v>
+      </c>
+      <c r="R8">
+        <v>24134</v>
+      </c>
+      <c r="S8">
+        <v>26981</v>
+      </c>
+      <c r="T8">
+        <v>27645</v>
+      </c>
+      <c r="U8">
+        <v>29907</v>
+      </c>
+      <c r="V8">
+        <v>35578</v>
+      </c>
+      <c r="W8">
+        <v>39893</v>
+      </c>
+      <c r="X8">
+        <v>42066</v>
+      </c>
+      <c r="Y8">
+        <v>41869</v>
+      </c>
+      <c r="Z8">
+        <v>40276</v>
+      </c>
+      <c r="AA8">
+        <v>36316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2488</v>
+      </c>
+      <c r="D9" s="5">
+        <v>43.4</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G9" t="s">
+        <v>235</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I9" t="s">
+        <v>168</v>
+      </c>
+      <c r="J9" t="s">
+        <v>169</v>
+      </c>
+      <c r="K9">
+        <v>18597</v>
+      </c>
+      <c r="L9">
+        <v>23880</v>
+      </c>
+      <c r="M9">
+        <v>27904</v>
+      </c>
+      <c r="N9">
+        <v>38959</v>
+      </c>
+      <c r="O9">
+        <v>51419</v>
+      </c>
+      <c r="P9">
+        <v>66042</v>
+      </c>
+      <c r="Q9">
+        <v>61157</v>
+      </c>
+      <c r="R9">
+        <v>72111</v>
+      </c>
+      <c r="S9">
+        <v>67088</v>
+      </c>
+      <c r="T9">
+        <v>73718</v>
+      </c>
+      <c r="U9">
+        <v>98759</v>
+      </c>
+      <c r="V9">
+        <v>129173</v>
+      </c>
+      <c r="W9">
+        <v>158226</v>
+      </c>
+      <c r="X9">
+        <v>165904</v>
+      </c>
+      <c r="Y9">
+        <v>144043</v>
+      </c>
+      <c r="Z9">
+        <v>128624</v>
+      </c>
+      <c r="AA9">
+        <v>107964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5">
+        <v>967.4</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" t="s">
+        <v>175</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" t="s">
+        <v>176</v>
+      </c>
+      <c r="J10" t="s">
+        <v>177</v>
+      </c>
+      <c r="K10">
+        <v>32381</v>
+      </c>
+      <c r="L10">
+        <v>33164</v>
+      </c>
+      <c r="M10">
+        <v>31371</v>
+      </c>
+      <c r="N10">
+        <v>34376</v>
+      </c>
+      <c r="O10">
+        <v>38103</v>
+      </c>
+      <c r="P10">
+        <v>35380</v>
+      </c>
+      <c r="Q10">
+        <v>35600</v>
+      </c>
+      <c r="R10">
+        <v>35312</v>
+      </c>
+      <c r="S10">
+        <v>26920</v>
+      </c>
+      <c r="T10">
+        <v>26285</v>
+      </c>
+      <c r="U10">
+        <v>27390</v>
+      </c>
+      <c r="V10">
+        <v>26683</v>
+      </c>
+      <c r="W10">
+        <v>23285</v>
+      </c>
+      <c r="X10">
+        <v>22026</v>
+      </c>
+      <c r="Y10">
+        <v>12980</v>
+      </c>
+      <c r="Z10">
+        <v>12745</v>
+      </c>
+      <c r="AA10">
+        <v>11502</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5">
+        <v>113</v>
+      </c>
+      <c r="D11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="G11" t="s">
+        <v>183</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I11" t="s">
+        <v>179</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="K11">
+        <v>4869</v>
+      </c>
+      <c r="L11">
+        <v>6356</v>
+      </c>
+      <c r="M11">
+        <v>6540</v>
+      </c>
+      <c r="N11">
+        <v>7762</v>
+      </c>
+      <c r="O11">
+        <v>8980</v>
+      </c>
+      <c r="P11">
+        <v>9682</v>
+      </c>
+      <c r="Q11">
+        <v>11243</v>
+      </c>
+      <c r="R11">
+        <v>13088</v>
+      </c>
+      <c r="S11">
+        <v>13222</v>
+      </c>
+      <c r="T11">
+        <v>15136</v>
+      </c>
+      <c r="U11">
+        <v>17578</v>
+      </c>
+      <c r="V11">
+        <v>19367</v>
+      </c>
+      <c r="W11">
+        <v>20905</v>
+      </c>
+      <c r="X11">
+        <v>22931</v>
+      </c>
+      <c r="Y11">
+        <v>22618</v>
+      </c>
+      <c r="Z11">
+        <v>21291</v>
+      </c>
+      <c r="AA11">
+        <v>19302</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5">
+        <v>167</v>
+      </c>
+      <c r="D12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="G12" t="s">
+        <v>188</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="K12">
+        <v>5191</v>
+      </c>
+      <c r="L12">
+        <v>6139</v>
+      </c>
+      <c r="M12">
+        <v>6310</v>
+      </c>
+      <c r="N12">
+        <v>7871</v>
+      </c>
+      <c r="O12">
+        <v>9437</v>
+      </c>
+      <c r="P12">
+        <v>11020</v>
+      </c>
+      <c r="Q12">
+        <v>12054</v>
+      </c>
+      <c r="R12">
+        <v>12393</v>
+      </c>
+      <c r="S12">
+        <v>13715</v>
+      </c>
+      <c r="T12">
+        <v>15450</v>
+      </c>
+      <c r="U12">
+        <v>19508</v>
+      </c>
+      <c r="V12">
+        <v>24939</v>
+      </c>
+      <c r="W12">
+        <v>26708</v>
+      </c>
+      <c r="X12">
+        <v>28157</v>
+      </c>
+      <c r="Y12">
+        <v>28201</v>
+      </c>
+      <c r="Z12">
+        <v>26248</v>
+      </c>
+      <c r="AA12">
+        <v>22294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5">
+        <v>922</v>
+      </c>
+      <c r="D13" s="5">
+        <v>54.1</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="G13" t="s">
+        <v>193</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I13" t="s">
+        <v>190</v>
+      </c>
+      <c r="J13" t="s">
+        <v>191</v>
+      </c>
+      <c r="K13">
+        <v>4015</v>
+      </c>
+      <c r="L13">
+        <v>4775</v>
+      </c>
+      <c r="M13">
+        <v>5872</v>
+      </c>
+      <c r="N13">
+        <v>6940</v>
+      </c>
+      <c r="O13">
+        <v>9627</v>
+      </c>
+      <c r="P13">
+        <v>13193</v>
+      </c>
+      <c r="Q13">
+        <v>13729</v>
+      </c>
+      <c r="R13">
+        <v>19203</v>
+      </c>
+      <c r="S13">
+        <v>20196</v>
+      </c>
+      <c r="T13">
+        <v>23116</v>
+      </c>
+      <c r="U13">
+        <v>30093</v>
+      </c>
+      <c r="V13">
+        <v>40043</v>
+      </c>
+      <c r="W13">
+        <v>49153</v>
+      </c>
+      <c r="X13">
+        <v>57229</v>
+      </c>
+      <c r="Y13">
+        <v>64612</v>
+      </c>
+      <c r="Z13">
+        <v>59141</v>
+      </c>
+      <c r="AA13">
+        <v>49891</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="240" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5">
+        <v>368</v>
+      </c>
+      <c r="D14">
+        <v>192.4</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I14" t="s">
+        <v>195</v>
+      </c>
+      <c r="J14" t="s">
+        <v>196</v>
+      </c>
+      <c r="K14">
+        <v>15190</v>
+      </c>
+      <c r="L14">
+        <v>16775</v>
+      </c>
+      <c r="M14">
+        <v>19778</v>
+      </c>
+      <c r="N14">
+        <v>21933</v>
+      </c>
+      <c r="O14">
+        <v>24778</v>
+      </c>
+      <c r="P14">
+        <v>27426</v>
+      </c>
+      <c r="Q14">
+        <v>26241</v>
+      </c>
+      <c r="R14">
+        <v>26882</v>
+      </c>
+      <c r="S14">
+        <v>23610</v>
+      </c>
+      <c r="T14">
+        <v>25465</v>
+      </c>
+      <c r="U14">
+        <v>33464</v>
+      </c>
+      <c r="V14">
+        <v>50520</v>
+      </c>
+      <c r="W14">
+        <v>67154</v>
+      </c>
+      <c r="X14">
+        <v>80355</v>
+      </c>
+      <c r="Y14">
+        <v>72718</v>
+      </c>
+      <c r="Z14">
+        <v>75062</v>
+      </c>
+      <c r="AA14">
+        <v>70779</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5">
+        <v>551</v>
+      </c>
+      <c r="D15">
+        <v>174.9</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="G15" t="s">
+        <v>203</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="K15">
+        <v>20858</v>
+      </c>
+      <c r="L15">
+        <v>24863</v>
+      </c>
+      <c r="M15">
+        <v>25260</v>
+      </c>
+      <c r="N15">
+        <v>27801</v>
+      </c>
+      <c r="O15">
+        <v>33407</v>
+      </c>
+      <c r="P15">
+        <v>40106</v>
+      </c>
+      <c r="Q15">
+        <v>42930</v>
+      </c>
+      <c r="R15">
+        <v>51871</v>
+      </c>
+      <c r="S15">
+        <v>58063</v>
+      </c>
+      <c r="T15">
+        <v>66073</v>
+      </c>
+      <c r="U15">
+        <v>84652</v>
+      </c>
+      <c r="V15">
+        <v>109189</v>
+      </c>
+      <c r="W15">
+        <v>123944</v>
+      </c>
+      <c r="X15">
+        <v>129792</v>
+      </c>
+      <c r="Y15">
+        <v>114616</v>
+      </c>
+      <c r="Z15">
+        <v>108048</v>
+      </c>
+      <c r="AA15">
+        <v>96313</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="335" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5">
+        <v>107</v>
+      </c>
+      <c r="D16">
+        <v>399.5</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="I16" t="s">
+        <v>205</v>
+      </c>
+      <c r="J16" t="s">
+        <v>206</v>
+      </c>
+      <c r="K16">
+        <v>15269</v>
+      </c>
+      <c r="L16">
+        <v>17245</v>
+      </c>
+      <c r="M16">
+        <v>17908</v>
+      </c>
+      <c r="N16">
+        <v>19572</v>
+      </c>
+      <c r="O16">
+        <v>23528</v>
+      </c>
+      <c r="P16">
+        <v>28514</v>
+      </c>
+      <c r="Q16">
+        <v>31735</v>
+      </c>
+      <c r="R16">
+        <v>34952</v>
+      </c>
+      <c r="S16">
+        <v>33343</v>
+      </c>
+      <c r="T16">
+        <v>37161</v>
+      </c>
+      <c r="U16">
+        <v>44440</v>
+      </c>
+      <c r="V16">
+        <v>47122</v>
+      </c>
+      <c r="W16">
+        <v>51445</v>
+      </c>
+      <c r="X16">
+        <v>55842</v>
+      </c>
+      <c r="Y16">
+        <v>51553</v>
+      </c>
+      <c r="Z16">
+        <v>46332</v>
+      </c>
+      <c r="AA16">
+        <v>42599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5">
+        <v>232</v>
+      </c>
+      <c r="D17">
+        <v>100.1</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="G17" t="s">
+        <v>213</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I17" t="s">
+        <v>210</v>
+      </c>
+      <c r="J17" t="s">
+        <v>211</v>
+      </c>
+      <c r="K17">
+        <v>8162</v>
+      </c>
+      <c r="L17">
+        <v>9453</v>
+      </c>
+      <c r="M17">
+        <v>10234</v>
+      </c>
+      <c r="N17">
+        <v>11205</v>
+      </c>
+      <c r="O17">
+        <v>11557</v>
+      </c>
+      <c r="P17">
+        <v>12149</v>
+      </c>
+      <c r="Q17">
+        <v>12116</v>
+      </c>
+      <c r="R17">
+        <v>12738</v>
+      </c>
+      <c r="S17">
+        <v>18994</v>
+      </c>
+      <c r="T17">
+        <v>20616</v>
+      </c>
+      <c r="U17">
+        <v>25763</v>
+      </c>
+      <c r="V17">
+        <v>38830</v>
+      </c>
+      <c r="W17">
+        <v>41959</v>
+      </c>
+      <c r="X17">
+        <v>46735</v>
+      </c>
+      <c r="Y17">
+        <v>31670</v>
+      </c>
+      <c r="Z17">
+        <v>27683</v>
+      </c>
+      <c r="AA17">
+        <v>23175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2022</v>
+      </c>
+      <c r="D18">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="G18" t="s">
+        <v>218</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I18" t="s">
+        <v>215</v>
+      </c>
+      <c r="J18" t="s">
+        <v>216</v>
+      </c>
+      <c r="K18">
+        <v>12417</v>
+      </c>
+      <c r="L18">
+        <v>14587</v>
+      </c>
+      <c r="M18">
+        <v>16883</v>
+      </c>
+      <c r="N18">
+        <v>18438</v>
+      </c>
+      <c r="O18">
+        <v>21925</v>
+      </c>
+      <c r="P18">
+        <v>25103</v>
+      </c>
+      <c r="Q18">
+        <v>29155</v>
+      </c>
+      <c r="R18">
+        <v>40029</v>
+      </c>
+      <c r="S18">
+        <v>54187</v>
+      </c>
+      <c r="T18">
+        <v>64874</v>
+      </c>
+      <c r="U18">
+        <v>85374</v>
+      </c>
+      <c r="V18">
+        <v>129203</v>
+      </c>
+      <c r="W18">
+        <v>176303</v>
+      </c>
+      <c r="X18">
+        <v>200459</v>
+      </c>
+      <c r="Y18">
+        <v>188694</v>
+      </c>
+      <c r="Z18">
+        <v>178102</v>
+      </c>
+      <c r="AA18">
+        <v>160577</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="304" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="5">
+        <v>60</v>
+      </c>
+      <c r="D19">
+        <v>139.1</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G19" t="s">
+        <v>222</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I19" t="s">
+        <v>220</v>
+      </c>
+      <c r="J19" t="s">
+        <v>221</v>
+      </c>
+      <c r="K19">
+        <v>7966</v>
+      </c>
+      <c r="L19">
+        <v>8167</v>
+      </c>
+      <c r="M19">
+        <v>8342</v>
+      </c>
+      <c r="N19">
+        <v>8330</v>
+      </c>
+      <c r="O19">
+        <v>9200</v>
+      </c>
+      <c r="P19">
+        <v>10317</v>
+      </c>
+      <c r="Q19">
+        <v>11211</v>
+      </c>
+      <c r="R19">
+        <v>10518</v>
+      </c>
+      <c r="S19">
+        <v>8685</v>
+      </c>
+      <c r="T19">
+        <v>8537</v>
+      </c>
+      <c r="U19">
+        <v>8389</v>
+      </c>
+      <c r="V19">
+        <v>8158</v>
+      </c>
+      <c r="W19">
+        <v>8889</v>
+      </c>
+      <c r="X19">
+        <v>9369</v>
+      </c>
+      <c r="Y19">
+        <v>9227</v>
+      </c>
+      <c r="Z19">
+        <v>8638</v>
+      </c>
+      <c r="AA19">
+        <v>8279</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="5">
+        <v>291</v>
+      </c>
+      <c r="D20">
+        <v>142.6</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G20" t="s">
+        <v>227</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I20" t="s">
+        <v>225</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="K20">
+        <v>14445</v>
+      </c>
+      <c r="L20">
+        <v>13398</v>
+      </c>
+      <c r="M20">
+        <v>15666</v>
+      </c>
+      <c r="N20">
+        <v>15329</v>
+      </c>
+      <c r="O20">
+        <v>17384</v>
+      </c>
+      <c r="P20">
+        <v>18396</v>
+      </c>
+      <c r="Q20">
+        <v>16719</v>
+      </c>
+      <c r="R20">
+        <v>20420</v>
+      </c>
+      <c r="S20">
+        <v>21778</v>
+      </c>
+      <c r="T20">
+        <v>24296</v>
+      </c>
+      <c r="U20">
+        <v>27793</v>
+      </c>
+      <c r="V20">
+        <v>35628</v>
+      </c>
+      <c r="W20">
+        <v>46025</v>
+      </c>
+      <c r="X20">
+        <v>51597</v>
+      </c>
+      <c r="Y20">
+        <v>43770</v>
+      </c>
+      <c r="Z20">
+        <v>42615</v>
+      </c>
+      <c r="AA20">
+        <v>41562</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="192" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5">
+        <v>353</v>
+      </c>
+      <c r="D21">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G21" t="s">
+        <v>232</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="I21" t="s">
+        <v>229</v>
+      </c>
+      <c r="J21" t="s">
+        <v>230</v>
+      </c>
+      <c r="K21">
+        <v>5790</v>
+      </c>
+      <c r="L21">
+        <v>7002</v>
+      </c>
+      <c r="M21">
+        <v>8580</v>
+      </c>
+      <c r="N21">
+        <v>9375</v>
+      </c>
+      <c r="O21">
+        <v>10815</v>
+      </c>
+      <c r="P21">
+        <v>11425</v>
+      </c>
+      <c r="Q21">
+        <v>13034</v>
+      </c>
+      <c r="R21">
+        <v>15108</v>
+      </c>
+      <c r="S21">
+        <v>17034</v>
+      </c>
+      <c r="T21">
+        <v>18119</v>
+      </c>
+      <c r="U21">
+        <v>20676</v>
+      </c>
+      <c r="V21">
+        <v>23775</v>
+      </c>
+      <c r="W21">
+        <v>27356</v>
+      </c>
+      <c r="X21">
+        <v>29996</v>
+      </c>
+      <c r="Y21">
+        <v>30455</v>
+      </c>
+      <c r="Z21">
+        <v>27104</v>
+      </c>
+      <c r="AA21">
+        <v>27122</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new cities in the database.
</commit_message>
<xml_diff>
--- a/Data/Podaci.xlsx
+++ b/Data/Podaci.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/domagojrunjak/Documents/Zavrsni rad/zavrsni-rad/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E290B8D3-52F3-634D-99B1-47620705B65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDB7407-F26B-4345-BA54-6FA78CD6A599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-3100" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="351">
   <si>
     <t>Naziv županije</t>
   </si>
@@ -271,9 +271,6 @@
   </si>
   <si>
     <t>Naziv države</t>
-  </si>
-  <si>
-    <t>Hrvatska</t>
   </si>
   <si>
     <t>Hrvatska (službeni naziv: Republika Hrvatska) je europska država, u geopolitičkom smislu srednjeeuropska i  sredozemna država, a zemljopisno smještena u južnom dijelu Srednje Europe te u sjevernom dijelu Sredozemlja. Na sjeveru graniči sa Slovenijom i Mađarskom, na istoku sa Srbijom i Bosnom i Hercegovinom, na jugu s Crnom Gorom, a na zapadu s Italijom ima morsku granicu. Kopnena površina iznosi 56.542 km², a površina obalnog mora 31.067 km² što Hrvatsku svrstava među srednje velike europske zemlje.
@@ -312,9 +309,6 @@
   </si>
   <si>
     <t>Valuta</t>
-  </si>
-  <si>
-    <t>Euro</t>
   </si>
   <si>
     <t>Jezik</t>
@@ -1138,6 +1132,492 @@
   <si>
     <t>385 (0)40</t>
   </si>
+  <si>
+    <t>Velika Gorica</t>
+  </si>
+  <si>
+    <t>10410 Velika Gorica</t>
+  </si>
+  <si>
+    <t>Na povijesnoj i političkoj karti Velika Gorica prvi put spominje se 1228. godine kao sjedište župe. Otada do danas prolazila je burnu povijest nošena na krilima mjena u širem i užem okruženju. Od turskih najezdi, preko borbi s velmožama, pregovora s kraljevima i banovima, do svjetskih i lokalnih ratova koji su je činili dijelom različitih država i državnih uređenja, Turopolje i Velika Gorica mijenjali su se, ali i uvijek ostajali svoji. Često u povijesti Turopoljci su bili posljednja obrana Zagreba – od turskih osvajanja do Domovinskog rata u kojem su dali veliki doprinos, ne samo na Kupi kao posljednjoj obrani glavnog grada, već na svim ratištima diljem Hrvatske.
+Plodna dolina rijeke Save pružala je, i pruža, idealne uvjete za život. Pulsiranje rijeke, koja je tijekom stoljeća mijenjala tok, odražavalo se na izbor mjesta stanovanja, odnosno njegov značaj tijekom povijesti.
+U razdoblju neolitika ili mlađeg kamenog doba (6. – 5. tisućljeće prije Krista), na položaju Gradišće kod Starog Čiča, stočari i poljodjelci izgradili su prve zemuničke nastambe. Od tog doba tradicija naseljavanja, tj. života, na Gradišću traje, vjerojatno, sve do dolaska rimske civilizacije. Pripadnici korenovske kulture na Gradišću izrađuju posuđe za pripravu i čuvanje hrane, kamene polirane sjekire, kamene nožiće, strelice, strugala, žrvnjeve, utege za mreže, koštane igle itd. Posuđe je ukrašavano, uglavnom, urezanim trakastim ukrasom (dvije ili tri paralelne crte). Korenovska kultura pripada velikoj skupini srednjoeuropske linearnotrakaste keramike.
+Eneolitik ili bakreno doba (4. i 3. tisućljeće prije Krista) povezuje se s početkom formiranja indoeuropskih plemenskih zajednica. U to je vrijeme na ovom prostoru prisutna lasinjska kultura (Novo Čiče i Dubranec), dok se s istoka, dolinom rijeke Save, širi vučedolska kultura, čiji su ostaci pronađeni na lokalitetu Gradišće kraj Starog Čiča. Pripadnici vučedolske kulture potpuno su ovladali vještinom proizvodnje bakra. Vučedolska je kultura poznata po maštovitim i vrlo kvalitetnim keramičkim proizvodima, često potpuno prekrivenim ukrasima.
+Brončano doba (2200. – 750/700. g. prije Krista) obilježeno je proizvodnjom brončanog oružja, oruđa i nakita, te intenzivnim razvojem metalurgije, trgovine i obrta. Ranom brončanom dobu (2200 – 1600. g. prije Krista) pripadaju nalazi keramike iz Starog Čiča – rijetko ukrašena keramika vinkovačke skupine, te keramika ukrašena licenskim stilom. Licenska se keramika rasprostirala na velikom prostoru srednje Europe, a ukras se izrađivao utiskivanjem konopa ili nazubljenog kotačića na stijenku nepečene posude. Osnovni oblik licenske kulture bio je vrčkuglastog tijela i ljevkastog vrata s ručkom koja je spajala tijelo i vrat. Pojava ove keramike objašnjava se seobama stočara u ranom brončanom dobu.
+Kasno brončano doba ili razdoblje tzv. kulture polja sa žarama (urnama) traje od 1300 – 750/700. g. prije Krista. Nositelji ove europske kulturne pojave pripadaju indoeuropskoj skupini, a odlikuje ih obred spaljivanja mrtvih im pokapanje ostataka u žarama (urnama), s prilozima nakita, oružja i oruđa. Na ovom je prostoru to razdoblje obilježeno kulturnim skupinama Virovitica (13. st. prije Krista) i Zagreb (kraj 13. te 12. i 11. st. prije Krista). U 10. st. prije Krista do završetka kasnog brončanog doba ovdje žive nositelji kulturne skupine Velika Gorica, koji su razlučeni na temelju arheoloških nalaza iz nekropole Visoki brijeg u Velikoj Gorici. Jedna od zanimljivosti ove nekropole su kuglaste žare (urne) s okruglom rupom koju neki autori tumače kao vezu sa zagrobnim svijetom – prolaz kroz koji je duša mogla izaći i ući. Kao prilozi u grobovima nađeni su brončani mačevi, koplja, šuplje sjekire, noževi itd.
+Sredinom 8. st. prije Krista širi se halštatska kultura – počinje željezno doba Europe. Latenska kultura mlađe faze željeznog doba dolazi do izražaja pojavom keltskih plemena u ovom dijelu današnje Hrvatske. Utjecaj keltske kulture postaje dominantan od kraja 2. do početka 1. st. prije Krista širenjem plemena Tauriska prema istoku.
+Rimsko osvajanje Panonije, a time i uključivanje ovih krajeva u sustav rimske civilizacije, započinje u posljednjoj trećini 1. st. prije Krista. Panonija je bila nastanjena plemenima ilirske kulturne tradicije s više ili manje keltskih kulturnih elemenata. Zlatno doba Carstva započinje vladavinom Augusta (utemeljitelj carstva – vladao od 31. g. prije Krista – 14. g. poslije Krista), a završava u 2. st. poslije Krista za vladavine Marka Aurelija (161. – 180. g.). U tom je razdoblju i potpuno pokoreno područje na kojem je bila Andautonija (današnje Šćitarjevo), nakon gušenja ustanka u Panoniji i Dalmaciji (6. – 9. g. poslije Krista) što je učinio Tiberije (Augustov nasljednik).
+Provala germanskih plemena 166. g. koja je opustošila Panoniju, bila je nagovještaj početka kraja Carstva. POkušajem cara Dioklecijana (284. – 305.) da gospodarski i upravno reformira državu nakratko se smiruju građanski ratovi i gospodarska nestabilnost. Njegove je reforme uspješno nastavio Konstantin Veliki (306. – 337.), čiji su nasljednici Carstvo podijelili na Istočno i Zapadno, ali nisu uspjeli zaustaviti nadiranje barabarskih plemena i sveopću nestabilnost, što je dovelo i do konačne političke i vojne propasti Zapadnog Rimskog Carstva 476. g.
+Dolaskom Rimljana prvi put je urbanizirano međurječje Save i Kupe. Urbanizacija je provedena izgradnjom glavnog naselja na Savi i povezivanjem prostora sustavom cesta, puteva i mostova. Preko ovog područja Rimljani grade dvije državne ceste – jednu iz Akvileje, preko Emone (Ljubljane) za Sisciju (Sisak) i drugu iz Dalmacije, preko Siscije za Poetovio (Ptuj). Trasa prve ceste prolazila je kroz (današnje) Gornju Lomnicu, Petrovinu, Okuje, Mraclin i u Buševcu se spajala s cestom Siscia – Poetovio, čija je trasa bila Sisak, Sela, Dužica, Ogulinec, Buševec, Vukovina, Staro Čiče, Novo Čiče, Bapče, Šćitarjevo (Andautonija) i dalje prema sjeveru. Osim državnih cesta, na području Andautonije postojale su i lokalne prometnice koje su povezivale Andautoniju s brojnim manjim naseljima na području (današnjih) Veleševca, Turopoljskog luga, Buševca, Novog Čiča, Velike Gorice, Odre itd. u kojima su živjeli starosjedioci i kolonizirano stanovništvo. Andautonija je, kao savska luka i mjesto na značajnim državnim prometnim pravcima, od samog svog početka imala veliku stratešku važnost.
+Ceste, ulice, kanalizacija, javne zgrade i stambena arhitektura Anadutonije građene su uglavnom od kamena koji je bio dovožen iz kamenoloma na Medvednici.
+Najbolje sačuvan i istražen dio Andautonije predstavlja gradsko kupalište – terme, otkrivene u dvorištu današnjeg župnog ureda. Terme su bile jedan od neizostavnih sadržaja svakoga rimskoga grada, u kojima se, osim kupanja, odvijao i društveni život građana. Pojedine prostorije, koje su svojom estetskom dotjeranošću trebale poslužiti što ugodnijem boravku, imale su zidove oslikane fresko slikarijama ili obložene mramorom, a podove popločene opekom ili crno-bijelim mozaicima. Vrlo su dobro sačuvani i ostaci hipokausta – sustava podnog i zidnog grijanja u termama.
+Smještaj teritorija Andautonije, odnosno položaj grada na važnim državnim prometnicama i rijeci Savi, te neposredna blizina centra provincije – grada Siscije, utjecao je na njezin nastanak, rast i razvoj, ali i na osjetljivost na destabilizaciju Carstva zbog unutarnjih nemira i barbarskih navala. U kasnoj antici mnoga stara središta, ako i nisu bila uništena, polako su se gasila, a organizacija života prilagođavala se novom dobu. Potkraj 4. st. započinje velika seoba naroda, pa bi se u tim događanjima mogao potražiti i početak kraja, ako ne i sam kraj Andautonije.
+Ovo vrijeme velikih promjena završava oko 800. g. kad je Karlo Veliki uspostavio granicu zapadne europske civilizacije na rijeci Drini. Iz tog vremena potječu i nalazi strarohrvatskih grobova u Velikoj Gorici (otkriveni početkom 20. st.) i Novom Čiču (1962. g.), te vjerojatno i u Petrovini. U Velikoj Gorici, na položaju Visoki Brijeg, pored paljevinskih prapovijesnih i rimskih grobova, pronađeno je i pet ranosrednjovjekovnih grobova s kosturima. Osim bojnih sjekira, strelica, noževa, metalnih dijelova opasača i ogrlica od staklenih perli u grobovima su pronađene i posude za jelo i piće, što ukazuje na još uvijek jako prisutnu pogansku tradiciju u načinu pokapanja.
+Navedeni ranosrednjovjekovni nalazi govore o prisustvu hrvatskog stanovništva na ovome području u vrijeme završetka formiranja zapadne europske civilizacije.
+Oslobođenjem od služenja zagrebačkom kastrumu, banskim i kraljevskim ispravama, u 13. st. je na ovom prostoru formirana zajednica plemića na temelju slobodnog posjeda. Godine 1278. u Hrvatskom saboru propisano je običajno pravo i povlastice, a taj je statut Plemenite općine Turopolje 1279. g. potvrdio i kralja Ladislav IV. Prema tom statutu turopoljskim je županom mogao postati samo onaj kojeg su zajednički izabrali i odobrili turopoljski plemići. Takve izborne, odnosno glavne skupštine (spravišča) održavale su se na dan sv. Jurja, 23. travnja, a od početka 17. st. na dan sv. Lucije (13. prosinca). Turopoljsko plemstvo izvodilo je svoje porijeklo iz povelje hercega Bele (kasnije kralj Bela IV.) iz 1225. g. koja je sačuvana u potvrđenom prijepisu iz 1466. g. Povelja govori o podizanju braće Buduna, Ivana, Levća i rođaka u plemiće. Ovu povelju, kao i privilegije stečene tijekom 13. st. turopoljsko je plemstvo nastojalo obraniti, pa je tražilo kraljevske potvrde.
+Početkom 15. st. počeli su upadi turske vojske na ovo područje, a prvi ozbiljniji upad u Turopolje zbio se 1422. g. u Petruševec i Rakitovec. Ponukani učestalošću osmanlijskih pljačkaško porobljivačkih upada turopoljski su plemenitaši odlučili izgraditi obrambenu utvrdu Lukavec, koja je, osim za obranu od Turaka, trebala poslužiti i za čuvanje dragocjenosti, imetka i važnih povijesnih dokumenata Plemenite općine.
+Od sredine 16. st. intenziviraju se turski upadi na područje Turopolja, a jedan od najtežih bio je onaj 24. kolovoza 1556. g. Poučeni teškim iskustvima, te uvidjevši potrebu za slogom, godine 1560. predstavnici turopoljskog plemstva su pred zagrebačkim Kaptolom obnovili bratstvo, te je ustanovljen red izbora župana, sudbena vlast i nasljedno pravo.
+Obnovljeno Turopoljsko bratstvo brojilo je 113 plemića, a 1570. g. pristupio mu je i slavni hrvatski ban Ivan Drašković sa svojim rođacima. Prestanak upada turskih postrojbi u Turopolje vezan je uz veličanstvenu pobjedu hrvatske vojske u bici kod Siska 22. lipnja 1593. g. Radi ojačanja svojih gospodarskih pozicija Velikogoričani su već početkom 17. st. od kralja tražili sajamske privilegije. Prvu takvu privilegiju dobili su 1602. godine, a drugu 1649. godine. Zbog velikih nereda i nemira tijekom priprema i održavanja turopoljskih spravišča i biranja župana tijekom prvih tridesetak godina 18. st. turopoljsko plemstvo je statutom bana Josipa Eszterhazyja iz 1736. g. izgubilo osobno pravo glasa, pa od tada pravo izbora župana i ostalih dužnosnika Plemenite općine imaju samo suci. Jedna od najvažnijih točki Eszterhazyjevog statuta bila je odredba prema kojoj su Turopoljci bili dužni u vrijeme mira držati na okupu stalnu plemićku vojnu četu od 120 ljudi, a u ratno vrijeme 300 ljudi. Upravo su te čete početkom 19. st. sudjelovale u obrani Hrvatske od Napoleonove agresije kojom je okupirano i Turopolje (1809 – 1813.). Nakon odlaska Francuza Turopoljci su obnovili svoju samoupravu sa sjedištem u Velikoj Gorici, a Hrvatski im je sabor iznova potvrdio njihova stara prava, uključujući i sazivanje spravišča, te izbor župana. Nakon završetka dugotrajne turske agresije, 17. i 18. st. bila su vrijeme obnove i izgradnje. Na području Turopolja grade se i obnavljaju crkve, kapele ali i javne palače. Turopolje je bilo žarište koje je koncentracijom izvorne narodne stvaralačke snage širilo svoj utjecaj na cjelokupno međurječje Save i Kupe gdje se tradicija gradnje drvenih crkava zadržala duboko u 20. st. Na ovom ih je području u 17. st. izgrađeno dvanaest, u 18. i 19. st. po šest, u 20. st. tri, a do danas ih je sačuvano samo jedanaest. Od zidanih crkava već 1642. g. izgrađena je u Šćitarjevu crkva sv. Martina Biskupa, oko 1714. crkva Gospe Snježne u Dubrancu, a 1779. crkva Pohoda Blažene Marije Djevice u Vukovini. Ubrzo po završetku obnove straog grada Lukavca (1750.) plemenitaši su započeli izgradnju znamenitog Turopoljskog grada koji je dovršen oko 1765. g. To je lijepa barokna jednokatnica visokoh krovišta s arkadnim trijemom u prizemlju, okrenuta prema gradskom parku. U vrijeme koje je prethodilo dolasku novog sustava, odnosno ukidanju plemstva i hrvatskom narodnom preporodu 1848. g. turopoljsko se plemstvo podijelilo. Jedan dio, pod vdstvom tadašnjeg župana Antuna Danijela Josipovića staje 1839. g. na stranu Mađara i ugarskog hegemonizma, a drugi se dio plemstva borio uz bana Josipa Jelačića i podupirao njegovu viziju Hrvatske. Na izvanrednom spravišču održanom 29. svibnja 1848. stari je župan smijenjen te je izabran Stjepan ml. Josipović pod čijim su vodstvom brojni Turopoljci sudjelovali 4. lipnja 1848. svečanom ustoličenju bana Jelačića. Stjepan ml. Josipović na župansku je dužnost biran sve do smrti (5. lipnja 1893.), a naslijedio ga je Ljudevit Josipović (unuk A. Danijela Josipovića) biran za župana do 1918. g. Od 1848. sjedište Plemenite općine nalazi se u Turopoljskom gradu (danas Muzej Turopolja) u Velikoj Gorici. Upravo u vrijeme županovanja Stjepana ml. Josipovića i Ljudevita Josipovića Velika Gorica i čitavo Turopolje doživljavaju uspon na svim područjima javnog života. Ubrzanom razvoju doprinijela je i izgradnja željezničke pruge 1862. g. na relaciji Zidani Most -–Zagreb – Velika Gorica – Sisak, kao i ranije uspostavljeni cestovni promet od Zagreba do Siska.
+Na području velikogoričkog kotara, sredinom 19. st., točnije 1857. g. bile su 1.633 kuće sa 17.590 stanovnika, a u samoj Velikoj Gorici 74 kuće s 479 duša. Pedesetak godina kasnije, na prijelazu stoljeća, Velika Gorica već ima 1.220 stanovnika što je razumljivo jer je u navedenom razdoblju bila ne samo općinsko nego i kotarsko mjesto. U prilog sve jačeg urbanog razvoja i jačanja velikogoričkog gospodarstva govori i obnova župne crkve Navještenja BDM, koju je na molbu župana Ljudevita Josipovića restaurirao arhitekt i graditelj Herman Bolle. Obnova je dovršena 1893. godine.
+Tijekom druge polovice 19. st. uređen je u Velikoj Gorici, ispred Turopoljskog grada, lijep perivoj, danas gradski park.Godine 1892. župan Stjepan ml. Josipović utemeljio je Pučku štedionicu, a njegov nasljednik Ljudevit Josipović zaslužan je za osnivanje podružnice Prve hrvatske štedionice u Velikoj Gorici. Postojanje i poslovanje ovih novčarskih ustanova doprinijelo je počecima razvoja industrije u Velikoj Gorici i mjestima oko nje. Već je 1894. zagrebački poduzetnik Filip Deutsch (sa sinovima) osnovao veliku poslovnu tvrtku, a nekoliko godina kasnije i dva parna mlina u Kurilovcu. Krajem 19. st. tvrtka je već imala proširene sve grane drvne proizvodnje i trgovine drvetom. Za zasluge u trgovini i veleobrtu (industriji) obitelj Deutsch 1910. godine dobija za sebe i svoje zakonite potomske plemstvo s pridjevom Maceljski.
+U posljednjim desetljećima 19. st. veliku je građevnu djelatnost razvio Nikola Hribar, koji je u to vrijeme izgradio više zgrada i kuća u Velikoj Gorici, kao i škole u Velikoj Gorici, Dubrancu, Lomnici, Mraclinu, Novom Čiču, Velikoj Mlaki i Šćitarjevu. Radio je na restauraciji župnih crkava u Velikoj Gorici i Dubrancu, kao i na mnogim kapelama na području Turopolja i Zagreba. Izgradio je i dom Hrvatskog sokola u Velikoj Gorici.
+O postupnom usponu Velike Gorice svjedoče i službena izvješća Zemaljske vlade u Zagrebu prema kojima je na području upravnog kotara Velika Gorica na prijelazu stoljeća djelaovalo 14 kulturno prosvjetnih društava s ukupno 467 članova. Među njima je na prvom mjestu Hrvatska čitaonica u Velikoj Gorici utemeljena 1885. godine. Treba spomenuti i pjevačko društvo “Lira” utemeljeno u Velikoj Gorici 1876. godine, Obrtnu zadrugu u Velikoj Gorici koja je poticala razvoj obrtničkih djelatnosti, te brojna vatrogasna društva, od kojih je prvo utemeljeno 1876. godine.
+Sve ove činjenice nesumljivo svjedoče da je Velika Gorica već krajem 19. st. imala sva obilježja modernog hrvatskog grada, ali i iskustva uspona i padova koji su je pratili u njenom razvoju.
+Stoljeće koje ostaje iza nas do sada je po mnogočemu posebno i znakovito. Velika Gorica je od malog seoskog trgovišta, od 2.871 stanovnika početkom stoljeća prerasla u grad od 31.614 stanovnika (1991.), dok danas s pripadajućim naseljima broji preko 60.000 stanovnika. U 20. stoljeću broj stanovnika u užem području grada Velika Gorica povećao se 11 puta, dok se na ukupnom prostoru udvostručio. Kroz jedno stoljeće živjela je u pet državnih zajednica Austro-Ugarskoj, Kraljevini Jugoslaviji, NDH, SFRJ i na kraju u samostalnoj Republici Hrvatskoj. U administrativno političkom smislu kao centar Turopolja bila je općinsko i kotarsko središte, te sjedište grada s 58 naselja. Pripadala je široj zajednici zagrebačkoj županiji, zajednici općina Zagreb, a u kraćem razdoblju ulazila je i u sam grad Zagreb, da bi konačno 1995. dobila status grada.
+Posljednja tri desetljeća od 1970. do danas potpuno su izmijenili sliku dotad poznate Velike Gorice.</t>
+  </si>
+  <si>
+    <t>Pula</t>
+  </si>
+  <si>
+    <t>52100 Pula</t>
+  </si>
+  <si>
+    <t>Grad Pula ima više od 3000 godina, a nastao je na brežuljku Kaštel gdje je nastalo prvo gradinsko naselje, utvrda Histra. Osim kružnog oblika dvije glavne gradske ulice, od prapovijesne gradine, ništa nije ostalo. Prava gradska povijest započinje s Rimljanima. Službeno je ime grada bilo Colonia Pietas Iulia Pola, a imao je sve funkcije i građevine tipične za naseobinu rimskih doseljenika.
+U doba seoba naroda u pulsku su se širu okolicu od VII. stoljeća stali naseljavati Slaveni i Hrvati. Poslije 1331. godine Pula više nije mogla uteći kandžama lava Sv. Marka. Mlečani u Puli nisu pokazivali zanimanje za gospodarski razvoj grada, jer im je najvažnija bila luka kao tranzitna točka na putu od Venecije duž istočne obale Jadrana prema Levantu. Česte epidemije kuge od XIV. stoljeća, kao i endemična malarija i druge bolesti, drastično su smanjile broj stanovnika tako da je u Puli na kraju XVII. stoljeća živjelo samo oko 600 ljudi. Međutim, od razdoblja humanizma i renesanse u europskoj su kulturnoj javnosti sve poznatiji postajali pulski antički spomenici: Arena, slavoluk Sergijevaca, Augustov hram(na slici), tako da su mnogi umjetnici i graditelji XVI., XVII. i XVIII. stoljeća boravili u Puli crtajući i opisujući rimske građevine koje su bile uzorom arhitekture od renesanse do klasicizma.
+Propašću Venecije Istra i Pula došle su pod austrijsku krunu. Od 1815. godine do kraja Prvog svjetskog rata Pula je bila dio austrijskog Primorja (Küstenland). Kad je 1856. godine otvoren Arsenal, tj. glavna baza austrijske ratne mornarice, započeo je suvremeni razvoj grada i cijele južne Istre. Nakon što je 1876. godine povezana željezničkom prugom sa linijom Beč - Trst Pula i obližnji Brijuni osjetili su početke turizma, a svi su članovi carske obitelji, na čelu s Franjom Josipom, bili pulski gosti.
+Dvadeseto je stoljeće u Puli bilo stoljeće višestrukih promjena vlasti, s odlascima i dolascima dijelova stanovništva, pojedinih društvenih i narodnosnih skupina, poglavito poslije Prvog i poslije Drugog svjetskog rata. Jako oštećena u bombardiranju tijekom Drugog svjetskog rata, Pula je u drugoj polovici XX. stoljeća ponovo procvjetala i razvila se u najveći istarski grad, značajan zbog dvije glavne gospodarske djelatnosti: industrije, na čelu s brodogradnjom i turizma.</t>
+  </si>
+  <si>
+    <t>44.87</t>
+  </si>
+  <si>
+    <t>13.85</t>
+  </si>
+  <si>
+    <t>Vinkovci</t>
+  </si>
+  <si>
+    <t>32100 Vinkovci </t>
+  </si>
+  <si>
+    <t>VK</t>
+  </si>
+  <si>
+    <t>Područje današnjih Vinkovaca i njegove bliže okolice ljudi nastanjuju već oko 7000 godina. Arheološka istraživanja dokazala su postojanje starije faze starčevačke kulture neolitika. Mlađa sopotska kultura (oko 4.250. do 3.350.g. pr. Kr) autohtona je kultura nazvana po lokalitetu Sopot nadomak grada. Rano razdoblje brončanog doba zastupljeno je specifičnom vinkovačkom kulturom (2.300. - 1.800. g. pr. Kr.). Starije željezno doba karakteristično je po naseljavanju Ilira. U mlađem željeznom dobu dominirala je keltsko-latenska kultura.
+Novo naselje Cibalae (ilirski: brežuljak) zasnovali su Rimljani na lokalitetu Hotel-Tržnica, kada su počeli sustavno osiguravati granicu (limes) na Dunavu zbog obrane od barbarskih plemena. Naselje se postupno romanizira te za cara Hadrijana (117.-138.g.) dobiva status municipija, Municipium Aelium Cibalae. Status kolonije grad najvjerojatnije dobiva vrijeme vladavine cara Karakale (196.-217.g.) i od tada postaje Colonia Aurelia Cibalae. Grad Cibalae ima veliko značenje za rimsku povijest, jer se tu u blizini 314. godine vodila bitka za prevlast i moć između careva Konstantina Velikog i Licinija. Značaj Cibala potvrđuje podatak da su u tom gradu rođena dva cara, braća i suvladari, Valentinijan I. (321.-375.) i Valens (328.-378.).
+Grad Cibalae stradavao je zajedno s propašću rimske civilizacije. Godine 378. razrušili su ga Zapadni Goti, poslije čega se nije oporavio. Slijedi provala Huna, te je grad pod vlašću Atile od 441. do 453. godine, nakon čega su grad poharali Istočni Goti i tu se zadržali dvadeset godina. Od 473. do 504. istočnu Slavoniju i Srijem zaposijedaju Gepidi, a zatim pripadne Bizantskom carstvu. Cibalae od velikog antičkog grada postupno postaju malo selo. Posljednji spomen Cibala nalazi se u darovnici cara Justinijana, koji Cibalae daruje benediktincima 527. godine. Ostatke grada ruše Avari 579. godine, a od 582. do 769. godine tu se nastanjuju plemena Avara i Slavena, čime konačno nestaju tragovi antičke civilizacije. Avarska dominacija je završena pobjedom Franaka 795. godine. Slavenski knezovi postaju franačkim vazalima.
+Naselje (u mađarskim spomenicima Zenthelye, Zenthylye, Zenthylya i sl.) uz rub ruševina antičkih Cibala dokazano postoji od XI. Stoljeća. O tome svjedoče arazni arheološkki ostaci ranoromaničke crkve sv. Ilija, koju je na lokalitetu Meraja otkrio i istražio arheolog Stojan Dimitrijević 1965. godine. Naselje Sveti Ilija vjerojatno je stradalo prilikom Tatara 1242. godine. Mjesto se oporavilo, pa je u XIV. Stoljeću sagrađena veća gotička crkva, koja se dijelom naslanja na temelje stare predromaničke crkve. Narodno ime Vinko/Vinkovci uz ono Sveti Ilija upisano je na strim zemljopisnim kartama iz 1592. i 1640. godine. Vinkovci se prvi put spominju u jednom izvještaju iz 1615. godine, uz napomenu da su nekada bili dobro nastanjeni, a pod Turcima su se rasuli u nekoliko sela.
+Srednjovjekovni posjedi mađarskoga plemstva u okolici Vinkovaca nestali su za vrijeme turske vladavine. Nekada poznato trgovište Sveti Ilija, sada Vinkovci postalo je malo selo, okruženo ostacima starih sela ili tzv. pustoselinama. Uz spaljenu gotičku crkvu sv. Ilije postojao je tzv. Vinkov sokak, zatim desetak kuća na istok, desetak kuća uz staru cestu od crkve na sjeverozapad. Prema jugu i dalje na istok, gdje je sada središte grada, bili su prazni prostori. Stare odlike toga naselja - plodno tlo, šumovito područje, rijeka Bosut s pritokama, voda stajačica sjeverno od mjesta i brežuljak Borinci, uz prometni značaj, bile su temelj budućeg razvitka.
+Nakon odlaska Turaka austrijske su vlasti nastojale što brže i što više naseliti područje uz tursku granicu, nazvano Koridorom, zatim Vojnom krajinom ili jednostavno Granicom. Stoga je naređeno ştanovništvu malih sela u prstenastom području oko grada Vinkovaca useljavanje u grad (koji zapravo još to nije bio). Također je poticano useljavanje Hrvata katolika iz Bosne i Like. Tijekom 18. stoljeća ovo se, uglavnom useljeno ratarsko stanovništvo, stopilo u starosjedioce Šokce, bez obzira jesu li se uselili kao Ličani, Bunjevci ili bosanski Hrvati.
+Barun JOSIP ŠOKČEVIĆ, hrvatski ban, podmaršal, učenik. Rođen je 7.ožujka 1811. godine u poznatoj graničarskoj obitelji u Vinkovcima koja je Monarhiji dala veći broj podčasnika i časnika. Nakon pučke škole i dva razreda realke (gimnazije) 1823. odlazi iz rodnog grada na vojnu akademiju u Bečko Novo Mjesto, koju završava izvanrednim uspjehom 1830. godine. Vojna karijera u Habsburškoj monarhiji bila mu je sjajna; počeo je službu kao zastavnik u pješačkoj pukovniji, brzo je napredovao u mirnodopsko i ratno vrijeme, u ljeto 1848. postaje pukovnik i zapovjednik 37. pješačke pukovnije u Lavovu, sastavljenom većinom od Mađara; s njom opsjeda i osvaja Veneciju te slama talijansku protutaustrijsku pobunu krajem godine. S 38 godina dobiva čin generala bojnika, dok u 46. godini svoga života postaje podmaršal pa je sa službovanja iz Slavonske vojne granice premješten u Vrhovnu vojnu komandu u Grazu. Kada je obolio tadašnji hrvatski ban Josip Jelačić (1858.) car Franjo Josip I. ga imenuje banovim zamjenikom i šalje u Zagreb. Poslije smrti bana Jelačića premješten je za zapovjednika Banatskog generalata sa sjedištem u Temišvaru. Uz brojna carska vojnička odlikovanja 1860. uzvišen je u stalež austrijskih baruna.
+U ljeto 1860. car ga imenuje za novog hrvatskog bana na preporuku Bosansko-srijemskog biskupa J. J. Strossmayera. To je godina velikih promjena u habsburškoj politici. Car odustaje od neoapsolutizma koju je provodio ministar Bach te narodima pod Austrijom obećava slobodni razvitak. Zato im za politiku prema Hrvatskoj odgovara podmaršal Šokčević koji ima obostrano povjerenje i narodno i austrijsko. Ban Šokčević je početkom srpnja svečano dočekan u Zagrebu. Odmah počinje politiku ponarođivanja službenog jezika u upravi koji je zadnjih 10-ak godina bio njemački. Činovnici moraju učiti hrvatski i prema narodu se ophoditi obzirno, u protivnom im prijeti otpust. Ta odredba vrijedi i za učitelje i profesore u školama, pa i u našoj vinkovačkoj Gimnaziji. Odmah se mijenja i stil odijevanja jer ban ukida zabranu narodnog odijevanja. Ban obećava svoje banovanje u Jelačićevu duhu.
+Na osnovi carske Listopadske diplome, ban Šokčević saziva najprije Bansku konferenciju od 55 hrvatskih uglednika da urede novi izborni zakon za Hrvatsku i daju hrvatske prijedloge o preuređenju Habsburške Monarhije. Hrvatski su zahtjevi isti kao i narodni zahtjevi 1848. godine, a to su cjelovita Hrvatska i federativna Monarhija. U duhu demokratizacije u cijeloj državi i u Hrvatskoj obnavljaju se političke stranke. No, car se predomislio početkom 1861. izdavši tzv. Veljački patent, kojim osniva Carevinsko vijeće u Beču i upravu državom ponovo centralizira s manjim ovlaštenjima uspostavljenim zemaljskim saborima. U tom se duhu održavaju Hrvatski sabori 1861. i 1865. pod predsjedanjem bana Šokčevića. Hrvatski sabornici nisu jedinstveni kako urediti odnose s Mađarima i Austrijancima, a pojavila se i starčevićanska opcija o samostalnoj Hrvatskoj.
+Iako je Hrvatska razjedinjena u njoj se polako budi gospodarski život ponajviše u gradovima Zagrebu, Rijeci, Karlovcu, Osijeku, Vukovaru i Zemunu. Rijeka Sava je glavna žila kucavica, grade se željezničke pruge, sam ban Šokčević predlaže trasu Vukovar-Vinkovci-Zagreb-Rijeka. U Zagrebu je 1864.godine organizirana Prva dalmatinsko-hrvatska-slavonska gospodarska izložba na prostoru gdje je današnji HNK, koja je pokazala da je Hrvatska krenula putem industrijalizacije, a na veleposjedima u Slavoniji pojavljuje se prva mehanizacija u obradi polja.
+Na Šokčevićevim putovanjima kroz Hrvatsku narod piše transparente:»Dao Bog dao Šokčeviću bane, da nam sreća sad po Tebi svane, zdravo bane, zdravo diko naša, u Tebi je prava nada naša!».
+Ban Šokčević je često svraćao u Vinkovce kako kao vojnik tako i kao ban. Kao banski zamjenik i ban 1858.,1860. i 1861. je svraćao majci Elizabeti, a posjećivao je i Gimnaziju. Tom je prilikom obilazio učionice, propitivao učenike sam ili s nastvanicima, raspitivao se o radu i poteškoćama. Izvori bilježe da je u svakom razredu dočekan kratkim učeničkim pozdravnim govorom a na izlasku bio počašćen uzvikom: Živio. Na kraju bi se ban zahvalio gimnazijskim nastavnicima na njihovom radu na oživljavanju narodnog osjećaja.
+Godine 1866. Austrija gubi rat s Pruskom i definitivno je izbačena iz igre oko njemačkog ujedinjena. Cijela je Monarhija u krizi, država se raspada, želeći opstati nosioci vlasti, Austrijanci pribjegavaju nagodbi s Mađarima. Hrvatska je prepuštena dogovoru s Mađarima. Car Franjo Josip I. bit će okrunjen za mađarskog kralja u Budimu. Na svečanost je pozvana i hrvatska delegacija na čelu s banom Josipom Šokčevićem. Ban se smatrao izigranim od Austrijanaca i podnosi ostavku. Dana 27. lipnja 1867. razriješen je banske dužnosti. Iduće je godine umirovljen od Vojne komande i cara, povlači se iz političkog i javnog života Hrvatske, seli u Graz, potom u Beč.
+Jednom je rođaku kasnije izjavio: «Takve nepravde nijesam mogao više trpjeti i zahvalio sam se; jer – kada ne mogu kako hoću, neću ni kako drugi hoće...Ovako je poštenije i časnije po mene».
+Umro je u Beču 16. studenog 1896. godine gotovo zaboravljen. Krajem svibnja 2002. posmrtni ostaci bana Šokčevića preneseni su u rodni grad Vinkovce, te sahranjeni u grobnoj kapelicu sv. Magdalene koju je dala sagraditi njegova majka Elizabeta.
+U razdoblju Marije Terezije (1740-1780) i Josipa II (1780-1790) došlo je do cijelog niza različitih promjena. Vinkovci su 1766. godine dobili status vojnog komuniteta, tj. dobili su određene pravne i ekonomske benificije i bili su na najboljem putu da se formiraju u jak ekonomski centar, ali se ubrzo ukida ovaj povlašteni status. 1780. godine u Vinkovcima je započela s radom gimnazija. Vojne vlasti izgrađuju niz upravnih i drugih zgrada. Brži razvoj Vinkovaca nastavlja se tek izgradnjom željezničkih pruga iza 1780. g., kada Vinkovci postaju sve važnije prometno središte na raskrižju željezničkih putova. Ovdje je bila i uprava velikog šumskog gospodarstva - Brodska imovna općina.
+Vinkovci su 1900.g imali oko 8.500 stanovnika. Kada je 1918. g. Hrvatska ušla u Državu Srba, Hrvata i Slovenaca, došlo je do nove organizacije uprave kojom su u 1921. g. ukinute županije, a osnovane oblasti. Nezadovoljstvo koje se pojavljuje među narodima u novostvorenoj državi 1929. g. dovodi do diktature vladara i ukidanja oblasti i oblasnih skupština. Bivši kotar Vinkovci ulazi u sastav Drinske banovine, no radom hrvatskih političkih stranaka 1931. g. kotarevi Vinkovci, Vukovar, Šid i Ilok pripojeni su Savskoj banovini.
+Nakon Drugog svjetskog rata u tada novoj Jugoslaviji osnivaju se kotarevi sa sjedištem u Vinkovcima, Vukovaru, Županji. U tom razdoblju usporavan je razvoj industrije na području Slavonije i zapadnog Srijema, ali marljivšću i upornošću njenih stanovnika i zahvaljujući prirodnom bogatstvima ovoga kraja razvila se napredna poljopriveda i neke industrijske grane.
+Raspadom socijalističke Jugoslavije u neovisnoj Hrvatskoj obnavlja se 1992. g. županija pod imenom Vukovarsko-srijemska u čijem se sastavu našao i grad Vinkovci.</t>
+  </si>
+  <si>
+    <t>45.28</t>
+  </si>
+  <si>
+    <t>18.80</t>
+  </si>
+  <si>
+    <t>Đakovo</t>
+  </si>
+  <si>
+    <t>31400 Đakovo</t>
+  </si>
+  <si>
+    <t>DJ</t>
+  </si>
+  <si>
+    <t>Brojni arheološki lokaliteti nalaze se u gradu i okolici. Oni su ispisali bogatu povijest ovoga grada. Iskopavanja iz 1997. godine potvrđuju život na širem području grada već u neolitiku, oko 5.500 godina prije Krista, koji kroz dugu i burnu povijest traje do današnjih dana.
+Đakovo se prvi puta spominje u poznatim pisanim dokumentima 1239. godine u darovnici hrvatskog kneza Kolomana bosanskom biskupu Ponsi, čime biskupi postaju gospodarima Đakova i Đakovštine. Od tada počinje povijest biskupije u Đakovu. Đakovo je i danas biskupski grad - sjedište Đakovačko-osječke nadbiskupije. Sam grad se u pojedinim periodima svoje povijesti spominje pod sličnim imenima: DYACO, DIACO, DYACOW...
+Godine 1536. Đakovo su zaposjeli Turci i vladali gotovo 150 godina - grad tada dobiva naziv JAKOVA. To je mračni dio povijesti grada. Srušene su skoro sve katoličke crkve i sagrađene džamije. Najpoznatija je Ibrahim-pašina džamija koja je nakon odlaska Turaka pretvorena u katoličku crkvu. Godine 1690. u grad se vraća biskup i tada počinje izgradnja grada.
+Poslije odlaska Turaka u Đakovu se gradi nova, skromnija katedrala i biskupski dvor. To je bila druga po redu od tri koliko ih je do sada u Đakovu sagrađeno. Gradili su ju biskupi Patačić i Bakić.
+Današnja katedrala-bazilika Sv. Petra sagrađena je u neogotičko-romanskom stilu. Biskup Strossmayer ju je počeo graditi 1866. godine u 52. godini života i 16. godini biskupske službe. Gradnja je trajala punih 16 godina (do 1882. godine), od toga 4 godine vanjski građevinski radovi, a 12 unutrašnje uređenje katedrale. Za gradnju katedrale potrošeno je 7 000 000 komada opeke koja je pečena u Đakovu. Kamen je dopreman iz Istre, Mađarske, Austrije, Italije i Francuske. Projektanti katedrale su bili arhitekti iz Beča Karlo Rősner i Fridrich Schmidt. Unutrašnje uređenje je povjereno njemačkim slikarima koji su živjeli u Rimu, ocu i sinu Alexandru-Maximilianu i Ludwigu Seitzu. Katedrala ima 7 oltara, a krase ju 43 fresko slike, 31 kip i 32 reljefa, te orgulje sa 73 registra, tri manuala i 5 486 svirala.
+Đakovačka biskupija i njeni biskupi ostavili su u gradu brojne dokaze svoga djelovanja. U gradu još i danas postoje brojni dokazi njihova djelovanja. Biskup Patčić 1706.god. obnavlja ergelu.
+Godine 1773. Đakovo postaje središte sjedinjenih biskupija Bosansko-đakovačke i Srijemske koje obuhvaćaju sve sjeveroistočne hrvatske krajeve. 
+Biskup Antun Mandić otvara, danas najstariju visokoškolsku ustanovu Slavonije i Baranje, Bogoslovno sjemenište. Poduzima i velike gospodarske zahvate na vlastelinstvu, posebice u uzgoju vinograda. Ime mu je sačuvano u nadaleko poznatim mandićevskim vinogradima. 
+Imenovanjem Josipa Jurja Strossmayera biskupom 1849. god. razvoj grada je u novom usponu. Biskupsko vlastelinstvo postaje uzorno gospodarstvo sa znatnim prihodima koji velikom biskupu omogućuje neviđene mecenske pothvate u Hrvatskoj (HAZU), a Đakovu s novom katedralom, te brojnim crkvenim i gospodarskim zdanjima daje novo lice. 
+Povijest Ergele Đakovo počinje osnivanjem biskupije darovnicom deset arapskih konja i jednim pastuhom, iako se za godinu osnivanja uzima 1506. Prema biskupu Bakiću uzgoj konja na vlastelinstvu postoji već 1374.god. Uzgoj traje i danas u Državnoj ergeli lipicanaca, koja se svrstava među najstarije u Europi, kao i kod sve većeg broja privatnih uzgajivača konja. Đakovo je oduvijek bio obrtnički grad. Godine 1813. osnovano je udruženje obrtnika CEH. Industrijski razvoj je počeo izgradnjom mlinova i ciglana, a brojni obrtnici raznih struka ponudom svojih proizvoda pridonijeli su da je Đakovo, posebno po svojim sajmovima, postalo trgovište poznato u cijeloj Slavoniji. Danas je Đakovo grad s preko 20.000 stanovnika, a s širim gradskim područjem broji preko 30.000 stanovnika.</t>
+  </si>
+  <si>
+    <t>45.31</t>
+  </si>
+  <si>
+    <t>18.41</t>
+  </si>
+  <si>
+    <t>Sinj</t>
+  </si>
+  <si>
+    <t>21230 Sinj</t>
+  </si>
+  <si>
+    <t>Najstarija povijest Cetine zapisana je u pećinama: na izvoru Cetine, u Biteliću, iznad Dabra, Rumina, u Otišiću, Vrdovu.Tu su živjeli prastanovnici naše regije. Kamene sjekire, žrvnjevi, noževi, strelice i lončarija u sinjskim muzejima oslikava kvalitet življenja tog vremena, što ga zovemo neolit. Brojne gomile nabacanog kamenja u našoj Krajini, zapravo su grobni humci. Ove gomile srećemo na podima (visoravnima) iznad polja, na istaknutim pozicijama, a potječu s prijelaza neolitika u metalno doba. Na otoku Dugišu, na Cetini, nadeni ostaci sojenica sežu u željezno doba.
+Brojne »gradine« na povišenim lokacijama često su ostaci najstarijih građevina u Krajini i zajedno s mogilama ih vezemo uz ilirsku nazočnost u Cetini. Iliri nemaju vlastitog pisma, pa o njima saznajemo iz rimskih zapisa.
+Oni spominju ratoborne Delmate, koji žive na prostoru izmedu Neretve i Krke, pa je Cetina njihova središnja zemlja.
+Slomivši otpor Delmata i zagospodarivši Cetinom, Rimljani su osnovali nekoliko naselja (vjerojatno na ilirskim temeljima) i povezali ih cestama.
+Obilje arheoloških nalaza gotovo na svim naseljenim lokalitetima svjedoci o neprekinutom kontinuitetu zivljenja u Cetini.
+U rimskom razdoblju najintenzivnije živi Tilurij -utvrđeni logor i grad na Gardunu, te Aequum na Čitluku.
+Šest je stoljeća Cetina ostala u sastavu Rimske imperije, a onda provale Avara i Slavena donose novo vrijeme, u kojem će Hrvati postati i ostati glavni etnički subjekt ove regije.
+U arheološkoj baštini stare hrvatske države najdragocjenija je crkva Sv. Spasa u Vrlici. Građena u IX., a dograđena u XIII. stoljeću, okružena s preko 1000 grobova i stećaka, biser je starohrvatske arhitekture. 
+Nažalost, na to nas vrijeme upozorava samo nekoliko spisa, koji svjedoče o njihovoj slavi. Pošto je obitelj Nelipića izumrla, u Cetini nije bilo snažne ličnosti, pa nastaju borbe oko njihova naslijeđa.
+To ide na ruku Turcima, pa vec početkom XVI. stoljeća upadaju u Cetinu. 1536. g. su je definitivno i osvojili i ovdje ostali 150 godina.
+Začuđuje da dugo tursko prisustvo u Cetini nije ostavilo znatnijih materijalnih tragova, ili upravo tu činjenicu objašnjava njihovo prisustvo. No tragovi postoje u toponomastici: Čitluk, Karakašica, Batljen, Surdup, Han i prezimenima: Atlaga, Alajbeg, Čabo, Malbaša, Strmo...
+Odlazeći iz Cetine Turci nisu žurili. 1686. g. su protjerani iz Sinja. Već slijedeće godine pokušali su osvojiti Sinj, ali nisu uspjeli. 
+Mirom u Karlovcima 1699. g. utvrdena je granica koja je zapadnu polovicu Sinjskog polja dodijelila Mlečanima, a istočnu Turcima.
+Dana 23. srpnja 1715. g. Mehmed paša s mnogobrojnom vojskom prikupljenom na Livanjskom polju (oko 70 000 momaka) prešla je Dinaru i utaborila se uz Cetinu. Razdvojivši se, dio vojske udari na Vrliku i osvoji je, a drugi dio opkoli Sinj. Juriš na Sinj počeo je 8. kolovoza. 700 boraca s nekoliko porodica i 8 fratara prestrašeno je gledalo, slušalo prijetnje i uvrede tisuća ratnika pod tvrđavom i molilo pred Marijinom slikom za pomoć. Karizma fra Pavla Vučkovica hrabrila je branitelje i odbila predaju. Poslije 8 dana opsade i bezbrojnih juriša, Turci su odbačeni. Mnoštvo ih pogibe, a većina pobježe, noću izmedu 14. i 15. kolovoza, točno na dan Velike Gospe.</t>
+  </si>
+  <si>
+    <t>43.70</t>
+  </si>
+  <si>
+    <t>16.63</t>
+  </si>
+  <si>
+    <t>Kutina</t>
+  </si>
+  <si>
+    <t>44320 Kutina</t>
+  </si>
+  <si>
+    <t>KT</t>
+  </si>
+  <si>
+    <t>Kutina, grad u Moslavini, 83 km jugoistočno od Zagreba. Leži na jugoistočnim padinama Moslavačke gore, na 149 m apsolutne visine, uz autocestu Zagreb–Lipovac i željezničku prugu Zagreb–Vinkovci.
+Jednobrodnu baroknu župnu crkvu sv. Marije Snježne sa zvonikom ispred glavnog ulaza, okruženu zidom koji na jednome dijelu ima trijem s dvjema zaobljenim kulama, dali su podići grof Karlo Erdődy i njegova žena (1729–69). Unutrašnjost crkve, oslikana iluzionističkim slikama (rad Josipa Görnera, 1779), ima raskošne drvene barokne oltare i propovjedaonicu te »Božji grob«. U Erdődyjev dvorac (pregrađen 1895) smješten je Muzej Moslavine (osnovan 1960; arheološki, kulturno-povijesni i etnografski odjel). Mnogobrojne drvene kuće tradicionalnoga moslavačkoga graditeljstva (kuća Pazdar i dr.). Sjeverno od Kutine ostatci srednjovjekovnoga grada i utvrde Blodyn (Balatin, Plovdin), a južno Kutinjca grada. Vinogradarstvo (škrlet, šipon). Petrokemijska (osn. 1968; tvornica dušičnih gnojiva, čađara, vapnara, glinara), metalna, drvna, prehrambena (mlin) industrija. Radiopostaja; tiskarstvo (Moslavački list). – Na lokalitetima Tomašica, Marić Gradina i Kaniška Iva, pronađeni su arheološki ostatci iz razdoblja mlađega kamenog doba i ranoga brončanog doba. Kontinuitet naseljavanja toga područja potvrđen je i na arheološkim lokalitetima Velika Mlinska, Donja Paklenica, Ribnjača i Voloderski bregi iz bakrenoga doba. Arheološki ostatci iz željeznoga doba potvrđuju prisutnost ilirskoga plemena Jasi, a na to su se područje poslije naseljavali Kelti, koji su se postupno stapali s mjesnim ilirskim stanovništvom. Tijekom rimskoga razdoblja to je područje bilo u sastavu provincije Panonije. Pretpostavka o postojanju rimskog naselja Varianis, smještenog između Siska i Pakraca, još uvijek nije znanstveno potvrđena.
+Kutina se u pisanim izvorima prvi put spominje 1256. kao Cotynna u lat. povelji kralja Bele IV., kojom se uređuju granice Garićke i Gračeničke župe. Kao župa Kutina (Kotinna) prvi se put spominje u popisu župa Zagrebačke biskupije iz 1334. Tada se spominje i župna crkva Svih svetih, dok 1488. izvori bilježe crkvu sv. Katarine. Tijekom kasnoga sr. vijeka često se spominje u izvorima (1364., 1400., 1424., 1464. i 1487) pod nazivima Kotenna, Kothennya, Kotenya i Katynna, dok se u jednoj ispravi Zagrebačkoga kaptola od 14. VIII. 1363. spominju Gornja, Donja i Velika Kutina. U razdoblju od XII. do XIV. st. Kutina je administrativno bila u sastavu Gračeničke županije. Tijekom razvijenog i kasnoga sr. vijeka bila je značajno trgovište i prometno čvorište. U tom su razdoblju njezini gospodari bili obitelji Rohović (Rohfy), Večerin, Geletić, Čupor, Bakač, plemići Bršljanovački, Roh de Decse te Auch. U doba vlasti nad tim područjem, obitelj Čupor svoje zemlje poklanjala je pustinjačkomu redu pavlina, koji je ostavio značajan trag u moslavačkoj kulturi. Potom je Kutina kao i cijela Moslavina bila vezana uz obitelj Széchényi i Erdődy. Nakon osman. osvajanja u Kutini je oko 1550. bila osnovana nahija, koja se u izvorima spominje pod nazivom Kutinovac. Zbog obrane od Osmanlija grad je bio opasan zidinama, a bile su sagrađene i utvrde Blodyn i Kutinjac grad. Nakon Karlovačkoga mira 1699. u grad se počelo vraćati izbjeglo stanovništvo. God. 1745. Kutina je postala sjedištem kotara pa je bila uključena u sastav Požeške županije. God. 1837. Ferdinand I. dodijelio je Kutini povelju kojom ju je proglasio trgovištem, a 1886. administrativno je pripala Bjelovarsko-križevačkoj županiji. Gospodarski napredak doživjela je nakon gradnje željeznice 1897. U podjeli Kraljevine SHS na oblasti 1924. Kutina je bila u sastavu Osječke oblasti, a nakon podjele na banovine 1931. ušla je u sastav Savske banovine. U razdoblju Banovine Hrvatske 1939–41. bila je sjedište istoimenoga kotara, a za Nezavisne Države Hrvatske bila je u sastavu velike župe Prigorje. Nekoć isključivo poljoprivredno i trg. naselje, u XX. st. razvila se u jako industr. središte Moslavine, posebice zbog prirodnih resursa i preradbe nafte i prirodnog plina.</t>
+  </si>
+  <si>
+    <t>16.78</t>
+  </si>
+  <si>
+    <t>Križevci</t>
+  </si>
+  <si>
+    <t>48260 Križevci</t>
+  </si>
+  <si>
+    <t>KŽ</t>
+  </si>
+  <si>
+    <t>Križevci su jedan od najstarijih gradova u kontinentalnoj Hrvatskoj. Tako će nam povijesna vrela posvjedočiti o pisanoj povijesti Križevaca već od 12. stoljeća kao županijskog središta, a od polovine 13. stoljeća, točnije od 1252., kao privilegiranog banskog, pa potom kraljevskog grada. I župnu crkvu svetog Križa vrela potvrđuju zarana, već 1232. godine, kao jednu od najstarijih crkvi u regiji. No ranija povijesna vrela izgubljena su, te bi se mogao steći dojam da na ovom mjestu naselje datira tek otkada ga povijest potvrđuje. Da nije tako ne svjedoče samo mnogoborojni arheološki nalazi, koji dokazuju kontinuitet života pod Kalnikom i uz križevačke potoke Korušku, Trstenik, Vrtlin i Glogovnicu; kroz tisuće godina, tu je važno križanje cesta, od kojih su neke nesumnjivo rimske, kao na primjer ona od Varaždinskih Toplica prema Sisku. No tu je i tradicija, legende i pučke predaje o nastanku mjesta, o imenu mjesta, neprovjereni, ali utemeljeni podaci o povijesnim događajima koji su se možda ovdje dogodili.
+Tako najpoznatija predaja, ona o čudu svetog Križa koju je zapisao Kvirin Vidačić, govori da su u 6. stoljeću, tek doseljeni Hrvati, još pogani, baš na ovom mjestu, trpeći žestoku žeđ, doživjeli viziju križa nad bunarom koji ih je sve okrijepio. Čim primiše Vjeru, nastane ovdje crkva, na mjestu gdje crkva istog titulara stoji i danas. Druga predaja, koju ne možemo dokazati, ali niti osporiti, govori o vremenu kralja Kolomana, te da su se predstavnici hrvatskog i mađarskog naroda susreli baš ovdje, kad ugovarahu uvjete mira i dinastički savez pod krunom svetg Stjepana. Neobično žilavo i živo predaja nam ocrtava Križevce kao najznatnije mjesto srednjovjekovne Slavonije, a ako sve i nije bilo točno kao što narod prenosi s naraštaja na naraštaj, opet je pažnje vrijedan svaki podatak predaje, tamo gdje nedostaju vrela. Da su Križevci bili od prvih zabilježenih plemenskih županija, činjenica je, jednako kao i da su u 14. stoljeću sjedište najveće županije, koja je površinom i življem veća od zagrebačke i varaždinske zajedno.
+Godine 1252. osnovao je Ban Stjepan Gornji grad kao kolonizatorsko naselje, odmah ga obdarivši širokom gradskim povlasticama, no prema predaji gradom je Križevce proglasio još Koloman stoljeće i pol ranije. Sljedećih će pet stoljeća povijest Križevaca biti povijest dva bliska, ali odvojena grada, Gornjeg i Donjeg te ta podjela i danas živi u svijesti građana, koji se, ne bez ponosa kako na zajedničku tako i na povijest svakog od ovih gradskih entiteta dijele na ‘Gornjograđane’ i ‘Donjograđane’. Ako je pak istina da je prva izgubljena povlastica još Kolomanova, onda su Križevci doista jedan od najstarijih gradova između Save i Drave.
+Razvoju grada pogoduje dobar položaj na križanju trgovačkih i vojničkih cesta, i široke gradske slobode koje uključuju pravo sajma, veliku razinu lokalne uprave, blagonaklonost kraljeva, stalno prisustvo podbana, sjedište kraljevskig suda itd. Povijest nas tijekom srednjovjekovnih stoljeća izvještava o važnom administrativnom i civilnom središtu, gradu koji je nesumnjivo ukrašen lijepim crkvama, samostanima, , utvrdom te bogatim trgovačkim i obrtničkim kućama. Od toga je nažalost malo očuvano, pored već spominjane crkve Sv. Križa, tu je samostan u Gornjem gradu, isprva augustinski, potom franjevački, da bi danas bio sjedište grkokatoliške biskupije. Povijest bilježi slavonske i hrvatske sabore, od kojih je neslavnu reputaciju stekao onaj kojeg pamtimo kao ‘Krvavi sabor križevački’. Malo znamo o tom događaju, obračunu kralja i protudvorskog pokreta hrvatskih i ugarskih velikaša, koji se, kako tradicija hoće, možda doista dogodio u crkvi Sv. Križa dana 27. veljače 1397. godine. Nedugo nakon ovog nemilog događaja kralj Sigismund svojom povlasticom još proširi gradske privilegije, te odobri podizanje bedema oko Donjeg grada. Ovom se važnom povlasticom Križevci ponovo u rangu izjednače s ostalim gradovima u okolici, Koprivnicom, Varaždinom itd., za kojima su, mada najstariji među njima, tijekom stoljeća malo zaostali u ovlastima samouprave.
+Nažalost, tužna stoljeća turskih ratova, koja ne samo iz čitavog križevačkog kraja, učine mrtvu pograničnu zonu spaljene zemlje, znatno oslabe ekonomsku bazu ovog bogatog trgovišta, velik dio Križevačke županije našao se iza granice turskog osvajanja, drugi dio opustošen i popaljen, tako da od velike bogate županije ostane tek nešto više nego ništa. Porezni dimovi svedeni na desetinu broja iz 15. stoljeća, više nisu mogli nositi ekonomski razvoj grada, koji, djelomice višekratno popaljen od Turaka, zaostane, te mu razvoj bude sasvim podređen vojnim obrambenim potrebama. Ipak, i u tim se vremenima Križevci žilavo odupiru uvijek sanjajući ljepšu budućnost i veće mogućnosti. U 17. stoljeću u grad dolaze pavlini, najobrazovaniji i najvredniji crkveni red u Hrvatskoj, moćni feudalci, ali i velika gospoda, koja su mnogo zaslužna da se u teškim vremenima ‘Reliquiae reliquiarum’ u Hrvatskoj nikad ne ugasi luč znanosti i prosvjete. Pavlinski samostan u Križevcima jedan je od posljednjih osnovanih u Hrvatskoj, a jedan Križevčanin, Nikola Benger, baš kroz palvinski red doživi najviše počasti, te postane najpoznatiji kroničar pavlinskog reda. Svoju je veliku ljubav za rodni grad pretočio 1730. godine u redove knjige ‘Regina Martyrum’, koja zbog živih i opširnih opisa Križevaca treba biti smatrana pretečom svih turističkih vodiča u Hrvatskoj. Pavlinski red doveo je ovamo i velikog Ivana Rangera, koji je upravo u gradu Križevcima ostavio svoja prva rijetka štafelajna djela koja je napravio po dolasku u Hrvatsku.
+Raskošno uređene, mada veličinom skromne, križevačke barkone crkve i kapele svjedoče o nikad izgubljenoj vjeri i želji da se nadiđe teška stvarnost. Raspoređene na prilazima, tvoreći oko grada križ, i ove crkve namjerno ili slučajno potvrđuju višestruko rimovanje imena grada s njegovim geografskim položajem i crkvenim patronom. Na požare i kužne pošasti koji su vjerno obilazili grad u najtežim stoljećima podsjećaju nas crkvice sv. Roka i sv. Florijana, na sajam koji se na gornjegradskom trgu održava još od vremena Arpadovića podsjeća crkva sv. Ladislava, koja kasnije patronat podijeli s trećim hrvatskim svecem, sv. Markom Križevčaninom, a na mnoga čuda koja su se dogodila po zagovoru Gospinu, podsjeća najljepša križevačka crkva, Majka Božja Koruška. Od civilnih građevina iz baroka su nam sačuvane raskošna županijska palača (danas Gradsko poglavarstvo), nekadašnja pavlinska apoteka u kojoj je danas Gradski muzej, te zgrada koju žitelji po tradiciji zovu Sabornicom (danas Likovna galerija). Zauvijek su izgubljene sve one karakteristične obrtničko trgovačke kuće u Gornjem gradu uglavnom s tri prozora, koje su mu davale onaj posebni seosko-gradski ugođaj o kojem svjedoči još pokoja stara fotografija. Mnoge stare zgrade uzornom su brigom vlasnika obnavljane i modernizirane, te im je danas teško prepoznati stariju jezgru, kao na primjer grkokatolička biskupija, u čijim zidovima leži blizu jednog tisućljeća, a danas je krasna kompilacija dvaju prvaka hrvatske arhitekture 19. stoljeća, Felbingera i Bollea. I najstarija zgrada u gradu, crkva Sv. Križa obnovljena je početkom 20. stoljeća u nastojanju da joj se obnovom vrati smisao koji je izgubila premještanjem sjedišta župe. U duhu moderne novo ruho dao joj je arhitekt Stjepan Podhorski, isti koji je gradu podario i krasnu zgradu Hrvatskoga doma. Razdvojena povijest Gornjeg i Donjeg grada bila je u ranijim stoljećima poticaj razvoja, jer su se naselja, svako svojim posebnim povlasticama i prednostima nadmetale u razvoju i napretku. Ali u težim stoljećima, kad je život stisnut iza malog obzidanog područja ‘unutarnjeg grada’, te daljim razvojem i promjenom strukture države, staro ustrojstvo postalo je neprimjereno. Stoga, točno pola tisućljeća nakon Stjepanove povlastice, uslijed reforme starih županija, kraljica Marija Terezija proglasi godine 1752. ujedinjenje grada, te novim Križevcima podijeli grb koji je bio sjedinjen stari grb Gornjeg i Donjeg grada. Spomen na odvojenu povijest oba grada blizanca ostao je, osim u ujednjenom grbu koji je i danas grb grada, u dobronamjernim susjedskim šalama ‘Gorjanaca’ i ‘Donjegrađana’, te u pluralnom imenu ‘Križevci’.
+U devetnaestom stoljeću Križevci, kao i čitava Hrvatska, doživljavaju brojne promjene. Sam grad se mijenja u svom vanjskom izgledu. Stare gradske zidine i ostaci tvrđave srušeni su uglavnom do sredine stoljeća pa grad sve više dobiva izgled modernog naselja čemu pridonosi i urbanistički plan iz 1861. godine. Ulice se popločavaju, izrađuju se šetnice i parkovi.
+Znatan je i porast stanovništva. Dok početkom stoljeća grad ima samo 1199 stanovnika, godine 1910. ih je 4886. Sve je veći broj Židova koji u svoje ruke preuzimaju trgovinu te se aktivno uključuju u sve tokove privrednog života grada, a 1895. podižu i sinagogu.
+Osjeća se sve jači zamah u privrednom životu. U gradu postoji pivnica, dvije tiskare, pivovara, paromlin, nekoliko hotela ili svratišta, a 1872. osniva se Štedionica. Otvaranje Gospodarskog i šumarskog učilišta 10. listopada 1860, prvog takve vrste na jugoistoku Evrope, u mnogome je pridonijelo napretku poljoprivrede, ne samo u Križevcima, već u čitavoj sjevernoj Hrvatskoj. Nedaleko grada prošla je 1870. i željeznica, na putu od Budimpešte preko Zagreba do Rijeke, no ona nije ispunila očekivanja Križevčana da će bolja prometna povezanost doprinijeti daljnjem napretku grada. Tokom cijelog devetnaestog stoljeća u gradu kraće ili duže vrijeme borave i rade razni znameniti Hrvati: Tituš Brezovački, Antun Nemčić, Mirko Bogović, Dragojlo Kušlan, Ljudevit Vukotinović, Josip Schlosser, Mojsije Baltić, Milutin Cihlar Nehajev, Gustav Bohutinsky, Fran Gudrum Oriovčanin, Oton Frangeš, Julije Drohobecky, da spomenemo samo neke. Mnogi od njih bili su predavači na Učilištu.
+Svakako najvažniji kulturni događaj u gradu sredinom stoljeća bilo je osnivanje Ilirske čitaonice 1838. godine, koja porijeklo vuče iz Narodnog kasina. U pedesetima će, za Bachova apsolutizma, njen rad privremeno prestati da bi ponovo započeo 1862. po imenom Narodne čitaonice. Privatna glazbena škola djeluje u Križevcima na samom početku XIX stoljeća, već od 1813. Pjevačko društvo “Zvono” postoji od 1863, a kasnije mu se, u glazbenom životu grada, pridružuje i “Slavuj”, koji okuplja slušatelje Gospodarskog učilišta. Postoji i amaterska kazališna družina sa dvadesetak članova.</t>
+  </si>
+  <si>
+    <t>16.54</t>
+  </si>
+  <si>
+    <t>Našice</t>
+  </si>
+  <si>
+    <t>31500 Našice </t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Našice se prvi puta spominju 1229. godine, a svjetovni gospodari su bili Abe, David Lacković, Ivan Korvin, Ivan i Nikola Gorjanski te iločki knezovi Ujlaky. U crkvenom pogledu vlasnici su bili templari, ivanovci i franjevci. Našice su bile pod Turcima u 16. i 17.stoljeću. Pred točno 230 godina našički posjed kupuju grofovi Pejačević i drže ga sve do 1945. godine.
+U Našicama treba razgledati crkvu sv. Antuna Padovanskog, knjižnicu Franjevačkog samostana znanstvenog značaja s 10 inkunabula, stari dvorac grofa Pejačevića iz 1811. godine građen po uzoru na postdamski dvorac Sanssouci te mauzolej i kapelicu grofa Pejačevića iz 1881. godine uz koji se nalazi i grob kontese Dore. Podsjetimo se tko je Dora. Kontesa Dora Pejačević školovana je u Dresdenu i Munchenu i rano pokazala iznimnu glazbenu darovitost. Učila je violinu i glasovir te u svom kratkom životu postala prva hrvatska skladateljica čiju glazbu izvode diljem svijeta. U dvorcu Pejačević, u kojem su rođena i dva hrvatska bana, danas je smješten Zavičajni muzej sa sobama posvećenim značajnim osobama našičkog kraja, zatim etnografska zbirka te poseban odjel lončarstva. Okružuje ga park s mnogobrojnim vrstama autohtonog i egzotičnog drveća i grmlja. Zaštićeni je hortikulturni spomenik s umjetnim jezerom iz pretprošlog stoljeća. Turizam se u Našicama zahvaljujući zemljopisnom položaju i ljepoti našičkog kraja u kojem se tipična slavonska ravnica spaja sa brežuljkastim dijelovima Krndije što je pridonijelo razvoju lovnog i ribolovnog turizma.</t>
+  </si>
+  <si>
+    <t>45.50</t>
+  </si>
+  <si>
+    <t>Županja</t>
+  </si>
+  <si>
+    <t>32270 Županja</t>
+  </si>
+  <si>
+    <t>ŽU</t>
+  </si>
+  <si>
+    <t>Područje Županje i županjske Posavine čovjek je trajno nastanio već u prapovijesnom razdoblju o čemu svjedoče arheološki nalazi koji su se ovdje pronašli slučajno ili su rezultat arheoloških iskopavanja.
+Prva zajednička naselja nastala su ovdje već u mlađem kamenom dobu – neolitu (oko 5000. do oko 3500. g. pr. Kr.) na povišenim gredama uz brojne manje vodotoke. Ti prvi “Županjci” koji su stanovali u zemunicama pripadali su nositeljima starčevačke kulture koji su ovamo doselili iz južne Vojvodine. Ostaci starčevačkog naselja pronađeni su u blizini Županje, na “Šlajsu”.
+Iako su arheološki nalazi iz bakrenog doba – neolitika (3500. – 2100. pr. Kr.) malobrojni, nema sumnje da je čovjek i tada stalno prisutan na tlu današnje Županje, kao i u brončano doba (2100. – 700. g. pr. Kr.) kada se alatke, oružje i nakit masovnije izrađuje od bronce. Isto se to može kazati i za starije željezno doba (700. – 500. g. pr. Kr.) i za mlade željezno doba koje traje od 500. g. pr. Kr. do 1. st. kada dolaskom Rimljana u Slavoniju i ovaj kraj ulazi u historijsko razdoblje.
+Ostaci materijalne kulture rimskog razdoblja u Županji su malobrojni, a svode se na slučajne površinske nalaze rimskog novca, ulomaka keramike, oruđa i oružja. Vjerojatno da u antičko doba ovdje nije bilo većeg naselja osim pojedinačnih građevina, možda poštanska postaja, uz cestu Siscia (Sisak) – Sirmium (Sremska Mitrovica).
+Za poznavanje prošlosti županjskog kraja od propasti Rimskog Carstva 476. pa do početka 13. st. (vrijeme velike seobe naroda, dolaska i trajnog naseljavanja Hrvata u Slavoniji) za sada ne znamo skoro ništa. Samo na temelju jednog iskopanog groba iz 10. st. (u Županji) ne mogu se donositi ozbiljniji zaključci.
+Od 1102. kada je Hrvatska ušla u državnu zajednicu s Madžarima pa do pada pod tursku vlast 1536., područje današnje Županje pripada vukovskoj županiji i u posjedu je feudalnih obitelji Gutt-Keledi, Sente Magoč i Talovaca. Županja se u to vrijeme i pod tim imenom još uvijek ne pojavljuje u pisanim izvorima, ali je sigurno da je postojala kao dio posjeda Selna koji je obuhvaćao tridesetak manjih naselja od kojih je veći dio bio razmješten na području današnjeg bošnjačkog atara. Tragovi tih naselja sačuvani su sve do danas u nazivlju zemljišta, a sama Županja vjerojatno se bila smjestila na tzv. “crkvenoj gredi” (Piškorevci, Veliki kraj) koja se pružala do Save. 
+U pisanim izvorima ime Županje prvi puta je zabilježeno 1554. na Merkatorovoj karti kao Županje Blato (Zupana blacia). Već činjenica da se Županja našla na ovoj karti upućuje na zaključak da je u to vrijeme bila veće i značajnije naselje u županjskoj Posavini.
+Podrijetlo imena Županje može se dovesti u svezu s pojmom župa, župan i prezimenom Županci (Ivan Županci, plemić koji se 1450. spominje kao vlasnik Aljmaša). Drugi dio naziva očito odražava konfiguraciju nizinskog, močvarnog i blatnog terena na kojem se Županja smjestila.
+Stanovništvo Županje u srednjem vijeku, u doturskom razdoblju činili su Hrvati katolici, ali je vjerojatno bilo i patarena (bogumila), pripadnika sekte koja je ovamo prodrla iz Bosne. To potvrđuje i podatak da u doturskom razdoblju na području današnje Županje nije bilo crkve ili župe, jer nije bilo dovoljno vjernika katolika za njihovo osnivanje. Da je patarenstvo u županjskoj Posavini bilo rašireno, mogla bi potvrditi i nastojanja katoličke crkve da ga iskorijeni osnivanjem samostana na Alšanu (kod Podgajaca) i u Lukovu (kod Lipovca). Isto tako i naziv sela Bošnjaci, koje je pod tim imenom u posjedovnim listinama prvi puta zabilježeno 1476., govori u prilog ovim autorima koji tvrde da je patarenstvo u županjskoj okolici bilo rašireno.
+Pod tursku je vlast Županje Blato, kao i veći dio Slavonije, došlo 1536. kada je Husrevbegova vojska prešla Savu kod Šamca i bez otpora zaposjela Posavinu. U Županjem Blatu kao većem naselju Turci su vjerojatno ostavili vojnu posadu i bez većih teškoća organizirali vlast. Patareni su brzo prihvatili islam, a vjerojatno i dio katolika, postajući dio povlaštenog sloja s mogućnošću napredovanja u vojsci i državnim službama. Katolici koji nisu prešli na islam postali su raja s teškim obvezama prema sultanu i novonastalom mjesnom plemstvu. S obzirom da su bili malobrojni, katolici Županjeg Blata za cijelog turskog perioda potpadali su pod tramošničku župu u Bosni.
+O Županjem Blatu za vrijeme turske vladavine od 1536. do 1691. nisu poznate nikakve pisane vijesti. Ovamo nije zašao ni neumorni turski putopisac Evlija Čelebija koji je posjetio svako značajnije mjesto u Slavoniji. Ne samo u pisanim spomenicima, nego ni u arhitekturi ili u toponomastici, ne nailazi se na tragove turskog razdoblja u Županjem Blatu i okolici, osim u jezičnoj terminologiji pa se i danas u svakodnevnom govornom jeziku rabe brojne riječi turskog podrijetla.
+Poslije poraza pod Bečom 1683. Turci su nakon dugotrajnog ratovanja bili prisiljeni na uzmak iz Slavonije. Svoje posljednje uporište, brodsku tvrđavu, morali su napustiti 1691. pa je time konačno cijela Slavonija oslobođena turske vlasti.
+Odlaskom Turaka došlo je do velikih promjena u strukturi stanovništva županjske Posavine. Starosjedioci, islamizirani patareni koji su s vremenom potpuno prihvatili tursku državnu misao, napustili su Županje Blato i povukli se u Bosnu. I dio starosjedilačkih katolika otišao je iz ovog naselja sklanjajući se u sela dalje od Save koja su bila sigurnija nego ovo granično područje. Na njihovo mjesto došao je novi živalj iz Bosne kojega je ovamo poslije vojne akcije u Bosni 1697. doveo princ Eugen Savojski. Zauzeli su zemljište izbjeglih katolika i muslimana i vrlo brzo se stopili sa starosjediocima s kojima ih je povezivao isti jezik, ista vjera, a i socijalni položaj, jer su i jedni i drugi sve donedavno bili raja.
+Do pokreta stanovništva u posavskom dijelu Slavonije ponovno će doći 1718. kada je Austrija osvojila bosansku Posavinu. Vjerujući da će osvojeno područje za stalno ostati u sastavu carevine, vlasti su poticale preseljavanje na desnu obalu Save gdje je bilo dosta napuštene i obradive zemlje. Neki rodovi iz Županje, Bošnjaka, Babine Grede i Štitara doista su prešli u bosansku Posavinu, ali kako 1739. Austrija gubi to područje mnogi su se tada vratili natrag. Onima kojima je dosadilo stalno seljakanje ostali su pa zato danas imamo neka ista prezimena u Županji i u prekosavskim selima.
+Poslije Karlovačkog mira 1699. kada je Sava postala stalnom granicom između dvaju carstava (osim u razdoblju 1718. – 1739.), austrijske vlasti su pristupile uređenju slavonsko – srijemske vojne granice. U većim, ili gospodarski i strategijski važnijim mjestima, stacionirane su vojne posade s kapetanom na čelu. Takva vojna posada postavit će se i u Županjem Blatu koje će zatim sve do razvojačenja Vojne granice biti sjedište 11. satnije (kumpanije) u sastavu 7. brodske pješačke pukovnije Županjsko stanovništvo uklopljeno je u vojno – graničarski sustav kojem su svi zdravstveno sposobni muškarci bili vojni obveznici od 16. do 60. godine života i u stalnoj pripravnosti. Iako nije bio kmet, kao njegov sunarodnjak u građanskoj Hrvatskoj, život graničara bio je vrlo težak, opterećen brojnim zabranama i pod prijetnjom batinanjima i za najmanji prekršaj.
+Poslije izgona Turaka, kada se život postupno normalizirao, a doseljenici iz Bosne povećali broj stanovnika pečujska biskupija osnovala je 1717. u Županjem Blatu župu kojoj su još pripadali Bošnjaci i Štitar. Prema opisu pečujskog biskupa Franje Nesselroda, koji je posjetio Županju 1729. župna crkva Sv. Ivana nalazila se u sredini sela, a građena je od hrastovine i pokrivena hrastovim grančicama blizini crkve je drveni toranj i u njemu zvono koje su župljani kupili za 30 forinti. Iz posjeta drugoga pečujskog biskupa Županjem Blatu 1755. saznajemo da je izgrađena nova, također drvena crkva i da selo broji 156 bračnih parova i 708 stanovnika.
+Polovicom 18. st. izvršeno je “stjerivanje” kuća u red (ušoravanje), odnosno suseljavanje manjih okolnih zaselaka u jedno selo i pod jednim nazivom. Tada je stari dio današnje Županje dobio urbanistički oblik koji je u osnovi sačuvan sve do danas.
+Kao kompanijsko mjesto Županje Blato je 1764. dobilo i školu u kojoj se nastava izvodila na njemačkom jeziku, a pohađalo ju je 40 učenika. Škola je međutim ubrzo ukinuta, a ponovno otvorena oko 1830. Kroz cijelo 18. st. Županje Blato se postupno formiralo kao važnije mjesto u Međubosuću: tu je sjedište satnije, kumpanije, župe, jedno vrijeme selo ima i školu, a tu je i solarski te tridesetnički ured, neka vrst carinarnice.
+Vijesti iz prve polovice 19. st. govore da je 1829. Županja imala 1829 stanovnika, da je oko 1830. dobila pučku školu i da se tu (pored današnjeg Muzeja) nalazi prijelazna postaja za tursku Bosnu s raštelom u kojem se obavljala trgovina između graničara i turskih podanika. U to vrijeme Savom od Siska do ušća u Dunav godišnje plovi 500 većih lađa koje pristaju i kod Županje, a redovito ovdje pristaju i komorski brodovi solarice dovozeći sol iz gornje Ugarske. Prvi hrvatski (i na Balkanu) parobrod “Sloga” koji je prometovao između Zemuna i Siska tijekom 1844. i 1845., kada je potopljen kod Bošnjaka, također je redovito pristajao kod Županje.
+Ideje hrvatskog preporodnog pokreta imale su odjeka i u Županji, a njihov konkretni odraz ogleda se u osnivanju Narodne čitaonice 1861.
+Vojna granica, taj specifični vojno-feudalni sustav, dokinuta je 1873. a 1881. kada je priključena banskoj Hrvatskoj. Sedma brodska pukovnija u čijem sastavu se nalazila i 11. županjska kumpanija, podijeljena je na kotareve, a Županja je određena za središte jednoga od njih. Cijeli kotarski aparat nalazio se u Županji, osim Kotarskog suda koji je smješten u Bošnjake. Tek 1911. sjedište Kotarskog suda bit će iz Bošnjaka preneseno u Županju. Ukidanjem Vojne granice ubrzan je proces raspadanja velikih zadružnih zajednica, što su vojne vlasti ranije sprječavale svim sredstvima jer se čitav vojno-graničarski sustav temeljio na instituciji zadruge.
+Nestankom Vojne granice došlo je i do velikih gospodarskih promjena prodorom novih i slobodnijih kapitalističkih odnosa. U županjskoj agrarnoj sredini te promjene vezane su uz iskorištavanje hrastovih šuma. Ovamo dolaze strani poduzetnici koji, znajući za potrebe europskog tržišta za kvalitetnom bačvarskom dužicom i taninskim ekstraktom, razvijaju snažnu drvno-preradivačku proizvodnju. Još sredinom 19. st. u okolici Županje (Bošnjaci) počelo se s eksploatacijom ogromnih slavonskih hrastova za izradu dužica, ali intenzivno iskorištavanje počinje 80-tih godina kada je u Županji podignuta Tvornica tanina.
+Ovu tvornicu, prvu i najveću te vrsti u Slavoniji i Srijemu, izgradili su udruženi engleski kapitalisti 1884. Uz nju, Englezi su izgradili i Tvornicu bačava potrebnih za transport taninskog ekstrakta. Županja nije slučajno odabrana za lokaciju ova dva i za ono vrijeme velika pogona: u okolici Županje nalazile su se ogromne površine hrastovih šuma. blizina Save osiguravala je jeftini transport, a jeftina je bila i radna snaga vješta poslovima oko drveta. Sve to navelo je Engleze da tu ulože kapital od oko 70000 funti sterlinga i izgrade Tvornicu tanina.
+Tvornica tanina i bačava dnevno je prerađivala 600 vagona sirovine. Dvadeset godina kasnije dnevna prerada drvene sirovine povećana je na 1200 vagona, što najzornije pokazuje kako se ubrzano i nemilosrdno iskorištavalo šumsko bogatstvo županjskog kraja. Tada je, oko 1910. u Tvornici tanina i bačava i na drugim poslovima bilo zaposleno oko 600 radnika od kojih su mnogi bili domaći ljudi, seljaci i nadničari koji su ovdje našli dodatne izvore novčane zarade.
+Izgradnjom Tvornice tanina i bačava došlo je do velikih promjena u županjskoj sredini navikloj da sin plete kotac kao što je to radio i otac. Iz drugih krajeva Hrvatske (Dalmacije, Like, Gorskog kotara), iz Slavonije pa i iz Slovačke, dolaze u Županju i njenu okolicu šumski radnici koji kao sezonci traže mogućnosti zarade. Tada su posebno bili cijenjeni Gorani (“Kranjci”, kako ih je narod zvao) koji su bih iskusni obrađivači drveta. Ovamo su dolazili u “partijama” nakon što su sa zakupcem šumskih parcela utvrdili uvjete pod kojima će “rušiti” i obraditi trupce u dužice ili u neku drugu vrstu (pragovi za pruge, npr.) građevnog materijala. Osim Gorana, na neki način kvalificiranih radnika, dolaze i radnici koji nalaze pomoćne poslove na tako velikom radilištu kao što je sječa, obrada i prerada hrastovih trupaca.
+Domaće seljačko stanovništvo u eksploataciji stoljetnih hrastovih šuma također nalazi izvor zarade. Udruženi u “partije” i s konjskim zapregama izvlače na “parizerima” ogromne klade do mjesta istovara. Kirijašenjem, kako se zvalo transportiranje hrastovih klada iz šume do istovarne postaje (“Lehštata”), domaće je stanovništvo dolazilo do značajne novčane zarade, tim važnije jer se ostvarivala u vrijeme kada se nisu obavljah najvažniji poljodjelski poslovi.
+Najbrojniji, šumski sezonski radnici, poslije obavljenog posla vraćali su se kući, ali su se mnogi odlučili za stalno naseliti u Županji i okolnim selima.
+To potvrđuju i ovi podaci: Županja je 1880. imala 2611 stanovnika, a 1900. već 3630. Za 20 godina županjsko stanovništvo se povećalo za preko 1000 osoba na što nije bitnije utjecao natalitet jer je bio samo nešto veći od mortaliteta, nego je doseljavanja iz drugih krajeva odnosno Austro-Ugarske. Poslije 1900. stanovništvo Županje stagnira čak i opada, što je u izravnoj vezi s eksploatacijom šumskih površina koje su do 1910. bile uglavnom posječene pa više nema gospodarskih razloga zbog kojih bi se migracija iz krajeva nastavila.
+Iako ovdje nisu vođene ratne operacije, i Županja je teško stradala Prvog svjetskog rata 1914. -1918. Mnogi Županjci, njih oko 60, ostavili su svoje kosti po raznim bojištima, a nestašica živežnih namirnica i bolesti još su više prorijedili županjsko stanovništvo. U ljeto 1915. pojavila se kolera koja je odnijela desetak života, a pred kraj rata u jesen 1918. izbila je epidemija od koje je u Županji umrlo 125 osoba svih životnih dobi.
+U novostvorenu državu Kraljevinu Srba, Hrvata i Slovenaca (od 1929. Kraljevina Jugoslavija), Županja je ušla kao sjedište županjskog kotara koji je sva sela od Strošinaca do Gundinaca. Već u prvim danima po dolasku srpske vojske pred kraj 1918. pokazalo se u kakvoj će državi i s kime Županjci živjeti. Bahati i okrutni “oslobodioci” terorizirali su stanovništvo na razne načine, a posegnuli su i za već zaboravljenim metodama javnog batinanja da bi, tobože, održali red i mir i prisili Županjce na poslušnost.
+U političkom životu Županje u Jugoslaviji između Prvog i Drugog svjetskog rata najvažniju je ulogu imala Radićeva Hrvatska republikanska seljačka stranka (od 1925. samo Hrvatska seljačka stranka) koja je na svim izborima premoćno pobjeđivala. Za listu dr. Mačeka na izborima 1935. glasovalo je skoro 90% birača, a 1938. čak preko 95% birača. U to vrijeme (prema popisu iz 1931.) Županja broji oko 3500 stanovnika, što je manje nego 1900. kada je u njoj živjelo 3630 osoba. Većina se bavi poljodjelstvom, a oko 1000 osoba zaposleno je u industriji i obrtu. Taj broj će se i smanjiti poslije prestanka s radom Tvornice tanina 1936. godine. Uoči Drugoga svjetskoga rata 85 posto stanovništva Županje činili su katolici, Hrvati. Po brojnosti zatim dolaze pravoslavci, u stvari Cigani, Romi, koji su se tada tako izjašnjavali pod pritiskom i utjecajem velikosrpske vlasti. Oko pet posto županjskih žitelja bili su Nijemci i Židovi koji su se bavili trgovinom, poduzetništvom i tercijarnim uslugama.
+Raspad Kraljevine Jugoslavije poslije “travanjskog rata” 1941. i uspostavu Nezavisne Države Hrvatske dočekali kao ostvarenje višestoljetnih težnji hrvatskoga naroda za neovisnom državom. Ustrojstvo nove vlasti nije teklo glatko, a neke radikalnije mjere koje sa ustaše poduzimale, shvaćene su kao nužne u tim prvim mjesecima tek uspostavljene države. Kasniji slijed događanja i neki neodmjereni postupci vlasti, osobito u pitanju deportacije i likvidacije Cigana, Židova i Srba. ali i domaćih ljudi koji su bili kritičniji prema politici koju su ustaše provodile, nisu kod Županjaca naišli na odobravanje. Ipak ogromna je većina u skladu s naputkom dr. Mačeka, ostala lojalna novim vlastima. Lijevo orijentirani pojedinci i malobrojni komunisti koji bili protiv nezavisne Hrvatske, djeluju u ilegali, uglavnom samostalno i nepovezano, do ljeta 1943. kada se aktivnije uključuju u antifašistički pokret čije je središte u zapadnom dijelu županjskog kotara bilo u šumi Merolino.
+Županja je za vrijeme rata (1941. -1945.) bila pošteđena ratnih operacija s izuzetkom nekoliko manjih vojnih i partizanskih i saboterskih akcija. Međutim, u jesen 1943. kroz sela županjske Posavine, doslovce, protutnjala je Prva kozačka divizija koju su činili ruski zarobljenici, crvenoarmejci, pod njemačkom komandom. “Čerkezi”, kako ih je narod nazivao, nemilosrdno su pljačkali, ubijali, palili i silovali da je predstojnik županjske kotarske i morao nadležne izvijestiti kako “mirno i nevino pučanstvo nema nigdje zaštite”. Ti “Čerkezi”, dezorjentirani vojnici bez budućnosti i nade da će se vratiti u Staljinov SSSR i tamo preživjeti, u malo vremena nanijeli su županjskom kraju najviše zla za vrijeme Drugoga svjetskoga rata. Partizanske jedinice, Osma crnogorska brigada, ušle su u Županju 13. travnja 1945. bez većih borbi, jer su domobransko-ustaške i njemačke snage već bile u povlačenju prema zapadu.
+Dolazak partizana dočekan je sa strahom, koji se ubrzo pokazao opravdanim. Preko noći preobučeni u partizane, srpsko-crnogorski četnici u hrvatskim, srijemsko-slavonskim selima počinili su brojne zločine ubijajući pripadnike HSS-a, domobrane i civile, samo zato što su Hrvati. To se dogodilo i u Županji neposredno poslije dolaska partizana kada je likvidirano više nevinih osoba, a mnogi su odvedeni na križni put, u smrt. Teror, ali drugim sredstvima, nastavljen je i u prvim poslijeratnim godinama u kojima se provodila nacionalizacija, nasilna kolektivizacija i tjeralo u seljačke zadruge zbog čega su mnogi ostali bez imovine i osnovnih sredstava za obradu zemlje. Poseban teret za županjskog seljaka bio je obvezan otkup (blaži izraz za nasilno oduzimanje) živežnih namirnica kojih nije imao dovoljno ni za vlastite, najosnovnije potrebe.
+Uslijed ubrzane industrijalizacije, Županja već u prvim godinama poslije Drugoga svjetskoga rata sve više dobiva izgled i sadržaje urbanizirane sredine, na što je odlučujuće utjecala izgradnja Sladorane i Mljekare. Sladorana se počela graditi 1942., ali je završena tek 1947. kada je i počela s preradom šećerne repe. Mljekara je izgrađena 1950. godine.          Izgradnja ove dvije tvornice prouzročila je i promjene u strukturi i broju županjskog stanovništva doseljavanjem radnika iz ratom pogođenih i pasivnih krajeva Hrvatske. Zbog njih se gradi uz Sladoranu i novo, radničko naselje (“kolonija”). Prema popisu iz 1953. Županja broji 5391 stanovnika dok je uoči Drugog svjetskoga rata imala nešto više od 3500. Tome značajnom povećanju u petnaestak godina doprinijeli su novopridošli radnici koji su našli zaposlenje u Sladorani i Mljekari.Sve do 1956. Županja je bila središte kotara u sastavu osječke oblasti kada se ove ukidaju i osnivaju novi kotarevi. Županja tada postaje samo jedna od većih općina u sastavu vinkovačkog kotara. Novom teritorijalno-administrativnom podjelom vinkovački kotar je ukinut 1961. a Županja se formira u središte županjske općine, do nove reorganizacije 1991. godine od kada ima status grada.
+Specifičan položaj županjske Posavine očituje se u njenoj, 89 kilometara dugoj, granici na Savi i petnaestak kilometara granice sa Srbijom – agresorom. Naši su se ljudi od prvog trena aktivno uključili u obranu Hrvatske, što potvrđuju i dva poginula redarstvenika u Borovom Selu: Mario Prusina i Mladen Čatić. Županjci su dali svoj obol i u pokušaju oslobađanja Mirkovaca. U suradnji s drugim hrvatskim postrojbama branili su istočni dio vinkovačkog atara od Privlake preko Đeletovaca sve do Lipovca. Šumski spačvanski bazen nalagao je specifične oblike ratovanja. Aktivno suprotstavljanje srbočetničkom agresoru spriječilo ga je u njegovu prodoru. Tuzlanski korpus trebao je forsirati Savu i s juga ući u Hrvatsku. Djelotvorna obrana onemogućila je ovaj naum u samom njegovu početku.
+Postrojbe 131. brigade znatno su pripomogle očuvanju hrvatskog područja u bosanskoj Posavini. U aktivnoj obrani županjske Posavine sudjelovali su: pričuvni i djelatni sastav postrojbi Ministarstva unutrašnjih poslova, odredi Narodne zaštite, Zbora narodne garde, 131. brigada Hrvatske vojske, Domobranska bojna Županja i 83. samostalna gardijska bojna HV.
+Drugi kritični period bio je znatno duži. Bosanski Srbi, u nemogućnosti da osvoje naša područja, dalekometnim topništvom pokušavali su slomiti moral naroda. Opća opasnost trajala je 1263 dana (27. travnja 1992. – 12. listopada 1995.). U tom razdoblju palo je 45.000 granata i projektila te je u gospodarskim, infrastrukturnim i stambenim objektima pričinjena šteta od cca 100 milijuna DEM. Za to vrijeme industrijska proizvodnja pala je na 40 posto dok je poljoprivredna smanjena gotovo za polovinu. Tijekom rata došlo je i do ljudskih žrtava: poginulo je 58 a ranjene su 122 osobe. Sve te žrtve svjedoče o našoj savjesti i svijesti, onoj čvrstoj i visokoj stijeni s koje se ponajbolje uočavaju svi naši vidici.</t>
+  </si>
+  <si>
+    <t>Daruvar</t>
+  </si>
+  <si>
+    <t>43500 Daruvar</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>Grad Daruvar je naselje s dugom urbanom povijesti, uskoro će navršiti dvije tisuće godina svojeg postojanja kao moderne cjeline, a njegova urbana jezgra mijenjala se u skladu s procesima koje su nosila različita povijesna razdoblja. Regionalno je središte županije u turizmu, te vinogradarstvu i voćarstvu.
+Najstarije poznato naselje, smješteno pored ljekovitih geotermalnih izvora na prostoru daruvarske kotline datira od 4. stoljeća prije Krista, iako arheološki nalazi kazuju da su ovi krajevi bili nastanjeni već u kamenom dobu.
+Za važnost koju ima kroz povijest, a i danas, neosporivu zaslugu imaju geotermalna vrela, čija je ljekovitost poznata od početka postojanja i života na ovim prostorima. Od vremena Rimljana, kada je ovdje obitavalo panonsko–keltsko pleme, koje su grčki i rimski pisci nazivali Iasi, u značenju ” Topličani” ili ” Iscjelitelji”, a sve prema velikom broju geotermalnih vrela s iscjeliteljskim svojstvima. Rimljani osnivaju svoje naselje pod imenom Aquae Balissae u značenju ”Vrlo jaka vrela”, tj. današnji Daruvar. Hrvati na ovo područje doseljavaju nakon propasti Zapadnog rimskog carstva i osnivaju naselje Probatica, kasnije Podborje.
+Ipak, presudno za razvoj grada i ljekovitih kupki bio je dolazak grofa Antuna Jankovića 1745. na ove prostore.
+On je gradu dao oblik koji i danas ima, te ga odredio kao termalno lječilište. Antun pl. Janković mijenja hrvatsko ime naselja Podborje, u mađarsko Daruvar, u značenju Ždralov grad ili točnije Ždralov dvorac, prema prelijepom baroknom dvorcu koji je započeo graditi 1771. god.
+Grof Janković naseljava svoje vlastelinstvo poljoprivrednicima i obrtnicima iz Hrvatske, Češke, Slovačke, Njemačke i Mađarske. Ovi prostori tako ponovo bivaju napučeni, s obzirom na dotadašnju rijetku naseljenost kao posljedicu ratova s Turcima. Doseljenicima je obećana besplatna zemlja i materijal za gradnju kuća.
+No ono čime su Jankovići obilježili svoje djelovanje, zasigurno je gradnja blatnih kupki na ljekovitim geotermalnim izvorima. Kaptirano je nekoliko izvora i 1772. godine izgrađena prva, Antunova kupka. Time je Daruvar postao poznato termalno lječilište sve do danas. Prirodni faktori vrela bili su presudni za taj kontinuitet lječilišta, a to je temperatura vode koja je 35 – 46°C te bogatstvo mineralnog blata. Djelovanje termalne vode je fizikalno, biološko i kemijsko.
+Od industrijskih objekata, od 1840. god. kad je sa radom započela Daruvarska pivovara, pa do 1918. godine, u Daruvaru je uz nju radila pilana i suknara, dok je glavna gospodarska grana bila šumarstvo.Mnogo brže od industrije razvijala se trgovina i ugostiteljstvo, zaslugom uspješnog rada termalnog lječilišta. Kotar Daruvar 1912. godine je imao 63 trgovca, 412 obrtnika, 68 ”sitničara”, 41 gostioničara i 92 krčmara. Takvom razvoju doprinijela je i izgradnja pruge Banova Jaruga – Daruvar – Barcs, otvorena uz nazočnost samog cara Franje Josipa 1897. godine.
+Nakon Prvog svjetskog rata u Daruvaru djeluje i ciglana, ljevaonica željeza i tvornica strojeva, pletionica, staklana, tiskara i jedna električna centrala zvana ”munjara”.
+U Domovinskom ratu grad Daruvar bio je jedan od glavnih točaka obrane Slavonije, a živote za domovinu je dalo 112 pripadnika MUP-a, HV-e i civila. U spomen žrtvama podignut je 1993. godine u parku grofa Jankovića Spomenik braniteljima Daruvara. 17. rujna se obilježava Dan branitelja Grada Daruvara i oslobođenje vojarne „Polom“.</t>
+  </si>
+  <si>
+    <t>45.59</t>
+  </si>
+  <si>
+    <t>17.23</t>
+  </si>
+  <si>
+    <t>Nova Gradiška</t>
+  </si>
+  <si>
+    <t>35400 Nova Gradiška</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>U svojoj relativno kratkoj, ali i bogatoj prošlosti (grad povjesničari često nazivaju i jednim od najmlađih hrvatskih gradova), Nova Gradiška je po svom povijesnom osnutku graničarsko naselje čiji su mještani oduvijek vodili neprekidnu borbu za nacionalnu opstojnost i neovisnost. Najprije s osvajačima Turcima, potom austrijskim i ugarskim nasrtajima, a u novijoj povijesti i veliko-srpskim režimima. U mirnodopskim razdobljima Novogradiščani jačaju gospodarsku i društvenu djelatnost.
+Nastanak naselja na području današnjeg grada polovicom 18. stoljeća povezuje se s odlukom carice Marije Terezije o učvršćivanju granice Carstva na jugu, osnivanjem slavonske Vojne Krajine , nakon izgona Turaka preko Save. Nova Gradiška je utemeljena 1. svibnja 1748. godine kao buduće zapovjedno mjesto Gradiške graničarske pukovnije. Izgradnjom novoosnovanog vojnog naselja rukovodio je potpukovnik Phillip Lewin Beck, zapovjednik pukovnije, koji je ”najprije crkvicu podići dao, zatim za pukovnika i podpukovnika kuće, te veliku stražu sa reštanom i gostionu…” Prvi objekti bili su od drveta, a Beck se ”trsio i ceste i putove i mostove praviti, škole uređivati, zanatlije i trgovce naseljavati…”.
+Nova Gradiška je osnovana u doba baroka, u duhu apsolutističkog vremena, kada se, diljem Hrvatske utemeljuju gradovi s ravnim paralelnim ulicama, sječenim pod pravim kutom, s prostranim središnjim četverokutnim glavnim trgom oko kojega se izgrađuju crkve, te javne i privatne zgrade.
+Nakon ukidanja vojne krajine (1871.) i njenog sjedinjenja s civilnom Hrvatskom (1881.) Nova Gradiška postaje kotarsko središte, prometno se povezuje sa Zagrebom (željeznička pruga 1888.) i sve intenzivnije razvija. Ubrzani gospodarski, društveni i kulturni život, gotovo preko noći mijenja karakter dotadašnjeg vojnog središta. U to je vrijeme izgrađena velebna pivovara na parni pogon, vlasnika Dragutina plemenitog Lobea (1873.) , prva u Hrvatskoj, otvaraju se pogoni za preradu drva, izradu opekarskih proizvoda, mlinovi – iz kojih nešto kasnije, niču i brojne tvornice (Kruljac i sinovi /pokućstvo/, Nektar / sirupi i likeri/, paromlin Matoković, nekoliko tvornica opeke, tvornica žeste i keramička tvornica u Cerniku.
+Jača nacionalni duh i politička borba s germanskim i ugarskim nasrtajima na Slavoniju. Osnivaju se hrvatska društva: Dobrovoljno vatrogasno društvo (1871, prvo u Slavoniji), Hrvatska čitaonica (1874.), HPD “Graničar” (1886.), Hrvatski sokol (1906.) i druga.
+Prva tiskara utemeljena je već 1882. godine, a samo godinu dana kasnije u njoj se tiska i prvi list – “Gradiščanin”. Početkom prošlog stoljeća grad se ponosi asfaltiranim nogostupima (1910.), a 1913. godine ulicama su zasvijetlile i prve električne žarulje , čime Nova Gradiška postaje šesti elektroficirani grad u Hrvatskoj. Uređuju se ulice, gradski park, promenada (šetalište), sajmište, groblje… Za brojne komunalne pothvate, iznimno velike za tada mali grad, posebno je zaslužan znameniti općinski načelnik Ivo Kramarić (1856.-1932.), koji je tu visoku dužnost obnašao, s manjim prekidima, od 1907. do 1927. godine.
+U vrijeme 2. Svjetskog rata Nova Gradiška je sjedište Velike župe Livac-Zapolje, koja je obuhvaćala kotare Nova Gradiška, Požega, Daruvar, Novska, Pakrac, Kostajnica i Prijedor.
+U poslijeratnoj socijalističko-komunističkoj Jugoslaviji razvoj grada se oslanjao, uglavnom, na prirodne potencijale, s posebnim naglaskom na razvoj drvne, prehrambene, tekstilne, metalne i kožarske industrije. Grade se velike tvornice: Stjepan Sekulić Jucko, Slavonija radinost, Nektar, PIK, Yukon, Zlata, Tang, Elting, Kožara i dr. Izgradnja tvornica i otvaranje tisuće radnih mjesta utjecalo je na preseljenje stanovnika iz obližnjih sela u grad. Grad se nekontrolirano širi, te se grade stambeni blokovi u naselju Urije-socrealistička arhitektura.
+1990. voljom hrvatskog naroda na višestranačkim izborima Hrvatska dobiva samostalnost i neovisnost. Na žalost, pobunjeni Srbi koji nisu prihvatili demokratske promjene i samostalnu državu Hrvatsku, organizirali su oružanu pobunu i uz potporu JNA okupirali trećinu teritorija RH. Od rujna 1991. do 3. siječnja 1992. Nova Gradiška je trpjela svakodnevna razaranja u kojima su potpuno uništeni ili oštećeni gotovi svi gospodarski objekti, crkve, škole, dječji vrtići, bolnica, tisuće obiteljskih domova i stanova. U Domovinskom ratu braneći domovinu diljem Hrvatske 250 hrvatskih branitelja iz Nove Gradiške i okolice dalo je svoj život. 107 branitelja iz drugih krajeva Hrvatske ostavilo je živote na novogradiškom ratištu.
+Pobjedom Hrvatske vojske u vojnoredarstvenoj akciji Bljesak 1. i 2. svibnja 1995. oslobođeno je okupirano područje zapadne Slavonije.
+Poslije Domovinskog rata Nova Gradiška suočena je s brojnim ratnim posljedicama-od saniranja ratnih šteta do zatvaranja tvornica što je uzrokovalo veliki broj nezaposlenih osoba. Posljednjih je godina pokrenut značajan gospodarski projekt Industrijski park koji nastoji privući ulaganja poslovnih partnera iz zemlje i inozemstva.</t>
+  </si>
+  <si>
+    <t>45.26</t>
+  </si>
+  <si>
+    <t>17.38</t>
+  </si>
+  <si>
+    <t>Knin</t>
+  </si>
+  <si>
+    <t>22300 Knin</t>
+  </si>
+  <si>
+    <t>Knin, grad u Dalmaciji, 71 km sjeveroistočno od Šibenika. Leži na desnoj obali rijeke Krke, na 220 m apsolutne visine. Čvorište je ličke, unske i zadarske željezničke pruge te cestâ koje iz unutrašnjosti Hrvatske vode k obali Jadranskoga mora.
+Metalna (vijci), tekstilna (konfekcija, rublje), drvna industrija; proizvodnja građevinskog materijala (opeka, elementi od gipsa). U blizini je ležište sadre i kamenolom vapnenca. Franjevački samostan (spominje se u XV. st.), crkva sv. Antuna Padovanskoga iz 1863. Zapadno od grada uzdiže se srednjovjekovna tvrđava (X. st.); konačan izgled dobila je početkom XVIII. st., kada je umjetnim prosjekom odijeljena od brda Sv. Spas, koje se sa sjeverne strane na nju nadovezuje. Tvrđava je jedna od najvećih fortifikacijskih građevina u Dalmaciji. U njoj je do II. svjetskog rata bio smješten Muzej hrvatskih starina. Podijeljena je na gornji, srednji i donji grad, koji su međusobno povezani pokretnim mostovima. U početku XVIII. st. na gradnji zidina radili su i domaći majstori (Ivan i Ignacije Macanović). U Domovinskome ratu tvrđava je devastirana (zbog ratne namjene), a katoličke crkve sv. Jakova i sv. Ante porušene su. – Arheološka nalazišta na području grada potvrđuju da su Knin i njegova okolica bili nastanjeni već u neolitiku i brončanom dobu. Iz rimskoga doba sačuvani su ostatci nekoliko rimskih grobova u podnožju kninske tvrđave, ostatci arhitekture na brdu Sv. Spas te ostatci obližnjeg rimskog logora Burnuma, sagrađenog u I. st. Nakon Rimljana tim su područjem vladali Ostrogoti (V–VI. st.), a za bizantske je vladavine (VI–VII. st.) na brdu Sv. Spas sagrađena utvrda. Mnogobrojni arheološki nalazi iz razdoblja starohrvatske umjetnosti i ranoga srednjega vijeka svjedoče o ranoj prisutnosti Hrvata na tom području.
+Knin prvi put spominje oko 950. bizantski car Konstantin VII. Porfirogenet, pod imenom Tenen (grč. τὸ Τενήν), kao grad i središte župe (grč. ἡ Τνήνα). U srednjovjekovnim latinskim izvorima naziva se i Tnin, Tenen, Tinninium, Tzena, Clino i sl. Srednjovjekovna utvrda podno brda Sv. Spas bila je kraljevski castrum i povremena prijestolnica hrvatskih vladarâ u X. i XI. st. (Trpimira, Muncimira, Svetoslava, Stjepana Držislava, Krešimira I.). Od polovice XI. st. Knin je postao prometno sjecište na putu iz dalmatinskih komuna prema Slavoniji i Bosni. Između 1040. i 1050. bila je osnovana Kninska biskupija, koje su biskupi nosili naslov »hrvatskoga biskupa« (episcopus Chroatensis) te su imali jurisdikciju do rijeke Drave. Za kralja Dmitra Zvonimira Knin je bio prijestolnica Hrvatskoga Kraljevstva, potom prijestolnica posljednjega hrvatskoga kralja Petra, a nakon njegove smrti ušao je u sastav Hrvatsko-Ugarskoga Kraljevstva (1102). Između 1076. i 1078. posvećena je prva kninska katedrala sv. Marije; oko nove katedrale sv. Bartula, posvećene između 1272. i 1274., poslije se razvio kninski kaptol. Od XII. do XIV. st. u Kninu i Zagrebu naizmjence su stolovali herceg i ban, održavali se dalmatinsko-hrvatski sabori i zasjedao Banski sud za Hrvatsku. Potkraj XIII. st. članovi hrvatskoga velikaškoga roda Bribirskih postali su gospodari Knina. Slabljenjem moći Mladina II. Bribirskoga kninski posjed preuzeo je rod Nelipčića, a nakon smrti kneza Nelipca (1344) hrvatsko-ugarski kralj Ludovik I. Anžuvinac. Od 1388. do 1392. bio je u sastavu Bosanskoga Kraljevstva. God. 1420. osmanska je vojska prvi put napala grad; 29. V. 1522. osvojio ga je bosanski sandžak-beg Husrev pa je Knin ušao u sastav Osmanskoga Carstva kao nahija u Bosanskom sandžaku. Od 1537. bio je u sastavu Kliškoga sandžaka, a od 1574. Krčko-ličkoga sandžaka. Premda su Mlečani 1648. nakratko bili zauzeli grad, sastavnim dijelom posjeda Mletačke Republike u Dalmaciji postao je nakon pobjede nad Osmanlijama 11. IX. 1688. Nakon pada Venecije (1797) i ukinuća francuskih Ilirskih pokrajina (1813) Knin je pripao Habsburškoj Monarhiji, a Rapalskim ugovorom (1920) ušao je u sastav Kraljevine SHS. U II. svjetskom ratu, pobjedom nad četničkim i njemačkim snagama u Kninskoj operaciji (26. XI. – 4. XII. 1944) te oslobođenjem Knina, partizanske su snage preuzele nadzor nad cijelom Dalmacijom. Polovicom 1990. Knin je bio žarište srpske pobune u Hrvatskoj. U kolovozu 1990. lokalne su vlasti poticale odcjepljenje od Hrvatske i uz pomoć Jugoslavenske narodne armije organizirale nadzor nad kninskim područjem. Hrvatsko stanovništvo bilo je prognano. Nakon samoproglašenja »Republike Srpske Krajine« (19. XII. 1991), Knin je bio njezin glavni grad. Oslobođen je 5. VIII. 1995. u operaciji Oluja. Srpske su se snage povukle, a zajedno s njima izbjegla je većina srpskog stanovništva.</t>
+  </si>
+  <si>
+    <t>Metković</t>
+  </si>
+  <si>
+    <t>20350 Metković</t>
+  </si>
+  <si>
+    <t>Metković se prvi put spominje 1422. u jednom spisu koji se čuva u dubrovačkom arhivu: flumaria Narrenti subtus Metchovich (...na rijeci Neretvi pod Metkovićem). Sudeći po arheološkim nalazima na brdu Predolcu, neposredno do grada, život je u njemu otpočeo još u pretpovijesno doba. Pretpostavlja se da su prvi poznati žitelji u donjem toku Neretve bili helenizirani Iliri Daorsi, koje su kasnije potisnuli ratoborni Ardijejci i Delmati. O njima  svjedoče mnogobrojne gradine i kamene gomile na okolnim brdima. U četvrtom stoljeću pr. Kr. stari Grci počeli su kolonizirati jadranske otoke i obalu, pa su zbog zgodna položaja utemeljili emporij (luku), tri kilometra sjeverozapadno od Metkovića. Bila je to u antici daleko poznata Narona, današnji Vid. Njezini su žitelji  trgovali s Ilirima u unutrašnjosti, prodavajući im oružje, posuđe, nakit i odjeću. Dobar strateški i komunikacijski položaj Narone uvidjeli su i Rimljani, koji su blizu nje podigli vojni tabor (možda u Mogorjelu kod Čapljine ?) za ratovanje protiv Ilira. Narona je vjerojatno za cara Augusta postala kolonija (Colonia Iulia Narona) i upravno središte (conventus Naronitanus). Devedesetih godina 20. st. u središtu Vida otkopani  su ostaci hrama na glavnome trgu (Augusteum), u kojemu je pronađeno 16 kipova bogova i božica, svi bez glava – kršćanska osveta, među kojima se ističe gotovo tri metra visoki kip divinizirana Augusta u carskoj odori. Kako je Narona bila biskupijsko središte, u njoj je pronađeno više starokršćanskih bazilika, od čega je vrijedna spomena dobro očuvana krstionica u bazilici na mjestu današnje crkve Sv. Vida.
+U ranom srednjem vijeku Poneretavlje su naselila slavenska i hrvatska plemena. Od Cetine do Neretve uzdiže se čuvena Paganija, zemlja nekrštenih gusara, kako nas u  10. st. izvješćuje bizantski car Konstantin Porfirogenet. Mlečani su jedno vrijeme plaćali Neretvanima danak za slobodnu plovidbu uz njihovu obalu. Vjeruje se da je hrvatski knez Domagoj podrijetlom bio Neretvanin.  Mletački kroničar zove ga "pessimus dux Slavorum". U 14. st. u dolinu Neretve spustili su se bosanski vladari, ponajprije Stjepan II. Kotromanić, pa kralj Tvrtko, pa herceg Stjepan Vukčić Kosača, pa knezovi Radivojevići-Jurjevići-Vlatkovići... Na puk smjerni nalegoše krajem 15. st. Turci. I danas blizu Metkovića nauzgor stoji moćna Norinska kula, o kojoj pjeva Andrija Kačić Miošić.
+Ulogu Narone preuzela je luka Drijeva, vjerojatno na desnoj obali Neretve blizu današnje Gabele. Drijeva su bila veliko trgovište svakojake robe, od sukna i voska do soli i začina, ali i robova. Često se spominje u zapisima dubrovačkih notara. Blizu Drijeva na povijesnu pozornicu u 15. st.  stupa i Metković, doduše kao maleno naselje bez velika značenja. Vjerojatno su njegov rast usporili Turci koji osvajaju Poneretavlje. Za njihove vlasti (1494. – 1685.) Metković se  ne spominje. Na zemljovidu prvi ga je zabilježio mletački kartograf Jacopo Gastaldi 1570. Glavna uloga bila je namijenjena susjednoj Gabeli, te Opuzenu i Kuli Norinskoj. Ta dva stoljeća ispunjena su čestim sukobima Turaka i Mlečana. Požarevačkim mirom 1718. utvrđena je granica između Turske carevine i Mletačke Republike (vidi dolje zemljovid iz 1787.).
+Mlečani su minirali i napustili Gabelu i osnovali neretvansku luku u Metkoviću na predjelu Unka. Metković se našao u kotaru Neretva, na čijem se čelu nalazio nadintendant sa sjedištem u Opuzenu. Naselje se polagano razvijalo, postajući središte poljodjelstva, stočarstva, lova i ribolova. Sredinom 18. st. Metković je imao oko četiristo duša. Nakon propasti Mletačke Republike za kratkotrajne francuske uprave došlo je do gradnje tzv. Napoleonove ceste (u narodu zvane francuskom i Marmontovom), čime je poraslo strateško i trgovačko značenje Metkovića. Upravo u to doba 1812. postao je općinsko središte za naselja na lijevoj obali Neretve. Ipak, istinski razvoj Metkovića otpočinje za vrijeme druge austrijske uprave. Lučki ured utemeljen je 1823. kao prva državna ustanova, a 1849. otvara se i poštanski ured. Izgradnjom cesta Mostar – Metković i Mostar – Sarajevo, Metković, čije pučanstvo je naraslo preko tisuću, postaje trgovačko i lučko naselje s razvijenim obrtom i ugostiteljstvom. Grad se širi od podnožja brda Predolca prema riječnoj dolini. Novosagrađena cesta postala je istodobno glavna gradska ulica.
+Val novih političkih promjena nakon autonomaša 1870. doveo je na vlast u Metkoviću narodnjake. Buđenju hrvatske nacionalne svijesti pomoglo je utemeljenje Hrvatske narodne čitaonice, koja će postati stožerom kulturne preobrazbe. U gradu se otvaraju zadruge, bankarske, brodarske  i osiguravateljske ispostave. Nakon okupacije Bosne i Hercegovine 1878. razvoj Metkovića postao je još brži. Obavlja se meliorizacija neretvanskih močvara i regulacija rijeke za sigurniju plovidbu. Nakon puštanja željezničke pruge Metković – Mostar, pa Mostar – Sarajevo, sagrađen je i 1895. željeznički most. Grad se širi i na desnoj obali Neretve. 
+U Prvom svjetskom ratu i nakon njega gospodarski zamah u Poneretavlju donekle stagnira. Ipak, metkovska luka postaje značajnim trgovinskim središtem (po prometu odmah nakon Sušaka). Prema popisu pučanstva 1931. Metković je imao gotovo tri tisuće žitelja. Širi se trgovački i ugostiteljski obrt, djeluje Gradska glazba, grad ima dvije kinodvorane, hotel "Zagreb", gradski park, Turističko društvo, carinarnice, duhansku, veterinarsku i zdravstvenu stanicu, pučku i građansku školu i mnoge upravne zgrade. Šaputa se i o postojanju nekoliko javnih kuća, što nije neobično s obzirom na jaki lučki promet.
+U Drugome svjetskom ratu Metković su više puta bombardirali saveznički zrakoplovi, pa je kraj rata dočekao u ruševnu stanju. U doba FNRJ i SFRJ Metković je postupno napredovao na gospodarskom, kulturnom, prosvjetnom i športskom planu, dok je imao poteškoća u razvoju političke demokracije. Godine 1971. Matica hrvatska bila je nositelj hrvatskoga političkog proljeća, koje je ugušeno policijskom presijom, pritiscima i zatvorskim kaznama glavnih članova. U velikosrpskoj agresiji na Hrvatsku Metković je 1991. – 1992. bio više puta bombardiran iz zrakoplova i topničkoga oružja. Glavne borbe za oslobođenje Jadrana i Južne Hrvatske iznijeli su pripadnici 116. brigade Hrvatske vojske. U zadnjem desetljeću nakon uspostave samostalne Republike Hrvatske  Metković nastavlja svoj urbani rast.</t>
+  </si>
+  <si>
+    <t>43.05</t>
+  </si>
+  <si>
+    <t>17.65</t>
+  </si>
+  <si>
+    <t>Imotski</t>
+  </si>
+  <si>
+    <t>21260 Imotski</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>Imotski je stari povijesni grad čije prvo spominjanje datira u 10. st. Nastao je na temeljima starohrvatske župe Emothe kao središte šire regije zvane Imotska krajina, koja se prostire na površini od 626 km2. Kroz mnoga stoljeća Imotski je njezino privredno, upravno i kulturno središte. Danas broji nešto više od 10.000 stanovnika. Klima je mediteransko-kontinentalna, ugodna za življenje.
+Stara gradska jezgra građena je klesanim kamenom, zbog čega Imotski mnogi smatraju jednim od najljepših dalmatinskih gradića. Nad gradom se nadvisuje staro hrvatska utvrda Topana sa zavjetnom crkvicom Gospe od Anđela iz 18. stoljeća. Gradsko područje obuhvaća i naselja Vinjani, Glavina i Medvidovića Draga. Svojim zapadnim rubom grad doslovce obuhvaća Modro jezero. Na udaljenosti od samo 1km u smjeru sjeverozapada nalazi se nadaleko poznato Crveno jezero, koje spada među najdublja u Europi. Zbog dojmljivosti i dramatičnosti Modrog i Crvenog jezera, oko njih su se isplele mnoge legende i vilinske priče koje su se pretvorile u dragocjeno etnološko nasljeđe. Osim ova dva jezera, uokolo se nalaze mnoge bezvodne vrtače nastale na mjestima negdašnjih jezera. Smatra se da je u ovom kraju nastala i narodna balada „Hasanaginica“ koja je prevedena na mnoge jezike i pripada svjetskoj književnoj baštini.
+Povijesni artefakti od prapovijesti do danas čuvaju seu Zavičajnom muzeju i Muzejskoj zbirci Franjevačkog samostana, te svjedoče o dugoj i burnoj prošlosti ovoga područja koje je oduvijek bilo na vjetrometini povijesnih previranja.
+Imotski ima sva obilježja primorskog grada, zahvaljujući ponajviše klimi i urbanoj arhitekturi stare gradske jezgre. Kamene kuće, strme uske ulice s kamenitim stepenicama svjedoci su nekadašnjeg izgleda ovog mjesta čija je stara jezgra i zaštićena. Nekoliko zgrada sa lijepim pročeljima i okovnim ogradama iz doba secesije, govore o stilskim strujanjima koja nisu mimoišla ni ovu sredinu.</t>
+  </si>
+  <si>
+    <t>43.45</t>
+  </si>
+  <si>
+    <t>17.22</t>
+  </si>
+  <si>
+    <t>Ogulin</t>
+  </si>
+  <si>
+    <t>47300 Ogulin</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>Utemeljenje Ogulina vezano je uz ime slavne obitelji Frankopan. Osnivač grada bio je Bernardin Frankopan, jedan od najmoćnijih velikaša svoga vremena. Sagradio je kaštel iznad samog ponora rijeke Dobre i tako postavio stabilne temelje daljnjeg razvoja grada.
+Vrijeme izgradnje ogulinske utvrde nije točno utvrđeno. No, poznata je isprava Bernardina Frankopana, osnivača Ogulina, koju je izdao u svom gradu Modrušu oko 1500-te godine kada je novosagrađenom gradu Ogulinu označio granice između Modruša i Vitunja. Dakle, prvi povijesni spomen o Ogulinu kazuje i njegovo današnje ime.
+Ogulin je već 1553. godine dospio u kraljevske ruke, a nekoliko godina kasnije postaje sjedište 13. kapetanije unutar novog obrambenog sustava tzv. Vojne krajine. Kakvo je Ogulin imao značenje u XV. i XVI. st. , osobito obrambeno, vidi se iz isprava toga vremena u kojima se ogulinska utvrda zove «ključem Kranjske». Stanovnici Ogulina bili su dobri vojnici, o čemu govori podatak da ih je zbog osobne hrabrosti i požrtvovnosti u borbi s Turcima od svake rabote oslobodio Vuk II., Krsto Frankopan Tržački, koji je 3. ožujka 1622. godine izdao povelju kojom ih je za sva vremena oslobodio obveza prema knezovima Frankopanima.
+U XVIII. st. dolazi do većih promjena u društveno-ekonomskom životu u Vojnoj krajini. Tako se na području Karlovačkog generalata osnivaju četiri pukovnije, od kojih je jedna u Ogulinu. Od 1746. godine krajišnici postaju redovna vojska. Ogulin postaje sjedište 3. ogulinske krajiške pješačke pukovnije, a time i štapsko mjesto. Razlog je to da je 1770. godine otvorena Glavna škola s njemačkim nastavnim jezikom za dječake i djevojčice, premda je školstvo do tada bilo u rukama crkvenih ustanova. Godine 1776. osnovana je Njemačka škola sa zadatkom obrazovanja kadrova za potrebe krajiških vlasti.
+Početkom XIX. st. dolazi do francuske okupacije ovog područja. Mirom, koji je sklopljen između Austrije i Francuske 1809. godine u Beču, ogulinsko područje pripalo je Ilirskim provincijama. Francuska uprava trajala je četiri godine. Potkraj 1813. godine Ogulin ponovno dolazi pod austrijsku upravu. Neprirodna organizacijska struktura Vojne krajine kao posebnog upravno-političkog područja u Hrvatskoj trajala je sve do sredine druge polovice XIX. st. Tek 1881. godine došlo je do razvojačenja i priključenja Vojne krajine Banskoj Hrvatskoj. U drugoj polovici XIX. st. Hrvatska je vezana uz mađarski dio Austro-Ugarske. Od 1873. godine Ogulin postaje središte Ogulinsko-slunjskog okružja. Prilikom reorganizacije županije 1886. godine u Hrvatskoj i Slavoniji osnovano je osam županija. Ogulin je tada središte Modruško-riječke županije, a u sastavu joj je bilo osam upravnih kotara: Ogulin, Slunj, Vojnić, Novi Vinodolski, Sušak, Delnice, Čabar, Vrbovsko i Grad Bakar. Obzirom na veliki priraštaj stanovništva i skromne mogućnosti za život dolazi do iseljavanja stanovništva. Krajem XIX. st. iseljenički valovi upućuju se prema zemljama zapadne Europe i Sjedinjenim Američkim Državama. Izgradnja željezničke pruge Zagreb – Rijeka (1873. godine) pomogla je u to vrijeme zaostalom i zapuštenom Ogulinu u bržem razvoju obrta i trgovine. Nakon Prvog svjetskog rata u novonastaloj Kraljevini SHS, ukinute su u Hrvatskoj i Slavoniji županije i osnovane oblasti, pa je područje nekadašnje Modruško-riječke potpalo pod Krajiško-primorsku oblast sa sjedištem u Karlovcu.
+Godine 1929. država koja je dobila ime Kraljevina Jugoslavija razdijeljena je u devet banovina. Ovom upravnom podjelom, Krajiško-primorska oblast ušla je u sklop Savske banovine. U vrijeme Nezavisne Države Hrvatske postojala je Velika župa Modruš (1941. –1946.), sa sjedištem u Ogulinu. Nakon Drugog svjetskog rata od 1945. – 1990. godine Hrvatska je bila u sklopu FNRJ, odnosno SFRJ. Ogulin je u tom razdoblju bio kotar, a nakon toga općina.
+Godine 1990. došlo je do prvih demokratskih izbora, konstituiranja novog Sabora, donošenja novog Ustava Hrvatske, kojim je određeno upravno-pravno ustrojstvo hrvatske države. Time je ostvarena devetstoljetna težnja hrvatskog naroda za potpunim suverenitetom i slobodom. Narod ovoga kraja dao je veliki doprinos u Domovinskom ratu, braneći svoju Hrvatsku, ponosno i vjerno kao i njegovi preci u prošlosti.</t>
+  </si>
+  <si>
+    <t>45.27</t>
+  </si>
+  <si>
+    <t>15.23</t>
+  </si>
+  <si>
+    <t>Delnice</t>
+  </si>
+  <si>
+    <t>51300 Delnice</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Najstariji povijesni zapisi o Delnicama vezani su uz obitelj Frankopan, njenu organizaciju vlasti i uprave i prema Gorskom kotaru. Delnice se prvi puta spominju u sudskoj ispravi Sabora 24. veljače 1482. godine, izdanoj zagrebačkim trgovcima, u kojoj su govorili da nisu dužni plaćati, u ono vrijeme tridesetnicu preko čijih posjeda putuju.
+Prvo delničko naselje bilo je potpuno čakavsko, smješteno nešto južnije od sadašnjeg lokaliteta u Lučicama. Učestali turski napadi imali su za posljedicu pljačku i spaljivanje goranskih naselja, gdje stradaju i Delnice.
+Nakon izbivanja sa svojih ognjišta, početkom 17. stoljeća obitelj Zrinski naseljava Delnice pučanstvom iz svojih pokupskih imanja Čabra, Broda i Gerova. Zajedno sa njima vraćaju se iz Kranjske potomci starih Delničana. Započinje gradnja novih Delnica ali na drugom mjestu, niže, uz cestu prema Brodu na Kupi, čime se stvaraju osnovni uvjeti za promet roba. U stoljeću obnove osnovana je katolička župa. Nove obitelji donijele su u taj, od starine čakavski kraj, kajkavsko narječje koje od tada čini južnu granicu kajkavskog narječja. Plodna goranska polja uz oživljavanje prometa postupno daju život Delnicama i Gorskom Kotaru. Pučanstvo, nešto kasnije nalazi zaradu u preradi drva.
+Obnova Delnica i cijelog Gorskog kotara zaustavljena je nakon neuspjele urote Zrinskih - Frankopana 1670. Vojska generala J. Herbersteina opljačkala je Gorski kotar, a veliki posjedi Zrinskih dolaze pod upravu Beča. Izgradnja prometnice Karlovac - Bakar - Rijeka, popularne “Karoline” zaobišla je Delnice i ponovo izazvala iseljavanje ljudi. Tek izgradnjom “Lujzijane”, prometnice koja je završena 1811., Delnice ponovno postaju središte ove regije. Intenzivira sa prerada drva, poljodjelstvo i stočarstvo, širi se sitno poduzetništvo, a od druge polovice 19. stoljeća javlja se delnička nošnja.
+Riječka željeznica postupno je vračala život Gorskom kotaru. Dio pučanstva od 1873. nalazi zaposlenje na njenoj trasi od Ogulina do Rijeke. Oživljava poljodjelstvo, stočarstvo i prerada drva. Prva škola u Delnicama utemeljena je 1836. Riječka željeznica nije mogla bitno promijeniti težak život Delničanima pa oni u ovo stoljeće ulaze s nimalo lakim životnim prilikama.
+Grad Delnice je danas sastavni dio Primorsko goranske županije kojoj osnovu gospodarstva čini šumarstvo i drvna industrija. Proizvodnja i prerada drva, ugostiteljstvo, trgovina, turizam i sve intenzivniji razvoj poduzetništva čine osnovu gospodarenja i pravce daljnjeg razvitka.</t>
+  </si>
+  <si>
+    <t>45.40</t>
+  </si>
+  <si>
+    <t>14.80</t>
+  </si>
+  <si>
+    <t>Makarska</t>
+  </si>
+  <si>
+    <t>21300 Makarska</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Makarska je među najstarijim gradovima na hrvatskom dijelu Jadrana. Uz rubove grada, na podnožju masiva planine Biokovo (1762 n/m) život se organizirao još u prapovijesti. Među arheološkim lokalitetima najstarija je pećina Bubnjavača iznad svetišta Vepric, nastanjena u kontinuitetu od 6000. g. pr. Kr. Njeni stanovnici pripadali su mediteranskoj rasi, a ekonomsku osnovicu imali u lovu i ribolovu, te stočarstvu. Zemljano posuđe su ukrašavali rubovima školjaka i predmeta, svojstveno rasprostranjenoj impresso kulturi starijeg neolitika.
+Lokaliteti u podplaninskim zaseocima Makru i Kotišini potvrđuju život u brončanom dobu (2200.-800. pr. Kr.). Stanovništvo se pokapalo u kamenim tumulima, brojnim na širem podplaninskom pojasu. U tom razdoblju dolazi do migracija Indoeuropljana na širi prostor današnje Europe. Ratne aktivnosti, potraga za rudama i jačanje trgovine, potakle su organiziranje života na uzdignutim utvrđenim gradinama. Ostaci takve utvrde, s koje se nadzirao prostrani kopneni i morski prostor, sačuvani su na makarskom poluotoku Sv. Petar. Arheološka istraživanja potvrdila su da je njegova zaravan bila nastanjena od sredine 3. tisućljeća pr. Kr. Naselje se oko 1200. g. pr. Kr. razvija kao fenička kolonija Mukron. Dolazak Feničana s istočnog Sredozemlja potaknut je izlovom morskih puževa grimizara, od čijih su žlijezda izrađivali skupocjenu boju. Tadašnju prethodnicu Makarske naznačava i nalaz keftiu ingota, sirova bronce u izgledu minijaturne volovske kože. U europskoj se znanosti još od 1906. vezuje za Makarsku kao dokaz kontakata s egejskim prostorom.
+U osvitu antičkog razdoblja Ardijejci, domorodačko ilirsko stanovništvo, ima trgovačke dodire s Grcima na susjednim otocima Hvaru i Visu. Dokazuju ih luksuzna helenistička keramika (3.-1. st. pr. Kr.) pronađena na Sv. Petru. Država Ardijejaca propada  135 g. pr. Kr. u ratu s civilizacijski naprednijim Rimljanima. 
+Utvrđeno ilirsko naselje na Sv. Petru u prvim stoljećima stabilne rimske vladavine gubi na važnosti. Grad se od 1. st. razvija u podnožju, na mjestu današnje Makarske. Ispočetka je imao status municipija, naselja s lokalnom samoupravom romaniziranog ilirskog stanovništva. Prema ostacima gradnji i brojnim nekropolama evidentiranih na dosta širokom pojasu, naselje je imalo razvedeni ili policentričan izgled. Vrhunac je imao tijekom kasne antike i razvojem kršćanstva, a 533. na koncilu u Saloni dodijeljen mu je status biskupije. Tada se u pisanom izvoru i spominje kao Muccurum. Uvjerljivo je tumačenje feničkog podrijetla naziva Muccurum, jer označava trgovište (makar) ili izvor (maqor) što karakterizira ovo naselje s lukom.    
+U trenutku najvećeg razvoja rimskoga grada započeo je bizantsko-gotski rat (535.-555.), osobito žestok na Jadranu. U vojnom planu cara Justinijana, branitelja pravovjernog kršćanstva nad arijanskim Gotima, reaktivirane su ranije utvrde s izvrsnim položajem za nadziranje kopnenih i pomorskih puteva. Stoga se i na Sv. Petar u Makarskoj podiže velika utvrda, čiji su prostrani ostaci arhitekture arheološki istraženi proteklih godina. Utvrda je prihvatila odbranu antičkog naselja u podnožju i bila pribježištem stanovništvu, a gradnjom crkve zadobila je i sakralni značaj. Iako historiografija osloncem na povjesničara Prokopija iz Cezareje navodi kako je Muccurum u ovome ratu 548. g. bio razoren, arheološki nalazi na Sv. Petru ipak upućuju na kontinuitet grada.  
+Makarska, kao Mucru, navodi se polovinom 7. st. u djelu Cosmographia kao važnije obalno naselje. Tijekom starohrvatskog razdoblja sa svojim Primorjem, poznatim pod nazivom Krajina, Paganija ili Neretvanska oblast, nalazi se u sklopu Južne ili Crvene Hrvatske. U izvoru 9. st. navodi se kao Mucules. Tada je, u vrijeme hrvatskog kneza Branimira (879.-892.), mletačka mornarica doživjela 18. IX. 887. g. težak poraz od strane Neretvana. U bitci koja se dogodila uz obalu Makarske, ili podno planine na mjestu zvanom Mucules, kako navodi pisani izvor, poginuo je dužd Petar Candiano. Stoga su duže vrijeme Mlečani hrvatskim vladarima i neretvanskim knezovima plaćali za nesmetanu plovidbu Jadranom. Republika Hrvatska datum ove pobjede slavi kao Dan hrvatske ratne mornarice.   
+Makarska se kao grad-utvrda to Mokron navodi i sredinom 10. st. u djelu De administrando imperio bizantskog cara Konstantina Porfirogeneta. Utvrda se odnosi na Sv. Petar, dok se naselje kao i u antičkom razdoblju nalazilo na mjestu današnjeg grada.
+Makarska se češće spominje u 14. i 15. st. u vrijeme plemstva Kačića. Pod vrhovnom je vlašću bosanskih banova i hrvatskih regionalnih gospodara, a potom moćnih hercegovačkih vladara iz obitelji Kosača. Važnost Makarske ogleda se u nastojanjima Venecije da je pridobije pod svoju upravu, i od koje se očekuje obnova utvrde. Važnost grada iskazuje i dolazak franjevaca, koji do 1468. na njegovom istočnom prilazu imaju samostan i crkvu Sv. Marije. Crkva je do danas sačuvala jednobrodni izgled i pravokutnu apsidu. Na zaravni poluotoka sv. Petar nalazio se kraće vrijeme pustinjački samostan augustinaca koji napuštaju krajem 15. st. 
+Herceg Stjepan Kosača predao je 1466. upravu nad Makarskom i Krajinom Veneciji. Međutim, njena je vlast bila kratkog vijeka jer su grad, najkasnije 1499., osvojile Osmanlije.
+Makarska je od kraja 15. st. do 1684. uglavnom pod vlašću Osmanlija. Grad koriste za lučku trgovinu i promet usmjeren unutrašnjošću. Kao granični grad često je napadan s mletačke, ali i osmanske strane, ovisno tko ga je držao pod kontrolom. U vrijeme Ciparskog rata (1570.-1573.) osobito je stradao franjevački samostan i crkva. Borbe je prikazao mletački kartograf G. F. Camocijo 1572. na crtežu Makarske utvrđene osmanskim zidinama i ojačane trima kulama. Podigao ih je 1568. graditelj Hajrudin, nakon što je sagradio most u Mostaru. Zidine su srušili Mlečani početkom Kandijskog rata (1646.-1669.), prilikom zauzimanja Makarske, kada su je i zapalili. Sačuvano je tek prizemlje južne kule na Marineti, dok je eminova kula porušena u 19. st. Stoga se 1703. izričito veli kako Makarska nema zidina i utvrda. Mlečani su 1647. poduzeli gradnju i danas sačuvanog obrambenog zida na Sv. Petru. Kulica na Zelenki, zazidane pećinice u Velikom Brdu, Makru, te Veliki kaštel u Kotišini pripadaju istom vremenskom sloju utvrđivanja ponegdje potpomognutog privremenom mletačkom upravom.
+Makarska je kraj osmanske vlasti dočekala kao siromašan i opustio gradić. Za 1695. g. navodi joj se svega 171 stanovnik, čiji broj već 1703. iznosi oko 1000. Pod vlašću Venecije (1684.-1797.) grad dobiva prepoznatljive urbanističke i barokne arhitektonske obrise stare jezgre koje je sačuvao do danas. Dolazi do procvata likovne, književne i glazbene umjetnosti okrenute Zapadu. Barokna katedrala sv. Marka i sv. Jeronima podiže se 1700.-1758. inicijativom biskupa Nikole Bijankovića (1695.-1730.) i prema nacrtima vodećih mletačkih vojnih inženjera (G. de Varanneo, G. D' Andrea, F. Melchiori, B. Riviera). Njena unutrašnjost iskazuje inventivnost venecijanskog baroknog stila pojačana reprezentativnim glavnim oltarom kipara P. Onighe. U njoj je i oltar zaštitnika grada Sv. Klementa, čije je tijelo prenijeto iz Rima 1725.
+Istovremeno se na zakošenom terenu oblikuje i Gradski trg uz katedralu te podižu barokne palače Karalipeo Mrkušić i Babić-Lozina. Gradi se 1755. česma s najstarijim kamenim grbom Makarske i grbom providura A. Balbija. U središtu trga postavljen je 1767. štandarac s reljefom Sv. Marka za zastavu Mletačke Republike. 
+Od trga prema zapadu formira se Kalalarga, komunikacija na koju se okomito vezuju uličice. U njoj se grade kamene palače Alačević, Miličić, Vuković i dr. u stilu dalmatinskog baroka, prepoznatljivog po utjecaju dubrovačke i mletačke rezidencijalne arhitekture. Na istočnom rubu grada, uz vrtove samostana i morsko žalo, obitelj Ivanišević gradi palaču s trijemom i galerijom s koje se pružao pogled na more. Na suprotnoj strani obale i obitelj Ivičević od 1773. podiže ladanjski kompleks, poznatiji kao palača Tonoli. Zajedno s palačama u staroj jezgri među najljepšim su primjerima stambene barokne arhitekture 18. st. u Dalmaciji, čija je brojnost i karakteristična za Makarsku.  
+Na obali je dovršena 1758. samostanska crkva sv. Filipa Nerija, iznimna u jedinstvenosti baroknih svodova, prozora i bočnih oltara. Franjevačkoj crkvi pridodana je 1694. kapela Sv. Ante Padovanskog i 1705. oltar u njoj. Slike u njoj, monumentalni Posljednji sud Antonia Molinarija iz 1680.-1681., te oltarni poliptih Uznesenja Marijina flamanskog slikara Pietra de Costera iz 1680., predstavljaju vrhunska slikarska ostvarenja. Franjevci podižu 1712.-1715. najveći i najljepši makarski zvonik, rastvorenih bifora na gornjim katovima i ljudskim glavama u središtu lukova, djelo protomajstora Andrije Ruspinija i Vicka Paniga. Dovršen je i četverokrilni klaustar za molitvu i meditaciju redovnika. Na poluotoku Sv. Petar obnavlja se crkva u baroknim oblicima, a u zaseocima iznad grada podižu nove crkve. U Velikom Brdu gradi se župna crkva sv. Jeronima (1716.-1745.), dok se u Kotišini proširuje crkva sv. Ante i podiže crkva sv. Andrije. Crkva sv. Ivana u Makru podignuta je 1854. na ostacima ranije crkve iz 16.-17. st. O tome govori latiničko-bosanički natpis uzidan u njezino pročelje, najraniji dokaz književnog rada na hrvatskome jeziku u Makarskom primorju.
+Nakon pada Mletačke republike 1797. predstavnici Makarske i lokalna skupština podržavali su vlast Austrije u nadi za sjedinjenje s kontinentalnom Hrvatskom. Priključenje Austriji iste je godine proglasio u makarskoj katedrali general Matija Rukavina. Međutim, njena vlast je bila kratkotrajna, jer već 1806. Makarsku zauzima francuska vojska.  Pobune i nemire izazvane nezadovoljstvom stanovništva francuskom upravom u gradu i Primorju strogo je kažnjavao vojni zapovjednik Dalmacije general Auguste Marmont. Zamisli nove vlasti o poboljšanju javnog života teško su bile provodive u ratnim okolnostima. U francusko-ruskom sukobu sredinom 1807. Makarska je višednevno bombardirana od strane ruskog brodovlja. Jedan je očevidac navodi kako je uništavanje grada bilo nerazborito i s namjerom da mu se nanese što veća šteta. Posljedice ovih stradavanja bile su vidljive iz opisa Makarske od strane austrijskih pisaca još sredinom 19. st.  
+Kratkotrajna francuska vlast u Makarskoj obilježena je monumentalnim spomenikom francuskoj vojsci u obliku kamene piramide. Postavljen je 1809. u Mandraću kod franjevačkog samostana, ali je premješten 1818. izvan zapadnog ulaza u grad. Narod ga je prozvao Napoleonovim spomenikom, kako se i danas naziva. Njegovim premještajem uz cestu nadomak Makarske Austrija je označila početak izgradnje kolne ceste, iako je ona od strane Francuza idejno trasirana i djelomično izvedena na širem području. 
+Na početku dugotrajne i mirnije tzv. Druge austrijske vlasti (1813.-1918.) Dalmacija još uvijek usporena u gospodarskom razvoju. Makarska je uvelike oslonjena na trgovinu solju s turskom Bosnom u zaleđu. Uz to, Makarsko primorje pogodila je u proljeće 1815. velika epidemija kuge. U Makarskoj, koja je tada imala 1575 stanovnika, u tromjesečnoj epidemiji umrlo ih je više od trećine. Do demografskog oporavka u razini stanja prije epidemije dolazi tek sredinom 19. st., te s prirastom stanovništva u idućih desetak godina.
+Makarska je na izborima 1865. pripala stranci Narodnjaka, čime se iskazala usmjerenost nacionalnom preporodu te najavio istaknuti kontinuitet njene političke aktivnosti. Onodobno Općinsko vijeća donjelo je 24. listopada 1865. odluku o uvođenju hrvatskoga jezika u službenu uporabu. Taj datum ujedno predstavlja i Dan grada Makarske.
+Građanstvo je društveno podijeljeno okupljanjem oko buržoaskog, i potom autonomaškog Casina ili, od 1869., narodnjačke Makarsko-primorske čitaonice.  
+Grad se nadopunio javnim i profanim gradnjama u svom odranije ocrtanom opsegu. Njegovu slikovitost naznačile su neostilska Općinska palača iz druge polovice stoljeća prema nacrtu splitskog arhitekta E. Vecchiettija, te Kačić-Pekina i Ivaniševićeva palača iz 1897. na Marineti. Pogledom s mora dominira zgrada Građanske škole iznad trga i katedrale dovršena 1879. g., a započeta gradnjom za biskupsko Sjemenište od strane makarskog biskupa Fabijana Blaškovića (1777.-1819.).
+Izvan istočne strane grada uređuje se gradsko groblje Sv. Križa utemeljeno 1832. Podižu se javni ili gospodarski objekti, poput svjetionika Sv. Petar 1884. Preuređuje se 1869. gradska obala, te 1892. zasađuje drvoredom. Pošumljava se poluotok Sv. Petar na kojemu se probiveni uski putevi. Makarska je 1897. izgradila vodovod po cijelom gradu.
+U kvadratičnom središtu trga niže katedrale postavljen je 1890. brončani kip pjesniku fra Andriji Kačiću Miošiću, djelo Ivana Rendića. Dugo se nalazio unutar hortikulturalne cjeline s fontanom i rubnim alegorijskim figurama. 
+Makarska je 20. stoljeće dočekala kao grad u gospodarskom usponu. Paromlin je otvoren 1901., a tvornice tjestenine i za preradu ribe 1904. i 1905. Morskim je putem bila dobro povezana s Jadranom, a u njenu je luku tjedno uplovljavalo više od 30 parobroda. Na isušenoj močvarnoj prevlaci Sv. Petra u Donjoj luci započeo se oblikovati Općinski vrt, živopisni perivoj s ribnjakom nazvan parkom Franje Josipa I., ali je zapušten u dolazećem vremenu. U Vepricu, zapadno od grada, biskup J. Carić utemeljeno je 1909. svetište Gospe Lurdske, znamenito hodočasničko mjesto. Iste godine Makarsku je posjetio prijestolonasljednik krune F. Ferdinand. Nakon obilaska franjevačkog samostana ponudio je pomoć za obnovu njegovih starijih dijelova. 
+U Prvom svjetskom ratu (1914.-1918.) Makarska nije bila izložena borbama, ali je osjećala tešku oskudicu. Grad je ipak organizirao svekoliku pomoć, medicinsku i opskrbom. Propašću austrougarske monarhije, koja je pod vlašću habsburške monarhije hrvatskim zemljama jamčila cjelokupnost, Makarska se od 1. studenoga 1918. našla u Državi Slovenaca, Hrvata i Srba te je uprava predana u ruke Narodnog vijeća. Stvaranjem Kraljevine Srba, Hrvata i Slovenaca 1. prosinca 1918. Makarska dijeli sudbinu hrvatskih krajeva koji su se našli u okviru nastale državne tvorevine, od 1929. pod nazivom Kraljevine Jugoslavije. 
+U gradu se postepeno razvija turizam i u tu svrhu grade manji kompleksi. Tek su pojedine gradnje iznimna arhitektonska ostvarenja, poput nove franjevačke crkve iz 1938.-1940., podignute prema nacrtu arhitekta S. Podhorskog. U Donjoj luci grade se građanske vile (Irena, Grle, Illeana, Nemčić, Pavlinović i dr.).
+Brzim raspadom Kraljevine Jugoslavije početkom Drugog svjetskog rata u travnju 1941. Makarska je 10. lipnja ušla u sastav Velike župe Cetina unutar novoosnovane Nezavisne države Hrvatske. Njena upravna i vojna vlast umnogome je bila ometana okupacijskim talijanskim snagama sve do kapitulacije Italije u rujnu 1943. U studenome u Makarsku dolazi njemačka vojska što je potaknulo brojna saveznička bombardiranja grada. Nakon odlaska hrvatske i njemačke vojne posade u razorenu Makarsku 20. listopada 1944. ulaze partizani. Završetkom Drugog svjetskog rata u svibnju 1945. Makarska, kao i Republika Hrvatska, u sastavu je nove državne zajednice Federativne Narodne Republike Jugoslavije, od 1963. pod nazivom Socijalistička Federativna Republika Jugoslavija. 
+Slijedom referenduma u kojemu se hrvatski narod opredjelio za samostalnu i neovisnu državu Sabor Republike Hrvatske je 25. lipnja 1991. donio Ustavnu odluku o suverenosti i samostalnosti Republike Hrvatske kojim se uspostavlja kao neovisna država. Sve državnopravne veze s Jugoslavijom raskinute su 8. listopada 1991. u danima započetog Domovinskog rata za ostvarenje proglašene neovisnosti. Makarska je sa svojim Primorjem dala ogroman doprinos pobjedi Hrvatske u Domovinskom ratu nad velikosrpskom agresijom, okončanim u kolovozu 1995. Osnutak 156. makarsko-vrgoračke brigade Hrvatske vojske 21. prosinca 1991., osobito ključne za provedbu vojnih akcija u dolini Neretve i na Dubrovačkom području, bio je rezultat ustrojenih postrojbi u gradu još polovinom godine. 
+Makarska je poznata u svijetu po svojoj kulturnoj baštini, osobito naslijeđu franjevačkog samostana. Osim svoje arhitekture i umjetnina znamenita je samostanska knjižnica, formirana je od 15. st. Među oko 100.000 svezaka čuva i 24 inkunabule ili knjige tiskane u 15. st. Bogata knjižna ostavština, izdavačka djelatnost te arhivska građa, među kojom je i 369 osmanskih isprava pisanih arabicom, dijelom je nasljeđe Filozofskog učilišta franjevaca u Makarskoj od 1708., te Visoke bogoslovije od 1736. s kontinuitetom sve do 1999. Monumentalni mozaik Krista Svevladara s prikazom hrvatskih svetaca u svetištu nove crkve franjevaca izradio je 1999. priznati hrvatski umjetnik J. Biffel. Malakološki muzej u samostanu utemeljen je 1963., Institut Planina i more 1979., dok je Botanički vrt u Kotišini osnovan 1984. također zaslugom fra J. Radića.
+Današnju Makarsku, kao priznatu turističku destinaciju, predstavljaju i ostvarenja suvremenih arhitekata poput A. Rožića. Spomenici zaslužnim osobama i razdobljima postavljaju se kao memorijalni akcenti u urbanistički zacrtanom prostoru. Spomenik revolucije, djelo M Salaja, podignut je 1974. na Glavici. Prvom predsjedniku samostalne Hrvatske dr. F. Tuđmanu spomenik je 2004. izradio K. Hraste, dok je iste godine postavljen spomenik hrvatskim braniteljima K. Kovačića. Česme na Trgu 156. brigade Hrvatske vojske i na Trakačama postavio je 2004. Grad Makarska. Skulpturu sv. Petra, na istočnoj strani poluotoka kojemu je titularom, izradio je 2009. T. Kršnjavi. Spomenik fra Anti Antiću P. Barišića podiže se 2005. uz crkvu u Velikom Brdu, a u Kotišini se uređuje Spomen-dom o. P. Perice. Današnji izgled gradskog groblja s brojnim neostilskim spomenicima iz druge polovine 19. st. rezultat je uređenja 2004. unutar hortikulture. 
+U Makarskoj djeluju Gradski muzej, Gradska galerija Antun Gojak i Gradska knjižnica (čiji je osnivač Grad), Ogranak Matice hrvatske te druge kulturne i sportske udruge . Među njima je osobito poznat HRNK Zmaj osnovan 1921. 
+Nastojanje Grada Makarske ka obnovi svoje povijesne i arhitektonske baštine prepoznatljivo je u dovršenom projektu Revitalizacija kulturno-povijesne baštine zaseoka Kotišina, ostvarenom uz pomoć sredstava iz fondova EU, kao i skorašnjoj izradi arheološkog parka na Sv. Petru s konzerviranim rimskim ostacima kao najstarije arhitekture u gradu.</t>
+  </si>
+  <si>
+    <t>43.29</t>
+  </si>
+  <si>
+    <t>Slatina</t>
+  </si>
+  <si>
+    <t>33520 Slatina</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>Slatina i slatinski kraj naseljavani su od najstarijih vremena što potvrđuju i arheološka nalazišta u slatinskoj okolici (Zvonimirovo, Nova Bukovica, Voćin, čađavica, Macute, Sladojevci, Slatina). Kontinuitet naseljavanja potvrđuje poznata rimska karta iz 3. st. n.e., na kojoj se u vrijeme rimskog vladanja Panonije na slatinskom području spominje naselje Marinianis.
+U pisanom se dokumentu grad Slatina spominje po prvi put u ispravi zagrebačkog biskupa Mihovila izdanoj 1. rujna 1297. godine u Požegi. Ime grada napisano je u inačici Zalathnuk. Slatina je u to vrijeme bila dobro Zagrebačke biskupije u sastavu Arhiđakonata Vaška. U 14. je stoljeću u Slatini bila župna crkva Svih Svetih, smještena negdje oko današnjeg parka. Crkva je imala pokrajne oltare posvećene sv. Juraju, Blaženoj Djevici Mariji, sv. Katarini, kapele posvećene Blaženoj Djevici Mariji i Jeleni i jedan oltar posvećen nekoj bratovštini. Po uvođenju županijskog uređenja Slatina je pripala Križevačkoj županiji.
+U vrijeme feudalizma Slatina je bila biskupijsko trgovište koje je imalo župnu crkvu i drvenu utvrdu – castellum smještenu na uzvišenju uz riječicu Javoricu (nedaleko od današnjeg ulaza u Slatinu- mosta) i koje se razvijalo u maleni srednjevjekovni gradić s podgrađem. Od plemića koji su potjecali ili živjeli u Slatini poznati su vlastelini Slatinski – de Zalatnoky , Georgius Hoberdancz de Zalathnuk, kao i vlastelinski župan Jane de Chanyk, koji je pred kraj 15. stoljeća jedno vrijeme bio čelni čovjek Slatine. Iz toga vremena potječe i prvi gradski grb, s motivom zvijezde Danice i ležećeg nasmijanoga polumjeseca, koji je i danas službeni grb grada Slatine. Poznato je da je već u to vrijeme jedan slatinski đak bio student na sveučilištu u Beču. Pred nadolazećom najezdom Osmanlija Slatina je dodatno pojačala osiguranje i obranu. U borbama s Osmanlijama u Bosni svojom se hrabrošću isticao Ivan Hoberdanc iz Slatine, te ga je kralj Ferdinand 1529. godine bio postavio za krajiškog kapetana i vrhovnog zapovjednika obrane Slavonije. U naletu osmanske vojske, paljenju, rušenju i pljački brojno je domorodačko stanovništvo većim dijelom otišlo sa svojih ognjišta.
+Pod takvim je okolnostima i utvrđeni grad Slatina pao pod osmansku vlast 1544. godine. Jedan manji dio domaćega stanovništva je prihvatio islam i ostao živjeti unutar utvrde, a neznatan broj pridružio se katoličkom stanovništvu koje je nastavilo živjeti u teškim uvjetima u močvarnim predjelima uz Dravu. Nakon okupacije Slatina je pripala Požeškom sandžaku, a u Slatini je stolovao aga, bile su dvije džamije – jedna velika vjerojatno stara župna crkva pretvorena u džamiju i manja, Balijeva podignuta kao zadužbina. Od vjerskih su službenika bili dva imama i hatib, mujezin i kajim. Kako je Slatina bila pogranično područje pojačana je obrana Slatine. Utvrda je bila opasana jarkom i utvrđena drvenim palisadama, a u njoj je bilo stalno smješteno oko 200 vojnika od kojih je veći broj bio konjanika. U graničnom području mir je bio kratkotrajan – tu je haračila turska vojska i uzvraćale su napadima hrvatske čete. Slatinski je kraj oslobođen od turskoga vladanja pred kraj 17. stoljeća. U tim je borbama porušen i stari slatinski grad. Posljednje su borbe s Turcima vođene 1684. godine na području kod šume Turbina, između Slatine i Medinaca, kad se uslijed nadmoćne hrvatske vojske turska posada predala.. Nakon odlaska Turaka Slatina je bila porušena, a ostao je samo toranj stare crkve Svih Svetih. Uspostavljena je vojna uprava na cijelom području.
+Po uspostavi civilnih organa vlasti Slatina je pripala Virovitičkoj županiji i imala je samo oko 50 kućanstava. Narod se bavio tradicijskim uzgojem stoke i obradom zemlje, a u okolnim je selima bila razvijena domaća radinost. Od 1750. godine vlasnik Slatine postao je Marko Aleksandar barun Pejačević. Povijesno gledajući, Slatina svoj prepoznatljivi razvoj u velikoj mjeri zahvaljuje ovoj imućnoj našičkoj plemićkoj obitelji. Danas su još dijelom sačuvani objekti u samom središtu grada koje su Pejačevići podigli kao stambene zgrade, ali i kao neophodne gospodarske objekte, te oko njih zasadili park s egzotičnim stablima, među kojima se i danas ističe mamutovac – sekvoja, kao jedan od simbola Slatine. Na molbu grofa Pejačevića kralj Franjo III proglasio je Slatinu 1808. godine trgovištem, što je doprinijelo povećanju prihoda i daljnjem razvoju mjesta. Slatina je tada prvi put dobila pravo održavanja sajmova na Petrovo, Pavlovo i Nikolinje, po starom kalendaru. Isto pravo kralj je obnovio 1822. godine. Pejačevići su 1822. godine u Sladojevcima potaknuli i gradnju prve škole na slatinskom području, koju su pohađali i učenici iz Slatine. Za vrijeme gotovo stogodišnjeg gospodarenja ovim krajem (1750.-1841.) Pejačevići će ostati zabilježeni kao obitelj koja je učinila značajne pozitivne pomake u životu i napretku cijeloga slatinskog kraja.
+Njemački knezovi Schaumburg –Lippe kupili su 1841. godine slatinsko imanje od Pejačevića. Svojim su dolaskom dodatno ubrzali gospodarski razvoj grada i okolice. U središtu Slatine sagradili su veliki vinski podrum i pecaru alkohola i zasadili su nove nasade vinove loze u okolici. U pecari je, kao sjećanje na prvu slatinsku crkvu, postavljen maleni oltar posvećen sv. Ani i Joakimu. Schaumburg-Lippe je poticao naseljavanje Mađara, Nijemaca i Slovaka u Slavoniju, koji su donijeli u slatinski kraj kulturne običaje europskih gradova. U Slatini su otvarali obrtničke radionice, a pojedini su doselili s ciljem unapređivanja rada prvih industrijskih pogona (pilana je otvorena 1885.), paromlin (1863.), ciglana oko (1890.) ispod današnje željezničke stanice, tvornica pjenušca i sl.), koji su otvoreni u Slatini kao blagi odraz industrijske revolucije toga vremena u Europi. U velikom je podrumu sve do 1912. godine radila tvornica pjenušavog vina – šampanjca. Za svoje vino i pjenušac dobio je Schaumburg-Lippe priznanje na gospodarskim izložbama u Zagrebu i Budimpešti. Pjenušac je proizvodio od vina sorte Kadarka.
+U drugoj polovici 19. stoljeća sagrađene su i prve tvrde cestovne prometnice, a 1885. godine puštena je u promet i prva željeznička pruga – vicinalna pruga od Suhopolja do Slatine, kao ogranak pruge Barč – Pakrac te 1895. pruga Našice – Slatina – Noskovci, gdje je pripojena Slavonsko podravskoj željeznici. Od Noskovaca do dravske obale otvorena je 1901. godine. Novodoseljeni su stanovnici sagradili i nove vjerske objekte, (1858. godine osnovana je Slatinska židovska općina, a sinagoga je sazidana 1884. godine. 1897. godine sagrađena je evangelička crkva u Slatini). Uz većinsko (70%) rimokatoličko stanovništvo i znatan broj pravoslavnih vjernika Slatina je pred kraj 19. stoljeća postala višereligijska sredina. Godine 1870. u Slatini je otvoren ured kotarske oblasti, ali pravi statusni napredak grada obilježava godina 1886. kada je Slatina postala sjedište novoosnovanog Kotara Slatina s tri upravne općine: Slatina, Gornji Miholjac i Voćin. Slatinskom su kotaru 1894. godine dodane još tri nove upravne općine:Nova Bukovica, Drenovac i Sopje.
+Kotarska uprava imala je sjedište u reprezentativnoj zgradi u samom središtu Slatine, koju i danas Slatinčani zovu «Stari kotar», a ponekad, s razlogom, i «Stara škola». U toj je zgradi bila i gradska uprava, pučka škola, prva knjižnica, gruntovnica, općinski sud i sl. Godine 1899. nadozidan je prvi kat istog zdanja za potrebe proširenja prostora za pučku školu. U zgradi je od 1917. godine radila i Viša pučka škola, od 1922.god. Šegrtska škola, od 1924. godine Građanska škola, a nakon drugoga svjetskoga rata bile su tu smještene udruge te osnovna škola sve do 1981. godine.
+Grad je krajem 19. stoljeća imao već mnoge gradske atribute:
+Slatinsku štedionicu (1873.), Narodnu čitaonicu (1896.), Obrtničku zadrugu (1882.) kao prvu profesionalnu udrugu u Slatini, te ostale građanske udruge – Dobrovoljno vatrogasno društvo (1874.), Učiteljsko društvo Kotara slatinskog (1896.), Hrvatsko pjevačko društvo «Zrinski» (1900.), Hrvatski sokol (1907.) Nogometni športski klub «Orao», poštanski ured (oko 1856.), zdravstvene ustanove – ljekarnu «K sv. ćirilu i Metodu» (1874.) Zdravstvena općina Slatina, tj. «Občinska pošastna bolnica Slatina s šest postelja» (1894.), veterinarski kotar (1893.), Hotel Böhm, Hotel Šandl, Hotel Slatina, tiskaru Bauer (oko 1885.) i dr.
+Današnja Slatina izrasla je iz malenog gradića čiji su smjer razvoja postavile plemićke obitelji koje su kroz povijest bile vlasnici slatinskih imanja. Posljednja među njima bila je obitelja grof Ivana Draškovića Trakošćanskog koji su slatinsko imanje 1914. godine kupili od kneza Schaumburg-Lippe. Slatina je u to vrijeme bila središte kotara, u kojem se stalno povečavao broj stanovnika (od 1880. do 1914. broj stanovnika povećan je za 50,42% ili 12000 stanovnika) i koji je postao poznat po dobrim konjima, velikim vinogradima, šumskim površinama punim divljači, domaćem pjenušcu, lovačkim psima i velikom sajmu. Grad je u to vrijeme bio prometno, upravno, gospodarsko i kulturno središte ovoga dijela Hrvatske. Draškovići su bili veliki izvoznici drva, poljoprivrednih proizvoda i stoke. Bili su vlasnici velikih površina zemlje na slatinskom području sve do vremena Drugoga svjetskoga rata, tj. sve do agrarne reforme.
+«Draškovićev dvorac» ili «Vila Margold», sagrađen je kao prvi slatinski mlin na valjke. U njemu je od sredine 19. stoljeća svoj prvi molitveni dom u Slatini imala slatinska židovska zajednica. U ovome su objektu stanovali vlastelinski službenici početkom 20. stoljeća. Nakon toga objekat je imao različite namjene. Tu je bio dječji dom poslije Drugog svjetskoga rata, jedno vrijeme Srednja škola, kao i stanovi za njihove profesore. Nakon obnove krajem osamdesetih godina svoj su prostor sve do 1991. godine tu imali Zavičajni muzej Slatina, Gradsko kazalište «Franjo Sertić Bijeli», Slatinski šahovski klub, a na prvome je katu bila svečana gradska dvorana za vjenčanja.
+Grad Slatina se razvijao na sjecištu važnih prometnica, koje su povezivale europske krajeve sa sjevera i juga i hrvatske istočne i zapadne krajeve. Kroz svoju je dugu pisanu povijest grad nosio svoje staro ime Slatina pisano u više inačica (Saladnah, Slatinaj, Zalathnuk i sl.), a godine 1921. dobio je naziv Podravska Slatina. Grad i njegovi stanovnici su s tim imenom prolazili kroz mnogobrojne borbe i svjedočili su raznim teškim i ljudskim i ratnim borbama i sudbinama kroz Drugi svjetski rat, vrijeme Hrvatskog proljeća, Domovinski rat. Kada je 1991. godine Hrvatska postala samostalna država Slatini je 1992. godine vraćeno njezino staro povijesno ime, a grad je za svoga zaštitnika odabrao sv. Josipa, glavnog patrona svoje župne crkve, čiji dan – 19. ožujka građani Slatine raznolikim programima obilježavaju od tada svake godine.</t>
+  </si>
+  <si>
+    <t>45.70</t>
+  </si>
+  <si>
+    <t>17.71</t>
+  </si>
+  <si>
+    <t>Republika Hrvatska</t>
+  </si>
+  <si>
+    <t>Euro
+(Do 14.1.2023. Hrvatska kuna)</t>
+  </si>
 </sst>
 </file>
 
@@ -1184,7 +1664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1199,6 +1679,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1481,7 +1964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -2413,19 +2896,19 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="106.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="69.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.83203125" customWidth="1"/>
@@ -2446,25 +2929,25 @@
         <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" t="s">
         <v>85</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>89</v>
-      </c>
-      <c r="K1" t="s">
-        <v>91</v>
       </c>
       <c r="L1" t="s">
         <v>22</v>
@@ -2493,7 +2976,7 @@
     </row>
     <row r="2" spans="1:19" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>349</v>
       </c>
       <c r="B2">
         <v>56594</v>
@@ -2502,28 +2985,28 @@
         <v>68.7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="L2">
         <v>2181499</v>
@@ -2559,8 +3042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B507D620-4341-924E-8188-4E502D276425}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="113" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2584,96 +3067,96 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>94</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>95</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>96</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>97</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>98</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
         <v>99</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" t="s">
         <v>100</v>
       </c>
-      <c r="I1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>101</v>
       </c>
-      <c r="K1" t="s">
-        <v>117</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>102</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>103</v>
-      </c>
-      <c r="N1" t="s">
-        <v>104</v>
-      </c>
-      <c r="O1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="J2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2683,10 +3166,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E265F14-DFAD-2341-A15B-FDB6F5CC7122}">
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2707,10 +3190,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>52</v>
@@ -2719,61 +3202,61 @@
         <v>51</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" t="s">
         <v>128</v>
-      </c>
-      <c r="H1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J1" t="s">
-        <v>130</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>141</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="U1" s="4" t="s">
         <v>25</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>26</v>
@@ -2802,22 +3285,22 @@
         <v>641.20000000000005</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K2">
         <v>48266</v>
@@ -2885,22 +3368,22 @@
         <v>47.7</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>238</v>
-      </c>
       <c r="G3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" t="s">
         <v>133</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="I3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J3" t="s">
-        <v>135</v>
       </c>
       <c r="K3">
         <v>5457</v>
@@ -2968,22 +3451,22 @@
         <v>421.4</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="G4" t="s">
-        <v>137</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="I4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K4">
         <v>15738</v>
@@ -3051,22 +3534,22 @@
         <v>401.4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" t="s">
+        <v>149</v>
+      </c>
+      <c r="J5" t="s">
         <v>150</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I5" t="s">
-        <v>151</v>
-      </c>
-      <c r="J5" t="s">
-        <v>152</v>
       </c>
       <c r="K5">
         <v>24865</v>
@@ -3134,22 +3617,22 @@
         <v>59.9</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>155</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="J6" t="s">
         <v>156</v>
-      </c>
-      <c r="I6" t="s">
-        <v>157</v>
-      </c>
-      <c r="J6" t="s">
-        <v>158</v>
       </c>
       <c r="K6">
         <v>11560</v>
@@ -3217,22 +3700,22 @@
         <v>91.8</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="G7" t="s">
-        <v>161</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="I7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K7">
         <v>4554</v>
@@ -3300,22 +3783,22 @@
         <v>187.9</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="G8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="G8" t="s">
-        <v>166</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="I8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K8">
         <v>10128</v>
@@ -3383,22 +3866,22 @@
         <v>43.4</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K9">
         <v>18597</v>
@@ -3466,22 +3949,22 @@
         <v>967.4</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="G10" t="s">
+        <v>173</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="I10" t="s">
         <v>174</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="J10" t="s">
         <v>175</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="I10" t="s">
-        <v>176</v>
-      </c>
-      <c r="J10" t="s">
-        <v>177</v>
       </c>
       <c r="K10">
         <v>32381</v>
@@ -3546,25 +4029,25 @@
         <v>113</v>
       </c>
       <c r="D11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G11" t="s">
         <v>181</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="H11" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="G11" t="s">
-        <v>183</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="I11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K11">
         <v>4869</v>
@@ -3629,25 +4112,25 @@
         <v>167</v>
       </c>
       <c r="D12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G12" t="s">
         <v>186</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="H12" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="G12" t="s">
-        <v>188</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="I12" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K12">
         <v>5191</v>
@@ -3715,22 +4198,22 @@
         <v>54.1</v>
       </c>
       <c r="E13" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="G13" t="s">
+        <v>191</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="G13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="I13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K13">
         <v>4015</v>
@@ -3798,22 +4281,22 @@
         <v>192.4</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="G14" t="s">
+        <v>196</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="G14" t="s">
-        <v>198</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="I14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K14">
         <v>15190</v>
@@ -3881,22 +4364,22 @@
         <v>174.9</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="G15" t="s">
+        <v>201</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="G15" t="s">
-        <v>203</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="I15" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K15">
         <v>20858</v>
@@ -3964,22 +4447,22 @@
         <v>399.5</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G16" t="s">
+        <v>206</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="G16" t="s">
-        <v>208</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="I16" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K16">
         <v>15269</v>
@@ -4047,22 +4530,22 @@
         <v>100.1</v>
       </c>
       <c r="E17" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="G17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="G17" t="s">
-        <v>213</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="I17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J17" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K17">
         <v>8162</v>
@@ -4130,22 +4613,22 @@
         <v>79.400000000000006</v>
       </c>
       <c r="E18" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G18" t="s">
+        <v>216</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="G18" t="s">
-        <v>218</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="I18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K18">
         <v>12417</v>
@@ -4213,22 +4696,22 @@
         <v>139.1</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G19" t="s">
+        <v>220</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>224</v>
-      </c>
       <c r="I19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K19">
         <v>7966</v>
@@ -4296,22 +4779,22 @@
         <v>142.6</v>
       </c>
       <c r="E20" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="G20" t="s">
+        <v>225</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="G20" t="s">
-        <v>227</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="I20" t="s">
-        <v>225</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>191</v>
+        <v>223</v>
+      </c>
+      <c r="J20" s="8">
+        <v>18070</v>
       </c>
       <c r="K20">
         <v>14445</v>
@@ -4379,22 +4862,22 @@
         <v>76.900000000000006</v>
       </c>
       <c r="E21" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G21" t="s">
+        <v>230</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="G21" t="s">
-        <v>232</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>233</v>
-      </c>
       <c r="I21" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J21" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K21">
         <v>5790</v>
@@ -4446,6 +4929,1500 @@
       </c>
       <c r="AA21">
         <v>27122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>256</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
+        <v>187</v>
+      </c>
+      <c r="D22">
+        <v>326.60000000000002</v>
+      </c>
+      <c r="E22" t="s">
+        <v>257</v>
+      </c>
+      <c r="F22" t="s">
+        <v>237</v>
+      </c>
+      <c r="G22" t="s">
+        <v>232</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="I22" s="8">
+        <v>45717</v>
+      </c>
+      <c r="J22" s="8">
+        <v>16075</v>
+      </c>
+      <c r="K22">
+        <v>12534</v>
+      </c>
+      <c r="L22">
+        <v>13822</v>
+      </c>
+      <c r="M22">
+        <v>14716</v>
+      </c>
+      <c r="N22">
+        <v>17056</v>
+      </c>
+      <c r="O22">
+        <v>18998</v>
+      </c>
+      <c r="P22">
+        <v>20840</v>
+      </c>
+      <c r="Q22">
+        <v>20124</v>
+      </c>
+      <c r="R22">
+        <v>22544</v>
+      </c>
+      <c r="S22">
+        <v>23717</v>
+      </c>
+      <c r="T22">
+        <v>24965</v>
+      </c>
+      <c r="U22">
+        <v>25804</v>
+      </c>
+      <c r="V22">
+        <v>28392</v>
+      </c>
+      <c r="W22">
+        <v>47104</v>
+      </c>
+      <c r="X22">
+        <v>56884</v>
+      </c>
+      <c r="Y22">
+        <v>63517</v>
+      </c>
+      <c r="Z22">
+        <v>63517</v>
+      </c>
+      <c r="AA22">
+        <v>61075</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" ht="192" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>259</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="5">
+        <v>971</v>
+      </c>
+      <c r="D23">
+        <v>53.8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>260</v>
+      </c>
+      <c r="F23" t="s">
+        <v>253</v>
+      </c>
+      <c r="G23" t="s">
+        <v>220</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="I23" t="s">
+        <v>262</v>
+      </c>
+      <c r="J23" t="s">
+        <v>263</v>
+      </c>
+      <c r="K23">
+        <v>3628</v>
+      </c>
+      <c r="L23">
+        <v>10601</v>
+      </c>
+      <c r="M23">
+        <v>25390</v>
+      </c>
+      <c r="N23">
+        <v>31498</v>
+      </c>
+      <c r="O23">
+        <v>36143</v>
+      </c>
+      <c r="P23">
+        <v>59498</v>
+      </c>
+      <c r="Q23">
+        <v>38591</v>
+      </c>
+      <c r="R23">
+        <v>44219</v>
+      </c>
+      <c r="S23">
+        <v>20812</v>
+      </c>
+      <c r="T23">
+        <v>28259</v>
+      </c>
+      <c r="U23">
+        <v>37099</v>
+      </c>
+      <c r="V23">
+        <v>47156</v>
+      </c>
+      <c r="W23">
+        <v>56153</v>
+      </c>
+      <c r="X23">
+        <v>62378</v>
+      </c>
+      <c r="Y23">
+        <v>58594</v>
+      </c>
+      <c r="Z23">
+        <v>57460</v>
+      </c>
+      <c r="AA23">
+        <v>52220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>264</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="5">
+        <v>327</v>
+      </c>
+      <c r="D24">
+        <v>94.2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>265</v>
+      </c>
+      <c r="F24" t="s">
+        <v>251</v>
+      </c>
+      <c r="G24" t="s">
+        <v>266</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="I24" t="s">
+        <v>268</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="K24">
+        <v>4493</v>
+      </c>
+      <c r="L24">
+        <v>5773</v>
+      </c>
+      <c r="M24">
+        <v>7315</v>
+      </c>
+      <c r="N24">
+        <v>8123</v>
+      </c>
+      <c r="O24">
+        <v>9832</v>
+      </c>
+      <c r="P24">
+        <v>11670</v>
+      </c>
+      <c r="Q24">
+        <v>12640</v>
+      </c>
+      <c r="R24">
+        <v>16038</v>
+      </c>
+      <c r="S24">
+        <v>18633</v>
+      </c>
+      <c r="T24">
+        <v>20834</v>
+      </c>
+      <c r="U24">
+        <v>25313</v>
+      </c>
+      <c r="V24">
+        <v>31605</v>
+      </c>
+      <c r="W24">
+        <v>35944</v>
+      </c>
+      <c r="X24">
+        <v>38580</v>
+      </c>
+      <c r="Y24">
+        <v>35912</v>
+      </c>
+      <c r="Z24">
+        <v>35312</v>
+      </c>
+      <c r="AA24">
+        <v>30842</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" ht="395" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>270</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5">
+        <v>139</v>
+      </c>
+      <c r="D25">
+        <v>169.2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>271</v>
+      </c>
+      <c r="F25" t="s">
+        <v>249</v>
+      </c>
+      <c r="G25" t="s">
+        <v>272</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="I25" t="s">
+        <v>274</v>
+      </c>
+      <c r="J25" t="s">
+        <v>275</v>
+      </c>
+      <c r="K25">
+        <v>8087</v>
+      </c>
+      <c r="L25">
+        <v>9065</v>
+      </c>
+      <c r="M25">
+        <v>8752</v>
+      </c>
+      <c r="N25">
+        <v>10412</v>
+      </c>
+      <c r="O25">
+        <v>12233</v>
+      </c>
+      <c r="P25">
+        <v>13803</v>
+      </c>
+      <c r="Q25">
+        <v>14215</v>
+      </c>
+      <c r="R25">
+        <v>15602</v>
+      </c>
+      <c r="S25">
+        <v>17432</v>
+      </c>
+      <c r="T25">
+        <v>18381</v>
+      </c>
+      <c r="U25">
+        <v>21507</v>
+      </c>
+      <c r="V25">
+        <v>25251</v>
+      </c>
+      <c r="W25">
+        <v>27304</v>
+      </c>
+      <c r="X25">
+        <v>29493</v>
+      </c>
+      <c r="Y25">
+        <v>30092</v>
+      </c>
+      <c r="Z25">
+        <v>27745</v>
+      </c>
+      <c r="AA25">
+        <v>23577</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="304" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>276</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="5">
+        <v>121</v>
+      </c>
+      <c r="D26">
+        <v>193.4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>277</v>
+      </c>
+      <c r="F26" t="s">
+        <v>252</v>
+      </c>
+      <c r="G26" t="s">
+        <v>216</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="I26" t="s">
+        <v>279</v>
+      </c>
+      <c r="J26" t="s">
+        <v>280</v>
+      </c>
+      <c r="K26">
+        <v>7600</v>
+      </c>
+      <c r="L26">
+        <v>8256</v>
+      </c>
+      <c r="M26">
+        <v>9025</v>
+      </c>
+      <c r="N26">
+        <v>10089</v>
+      </c>
+      <c r="O26">
+        <v>11543</v>
+      </c>
+      <c r="P26">
+        <v>13205</v>
+      </c>
+      <c r="Q26">
+        <v>13770</v>
+      </c>
+      <c r="R26">
+        <v>14829</v>
+      </c>
+      <c r="S26">
+        <v>15526</v>
+      </c>
+      <c r="T26">
+        <v>16864</v>
+      </c>
+      <c r="U26">
+        <v>18687</v>
+      </c>
+      <c r="V26">
+        <v>20598</v>
+      </c>
+      <c r="W26">
+        <v>23849</v>
+      </c>
+      <c r="X26">
+        <v>25985</v>
+      </c>
+      <c r="Y26">
+        <v>25373</v>
+      </c>
+      <c r="Z26">
+        <v>24826</v>
+      </c>
+      <c r="AA26">
+        <v>23452</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" ht="240" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>281</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="5">
+        <v>66</v>
+      </c>
+      <c r="D27">
+        <v>294.8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>282</v>
+      </c>
+      <c r="F27" t="s">
+        <v>238</v>
+      </c>
+      <c r="G27" t="s">
+        <v>283</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="I27" t="s">
+        <v>146</v>
+      </c>
+      <c r="J27" t="s">
+        <v>285</v>
+      </c>
+      <c r="K27">
+        <v>7177</v>
+      </c>
+      <c r="L27">
+        <v>7067</v>
+      </c>
+      <c r="M27">
+        <v>7795</v>
+      </c>
+      <c r="N27">
+        <v>9008</v>
+      </c>
+      <c r="O27">
+        <v>11119</v>
+      </c>
+      <c r="P27">
+        <v>12866</v>
+      </c>
+      <c r="Q27">
+        <v>13380</v>
+      </c>
+      <c r="R27">
+        <v>14991</v>
+      </c>
+      <c r="S27">
+        <v>16597</v>
+      </c>
+      <c r="T27">
+        <v>17242</v>
+      </c>
+      <c r="U27">
+        <v>18804</v>
+      </c>
+      <c r="V27">
+        <v>21128</v>
+      </c>
+      <c r="W27">
+        <v>23202</v>
+      </c>
+      <c r="X27">
+        <v>24829</v>
+      </c>
+      <c r="Y27">
+        <v>24597</v>
+      </c>
+      <c r="Z27">
+        <v>22760</v>
+      </c>
+      <c r="AA27">
+        <v>19601</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>286</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="5">
+        <v>72</v>
+      </c>
+      <c r="D28">
+        <v>264.2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>287</v>
+      </c>
+      <c r="F28" t="s">
+        <v>241</v>
+      </c>
+      <c r="G28" t="s">
+        <v>288</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="I28" s="8">
+        <v>46020</v>
+      </c>
+      <c r="J28" t="s">
+        <v>290</v>
+      </c>
+      <c r="K28">
+        <v>12438</v>
+      </c>
+      <c r="L28">
+        <v>12769</v>
+      </c>
+      <c r="M28">
+        <v>13752</v>
+      </c>
+      <c r="N28">
+        <v>15798</v>
+      </c>
+      <c r="O28">
+        <v>17709</v>
+      </c>
+      <c r="P28">
+        <v>19108</v>
+      </c>
+      <c r="Q28">
+        <v>18319</v>
+      </c>
+      <c r="R28">
+        <v>19230</v>
+      </c>
+      <c r="S28">
+        <v>19729</v>
+      </c>
+      <c r="T28">
+        <v>20575</v>
+      </c>
+      <c r="U28">
+        <v>21793</v>
+      </c>
+      <c r="V28">
+        <v>22534</v>
+      </c>
+      <c r="W28">
+        <v>22772</v>
+      </c>
+      <c r="X28">
+        <v>22676</v>
+      </c>
+      <c r="Y28">
+        <v>22324</v>
+      </c>
+      <c r="Z28">
+        <v>21122</v>
+      </c>
+      <c r="AA28">
+        <v>18949</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" ht="112" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>291</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="5">
+        <v>70</v>
+      </c>
+      <c r="D29">
+        <v>205.2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>292</v>
+      </c>
+      <c r="F29" t="s">
+        <v>249</v>
+      </c>
+      <c r="G29" t="s">
+        <v>293</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="I29" t="s">
+        <v>295</v>
+      </c>
+      <c r="J29" s="8">
+        <v>18100</v>
+      </c>
+      <c r="K29">
+        <v>3076</v>
+      </c>
+      <c r="L29">
+        <v>3746</v>
+      </c>
+      <c r="M29">
+        <v>4035</v>
+      </c>
+      <c r="N29">
+        <v>6259</v>
+      </c>
+      <c r="O29">
+        <v>7992</v>
+      </c>
+      <c r="P29">
+        <v>9238</v>
+      </c>
+      <c r="Q29">
+        <v>9244</v>
+      </c>
+      <c r="R29">
+        <v>10810</v>
+      </c>
+      <c r="S29">
+        <v>12736</v>
+      </c>
+      <c r="T29">
+        <v>13616</v>
+      </c>
+      <c r="U29">
+        <v>14665</v>
+      </c>
+      <c r="V29">
+        <v>15366</v>
+      </c>
+      <c r="W29">
+        <v>15629</v>
+      </c>
+      <c r="X29">
+        <v>17432</v>
+      </c>
+      <c r="Y29">
+        <v>17320</v>
+      </c>
+      <c r="Z29">
+        <v>16224</v>
+      </c>
+      <c r="AA29">
+        <v>14291</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>296</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="5">
+        <v>182</v>
+      </c>
+      <c r="D30">
+        <v>50.2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>297</v>
+      </c>
+      <c r="F30" t="s">
+        <v>251</v>
+      </c>
+      <c r="G30" t="s">
+        <v>298</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="I30" s="8">
+        <v>45070</v>
+      </c>
+      <c r="J30" s="8">
+        <v>18700</v>
+      </c>
+      <c r="K30">
+        <v>3831</v>
+      </c>
+      <c r="L30">
+        <v>4337</v>
+      </c>
+      <c r="M30">
+        <v>4280</v>
+      </c>
+      <c r="N30">
+        <v>5161</v>
+      </c>
+      <c r="O30">
+        <v>5347</v>
+      </c>
+      <c r="P30">
+        <v>5019</v>
+      </c>
+      <c r="Q30">
+        <v>4747</v>
+      </c>
+      <c r="R30">
+        <v>5103</v>
+      </c>
+      <c r="S30">
+        <v>6537</v>
+      </c>
+      <c r="T30">
+        <v>7391</v>
+      </c>
+      <c r="U30">
+        <v>9339</v>
+      </c>
+      <c r="V30">
+        <v>11476</v>
+      </c>
+      <c r="W30">
+        <v>12679</v>
+      </c>
+      <c r="X30">
+        <v>14435</v>
+      </c>
+      <c r="Y30">
+        <v>16383</v>
+      </c>
+      <c r="Z30">
+        <v>12090</v>
+      </c>
+      <c r="AA30">
+        <v>9153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="256" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>300</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="5">
+        <v>156</v>
+      </c>
+      <c r="D31">
+        <v>64.7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>301</v>
+      </c>
+      <c r="F31" t="s">
+        <v>242</v>
+      </c>
+      <c r="G31" t="s">
+        <v>302</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="I31" t="s">
+        <v>304</v>
+      </c>
+      <c r="J31" t="s">
+        <v>305</v>
+      </c>
+      <c r="K31">
+        <v>2278</v>
+      </c>
+      <c r="L31">
+        <v>3467</v>
+      </c>
+      <c r="M31">
+        <v>4017</v>
+      </c>
+      <c r="N31">
+        <v>5031</v>
+      </c>
+      <c r="O31">
+        <v>5881</v>
+      </c>
+      <c r="P31">
+        <v>7215</v>
+      </c>
+      <c r="Q31">
+        <v>7056</v>
+      </c>
+      <c r="R31">
+        <v>8078</v>
+      </c>
+      <c r="S31">
+        <v>9553</v>
+      </c>
+      <c r="T31">
+        <v>10002</v>
+      </c>
+      <c r="U31">
+        <v>11228</v>
+      </c>
+      <c r="V31">
+        <v>12355</v>
+      </c>
+      <c r="W31">
+        <v>13546</v>
+      </c>
+      <c r="X31">
+        <v>14210</v>
+      </c>
+      <c r="Y31">
+        <v>13243</v>
+      </c>
+      <c r="Z31">
+        <v>11633</v>
+      </c>
+      <c r="AA31">
+        <v>10105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>306</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="5">
+        <v>239</v>
+      </c>
+      <c r="D32">
+        <v>48.9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>307</v>
+      </c>
+      <c r="F32" t="s">
+        <v>247</v>
+      </c>
+      <c r="G32" t="s">
+        <v>308</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="J32" t="s">
+        <v>311</v>
+      </c>
+      <c r="K32">
+        <v>3039</v>
+      </c>
+      <c r="L32">
+        <v>3756</v>
+      </c>
+      <c r="M32">
+        <v>4265</v>
+      </c>
+      <c r="N32">
+        <v>4611</v>
+      </c>
+      <c r="O32">
+        <v>5369</v>
+      </c>
+      <c r="P32">
+        <v>6390</v>
+      </c>
+      <c r="Q32">
+        <v>6246</v>
+      </c>
+      <c r="R32">
+        <v>7110</v>
+      </c>
+      <c r="S32">
+        <v>8808</v>
+      </c>
+      <c r="T32">
+        <v>10181</v>
+      </c>
+      <c r="U32">
+        <v>12081</v>
+      </c>
+      <c r="V32">
+        <v>14581</v>
+      </c>
+      <c r="W32">
+        <v>16351</v>
+      </c>
+      <c r="X32">
+        <v>17071</v>
+      </c>
+      <c r="Y32">
+        <v>15833</v>
+      </c>
+      <c r="Z32">
+        <v>14229</v>
+      </c>
+      <c r="AA32">
+        <v>11690</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" ht="272" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>312</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="5">
+        <v>33</v>
+      </c>
+      <c r="D33">
+        <v>6.5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>313</v>
+      </c>
+      <c r="F33" t="s">
+        <v>250</v>
+      </c>
+      <c r="G33" t="s">
+        <v>206</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="I33" s="8">
+        <v>44040</v>
+      </c>
+      <c r="J33" s="8">
+        <v>16200</v>
+      </c>
+      <c r="K33">
+        <v>10637</v>
+      </c>
+      <c r="L33">
+        <v>11284</v>
+      </c>
+      <c r="M33">
+        <v>10660</v>
+      </c>
+      <c r="N33">
+        <v>12294</v>
+      </c>
+      <c r="O33">
+        <v>13179</v>
+      </c>
+      <c r="P33">
+        <v>14621</v>
+      </c>
+      <c r="Q33">
+        <v>13320</v>
+      </c>
+      <c r="R33">
+        <v>15482</v>
+      </c>
+      <c r="S33">
+        <v>17048</v>
+      </c>
+      <c r="T33">
+        <v>18662</v>
+      </c>
+      <c r="U33">
+        <v>20164</v>
+      </c>
+      <c r="V33">
+        <v>20872</v>
+      </c>
+      <c r="W33">
+        <v>21854</v>
+      </c>
+      <c r="X33">
+        <v>23025</v>
+      </c>
+      <c r="Y33">
+        <v>15190</v>
+      </c>
+      <c r="Z33">
+        <v>15407</v>
+      </c>
+      <c r="AA33">
+        <v>11633</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>315</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="5">
+        <v>298</v>
+      </c>
+      <c r="D34">
+        <v>51.2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>316</v>
+      </c>
+      <c r="F34" t="s">
+        <v>254</v>
+      </c>
+      <c r="G34" t="s">
+        <v>225</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="J34" t="s">
+        <v>319</v>
+      </c>
+      <c r="K34">
+        <v>1476</v>
+      </c>
+      <c r="L34">
+        <v>1694</v>
+      </c>
+      <c r="M34">
+        <v>1931</v>
+      </c>
+      <c r="N34">
+        <v>2230</v>
+      </c>
+      <c r="O34">
+        <v>2571</v>
+      </c>
+      <c r="P34">
+        <v>3014</v>
+      </c>
+      <c r="Q34">
+        <v>3271</v>
+      </c>
+      <c r="R34">
+        <v>3941</v>
+      </c>
+      <c r="S34">
+        <v>4658</v>
+      </c>
+      <c r="T34">
+        <v>5301</v>
+      </c>
+      <c r="U34">
+        <v>6358</v>
+      </c>
+      <c r="V34">
+        <v>8810</v>
+      </c>
+      <c r="W34">
+        <v>11097</v>
+      </c>
+      <c r="X34">
+        <v>13370</v>
+      </c>
+      <c r="Y34">
+        <v>15384</v>
+      </c>
+      <c r="Z34">
+        <v>16788</v>
+      </c>
+      <c r="AA34">
+        <v>15235</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" ht="176" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>320</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="5">
+        <v>156</v>
+      </c>
+      <c r="D35">
+        <v>58.5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>321</v>
+      </c>
+      <c r="F35" t="s">
+        <v>252</v>
+      </c>
+      <c r="G35" t="s">
+        <v>322</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="J35" t="s">
+        <v>325</v>
+      </c>
+      <c r="K35">
+        <v>3127</v>
+      </c>
+      <c r="L35">
+        <v>3538</v>
+      </c>
+      <c r="M35">
+        <v>3704</v>
+      </c>
+      <c r="N35">
+        <v>4307</v>
+      </c>
+      <c r="O35">
+        <v>4827</v>
+      </c>
+      <c r="P35">
+        <v>5410</v>
+      </c>
+      <c r="Q35">
+        <v>5693</v>
+      </c>
+      <c r="R35">
+        <v>5911</v>
+      </c>
+      <c r="S35">
+        <v>6879</v>
+      </c>
+      <c r="T35">
+        <v>7147</v>
+      </c>
+      <c r="U35">
+        <v>7362</v>
+      </c>
+      <c r="V35">
+        <v>8084</v>
+      </c>
+      <c r="W35">
+        <v>8911</v>
+      </c>
+      <c r="X35">
+        <v>9935</v>
+      </c>
+      <c r="Y35">
+        <v>10213</v>
+      </c>
+      <c r="Z35">
+        <v>10764</v>
+      </c>
+      <c r="AA35">
+        <v>9153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" ht="335" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>326</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="5">
+        <v>23</v>
+      </c>
+      <c r="D36">
+        <v>538.1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>327</v>
+      </c>
+      <c r="F36" t="s">
+        <v>239</v>
+      </c>
+      <c r="G36" t="s">
+        <v>328</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="J36" t="s">
+        <v>331</v>
+      </c>
+      <c r="K36">
+        <v>12927</v>
+      </c>
+      <c r="L36">
+        <v>14594</v>
+      </c>
+      <c r="M36">
+        <v>16154</v>
+      </c>
+      <c r="N36">
+        <v>18203</v>
+      </c>
+      <c r="O36">
+        <v>19172</v>
+      </c>
+      <c r="P36">
+        <v>19597</v>
+      </c>
+      <c r="Q36">
+        <v>18542</v>
+      </c>
+      <c r="R36">
+        <v>20594</v>
+      </c>
+      <c r="S36">
+        <v>17488</v>
+      </c>
+      <c r="T36">
+        <v>18090</v>
+      </c>
+      <c r="U36">
+        <v>18315</v>
+      </c>
+      <c r="V36">
+        <v>17737</v>
+      </c>
+      <c r="W36">
+        <v>17012</v>
+      </c>
+      <c r="X36">
+        <v>16732</v>
+      </c>
+      <c r="Y36">
+        <v>15054</v>
+      </c>
+      <c r="Z36">
+        <v>13915</v>
+      </c>
+      <c r="AA36">
+        <v>12246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" ht="256" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>332</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="5">
+        <v>22</v>
+      </c>
+      <c r="D37">
+        <v>230.9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>333</v>
+      </c>
+      <c r="F37" t="s">
+        <v>243</v>
+      </c>
+      <c r="G37" t="s">
+        <v>334</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="J37" t="s">
+        <v>337</v>
+      </c>
+      <c r="K37">
+        <v>6929</v>
+      </c>
+      <c r="L37">
+        <v>7289</v>
+      </c>
+      <c r="M37">
+        <v>6797</v>
+      </c>
+      <c r="N37">
+        <v>7007</v>
+      </c>
+      <c r="O37">
+        <v>7172</v>
+      </c>
+      <c r="P37">
+        <v>7651</v>
+      </c>
+      <c r="Q37">
+        <v>7322</v>
+      </c>
+      <c r="R37">
+        <v>7337</v>
+      </c>
+      <c r="S37">
+        <v>6609</v>
+      </c>
+      <c r="T37">
+        <v>7592</v>
+      </c>
+      <c r="U37">
+        <v>7652</v>
+      </c>
+      <c r="V37">
+        <v>7291</v>
+      </c>
+      <c r="W37">
+        <v>6817</v>
+      </c>
+      <c r="X37">
+        <v>6858</v>
+      </c>
+      <c r="Y37">
+        <v>6262</v>
+      </c>
+      <c r="Z37">
+        <v>5952</v>
+      </c>
+      <c r="AA37">
+        <v>5135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>338</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="5">
+        <v>352</v>
+      </c>
+      <c r="D38">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E38" t="s">
+        <v>339</v>
+      </c>
+      <c r="F38" t="s">
+        <v>252</v>
+      </c>
+      <c r="G38" t="s">
+        <v>340</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="J38" s="8">
+        <v>17020</v>
+      </c>
+      <c r="K38">
+        <v>2175</v>
+      </c>
+      <c r="L38">
+        <v>2331</v>
+      </c>
+      <c r="M38">
+        <v>2448</v>
+      </c>
+      <c r="N38">
+        <v>2690</v>
+      </c>
+      <c r="O38">
+        <v>2841</v>
+      </c>
+      <c r="P38">
+        <v>3138</v>
+      </c>
+      <c r="Q38">
+        <v>3138</v>
+      </c>
+      <c r="R38">
+        <v>3272</v>
+      </c>
+      <c r="S38">
+        <v>3242</v>
+      </c>
+      <c r="T38">
+        <v>3497</v>
+      </c>
+      <c r="U38">
+        <v>4550</v>
+      </c>
+      <c r="V38">
+        <v>7121</v>
+      </c>
+      <c r="W38">
+        <v>9556</v>
+      </c>
+      <c r="X38">
+        <v>11958</v>
+      </c>
+      <c r="Y38">
+        <v>13716</v>
+      </c>
+      <c r="Z38">
+        <v>13834</v>
+      </c>
+      <c r="AA38">
+        <v>13301</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>343</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="5">
+        <v>69</v>
+      </c>
+      <c r="D39">
+        <v>167.8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>344</v>
+      </c>
+      <c r="F39" t="s">
+        <v>245</v>
+      </c>
+      <c r="G39" t="s">
+        <v>345</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="J39" t="s">
+        <v>348</v>
+      </c>
+      <c r="K39">
+        <v>5464</v>
+      </c>
+      <c r="L39">
+        <v>6625</v>
+      </c>
+      <c r="M39">
+        <v>6548</v>
+      </c>
+      <c r="N39">
+        <v>8372</v>
+      </c>
+      <c r="O39">
+        <v>9188</v>
+      </c>
+      <c r="P39">
+        <v>10201</v>
+      </c>
+      <c r="Q39">
+        <v>10290</v>
+      </c>
+      <c r="R39">
+        <v>11929</v>
+      </c>
+      <c r="S39">
+        <v>11805</v>
+      </c>
+      <c r="T39">
+        <v>12509</v>
+      </c>
+      <c r="U39">
+        <v>12598</v>
+      </c>
+      <c r="V39">
+        <v>13475</v>
+      </c>
+      <c r="W39">
+        <v>14638</v>
+      </c>
+      <c r="X39">
+        <v>15844</v>
+      </c>
+      <c r="Y39">
+        <v>14819</v>
+      </c>
+      <c r="Z39">
+        <v>13686</v>
+      </c>
+      <c r="AA39">
+        <v>11503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added years for history and new cities.
</commit_message>
<xml_diff>
--- a/Data/Podaci.xlsx
+++ b/Data/Podaci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/domagojrunjak/Documents/Zavrsni rad/zavrsni-rad/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDB7407-F26B-4345-BA54-6FA78CD6A599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8414F799-B812-D145-BE0F-80F85D310919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3100" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-3100" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Županije" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="366">
   <si>
     <t>Naziv županije</t>
   </si>
@@ -333,45 +333,6 @@
 S prosječno 2.600 sunčanih sati u godini jadranska je obala jedna od najsunčanijih u Sredozemlju, a prosječna temperatura mora ljeti je od 25 °C do 27 °C, što Hrvatsku čini turistički atraktivnom lokacijom.</t>
   </si>
   <si>
-    <t>Kameno doba</t>
-  </si>
-  <si>
-    <t>Metalno doba</t>
-  </si>
-  <si>
-    <t>Doba Grka, Ilira i Rimljana</t>
-  </si>
-  <si>
-    <t>Dolazak Hrvata</t>
-  </si>
-  <si>
-    <t>Hrvatsko Kraljevstvo</t>
-  </si>
-  <si>
-    <t>Personalna unija s Ugarskom</t>
-  </si>
-  <si>
-    <t>Ratovi s Osmanlijama</t>
-  </si>
-  <si>
-    <t>Habsburška monarhija</t>
-  </si>
-  <si>
-    <t>Hrvatski narodni preporod</t>
-  </si>
-  <si>
-    <t>Prva Jugoslavija</t>
-  </si>
-  <si>
-    <t>Nezavisna država Hrvatska</t>
-  </si>
-  <si>
-    <t>SFR Jugoslavija</t>
-  </si>
-  <si>
-    <t>Neovisna Hrvatska</t>
-  </si>
-  <si>
     <t xml:space="preserve">Na prostoru Hrvatske je otkriveno pedesetak nalazišta čovjeka kamenog doba. U pećini Šandalja I u blizini Pule pronađeni su najstariji predmeti oblikovani rukom na tlu Hrvatske. Izrađeni su od kamena, a obrađeni okresivanjem. Najvažnije nalazište otkrio je Dragutin Gorjanović-Kramberger 1899. godine u spilji na Hušnjakovom brdu kraj Krapine gdje je našao ostatke neandertalskog čovjeka i njegova oruđa. Nalazišta krapinskog pračovjeka jedno je od najvažnijih u Europi. Živio je oko 130 tisuća godina prije Krista.
 Ljudi mlađeg kamenog doba na prostoru Hrvatske su živjeli u plodnim nizinama rijeka i uz Jadransko more. Prema prostoru najvažnijih nalazišta razlikujemo četiri kulture. Starčevačka kultura se prostirala dijelom sjeverne Hrvatske, a nositelji su ratari i stočari koji su živjeli u sojenicama i proizvodili keramiku koju su bojali crvenom bojom. Sopotska kultura prostirala se na prostoru Slavonije. Danilska kultura se prostirala uz obale Jadrana. Hvarska kultura se prostirala južnim dalmatinskim otocima. Danilska i Hvarska kultura pripadaju krugu impresso keramike koja se odlikuje posudama crveno smeđe boje ukrašenima otiscima školjaka, morskim puževa i zarezima učinjenim oštrim predmetima. </t>
   </si>
@@ -406,18 +367,12 @@
 Jedini dio hrvatskoga prostora koji se samostalno razvijao bila je Dubrovačka Republika koja je s 200 brodova imala jednu od najvećih trgovačkih mornarica u Europi. Isusovac Bartol Kašić piše 1604. godine prvu gramatiku hrvatskog jezika. Isusovci osnivaju 1607. godine gimnaziju u Zagrebu. Kralj Leopold I. dodijelio joj je naslov akademije čime je osnovano Sveučilište u Zagrebu, najstarije sveučilište s neprekinutim djelovanjem u Jugoistočnoj Europi. Najvažniji hrvatski barokni književnik Ivan Gundulić djeluje u Dubrovniku, a povjesničar Ivan Lučić spada u sam vrh europske povijesne znanosti sedamnaestog stoljeća. </t>
   </si>
   <si>
-    <t>Oslobađanje Hrvatske od Osmanlija</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nakon pobjede nad Osmanlijama kod Beča 1683. godine organizira se Sveta liga, savez Habsburške Monarhije, Mletačke Republike i Poljske. Oslobađanje Slavonije organizira franjevac Luka Ibrišimović, a u Lici otpor organizira Marko Mesić. Mirom u Srijemskim Karlovcima 1699. godine velik dio hrvatskog prostora je oslobođen vlasti Osmanlija. Ipak oslobođeni prostor je postao dio Vojne Krajne. Mir u Požarevcu 1718. godine označio je kraj vojne opasnosti od Osmanskog Carstva. Hrvatski sabor 1712. godine prihvaća Pragmatičku sankciju. Provodi se plansko naseljavanje s kojim u Hrvatsku dolaze Nijemci, Česi, Slovaci i Srbi.
 Marija Terezija provodi brojne upravne, porezne i vojne reforme. Osniva se Hrvatsko kraljevsko vijeće 1767. godine, prva moderna vlada. Za vrijeme cara Josipa II. provodi se snažna germanizacija pa se hrvatsko plemstvo okreće suradnji s ugarskim. Na zajedničkom Ugarskom saboru 1790. godine od hrvatske je strane predložena veća financijska ovisnost te podvrgnost Ugarskom kraljevskom vijeću što su Mađari oduševljeno prihvatili. U to vrijeme nastaje ideja o jedinstvenoj mađarskoj nacionalnoj državi od Karpata do Jadrana kao odgovor na germanizaciju Beča u kojoj bi mađarski jezik postao službeni za sve. Hrvatski izaslanici na Saboru odlučno odbijaju uvođenje mađarskog jezika kao službenog. Po prvi puta izbio je spor oko jezika koji će se u sljedećem stoljeću smatrati glavnim obilježjem nacije. Požunskim mirom 1805. godine hrvatska obala dolazi pod francusku vlast te su organizirane Ilirske pokrajine. Na Bečkom kongresu 1815. godine Dalmacija i Istra dolaze pod austrijsku vlast ali nisu sjedinjene s ostatkom Hrvatske. </t>
   </si>
   <si>
     <t xml:space="preserve">Razjedinjenost hrvatskih zemalja pokazao je osnovni cilj hrvatske politike u 19. stoljeću – ujedinjenje hrvatskih krajeva u jedinstvenu cjelinu. Zagrebački biskup Maksimilijan Vrhovac pomaže pretpreporodne napore. Ljudevit Gaj stvara krug građanskih intelektualaca koji postaje jezgra kulturnog i nacionalnog preporoda Hrvatske. Pripadnici tog pokreta nazivaju se ilircima, a pokret se naziva Ilirskim pokretom. Grof Janko Drašković piše Disertaciju, prvi hrvatski politički program. U Zagrebu 1835. godine počinju izlaziti Novine horvatske. Objavljena je pjesma Horvatska domovina Antuna Mihanovića koja će poslije postati hrvatska himna. Matica ilirska osnovana je 1842. godine. Ivan Kukuljević Sakcinski održava 1843. godine u Hrvatskom saboru prvi zastupnički govor na hrvatskom jeziku. Srpanjske žrtve svečano su pokopane 1845. godine. Hrvatski sabor jednoglasno je 1847. godine proglasio hrvatski jezik službenim.
 Revolucionarne 1848. godine formulirana su Zahtijevanja naroda. Hrvatskim banom postaje Josip Jelačić. U Hrvatskoj je 25. travnja 1848. godine ukinuto kmetstvo. Osnovano je Bansko vijeće te je sazvan prvi zastupnički Sabor u hrvatskoj povijesti. Jelačić je s hrvatskom vojskom prešao Dravu i zaratio s Mađarima. Nakon revolucije 1849. godine Franjo Josip proglašava oktroirani Ustav. Započeta je snažna germanizacija. Na Saboru 1861. godine grupiraju se političke stranke: Narodna stranka, Stranka prava i Unionistička stranka. </t>
-  </si>
-  <si>
-    <t>Hrvatsko-ugarska nagodba</t>
   </si>
   <si>
     <t xml:space="preserve">Hrvatsko-ugarska nagodba sklopljena je 1868. godine kojom su uređena zajednička pitanja, a prevagnuli su mađarski interesi. Ugarska je priznala Kraljevini Hrvatskoj položaj političkog naroda i teritorijalnu cjelokupnost. Hrvatska je slala zastupnike u Ugarski sabor te je bila financijski oštećena i podređena Ugarskoj. Riječkom krpicom Rijeka dolazi pod mađarsku vlast. Propala je Kvaternikova Rakovička buna. U ovom razdoblju djeluje Ante Starčević, otac domovine. U Dalmaciji se vodi politička borba narodnjaka i autonomaša. U Istri djeluje Juraj Dobrila. Banom postaje Ivan Mažuranić koji provodi modernizaciju zemlje. Godine 1874. godine utemeljeno je moderno Sveučilište u Zagrebu. Godine 1881. Vojna Krajina je sjedinjena s ostatkom Hrvatske. Dolaskom na vlast bana Khuen-Hédervárya 1883. godine sljedećih dvadeset godina provodi se jaka mađarizacija. Srpska manjina dobiva privilegirani položaj. Održani su veliki protumađarski prosvjedi 1903. godine. </t>
@@ -1617,6 +1572,114 @@
   <si>
     <t>Euro
 (Do 14.1.2023. Hrvatska kuna)</t>
+  </si>
+  <si>
+    <t>Zaprešić</t>
+  </si>
+  <si>
+    <t>10290 Zaprešić</t>
+  </si>
+  <si>
+    <t>O naseljenosti zaprešićkoga kraja još u pretpovijesti svjedoče kamene sjekire iz neolitika nađene u Brdovcu i bakrene sjekire iz eneolitika nađene u Mariji Gorici. Ljudi željeznog doba halštata ostavili su tragove na Sv. Križu, a zanimljivi antički ostaci pronađeni su u Drenju.
+U rimsko doba kroz ovaj je kraj prolazila prometnica Emona (Ljubljana) – Neviodunum – (Drnovo kraj Krškog, do kojeg je tada i Sava bila plovna) – Siscia (Sisak). U Drenju je bio prijelaz preko Save, kojim se lokalna cesta uz Sutlu spajala s državnom cestom Emona – Siscia.
+Nakon dugih stoljeća tišine, novo se srednjovjekovno društvo počinje ustrojavati krajem 11. stoljeća. Tada je Ača, pouzdanik kralja Ladislava, oko 1094. od kralja dobio područja s istočne i zapadne strane Medvednice da bi štitio novoosnovanu biskupiju. Na njezinim zapadnim rubovima počinjao je posjed koji se pružao uz Savu pa sve do Sutle, od kojeg se razvilo susedgradsko-stubičko vlastelinstvo, drugo najveće svjetovno vlastelinstvo u Zagrebačkoj županiji.
+Tijekom 15.-16. stoljeća na vlastelinstvo dalekih Ačinih nasljednika doseljavaju se izbjeglice pred Osmanlijama. Neki od njih bježali su iz Pounja i Like, a potomci su im do sada sačuvali ikavicu. S ovim izbjeglicama došli su i franjevci, za koje je vlastelin Susedgrada Zylagy izgradio samostan u Mariji Gorici. To su isti oni fratri, koji su često, čak i u saborskim spisima, krivo nazivani brdovečki fratri. Tek što su se snašli u novom samostanu, okolicu je uz stalnu osmansku prijetnju, potreslo još jedno krvavo zbivanje. Opterećeni kmetovi na čije učestale žalbe nije bilo odgovora, godine 1573. podigli su najveću seljačku bunu ikada viđenu ne samo u Zagrebačkoj županiji nego i znatno šire. Jedan od njezinih vođa bio je Ilija Gregorić, rođen upravo u Mariji Gorici. Negdje oko 1575. godine počinje osipanje ogromnog vlastelinstva. Heningovci tada svoj dio dijele u pet dijelova, na kojima se kasnije često mijenjaju vlasnici.
+Posjedi se drobe u niz malih vlastelinstava. Posljedica je bila da je u 17. i 18. stoljeću ovdje živio niz sitnih plemića. Podsjetnik na njih brojne su jednostavne kurije, podignute na desecima malih posjeda, a mnoge su ušle i u 20. stoljeće.
+Zahvaljujući dobrom prometnom položaju, ovdje se vrlo rano javlja naselje, koje je već 1334. bilo dovoljno veliko da u njemu bude podignuta župna crkva Sv. Petra. Potvrđeno je to i trasom prve željezničke pruge u Hrvatskoj, koja je prošla ovuda.
+U Zaprešiću je 1920. osnovana Industrija mesnih proizvoda d.d., uz Sljeme i petrinjski Gavrilović, najstarija naša mesna industrija.
+U zaprešićkom kraju sačuvani su neki od najljepših dijelova naše kulturne, povijesne i umjetničke baštine. Posebnu grupu čine dvorci, nastajali tijekom 18. i 19. stoljeća, koji govore o baroknom europskom ukusu svojih naručitelja, a pripadaju među najljepše primjerke u sjeverozapadnoj Hrvatskoj. Prema kategorizaciji povjesničara umjetnosti dva su nulte kategorije (Gornja Bistra, Januševec), prve je kategorije Lužnica, a druge su kategorije Laduč i Novi dvori.</t>
+  </si>
+  <si>
+    <t>45.86</t>
+  </si>
+  <si>
+    <t>15.81</t>
+  </si>
+  <si>
+    <t>Omiš</t>
+  </si>
+  <si>
+    <t>21310 Omiš</t>
+  </si>
+  <si>
+    <t>Materijalni ostaci ljudskog prisustva na širem području Omiša sežu u prapovijest, a brojne gomile i naselja gradinskog tipa na strateški istaknutim položajima Primorske kose i Omiške Dinare svjedoci su guste naseljenosti područja u kasnobrončanom i željeznom dobu, koje povijesni izvori vežu uz razdoblje delmatskih Onastina.
+Povijesno središte Omiša, sudeći po materijalnim ostacima oduvijek je bilo smješteno na istočnoj obali Cetine, gdje nam povijesni izvori potvrđuju postojanje Oneuma, antičkog naselja tijekom 1. stoljeća. Mramorni portret cara Tiberija te natpisi s Tiberijevim i Klaudijevim posvetama ukazuju na monumentalne građevine javnog i religijskog karaktera u dobro utvrđenom Oneumu. Svoje današnje ime Omiš duguje izvedenici iz srednjovjekovnog (Dalmissum, Olmisi), odnosno mletačkog imena Almissa.
+Omišani su kao odlični pomorci kroz povijest nadzirali plovidbu Jadranom te im je, osobito u srednjem vijeku za vladavine Kačića (12. – 13. stoljeće), ubiranje tributa za slobodnu plovidbu bilo jedan od osnovnih oblika privređivanja. Kao samostalni kneževi spominju se Miroslav, Desislav, Brečko, Hodimir i Nikola, koji svoje ugovore ovjeravaju općinskim pečatima sa zidinama i kulama te natpisom Sigilum Comunis Dalmensis. Imali su i vlastite pečate s prikazom srednjovjekovnog viteza na konju.
+Nakon Kačića, neki od istaknutijih gospodara Omiša su bili knezovi Šubići, bosanski velmoža Hrvoje Vukčić Hrvatinić, ban Ivaniš Nelipić, obitelj Matka Talovca koja je gospodarila Omišem pod krunom kralja Žigmunda te bosanski vojvoda Stjepan Kosača. U razvijenom srednjem vijeku i dalje je naglašeno gusarenje i pljačka na moru, a o opasnostima od omiških gusara govori i podatak da dubrovački statut zabranjuje prodaju brodova Omišanima.
+Nakon što je Ladislav Napuljski 1409. g. prodao Dalmaciju Mletačkoj Republici, godine 1444. i Omiš je priznao vlast Mlečana, u čijemu sastavu ostaje do 1797. g. Nakon propasti Venecije, Omiš je pripao Austriji do 1805. g., a od 1805. – 1813. g. francuskoj upravi. Padom Napoleona uslijedila je austrijska upravu do kraja Prvog svjetskog rata. Od 1918. g. pa do kraja Drugog svjetska rata povijest Omiša obilježena je državnim upravama Kraljevine SHS i Kraljevine Jugoslavije, nakon čega je uslijedilo razdoblje SFRJ do osamostaljenja Hrvatske u Domovinskom ratu (1991. – 1995.).</t>
+  </si>
+  <si>
+    <t>43.44</t>
+  </si>
+  <si>
+    <t>16.69</t>
+  </si>
+  <si>
+    <t>Petrinja</t>
+  </si>
+  <si>
+    <t>44250 Petrinja</t>
+  </si>
+  <si>
+    <t>Prošlost grada Petrinje i Banovine kao graničnog područja, ostavila je brojne tragove u spomeničkoj baštini. Od kulturne baštine pod zaštitom najznačajnija je gradska jezgra Petrinje, odnosno niz jednokatnih kuća i javnih građevina koji obrubljuju središnji gradski park, građenih u stilu kasnog baroka i klasicizma. Međutim, uslijed ratnih razaranja te potom neriješenih imovinsko-pravnih odnosa veći dio objekata u gradskoj jezgri zahtjeva kompletnu obnovu. Na današnjoj lokaciji grada, kontinuitet naseljenosti može se pratiti od 1592. godine, kada je na samom ušću Petrinjčice u Kupu izgrađena turska utvrda koja je srušena 1728. godine. Izvan tvrđave već u prvoj polovici 18. st. postoje predgrađa Kaverlin, Majdanci i Kaniža. Druga polovica 18. st., obilježena je gospodarskim poletom i razvojem što je utjecalo na procvat graditeljskih aktivnosti i izgradnju grada u razdoblju od 1788. do 1793. godine. U tom periodu formirane su glavne ulice grada kakav poznajemo danas sa prepoznatljivim primjerima barokne i klasicističke izgradnje.
+Petrinja, stoljećima važno gospodarsko, prosvjetno i kulturno središte Banovine, a danas i cijele Sisačko-moslavačke županije, prema nekim povjesničarima postojalo je već u zadnjim stoljećima opstanka Rimskog Carstva (3. i 4. st. n.e.), a njezin naziv svoj korijen najvjerojatnije vuče ili od latinizirane grčke riječi petrus (kamen) ili pak po crkvi sv. Petra što se na tim prostorima nalazila još od vremena Sisačke biskupije.
+Posebne razvojne okolnosti svrstale su Petrinju među rijetka europska naselja koja služe kao svojevrstan primjer prestanka postojanja već jednom aktivne urbane strukture na izvornoj lokaciji i njezina preseljenja sa starog na novi prostor. Stoga se u geografskom smislu prostorni hod Petrinje u prošlosti razlikuje od povijesno-prostornih iskustava obližnjeg Siska ili primjerice Karlovca, gdje je zadržan kontinuitet povijesnih pravaca kretanja, gdje aktivna urbana masa nije varirala pa je takvo stanje obilježilo njihovu trajnost i stalnost opstojanja u određenom već zadanom lokacijskom prostoru. Na izvornoj i prvoj lokaciji u neposrednoj blizini današnjeg naselja Jabukovca.
+Stara srednjovjekovna Petrinja već je 1240. godine bila poznato i dobro naseljeno mjesto, koje je slavonski herceg Koloman iste godine udijelio povlastice slične onima što ih tada dobivaju i ostali slobodni kraljevski gradovi. Međutim, nakon pada Bosne 1463. godine uslijed osmanlijskih prodora i pustošenja, ponajprije u rubnim dijelovima Habsburške Monarhije, mnoge utvrde i stari gradovi, među kojima je bila i Stara Petrinja, bili su razoreni i napušteni.
+Poslije propasti Austro-Ugarske Monarhije (1918.) i stvaranja nove države Kraljevine Srba, Hrvata i Slovenaca, odnosno Jugoslavije, Petrinja od 1924. godine pripada Karlovačkoj oblasti, a od 1929. Savskoj Banovini. U gradu je djelovalo više dobrotvornih, kulturno-prosvjetnih i vjerskih društava, kao npr. Gospojinsko društvo Dobrotvor od 1904. godine, Ženska udruga za promicanje kućne industrije od 1908. god., Hrvatska žena od 1921. god., Seljačka sloga od 1922. god., Društvo Hrvatica „Katarine grofice Zrinske“ od 1929. god., Klub prijatelja Engleske od 1934. god., Društvo prijatelja Francuske „Cercle Francais“ od 1924. god. i dr.
+Petrinja je još od 19. stoljeća zapažena po svojim mnogobrojnim sportskim društvima. Osim Streljačkog društva utemeljenog 1816. god. tu djeluje Sklizalačko društvo utemeljeno 1881. god., Biciklističko društvo 1891. god., Hrvatski sokol 1906. god., Srpski sokol 1907. god., Nogometni klub Slaven 1910. god., Hrvatski nogometni klub Jelačić 1913. god., Hrvatsko planinarsko društvo Zrin 1922. god., Kuglaški klub Jelačić 1932. god. i sl.
+Prema popisu stanovništva iz 1930. godine Petrinja ima 6137 žitelja. Tijekom i neposredno poslije Drugog svjetskog rata i Petrinja proživljava sve strahote koje rat sa sobom donosi. Unatoč tome što se podosta petrinjskih Hrvata priključuje antifašističkom pokretu 1914.-1945., nestankom Nezavisne države Hrvatske (1945.) i obnovom Druge Jugoslavije, veći dio petrinjskih Hrvata od novih vlasti je progonjen i u mnogočemu sveden na narod drugog reda. Početkom 1963. godine donesen je Statut općine Petrinja u kojem su obuhvaćena 22 sela i naselja. Godine 1981. proveden je popis stanovništva po kojem je općina Petrinja imala 33.570 stanovnika.
+Početkom 1990. godine u Petrinji počinje osnivanje prvih političkih stranaka i početak novog političkog uređenja i demokracije. Prvi nemiri počeli su 28. rujna 1990. kada je grupa naoružanih Srba pozivala na ustanak. Agresija na Banovinu počela je u ljeto 1991. godine. Predsjednik Republike Hrvatske dr. Franjo Tuđman obišao je 25. kolovoza 1991. godine Petrinju i bojište u Peckom. Politički nemiri trajali su do 2. rujna 1991. kada je izveden prvi tenkovski napad na samo središte grada. Od tada pa do 21. rujna vodile su se borbe za Petrinju koja je toga dana pala. Nakon 21. rujna 1991. godine Petrinjci se nalaze u progonstvu, a grad se i dalje razara.</t>
+  </si>
+  <si>
+    <t>45.44</t>
+  </si>
+  <si>
+    <t>16.28</t>
+  </si>
+  <si>
+    <t>Kameno doba</t>
+  </si>
+  <si>
+    <t>Metalno doba</t>
+  </si>
+  <si>
+    <t>Doba Grka, Ilira i Rimljana</t>
+  </si>
+  <si>
+    <t>Dolazak Hrvata</t>
+  </si>
+  <si>
+    <t>Hrvatsko Kraljevstvo</t>
+  </si>
+  <si>
+    <t>Personalna unija s Ugarskom</t>
+  </si>
+  <si>
+    <t>Ratovi s Osmanlijama</t>
+  </si>
+  <si>
+    <t>Habsburška monarhija</t>
+  </si>
+  <si>
+    <t>Oslobađanje Hrvatske od Osmanlija</t>
+  </si>
+  <si>
+    <t>Hrvatski narodni preporod</t>
+  </si>
+  <si>
+    <t>Hrvatsko-ugarska nagodba</t>
+  </si>
+  <si>
+    <t>Prva Jugoslavija</t>
+  </si>
+  <si>
+    <t>Nezavisna država Hrvatska</t>
+  </si>
+  <si>
+    <t>SFR Jugoslavija</t>
+  </si>
+  <si>
+    <t>Neovisna Hrvatska</t>
   </si>
 </sst>
 </file>
@@ -2976,7 +3039,7 @@
     </row>
     <row r="2" spans="1:19" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="B2">
         <v>56594</v>
@@ -2997,7 +3060,7 @@
         <v>83</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>86</v>
@@ -3042,8 +3105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B507D620-4341-924E-8188-4E502D276425}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3059,7 +3122,7 @@
     <col min="9" max="9" width="55.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="48.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="67.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="52.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="82.1640625" bestFit="1" customWidth="1"/>
@@ -3067,96 +3130,96 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>351</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>352</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>353</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>354</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>355</v>
       </c>
       <c r="F1" t="s">
-        <v>96</v>
+        <v>356</v>
       </c>
       <c r="G1" t="s">
-        <v>97</v>
+        <v>357</v>
       </c>
       <c r="H1" t="s">
-        <v>98</v>
+        <v>358</v>
       </c>
       <c r="I1" t="s">
-        <v>112</v>
+        <v>359</v>
       </c>
       <c r="J1" t="s">
-        <v>99</v>
+        <v>360</v>
       </c>
       <c r="K1" t="s">
-        <v>115</v>
+        <v>361</v>
       </c>
       <c r="L1" t="s">
-        <v>100</v>
+        <v>362</v>
       </c>
       <c r="M1" t="s">
-        <v>101</v>
+        <v>363</v>
       </c>
       <c r="N1" t="s">
-        <v>102</v>
+        <v>364</v>
       </c>
       <c r="O1" t="s">
-        <v>103</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3166,10 +3229,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E265F14-DFAD-2341-A15B-FDB6F5CC7122}">
-  <dimension ref="A1:AA39"/>
+  <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView topLeftCell="H1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3190,10 +3253,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>52</v>
@@ -3202,61 +3265,61 @@
         <v>51</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="H1" t="s">
         <v>78</v>
       </c>
       <c r="I1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="J1" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="U1" s="4" t="s">
         <v>25</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>26</v>
@@ -3285,22 +3348,22 @@
         <v>641.20000000000005</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="G2" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="J2" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="K2">
         <v>48266</v>
@@ -3368,22 +3431,22 @@
         <v>47.7</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="G3" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="I3" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="J3" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="K3">
         <v>5457</v>
@@ -3451,22 +3514,22 @@
         <v>421.4</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="G4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="I4" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="J4" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="K4">
         <v>15738</v>
@@ -3534,22 +3597,22 @@
         <v>401.4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="G5" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="I5" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="J5" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="K5">
         <v>24865</v>
@@ -3617,22 +3680,22 @@
         <v>59.9</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="G6" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="I6" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="J6" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="K6">
         <v>11560</v>
@@ -3700,22 +3763,22 @@
         <v>91.8</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="G7" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="I7" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="J7" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="K7">
         <v>4554</v>
@@ -3783,22 +3846,22 @@
         <v>187.9</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="G8" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="I8" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="J8" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="K8">
         <v>10128</v>
@@ -3866,22 +3929,22 @@
         <v>43.4</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="G9" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="I9" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="J9" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="K9">
         <v>18597</v>
@@ -3949,22 +4012,22 @@
         <v>967.4</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="G10" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="I10" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="J10" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="K10">
         <v>32381</v>
@@ -4029,25 +4092,25 @@
         <v>113</v>
       </c>
       <c r="D11" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="G11" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="I11" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="K11">
         <v>4869</v>
@@ -4112,25 +4175,25 @@
         <v>167</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="G12" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="K12">
         <v>5191</v>
@@ -4198,22 +4261,22 @@
         <v>54.1</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="G13" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="I13" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="J13" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="K13">
         <v>4015</v>
@@ -4281,22 +4344,22 @@
         <v>192.4</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="G14" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="I14" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="J14" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="K14">
         <v>15190</v>
@@ -4364,22 +4427,22 @@
         <v>174.9</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="G15" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K15">
         <v>20858</v>
@@ -4447,22 +4510,22 @@
         <v>399.5</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="G16" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="I16" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="J16" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="K16">
         <v>15269</v>
@@ -4530,22 +4593,22 @@
         <v>100.1</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="G17" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="I17" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="J17" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="K17">
         <v>8162</v>
@@ -4613,22 +4676,22 @@
         <v>79.400000000000006</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="G18" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="I18" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="J18" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="K18">
         <v>12417</v>
@@ -4696,22 +4759,22 @@
         <v>139.1</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="G19" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="I19" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="J19" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="K19">
         <v>7966</v>
@@ -4779,19 +4842,19 @@
         <v>142.6</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="G20" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="I20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J20" s="8">
         <v>18070</v>
@@ -4862,22 +4925,22 @@
         <v>76.900000000000006</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="G21" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="I21" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="J21" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="K21">
         <v>5790</v>
@@ -4933,7 +4996,7 @@
     </row>
     <row r="22" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -4945,16 +5008,16 @@
         <v>326.60000000000002</v>
       </c>
       <c r="E22" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="F22" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="G22" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="I22" s="8">
         <v>45717</v>
@@ -5016,7 +5079,7 @@
     </row>
     <row r="23" spans="1:27" ht="192" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
@@ -5028,22 +5091,22 @@
         <v>53.8</v>
       </c>
       <c r="E23" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="F23" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="G23" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="I23" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="J23" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="K23">
         <v>3628</v>
@@ -5099,7 +5162,7 @@
     </row>
     <row r="24" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="B24" t="s">
         <v>16</v>
@@ -5111,22 +5174,22 @@
         <v>94.2</v>
       </c>
       <c r="E24" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="F24" t="s">
+        <v>236</v>
+      </c>
+      <c r="G24" t="s">
         <v>251</v>
       </c>
-      <c r="G24" t="s">
-        <v>266</v>
-      </c>
       <c r="H24" s="2" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="I24" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="K24">
         <v>4493</v>
@@ -5182,7 +5245,7 @@
     </row>
     <row r="25" spans="1:27" ht="395" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B25" t="s">
         <v>14</v>
@@ -5194,22 +5257,22 @@
         <v>169.2</v>
       </c>
       <c r="E25" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="F25" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="G25" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="I25" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="J25" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="K25">
         <v>8087</v>
@@ -5265,7 +5328,7 @@
     </row>
     <row r="26" spans="1:27" ht="304" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
@@ -5277,22 +5340,22 @@
         <v>193.4</v>
       </c>
       <c r="E26" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="F26" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="G26" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="I26" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="J26" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="K26">
         <v>7600</v>
@@ -5348,7 +5411,7 @@
     </row>
     <row r="27" spans="1:27" ht="240" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
@@ -5360,22 +5423,22 @@
         <v>294.8</v>
       </c>
       <c r="E27" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="F27" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="G27" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="I27" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="J27" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="K27">
         <v>7177</v>
@@ -5431,7 +5494,7 @@
     </row>
     <row r="28" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -5443,22 +5506,22 @@
         <v>264.2</v>
       </c>
       <c r="E28" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="F28" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="G28" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="I28" s="8">
         <v>46020</v>
       </c>
       <c r="J28" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="K28">
         <v>12438</v>
@@ -5514,7 +5577,7 @@
     </row>
     <row r="29" spans="1:27" ht="112" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B29" t="s">
         <v>14</v>
@@ -5526,19 +5589,19 @@
         <v>205.2</v>
       </c>
       <c r="E29" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="F29" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="G29" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="I29" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="J29" s="8">
         <v>18100</v>
@@ -5597,7 +5660,7 @@
     </row>
     <row r="30" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="B30" t="s">
         <v>16</v>
@@ -5609,16 +5672,16 @@
         <v>50.2</v>
       </c>
       <c r="E30" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="F30" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="G30" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="I30" s="8">
         <v>45070</v>
@@ -5680,7 +5743,7 @@
     </row>
     <row r="31" spans="1:27" ht="256" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -5692,22 +5755,22 @@
         <v>64.7</v>
       </c>
       <c r="E31" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="F31" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="G31" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="I31" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="J31" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="K31">
         <v>2278</v>
@@ -5763,7 +5826,7 @@
     </row>
     <row r="32" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -5775,22 +5838,22 @@
         <v>48.9</v>
       </c>
       <c r="E32" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="F32" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="G32" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="J32" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="K32">
         <v>3039</v>
@@ -5846,7 +5909,7 @@
     </row>
     <row r="33" spans="1:27" ht="272" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="B33" t="s">
         <v>15</v>
@@ -5858,16 +5921,16 @@
         <v>6.5</v>
       </c>
       <c r="E33" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="F33" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="G33" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="I33" s="8">
         <v>44040</v>
@@ -5929,7 +5992,7 @@
     </row>
     <row r="34" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="B34" t="s">
         <v>19</v>
@@ -5941,22 +6004,22 @@
         <v>51.2</v>
       </c>
       <c r="E34" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="F34" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="G34" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="J34" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="K34">
         <v>1476</v>
@@ -6012,7 +6075,7 @@
     </row>
     <row r="35" spans="1:27" ht="176" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
@@ -6024,22 +6087,22 @@
         <v>58.5</v>
       </c>
       <c r="E35" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="F35" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="G35" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="J35" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="K35">
         <v>3127</v>
@@ -6095,7 +6158,7 @@
     </row>
     <row r="36" spans="1:27" ht="335" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
@@ -6107,22 +6170,22 @@
         <v>538.1</v>
       </c>
       <c r="E36" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="F36" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="G36" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="J36" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="K36">
         <v>12927</v>
@@ -6178,7 +6241,7 @@
     </row>
     <row r="37" spans="1:27" ht="256" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
@@ -6190,22 +6253,22 @@
         <v>230.9</v>
       </c>
       <c r="E37" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="F37" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="G37" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="J37" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="K37">
         <v>6929</v>
@@ -6261,7 +6324,7 @@
     </row>
     <row r="38" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="B38" t="s">
         <v>17</v>
@@ -6273,19 +6336,19 @@
         <v>37.799999999999997</v>
       </c>
       <c r="E38" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="F38" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="G38" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="J38" s="8">
         <v>17020</v>
@@ -6344,7 +6407,7 @@
     </row>
     <row r="39" spans="1:27" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -6356,22 +6419,22 @@
         <v>167.8</v>
       </c>
       <c r="E39" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="F39" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="G39" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="J39" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="K39">
         <v>5464</v>
@@ -6423,6 +6486,255 @@
       </c>
       <c r="AA39">
         <v>11503</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" ht="304" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>336</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="5">
+        <v>449</v>
+      </c>
+      <c r="D40">
+        <v>53.8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>337</v>
+      </c>
+      <c r="F40" t="s">
+        <v>222</v>
+      </c>
+      <c r="G40" t="s">
+        <v>217</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="J40" t="s">
+        <v>340</v>
+      </c>
+      <c r="K40">
+        <v>3120</v>
+      </c>
+      <c r="L40">
+        <v>3334</v>
+      </c>
+      <c r="M40">
+        <v>3634</v>
+      </c>
+      <c r="N40">
+        <v>4280</v>
+      </c>
+      <c r="O40">
+        <v>4660</v>
+      </c>
+      <c r="P40">
+        <v>5058</v>
+      </c>
+      <c r="Q40">
+        <v>5404</v>
+      </c>
+      <c r="R40">
+        <v>5810</v>
+      </c>
+      <c r="S40">
+        <v>6284</v>
+      </c>
+      <c r="T40">
+        <v>6540</v>
+      </c>
+      <c r="U40">
+        <v>7484</v>
+      </c>
+      <c r="V40">
+        <v>9101</v>
+      </c>
+      <c r="W40">
+        <v>12773</v>
+      </c>
+      <c r="X40">
+        <v>20720</v>
+      </c>
+      <c r="Y40">
+        <v>23125</v>
+      </c>
+      <c r="Z40">
+        <v>25223</v>
+      </c>
+      <c r="AA40">
+        <v>24133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" ht="176" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>341</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="5">
+        <v>53</v>
+      </c>
+      <c r="D41">
+        <v>266.2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>342</v>
+      </c>
+      <c r="F41" t="s">
+        <v>237</v>
+      </c>
+      <c r="G41" t="s">
+        <v>201</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="J41" t="s">
+        <v>345</v>
+      </c>
+      <c r="K41">
+        <v>8153</v>
+      </c>
+      <c r="L41">
+        <v>9255</v>
+      </c>
+      <c r="M41">
+        <v>10038</v>
+      </c>
+      <c r="N41">
+        <v>11212</v>
+      </c>
+      <c r="O41">
+        <v>12788</v>
+      </c>
+      <c r="P41">
+        <v>13791</v>
+      </c>
+      <c r="Q41">
+        <v>14283</v>
+      </c>
+      <c r="R41">
+        <v>15344</v>
+      </c>
+      <c r="S41">
+        <v>15122</v>
+      </c>
+      <c r="T41">
+        <v>15094</v>
+      </c>
+      <c r="U41">
+        <v>17637</v>
+      </c>
+      <c r="V41">
+        <v>15880</v>
+      </c>
+      <c r="W41">
+        <v>15056</v>
+      </c>
+      <c r="X41">
+        <v>15630</v>
+      </c>
+      <c r="Y41">
+        <v>15472</v>
+      </c>
+      <c r="Z41">
+        <v>14936</v>
+      </c>
+      <c r="AA41">
+        <v>14139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" ht="350" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>346</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="5">
+        <v>53</v>
+      </c>
+      <c r="D42">
+        <v>379.3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>347</v>
+      </c>
+      <c r="F42" t="s">
+        <v>223</v>
+      </c>
+      <c r="G42" t="s">
+        <v>120</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="J42" t="s">
+        <v>350</v>
+      </c>
+      <c r="K42">
+        <v>18448</v>
+      </c>
+      <c r="L42">
+        <v>20403</v>
+      </c>
+      <c r="M42">
+        <v>21091</v>
+      </c>
+      <c r="N42">
+        <v>24958</v>
+      </c>
+      <c r="O42">
+        <v>27873</v>
+      </c>
+      <c r="P42">
+        <v>29633</v>
+      </c>
+      <c r="Q42">
+        <v>28383</v>
+      </c>
+      <c r="R42">
+        <v>29808</v>
+      </c>
+      <c r="S42">
+        <v>24293</v>
+      </c>
+      <c r="T42">
+        <v>25070</v>
+      </c>
+      <c r="U42">
+        <v>27465</v>
+      </c>
+      <c r="V42">
+        <v>30545</v>
+      </c>
+      <c r="W42">
+        <v>33124</v>
+      </c>
+      <c r="X42">
+        <v>35151</v>
+      </c>
+      <c r="Y42">
+        <v>23413</v>
+      </c>
+      <c r="Z42">
+        <v>24671</v>
+      </c>
+      <c r="AA42">
+        <v>19950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>